<commit_message>
qCRMWeb examples: How to display tabbed form
</commit_message>
<xml_diff>
--- a/Vitae/Library/Resources/SharedResource.xlsx
+++ b/Vitae/Library/Resources/SharedResource.xlsx
@@ -1,22 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22325"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\Vitae\Library\Resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\Various\Vitae\Library\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73F342F1-708A-4CE6-90A7-8E9BB5894835}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="30220" windowHeight="19620" xr2:uid="{27DE1AD4-C3A1-49ED-BBBC-B59C1C3E1A78}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="30225" windowHeight="19620" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="en" sheetId="3" r:id="rId1"/>
     <sheet name="de" sheetId="4" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">de!$A$1:$B$20</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">en!$A$1:$B$20</definedName>
+  </definedNames>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -34,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="54">
   <si>
     <t>City</t>
   </si>
@@ -84,15 +87,9 @@
     <t>StreetNo</t>
   </si>
   <si>
-    <t>Street number</t>
-  </si>
-  <si>
     <t>StreetNoRequired</t>
   </si>
   <si>
-    <t>A street number is required</t>
-  </si>
-  <si>
     <t>StreetRequired</t>
   </si>
   <si>
@@ -162,15 +159,9 @@
     <t>CountryCode</t>
   </si>
   <si>
-    <t>Country code</t>
-  </si>
-  <si>
     <t>CountryName</t>
   </si>
   <si>
-    <t>Country name</t>
-  </si>
-  <si>
     <t>CountryRequired</t>
   </si>
   <si>
@@ -180,16 +171,40 @@
     <t>Land</t>
   </si>
   <si>
-    <t>Ländercode</t>
-  </si>
-  <si>
     <t>Ein Land wird benötigt</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Code</t>
+  </si>
+  <si>
+    <t>Value</t>
+  </si>
+  <si>
+    <t>Number</t>
+  </si>
+  <si>
+    <t>A number is required</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>EmailRequired</t>
+  </si>
+  <si>
+    <t>Eine Email wird benötigt</t>
+  </si>
+  <si>
+    <t>An email address is required</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -226,7 +241,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -537,343 +552,401 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A856D1D0-AC13-4482-816F-C6D9365F83AB}">
-  <dimension ref="A1:B19"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:B19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="31.6328125" customWidth="1"/>
-    <col min="2" max="2" width="57.54296875" customWidth="1"/>
+    <col min="1" max="1" width="31.5703125" customWidth="1"/>
+    <col min="2" max="2" width="57.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A2" s="1" t="s">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B3" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A3" s="1" t="s">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B7" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A4" s="1" t="s">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B8" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A5" s="1" t="s">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B9" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A6" s="1" t="s">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B10" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A7" s="1" t="s">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B11" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A8" s="1" t="s">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B12" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A9" s="1" t="s">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="B13" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A10" s="1" t="s">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="B14" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A11" s="1" t="s">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="B15" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A12" s="1" t="s">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="B16" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A13" s="1" t="s">
+      <c r="B17" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B13" s="1" t="s">
+      <c r="B18" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A14" s="1" t="s">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="B19" s="1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A15" s="1" t="s">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B15" s="1" t="s">
+      <c r="B20" s="1" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A16" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A17" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A18" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A19" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>46</v>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>53</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:B20">
+    <sortState ref="A2:B20">
+      <sortCondition ref="A1:A20"/>
+    </sortState>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{84BDAEB0-85CE-42DD-A976-DD4575ED3F45}">
-  <dimension ref="A1:B19"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B19" sqref="A1:B19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="31.6328125" customWidth="1"/>
-    <col min="2" max="2" width="57.54296875" customWidth="1"/>
+    <col min="1" max="1" width="31.5703125" customWidth="1"/>
+    <col min="2" max="2" width="57.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B2" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B7" s="1" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="1" t="s">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B8" s="1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A3" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" s="1" t="s">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9" s="1" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A4" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" s="1" t="s">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B10" s="1" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A5" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5" s="1" t="s">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11" s="1" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A6" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B6" s="1" t="s">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B12" s="1" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A7" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B7" s="1" t="s">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B13" s="1" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A8" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B8" s="1" t="s">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B14" s="1" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A9" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B9" s="1" t="s">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B15" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A10" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B10" s="1" t="s">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B16" s="1" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A11" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B11" s="1" t="s">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B17" s="1" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A12" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B12" s="1" t="s">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B18" s="1" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A13" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B13" s="1" t="s">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B19" s="1" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A14" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B14" s="1" t="s">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B20" s="1" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A15" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A16" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A17" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A18" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A19" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>49</v>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>52</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:B20">
+    <sortState ref="A2:B20">
+      <sortCondition ref="A1:A20"/>
+    </sortState>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
New scss from resumee
</commit_message>
<xml_diff>
--- a/Vitae/Library/Resources/SharedResource.xlsx
+++ b/Vitae/Library/Resources/SharedResource.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22325"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\Various\Vitae\Library\Resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\Vitae\Library\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CD251A3-2025-4256-A2CA-3A42D04A6E81}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="30225" windowHeight="19620" activeTab="1"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="30220" windowHeight="19620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="en" sheetId="3" r:id="rId1"/>
@@ -24,20 +25,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="56">
   <si>
     <t>City</t>
   </si>
@@ -199,12 +192,18 @@
   </si>
   <si>
     <t>An email address is required</t>
+  </si>
+  <si>
+    <t>Select</t>
+  </si>
+  <si>
+    <t>Auswählen</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -241,7 +240,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -552,20 +551,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B22"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:B23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A29" sqref="A29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="31.5703125" customWidth="1"/>
-    <col min="2" max="2" width="57.5703125" customWidth="1"/>
+    <col min="1" max="1" width="31.54296875" customWidth="1"/>
+    <col min="2" max="2" width="57.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>45</v>
       </c>
@@ -573,7 +572,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -581,7 +580,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -589,7 +588,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>39</v>
       </c>
@@ -597,7 +596,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>40</v>
       </c>
@@ -605,7 +604,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>41</v>
       </c>
@@ -613,7 +612,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
         <v>3</v>
       </c>
@@ -621,7 +620,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
         <v>4</v>
       </c>
@@ -629,7 +628,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
         <v>6</v>
       </c>
@@ -637,7 +636,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
         <v>7</v>
       </c>
@@ -645,7 +644,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
         <v>9</v>
       </c>
@@ -653,7 +652,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
         <v>10</v>
       </c>
@@ -661,7 +660,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
         <v>11</v>
       </c>
@@ -669,7 +668,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
         <v>12</v>
       </c>
@@ -677,7 +676,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
         <v>14</v>
       </c>
@@ -685,7 +684,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
         <v>15</v>
       </c>
@@ -693,7 +692,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
         <v>16</v>
       </c>
@@ -701,7 +700,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A18" s="1" t="s">
         <v>17</v>
       </c>
@@ -709,7 +708,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A19" s="1" t="s">
         <v>19</v>
       </c>
@@ -717,7 +716,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A20" s="1" t="s">
         <v>21</v>
       </c>
@@ -725,7 +724,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A21" s="1" t="s">
         <v>50</v>
       </c>
@@ -733,7 +732,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A22" s="1" t="s">
         <v>51</v>
       </c>
@@ -741,9 +740,17 @@
         <v>53</v>
       </c>
     </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A23" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:B20">
-    <sortState ref="A2:B20">
+  <autoFilter ref="A1:B20" xr:uid="{00000000-0009-0000-0000-000000000000}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B20">
       <sortCondition ref="A1:A20"/>
     </sortState>
   </autoFilter>
@@ -752,20 +759,20 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B22"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:B23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="31.5703125" customWidth="1"/>
-    <col min="2" max="2" width="57.5703125" customWidth="1"/>
+    <col min="1" max="1" width="31.54296875" customWidth="1"/>
+    <col min="2" max="2" width="57.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>45</v>
       </c>
@@ -773,7 +780,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -781,7 +788,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -789,7 +796,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>39</v>
       </c>
@@ -797,7 +804,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>40</v>
       </c>
@@ -805,7 +812,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>41</v>
       </c>
@@ -813,7 +820,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
         <v>3</v>
       </c>
@@ -821,7 +828,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
         <v>4</v>
       </c>
@@ -829,7 +836,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
         <v>6</v>
       </c>
@@ -837,7 +844,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
         <v>7</v>
       </c>
@@ -845,7 +852,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
         <v>9</v>
       </c>
@@ -853,7 +860,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
         <v>10</v>
       </c>
@@ -861,7 +868,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
         <v>11</v>
       </c>
@@ -869,7 +876,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
         <v>12</v>
       </c>
@@ -877,7 +884,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
         <v>14</v>
       </c>
@@ -885,7 +892,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
         <v>15</v>
       </c>
@@ -893,7 +900,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
         <v>16</v>
       </c>
@@ -901,7 +908,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A18" s="1" t="s">
         <v>17</v>
       </c>
@@ -909,7 +916,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A19" s="1" t="s">
         <v>19</v>
       </c>
@@ -917,7 +924,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A20" s="1" t="s">
         <v>21</v>
       </c>
@@ -925,7 +932,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A21" s="1" t="s">
         <v>50</v>
       </c>
@@ -933,7 +940,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A22" s="1" t="s">
         <v>51</v>
       </c>
@@ -941,9 +948,17 @@
         <v>52</v>
       </c>
     </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A23" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:B20">
-    <sortState ref="A2:B20">
+  <autoFilter ref="A1:B20" xr:uid="{00000000-0009-0000-0000-000001000000}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B20">
       <sortCondition ref="A1:A20"/>
     </sortState>
   </autoFilter>

</xml_diff>

<commit_message>
Working extra client side validation
</commit_message>
<xml_diff>
--- a/Vitae/Library/Resources/SharedResource.xlsx
+++ b/Vitae/Library/Resources/SharedResource.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="136">
   <si>
     <t>City</t>
   </si>
@@ -425,6 +425,18 @@
   </si>
   <si>
     <t>Ende</t>
+  </si>
+  <si>
+    <t>Add</t>
+  </si>
+  <si>
+    <t>Hinzufügen</t>
+  </si>
+  <si>
+    <t>Nationality</t>
+  </si>
+  <si>
+    <t>Nationalität</t>
   </si>
 </sst>
 </file>
@@ -802,10 +814,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B57"/>
+  <dimension ref="A1:B59"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:B57"/>
+      <selection activeCell="B59" sqref="B59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1268,6 +1280,22 @@
       </c>
       <c r="B57" s="1" t="s">
         <v>9</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A58" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="B58" s="1" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>134</v>
+      </c>
+      <c r="B59" t="s">
+        <v>134</v>
       </c>
     </row>
   </sheetData>
@@ -1283,10 +1311,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B57"/>
+  <dimension ref="A1:B59"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B58" sqref="B58"/>
+    <sheetView topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="B59" sqref="B59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1751,6 +1779,22 @@
         <v>41</v>
       </c>
     </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A58" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="B58" s="1" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>134</v>
+      </c>
+      <c r="B59" s="1" t="s">
+        <v>135</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:B24">
     <sortState ref="A2:B57">

</xml_diff>

<commit_message>
Working dynamic AJAX form!
</commit_message>
<xml_diff>
--- a/Vitae/Library/Resources/SharedResource.xlsx
+++ b/Vitae/Library/Resources/SharedResource.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22325"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\Various\Vitae\Library\Resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\Vitae\Library\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6411D96B-A7D2-4B2E-8321-1D4C665B2B01}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="30225" windowHeight="19620"/>
+    <workbookView xWindow="7500" yWindow="540" windowWidth="22500" windowHeight="14260" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="en" sheetId="3" r:id="rId1"/>
@@ -29,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="138">
   <si>
     <t>City</t>
   </si>
@@ -437,12 +438,18 @@
   </si>
   <si>
     <t>Nationalität</t>
+  </si>
+  <si>
+    <t>Remove</t>
+  </si>
+  <si>
+    <t>Entfernen</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -502,7 +509,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -813,20 +820,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B59"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:B60"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="B59" sqref="B59"/>
+      <selection activeCell="A61" sqref="A61"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="31.5703125" customWidth="1"/>
-    <col min="2" max="2" width="57.5703125" customWidth="1"/>
+    <col min="1" max="1" width="31.54296875" customWidth="1"/>
+    <col min="2" max="2" width="57.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>20</v>
       </c>
@@ -834,7 +841,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>51</v>
       </c>
@@ -842,7 +849,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>67</v>
       </c>
@@ -850,7 +857,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>44</v>
       </c>
@@ -858,7 +865,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>53</v>
       </c>
@@ -866,7 +873,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>95</v>
       </c>
@@ -874,7 +881,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
         <v>62</v>
       </c>
@@ -882,7 +889,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
         <v>63</v>
       </c>
@@ -890,7 +897,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
         <v>0</v>
       </c>
@@ -898,7 +905,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
         <v>0</v>
       </c>
@@ -906,7 +913,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
         <v>93</v>
       </c>
@@ -914,7 +921,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
         <v>17</v>
       </c>
@@ -922,7 +929,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
         <v>18</v>
       </c>
@@ -930,7 +937,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
         <v>101</v>
       </c>
@@ -938,7 +945,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
         <v>64</v>
       </c>
@@ -946,7 +953,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
         <v>109</v>
       </c>
@@ -954,7 +961,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
         <v>24</v>
       </c>
@@ -962,7 +969,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A18" s="1" t="s">
         <v>118</v>
       </c>
@@ -970,7 +977,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A19" s="1" t="s">
         <v>71</v>
       </c>
@@ -978,7 +985,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A20" s="1" t="s">
         <v>70</v>
       </c>
@@ -986,7 +993,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A21" s="1" t="s">
         <v>1</v>
       </c>
@@ -994,7 +1001,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A22" s="1" t="s">
         <v>72</v>
       </c>
@@ -1002,7 +1009,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A23" s="1" t="s">
         <v>36</v>
       </c>
@@ -1010,7 +1017,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A24" s="1" t="s">
         <v>116</v>
       </c>
@@ -1018,7 +1025,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A25" s="1" t="s">
         <v>34</v>
       </c>
@@ -1026,7 +1033,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A26" s="1" t="s">
         <v>2</v>
       </c>
@@ -1034,7 +1041,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A27" s="1" t="s">
         <v>3</v>
       </c>
@@ -1042,7 +1049,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>27</v>
       </c>
@@ -1050,7 +1057,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A29" s="1" t="s">
         <v>43</v>
       </c>
@@ -1058,7 +1065,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A30" s="1" t="s">
         <v>40</v>
       </c>
@@ -1066,7 +1073,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A31" s="1" t="s">
         <v>99</v>
       </c>
@@ -1074,7 +1081,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A32" s="1" t="s">
         <v>96</v>
       </c>
@@ -1082,7 +1089,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A33" s="1" t="s">
         <v>66</v>
       </c>
@@ -1090,7 +1097,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A34" s="1" t="s">
         <v>69</v>
       </c>
@@ -1098,7 +1105,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A35" s="1" t="s">
         <v>46</v>
       </c>
@@ -1106,7 +1113,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>29</v>
       </c>
@@ -1114,7 +1121,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A37" s="1" t="s">
         <v>104</v>
       </c>
@@ -1122,7 +1129,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A38" s="1" t="s">
         <v>81</v>
       </c>
@@ -1130,7 +1137,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A39" s="1" t="s">
         <v>78</v>
       </c>
@@ -1138,7 +1145,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A40" s="1" t="s">
         <v>55</v>
       </c>
@@ -1146,7 +1153,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A41" s="1" t="s">
         <v>48</v>
       </c>
@@ -1154,7 +1161,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A42" s="1" t="s">
         <v>58</v>
       </c>
@@ -1162,7 +1169,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A43" s="1" t="s">
         <v>115</v>
       </c>
@@ -1170,7 +1177,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A44" s="1" t="s">
         <v>4</v>
       </c>
@@ -1178,7 +1185,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A45" s="1" t="s">
         <v>112</v>
       </c>
@@ -1186,7 +1193,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A46" s="1" t="s">
         <v>111</v>
       </c>
@@ -1194,7 +1201,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A47" s="1" t="s">
         <v>25</v>
       </c>
@@ -1202,7 +1209,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
         <v>28</v>
       </c>
@@ -1210,7 +1217,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A49" s="1" t="s">
         <v>117</v>
       </c>
@@ -1218,7 +1225,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A50" s="1" t="s">
         <v>5</v>
       </c>
@@ -1226,7 +1233,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A51" s="1" t="s">
         <v>6</v>
       </c>
@@ -1234,7 +1241,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A52" s="1" t="s">
         <v>7</v>
       </c>
@@ -1242,7 +1249,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A53" s="1" t="s">
         <v>114</v>
       </c>
@@ -1250,7 +1257,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A54" s="1" t="s">
         <v>113</v>
       </c>
@@ -1258,7 +1265,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A55" s="1" t="s">
         <v>91</v>
       </c>
@@ -1266,7 +1273,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A56" s="1" t="s">
         <v>97</v>
       </c>
@@ -1274,7 +1281,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A57" s="1" t="s">
         <v>8</v>
       </c>
@@ -1282,7 +1289,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A58" s="1" t="s">
         <v>132</v>
       </c>
@@ -1290,7 +1297,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
         <v>134</v>
       </c>
@@ -1298,9 +1305,17 @@
         <v>134</v>
       </c>
     </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A60" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="B60" s="1" t="s">
+        <v>136</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:B24">
-    <sortState ref="A2:B57">
+  <autoFilter ref="A1:B24" xr:uid="{00000000-0009-0000-0000-000000000000}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B57">
       <sortCondition ref="A1:A24"/>
     </sortState>
   </autoFilter>
@@ -1310,20 +1325,20 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B59"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:B60"/>
   <sheetViews>
     <sheetView topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="B59" sqref="B59"/>
+      <selection activeCell="B60" sqref="B60"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="31.5703125" customWidth="1"/>
-    <col min="2" max="2" width="57.5703125" customWidth="1"/>
+    <col min="1" max="1" width="31.54296875" customWidth="1"/>
+    <col min="2" max="2" width="57.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>20</v>
       </c>
@@ -1331,7 +1346,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>51</v>
       </c>
@@ -1339,7 +1354,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>67</v>
       </c>
@@ -1347,7 +1362,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>44</v>
       </c>
@@ -1355,7 +1370,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>53</v>
       </c>
@@ -1363,7 +1378,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>95</v>
       </c>
@@ -1371,7 +1386,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
         <v>62</v>
       </c>
@@ -1379,7 +1394,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
         <v>63</v>
       </c>
@@ -1387,7 +1402,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
         <v>0</v>
       </c>
@@ -1395,7 +1410,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
         <v>0</v>
       </c>
@@ -1403,7 +1418,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
         <v>93</v>
       </c>
@@ -1411,7 +1426,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
         <v>17</v>
       </c>
@@ -1419,7 +1434,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
         <v>18</v>
       </c>
@@ -1427,7 +1442,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
         <v>101</v>
       </c>
@@ -1435,7 +1450,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
         <v>64</v>
       </c>
@@ -1443,7 +1458,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
         <v>109</v>
       </c>
@@ -1451,7 +1466,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
         <v>24</v>
       </c>
@@ -1459,7 +1474,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A18" s="1" t="s">
         <v>118</v>
       </c>
@@ -1467,7 +1482,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A19" s="1" t="s">
         <v>71</v>
       </c>
@@ -1475,7 +1490,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A20" s="1" t="s">
         <v>70</v>
       </c>
@@ -1483,7 +1498,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A21" s="1" t="s">
         <v>1</v>
       </c>
@@ -1491,7 +1506,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A22" s="1" t="s">
         <v>72</v>
       </c>
@@ -1499,7 +1514,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A23" s="1" t="s">
         <v>36</v>
       </c>
@@ -1507,7 +1522,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A24" s="1" t="s">
         <v>116</v>
       </c>
@@ -1515,7 +1530,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A25" s="1" t="s">
         <v>34</v>
       </c>
@@ -1523,7 +1538,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A26" s="1" t="s">
         <v>2</v>
       </c>
@@ -1531,7 +1546,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A27" s="1" t="s">
         <v>3</v>
       </c>
@@ -1539,7 +1554,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>27</v>
       </c>
@@ -1547,7 +1562,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A29" s="1" t="s">
         <v>43</v>
       </c>
@@ -1555,7 +1570,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A30" s="1" t="s">
         <v>40</v>
       </c>
@@ -1563,7 +1578,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A31" s="1" t="s">
         <v>99</v>
       </c>
@@ -1571,7 +1586,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A32" s="1" t="s">
         <v>96</v>
       </c>
@@ -1579,7 +1594,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A33" s="1" t="s">
         <v>66</v>
       </c>
@@ -1587,7 +1602,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A34" s="1" t="s">
         <v>69</v>
       </c>
@@ -1595,7 +1610,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A35" s="1" t="s">
         <v>46</v>
       </c>
@@ -1603,7 +1618,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>29</v>
       </c>
@@ -1611,7 +1626,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A37" s="1" t="s">
         <v>104</v>
       </c>
@@ -1619,7 +1634,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A38" s="1" t="s">
         <v>81</v>
       </c>
@@ -1627,7 +1642,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A39" s="1" t="s">
         <v>78</v>
       </c>
@@ -1635,7 +1650,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A40" s="1" t="s">
         <v>55</v>
       </c>
@@ -1643,7 +1658,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A41" s="1" t="s">
         <v>48</v>
       </c>
@@ -1651,7 +1666,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A42" s="1" t="s">
         <v>58</v>
       </c>
@@ -1659,7 +1674,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A43" s="1" t="s">
         <v>115</v>
       </c>
@@ -1667,7 +1682,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A44" s="1" t="s">
         <v>4</v>
       </c>
@@ -1675,7 +1690,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A45" s="1" t="s">
         <v>112</v>
       </c>
@@ -1683,7 +1698,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A46" s="1" t="s">
         <v>111</v>
       </c>
@@ -1691,7 +1706,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A47" s="1" t="s">
         <v>25</v>
       </c>
@@ -1699,7 +1714,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
         <v>28</v>
       </c>
@@ -1707,7 +1722,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A49" s="1" t="s">
         <v>117</v>
       </c>
@@ -1715,7 +1730,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A50" s="1" t="s">
         <v>5</v>
       </c>
@@ -1723,7 +1738,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A51" s="1" t="s">
         <v>6</v>
       </c>
@@ -1731,7 +1746,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A52" s="1" t="s">
         <v>7</v>
       </c>
@@ -1739,7 +1754,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A53" s="1" t="s">
         <v>114</v>
       </c>
@@ -1747,7 +1762,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A54" s="1" t="s">
         <v>113</v>
       </c>
@@ -1755,7 +1770,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A55" s="1" t="s">
         <v>91</v>
       </c>
@@ -1763,7 +1778,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A56" s="1" t="s">
         <v>97</v>
       </c>
@@ -1771,7 +1786,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A57" s="1" t="s">
         <v>8</v>
       </c>
@@ -1779,7 +1794,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A58" s="1" t="s">
         <v>132</v>
       </c>
@@ -1787,7 +1802,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
         <v>134</v>
       </c>
@@ -1795,9 +1810,17 @@
         <v>135</v>
       </c>
     </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A60" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="B60" s="1" t="s">
+        <v>137</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:B24">
-    <sortState ref="A2:B57">
+  <autoFilter ref="A1:B24" xr:uid="{00000000-0009-0000-0000-000001000000}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B57">
       <sortCondition ref="A1:A24"/>
     </sortState>
   </autoFilter>

</xml_diff>

<commit_message>
New design implemented (qCRM Web template)
</commit_message>
<xml_diff>
--- a/Vitae/Library/Resources/SharedResource.xlsx
+++ b/Vitae/Library/Resources/SharedResource.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22325"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\Vitae\Library\Resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\Various\Vitae\Library\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6411D96B-A7D2-4B2E-8321-1D4C665B2B01}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7500" yWindow="540" windowWidth="22500" windowHeight="14260" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7500" yWindow="540" windowWidth="22500" windowHeight="14265" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="en" sheetId="3" r:id="rId1"/>
@@ -30,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="159">
   <si>
     <t>City</t>
   </si>
@@ -444,12 +443,75 @@
   </si>
   <si>
     <t>Entfernen</t>
+  </si>
+  <si>
+    <t>PersonalData</t>
+  </si>
+  <si>
+    <t>Personal data</t>
+  </si>
+  <si>
+    <t>PersonalDetails</t>
+  </si>
+  <si>
+    <t>Personal details</t>
+  </si>
+  <si>
+    <t>Experience</t>
+  </si>
+  <si>
+    <t>Languages</t>
+  </si>
+  <si>
+    <t>Interests</t>
+  </si>
+  <si>
+    <t>CurriculumVitae</t>
+  </si>
+  <si>
+    <t>Curriculum Vitae</t>
+  </si>
+  <si>
+    <t>Persönliche Angaben</t>
+  </si>
+  <si>
+    <t>Erfahrung</t>
+  </si>
+  <si>
+    <t>Sprachen</t>
+  </si>
+  <si>
+    <t>Interessen</t>
+  </si>
+  <si>
+    <t>MyVitae</t>
+  </si>
+  <si>
+    <t>Mein Vitae</t>
+  </si>
+  <si>
+    <t>My Vitae</t>
+  </si>
+  <si>
+    <t>Awards</t>
+  </si>
+  <si>
+    <t>Errungenschaften</t>
+  </si>
+  <si>
+    <t>LoggedInAs</t>
+  </si>
+  <si>
+    <t>Logged in as</t>
+  </si>
+  <si>
+    <t>Eingeloggt als</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -509,7 +571,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -820,20 +882,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B60"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="A61" sqref="A61"/>
+    <sheetView topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="B69" sqref="B69"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="31.54296875" customWidth="1"/>
-    <col min="2" max="2" width="57.54296875" customWidth="1"/>
+    <col min="1" max="1" width="31.5703125" customWidth="1"/>
+    <col min="2" max="2" width="57.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>20</v>
       </c>
@@ -841,7 +903,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>51</v>
       </c>
@@ -849,63 +911,63 @@
         <v>51</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B4" s="1" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A4" s="1" t="s">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B5" s="1" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A5" s="1" t="s">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B6" s="1" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A6" s="1" t="s">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B7" s="1" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A7" s="1" t="s">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B8" s="1" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A8" s="1" t="s">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B9" s="1" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A9" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>0</v>
       </c>
@@ -913,409 +975,481 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="B12" s="1" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A12" s="1" t="s">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="B13" s="1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A13" s="1" t="s">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B13" s="1" t="s">
+      <c r="B14" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A14" s="1" t="s">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>145</v>
+      </c>
+      <c r="B15" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="B16" s="1" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A15" s="1" t="s">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B17" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A16" s="1" t="s">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="B16" s="1" t="s">
+      <c r="B18" s="1" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A17" s="1" t="s">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B17" s="1" t="s">
+      <c r="B19" s="1" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A18" s="1" t="s">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="B18" s="1" t="s">
+      <c r="B20" s="1" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A19" s="1" t="s">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>142</v>
+      </c>
+      <c r="B21" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B22" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A20" s="1" t="s">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B23" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A21" s="1" t="s">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B21" s="1" t="s">
+      <c r="B24" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A22" s="1" t="s">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B25" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A23" s="1" t="s">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="B23" s="1" t="s">
+      <c r="B26" s="1" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A24" s="1" t="s">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="B24" s="1" t="s">
+      <c r="B27" s="1" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A25" s="1" t="s">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>144</v>
+      </c>
+      <c r="B28" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B25" s="1" t="s">
+      <c r="B29" s="1" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A26" s="1" t="s">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>143</v>
+      </c>
+      <c r="B30" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B26" s="1" t="s">
+      <c r="B31" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A27" s="1" t="s">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B27" s="1" t="s">
+      <c r="B32" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A28" t="s">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
         <v>27</v>
       </c>
-      <c r="B28" s="1" t="s">
+      <c r="B33" s="1" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A29" s="1" t="s">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="B29" s="1" t="s">
+      <c r="B34" s="1" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A30" s="1" t="s">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="B30" s="1" t="s">
+      <c r="B35" s="1" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A31" s="1" t="s">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>134</v>
+      </c>
+      <c r="B36" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="B31" s="1" t="s">
+      <c r="B37" s="1" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A32" s="1" t="s">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="B32" s="1" t="s">
+      <c r="B38" s="1" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A33" s="1" t="s">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="B33" s="1" t="s">
+      <c r="B39" s="1" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A34" s="1" t="s">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="B34" t="s">
+      <c r="B40" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A35" s="1" t="s">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A42" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A43" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="B35" s="1" t="s">
+      <c r="B43" s="1" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A36" t="s">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
         <v>29</v>
       </c>
-      <c r="B36" s="1" t="s">
+      <c r="B44" s="1" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A37" s="1" t="s">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A45" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="B37" s="1" t="s">
+      <c r="B45" s="1" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A38" s="1" t="s">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A46" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="B38" t="s">
+      <c r="B46" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A39" s="1" t="s">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A47" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A48" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="B39" t="s">
+      <c r="B48" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A40" s="1" t="s">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A49" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="B40" s="1" t="s">
+      <c r="B49" s="1" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A41" s="1" t="s">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A50" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="B41" s="1" t="s">
+      <c r="B50" s="1" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A42" s="1" t="s">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A51" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="B42" s="1" t="s">
+      <c r="B51" s="1" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A43" s="1" t="s">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A52" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="B43" s="1" t="s">
+      <c r="B52" s="1" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A44" s="1" t="s">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A53" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B44" s="1" t="s">
+      <c r="B53" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A45" s="1" t="s">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A54" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="B45" s="1" t="s">
+      <c r="B54" s="1" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A46" s="1" t="s">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A55" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="B46" s="3" t="s">
+      <c r="B55" s="3" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A47" s="1" t="s">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A56" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B47" s="1" t="s">
+      <c r="B56" s="1" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A48" t="s">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
         <v>28</v>
       </c>
-      <c r="B48" s="1" t="s">
+      <c r="B57" s="1" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A49" s="1" t="s">
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A58" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="B49" s="1" t="s">
+      <c r="B58" s="1" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A50" s="1" t="s">
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A59" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B50" s="1" t="s">
+      <c r="B59" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A51" s="1" t="s">
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A60" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B51" s="1" t="s">
+      <c r="B60" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A52" s="1" t="s">
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A61" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B52" s="1" t="s">
+      <c r="B61" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A53" s="1" t="s">
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A62" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="B53" s="1" t="s">
+      <c r="B62" s="1" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A54" s="1" t="s">
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A63" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="B54" s="1" t="s">
+      <c r="B63" s="1" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A55" s="1" t="s">
+    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A64" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="B55" s="1" t="s">
+      <c r="B64" s="1" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A56" s="1" t="s">
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A65" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="B56" s="1" t="s">
+      <c r="B65" s="1" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A57" s="1" t="s">
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A66" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B57" s="1" t="s">
+      <c r="B66" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A58" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="B58" s="1" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A59" t="s">
-        <v>134</v>
-      </c>
-      <c r="B59" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A60" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="B60" s="1" t="s">
-        <v>136</v>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>151</v>
+      </c>
+      <c r="B67" s="1" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A68" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="B68" s="1" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A69" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="B69" s="1" t="s">
+        <v>157</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:B24" xr:uid="{00000000-0009-0000-0000-000000000000}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B57">
+  <autoFilter ref="A1:B24">
+    <sortState ref="A2:B66">
       <sortCondition ref="A1:A24"/>
     </sortState>
   </autoFilter>
@@ -1325,20 +1459,20 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:B60"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B69"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="B60" sqref="B60"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="B69" sqref="B69"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="31.54296875" customWidth="1"/>
-    <col min="2" max="2" width="57.54296875" customWidth="1"/>
+    <col min="1" max="1" width="31.5703125" customWidth="1"/>
+    <col min="2" max="2" width="57.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>20</v>
       </c>
@@ -1346,7 +1480,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>51</v>
       </c>
@@ -1354,473 +1488,545 @@
         <v>52</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B4" s="1" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A4" s="1" t="s">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B5" s="1" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A5" s="1" t="s">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B6" s="1" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A6" s="1" t="s">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B7" s="1" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A7" s="1" t="s">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B8" s="1" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A8" s="1" t="s">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B9" s="1" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A9" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B10" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B11" s="1" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A11" s="1" t="s">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="B12" s="1" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A12" s="1" t="s">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="B13" s="1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A13" s="1" t="s">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B13" s="1" t="s">
+      <c r="B14" s="1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A14" s="1" t="s">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>145</v>
+      </c>
+      <c r="B15" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="B16" s="1" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A15" s="1" t="s">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B17" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A16" s="1" t="s">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="B16" s="1" t="s">
+      <c r="B18" s="1" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A17" s="1" t="s">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B17" s="1" t="s">
+      <c r="B19" s="1" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A18" s="1" t="s">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="B18" s="1" t="s">
+      <c r="B20" s="1" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A19" s="1" t="s">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>142</v>
+      </c>
+      <c r="B21" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B22" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A20" s="1" t="s">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B23" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A21" s="1" t="s">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B21" s="1" t="s">
+      <c r="B24" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A22" s="1" t="s">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B25" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A23" s="1" t="s">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="B23" s="1" t="s">
+      <c r="B26" s="1" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A24" s="1" t="s">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="B24" s="1" t="s">
+      <c r="B27" s="1" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A25" s="1" t="s">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>144</v>
+      </c>
+      <c r="B28" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B25" s="1" t="s">
+      <c r="B29" s="1" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A26" s="1" t="s">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>143</v>
+      </c>
+      <c r="B30" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B26" s="1" t="s">
+      <c r="B31" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A27" s="1" t="s">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B27" s="1" t="s">
+      <c r="B32" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A28" t="s">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
         <v>27</v>
       </c>
-      <c r="B28" s="1" t="s">
+      <c r="B33" s="1" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A29" s="1" t="s">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="B29" s="1" t="s">
+      <c r="B34" s="1" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A30" s="1" t="s">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="B30" s="1" t="s">
+      <c r="B35" s="1" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A31" s="1" t="s">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>134</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="B31" s="1" t="s">
+      <c r="B37" s="1" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A32" s="1" t="s">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="B32" s="1" t="s">
+      <c r="B38" s="1" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A33" s="1" t="s">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="B33" s="1" t="s">
+      <c r="B39" s="1" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A34" s="1" t="s">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="B34" t="s">
+      <c r="B40" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A35" s="1" t="s">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A42" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A43" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="B35" s="1" t="s">
+      <c r="B43" s="1" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A36" t="s">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
         <v>29</v>
       </c>
-      <c r="B36" s="1" t="s">
+      <c r="B44" s="1" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A37" s="1" t="s">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A45" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="B37" s="1" t="s">
+      <c r="B45" s="1" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A38" s="1" t="s">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A46" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="B38" t="s">
+      <c r="B46" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A39" s="1" t="s">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A47" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A48" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="B39" t="s">
+      <c r="B48" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A40" s="1" t="s">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A49" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="B40" s="1" t="s">
+      <c r="B49" s="1" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A41" s="1" t="s">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A50" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="B41" s="1" t="s">
+      <c r="B50" s="1" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A42" s="1" t="s">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A51" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="B42" s="1" t="s">
+      <c r="B51" s="1" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A43" s="1" t="s">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A52" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="B43" s="1" t="s">
+      <c r="B52" s="1" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A44" s="1" t="s">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A53" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B44" s="1" t="s">
+      <c r="B53" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A45" s="1" t="s">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A54" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="B45" s="1" t="s">
+      <c r="B54" s="1" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A46" s="1" t="s">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A55" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="B46" s="1" t="s">
+      <c r="B55" s="1" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A47" s="1" t="s">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A56" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B47" s="1" t="s">
+      <c r="B56" s="1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A48" t="s">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
         <v>28</v>
       </c>
-      <c r="B48" s="1" t="s">
+      <c r="B57" s="1" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A49" s="1" t="s">
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A58" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="B49" s="1" t="s">
+      <c r="B58" s="1" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A50" s="1" t="s">
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A59" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B50" s="1" t="s">
+      <c r="B59" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A51" s="1" t="s">
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A60" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B51" s="1" t="s">
+      <c r="B60" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A52" s="1" t="s">
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A61" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B52" s="1" t="s">
+      <c r="B61" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A53" s="1" t="s">
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A62" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="B53" s="1" t="s">
+      <c r="B62" s="1" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A54" s="1" t="s">
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A63" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="B54" s="1" t="s">
+      <c r="B63" s="1" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A55" s="1" t="s">
+    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A64" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="B55" s="1" t="s">
+      <c r="B64" s="1" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A56" s="1" t="s">
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A65" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="B56" s="1" t="s">
+      <c r="B65" s="1" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A57" s="1" t="s">
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A66" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B57" s="1" t="s">
+      <c r="B66" s="1" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A58" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="B58" s="1" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A59" t="s">
-        <v>134</v>
-      </c>
-      <c r="B59" s="1" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A60" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="B60" s="1" t="s">
-        <v>137</v>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>151</v>
+      </c>
+      <c r="B67" s="1" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A68" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="B68" s="1" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A69" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="B69" s="1" t="s">
+        <v>158</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:B24" xr:uid="{00000000-0009-0000-0000-000001000000}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B57">
+  <autoFilter ref="A1:B24">
+    <sortState ref="A2:B66">
       <sortCondition ref="A1:A24"/>
     </sortState>
   </autoFilter>

</xml_diff>

<commit_message>
Skills & Tagsinput added
</commit_message>
<xml_diff>
--- a/Vitae/Library/Resources/SharedResource.xlsx
+++ b/Vitae/Library/Resources/SharedResource.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="384" uniqueCount="231">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="400" uniqueCount="238">
   <si>
     <t>City</t>
   </si>
@@ -722,6 +722,27 @@
   </si>
   <si>
     <t>Verliehen im</t>
+  </si>
+  <si>
+    <t>Skills</t>
+  </si>
+  <si>
+    <t>Category</t>
+  </si>
+  <si>
+    <t>Kategorie</t>
+  </si>
+  <si>
+    <t>Skillset</t>
+  </si>
+  <si>
+    <t>Kernkompetenz</t>
+  </si>
+  <si>
+    <t>Etc</t>
+  </si>
+  <si>
+    <t>…</t>
   </si>
 </sst>
 </file>
@@ -1099,10 +1120,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B96"/>
+  <dimension ref="A1:B100"/>
   <sheetViews>
-    <sheetView topLeftCell="A64" workbookViewId="0">
-      <selection activeCell="A93" sqref="A93:A96"/>
+    <sheetView topLeftCell="A82" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:B100"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1153,735 +1174,767 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>152</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>152</v>
+        <v>225</v>
+      </c>
+      <c r="B6" t="s">
+        <v>226</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>44</v>
+        <v>227</v>
+      </c>
+      <c r="B7" t="s">
+        <v>228</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>52</v>
+        <v>152</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>52</v>
+        <v>152</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>94</v>
+        <v>44</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>94</v>
+        <v>44</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>61</v>
+        <v>52</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>62</v>
+        <v>94</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>106</v>
+        <v>94</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>0</v>
+        <v>232</v>
+      </c>
+      <c r="B12" t="s">
+        <v>232</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>0</v>
+        <v>61</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>0</v>
+        <v>60</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>197</v>
-      </c>
-      <c r="B14" t="s">
-        <v>198</v>
+      <c r="A14" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>106</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>92</v>
+        <v>0</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>92</v>
+        <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>17</v>
+        <v>0</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>21</v>
+        <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>33</v>
+      <c r="A17" t="s">
+        <v>197</v>
+      </c>
+      <c r="B17" t="s">
+        <v>198</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>143</v>
-      </c>
-      <c r="B18" t="s">
-        <v>144</v>
+      <c r="A18" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>100</v>
+        <v>17</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>100</v>
+        <v>21</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="B20" t="s">
-        <v>64</v>
+        <v>18</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>108</v>
+      <c r="A21" t="s">
+        <v>143</v>
+      </c>
+      <c r="B21" t="s">
+        <v>144</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>24</v>
+        <v>100</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>24</v>
+        <v>100</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="B23" s="1" t="s">
-        <v>116</v>
+        <v>224</v>
+      </c>
+      <c r="B23" t="s">
+        <v>224</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>140</v>
+      <c r="A24" s="1" t="s">
+        <v>63</v>
       </c>
       <c r="B24" t="s">
-        <v>140</v>
+        <v>64</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="B25" t="s">
-        <v>79</v>
+        <v>108</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>108</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="B26" t="s">
-        <v>73</v>
+        <v>200</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>200</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>1</v>
+        <v>24</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>1</v>
+        <v>24</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="B28" t="s">
-        <v>72</v>
+        <v>116</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>116</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="B29" s="1" t="s">
-        <v>36</v>
+        <v>236</v>
+      </c>
+      <c r="B29" t="s">
+        <v>237</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A30" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="B30" s="1" t="s">
-        <v>114</v>
+      <c r="A30" t="s">
+        <v>140</v>
+      </c>
+      <c r="B30" t="s">
+        <v>140</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>142</v>
+      <c r="A31" s="1" t="s">
+        <v>70</v>
       </c>
       <c r="B31" t="s">
-        <v>142</v>
+        <v>79</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
-        <v>194</v>
+      <c r="A32" s="1" t="s">
+        <v>69</v>
       </c>
       <c r="B32" t="s">
-        <v>196</v>
+        <v>73</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
-        <v>34</v>
+        <v>1</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>34</v>
+        <v>1</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
-        <v>141</v>
+      <c r="A34" s="1" t="s">
+        <v>71</v>
       </c>
       <c r="B34" t="s">
-        <v>141</v>
+        <v>72</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
-        <v>2</v>
+        <v>36</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>2</v>
+        <v>36</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
-        <v>154</v>
+        <v>114</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>155</v>
+        <v>114</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A37" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B37" s="1" t="s">
-        <v>3</v>
+      <c r="A37" t="s">
+        <v>142</v>
+      </c>
+      <c r="B37" t="s">
+        <v>142</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>162</v>
-      </c>
-      <c r="B38" t="s">
-        <v>181</v>
+        <v>202</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>203</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>164</v>
+        <v>194</v>
       </c>
       <c r="B39" t="s">
-        <v>171</v>
+        <v>196</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
-        <v>167</v>
+      <c r="A40" s="1" t="s">
+        <v>214</v>
       </c>
       <c r="B40" t="s">
-        <v>172</v>
+        <v>219</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
-        <v>27</v>
-      </c>
-      <c r="B41" s="1" t="s">
-        <v>30</v>
+      <c r="A41" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="B41" t="s">
+        <v>216</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="B42" s="1" t="s">
-        <v>43</v>
+        <v>220</v>
+      </c>
+      <c r="B42" t="s">
+        <v>217</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="B43" s="1" t="s">
-        <v>40</v>
+        <v>221</v>
+      </c>
+      <c r="B43" t="s">
+        <v>218</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
-        <v>149</v>
+      <c r="A44" s="1" t="s">
+        <v>34</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>151</v>
+        <v>34</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>132</v>
+        <v>141</v>
       </c>
       <c r="B45" t="s">
-        <v>132</v>
+        <v>141</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
-        <v>98</v>
+        <v>2</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>98</v>
+        <v>2</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A47" t="s">
-        <v>168</v>
-      </c>
-      <c r="B47" t="s">
-        <v>184</v>
+      <c r="A47" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>155</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A48" t="s">
-        <v>169</v>
-      </c>
-      <c r="B48" t="s">
-        <v>173</v>
+      <c r="A48" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>170</v>
+        <v>162</v>
       </c>
       <c r="B49" t="s">
-        <v>174</v>
+        <v>181</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A50" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="B50" s="1" t="s">
-        <v>95</v>
+      <c r="A50" t="s">
+        <v>164</v>
+      </c>
+      <c r="B50" t="s">
+        <v>171</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A51" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="B51" s="1" t="s">
-        <v>65</v>
+      <c r="A51" t="s">
+        <v>167</v>
+      </c>
+      <c r="B51" t="s">
+        <v>172</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A52" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="B52" t="s">
-        <v>88</v>
+      <c r="A52" t="s">
+        <v>27</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
-        <v>136</v>
+        <v>43</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>137</v>
+        <v>43</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
-        <v>138</v>
+        <v>40</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>139</v>
+        <v>40</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A55" s="1" t="s">
-        <v>46</v>
+      <c r="A55" t="s">
+        <v>149</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>46</v>
+        <v>151</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A56" t="s">
-        <v>29</v>
-      </c>
-      <c r="B56" s="1" t="s">
-        <v>29</v>
+      <c r="A56" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B56" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A57" s="1" t="s">
-        <v>103</v>
+      <c r="A57" t="s">
+        <v>205</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>105</v>
+        <v>205</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A58" s="1" t="s">
-        <v>80</v>
+      <c r="A58" t="s">
+        <v>132</v>
       </c>
       <c r="B58" t="s">
-        <v>81</v>
+        <v>132</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
-        <v>157</v>
+        <v>98</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>158</v>
+        <v>98</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A60" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="B60" s="1" t="s">
-        <v>134</v>
+      <c r="A60" t="s">
+        <v>168</v>
+      </c>
+      <c r="B60" t="s">
+        <v>184</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A61" s="1" t="s">
-        <v>77</v>
+      <c r="A61" t="s">
+        <v>169</v>
       </c>
       <c r="B61" t="s">
-        <v>78</v>
+        <v>173</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A62" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="B62" s="1" t="s">
-        <v>55</v>
+      <c r="A62" t="s">
+        <v>170</v>
+      </c>
+      <c r="B62" t="s">
+        <v>174</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
-        <v>48</v>
+        <v>95</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>49</v>
+        <v>95</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
-        <v>57</v>
+        <v>65</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>59</v>
+        <v>65</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="B65" s="1" t="s">
-        <v>127</v>
+        <v>68</v>
+      </c>
+      <c r="B65" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
-        <v>4</v>
+        <v>136</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>4</v>
+        <v>137</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="B67" s="3" t="s">
-        <v>117</v>
+        <v>138</v>
+      </c>
+      <c r="B67" s="1" t="s">
+        <v>139</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
-        <v>25</v>
+        <v>46</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>25</v>
+        <v>46</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
-        <v>115</v>
+        <v>103</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>115</v>
+        <v>105</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B71" s="1" t="s">
-        <v>5</v>
+        <v>80</v>
+      </c>
+      <c r="B71" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
-        <v>6</v>
+        <v>157</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>6</v>
+        <v>158</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
-        <v>7</v>
+        <v>207</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>23</v>
+        <v>209</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A74" s="1" t="s">
-        <v>112</v>
+        <v>134</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>120</v>
+        <v>134</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A75" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="B75" s="1" t="s">
-        <v>119</v>
+        <v>77</v>
+      </c>
+      <c r="B75" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A76" t="s">
-        <v>165</v>
-      </c>
-      <c r="B76" t="s">
-        <v>183</v>
+      <c r="A76" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B76" s="1" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A77" t="s">
-        <v>191</v>
-      </c>
-      <c r="B77" t="s">
-        <v>192</v>
+      <c r="A77" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B77" s="1" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A78" s="1" t="s">
-        <v>122</v>
+        <v>57</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>118</v>
+        <v>59</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A79" t="s">
-        <v>160</v>
-      </c>
-      <c r="B79" t="s">
-        <v>179</v>
+      <c r="A79" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="B79" s="1" t="s">
+        <v>127</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A80" t="s">
-        <v>161</v>
-      </c>
-      <c r="B80" t="s">
-        <v>180</v>
+      <c r="A80" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B80" s="1" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A81" t="s">
-        <v>166</v>
-      </c>
-      <c r="B81" t="s">
-        <v>179</v>
+      <c r="A81" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="B81" s="3" t="s">
+        <v>117</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A82" s="1" t="s">
-        <v>90</v>
+        <v>25</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>90</v>
+        <v>25</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A83" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="B83" s="1" t="s">
-        <v>96</v>
+        <v>231</v>
+      </c>
+      <c r="B83" t="s">
+        <v>231</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A84" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B84" s="1" t="s">
-        <v>9</v>
+        <v>234</v>
+      </c>
+      <c r="B84" t="s">
+        <v>234</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A85" s="1" t="s">
-        <v>200</v>
+      <c r="A85" t="s">
+        <v>28</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>200</v>
+        <v>28</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A86" t="s">
-        <v>202</v>
+      <c r="A86" s="1" t="s">
+        <v>115</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>203</v>
+        <v>115</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A87" t="s">
-        <v>205</v>
+      <c r="A87" s="1" t="s">
+        <v>5</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>205</v>
+        <v>5</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A88" s="1" t="s">
-        <v>207</v>
+        <v>6</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>209</v>
+        <v>6</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A89" s="1" t="s">
-        <v>214</v>
-      </c>
-      <c r="B89" t="s">
-        <v>219</v>
+        <v>7</v>
+      </c>
+      <c r="B89" s="1" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A90" s="1" t="s">
-        <v>215</v>
-      </c>
-      <c r="B90" t="s">
-        <v>216</v>
+        <v>112</v>
+      </c>
+      <c r="B90" s="1" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A91" s="1" t="s">
-        <v>220</v>
-      </c>
-      <c r="B91" t="s">
-        <v>217</v>
+        <v>111</v>
+      </c>
+      <c r="B91" s="1" t="s">
+        <v>119</v>
       </c>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A92" s="1" t="s">
-        <v>221</v>
+      <c r="A92" t="s">
+        <v>165</v>
       </c>
       <c r="B92" t="s">
-        <v>218</v>
+        <v>183</v>
       </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A93" s="1" t="s">
-        <v>20</v>
+      <c r="A93" t="s">
+        <v>191</v>
       </c>
       <c r="B93" t="s">
-        <v>20</v>
+        <v>192</v>
       </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A94" s="1" t="s">
-        <v>224</v>
-      </c>
-      <c r="B94" t="s">
-        <v>224</v>
+        <v>122</v>
+      </c>
+      <c r="B94" s="1" t="s">
+        <v>118</v>
       </c>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A95" s="1" t="s">
-        <v>225</v>
+      <c r="A95" t="s">
+        <v>160</v>
       </c>
       <c r="B95" t="s">
-        <v>226</v>
+        <v>179</v>
       </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A96" s="1" t="s">
-        <v>227</v>
+      <c r="A96" t="s">
+        <v>161</v>
       </c>
       <c r="B96" t="s">
-        <v>228</v>
+        <v>180</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A97" t="s">
+        <v>166</v>
+      </c>
+      <c r="B97" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A98" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="B98" s="1" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A99" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="B99" s="1" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A100" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B100" s="1" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:B24">
-    <sortState ref="A2:B84">
+    <sortState ref="A2:B100">
       <sortCondition ref="A1:A24"/>
     </sortState>
   </autoFilter>
@@ -1892,10 +1945,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B96"/>
+  <dimension ref="A1:B100"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A67" workbookViewId="0">
-      <selection activeCell="B97" sqref="B97"/>
+    <sheetView tabSelected="1" topLeftCell="A76" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:B100"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1946,735 +1999,767 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>152</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>153</v>
+        <v>225</v>
+      </c>
+      <c r="B6" t="s">
+        <v>229</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>45</v>
+        <v>227</v>
+      </c>
+      <c r="B7" t="s">
+        <v>230</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>52</v>
+        <v>152</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>53</v>
+        <v>153</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>94</v>
+        <v>44</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>102</v>
+        <v>45</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>61</v>
+        <v>52</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>74</v>
+        <v>53</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>62</v>
+        <v>94</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>42</v>
+        <v>232</v>
+      </c>
+      <c r="B12" t="s">
+        <v>233</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>0</v>
+        <v>61</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>123</v>
+        <v>74</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>197</v>
-      </c>
-      <c r="B14" t="s">
-        <v>199</v>
+      <c r="A14" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>92</v>
+        <v>0</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>93</v>
+        <v>42</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>17</v>
+        <v>0</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>21</v>
+        <v>123</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>19</v>
+      <c r="A17" t="s">
+        <v>197</v>
+      </c>
+      <c r="B17" t="s">
+        <v>199</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>143</v>
-      </c>
-      <c r="B18" t="s">
-        <v>144</v>
+      <c r="A18" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>100</v>
+        <v>17</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>101</v>
+        <v>21</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="B20" t="s">
-        <v>75</v>
+        <v>18</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>109</v>
+      <c r="A21" t="s">
+        <v>143</v>
+      </c>
+      <c r="B21" t="s">
+        <v>144</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>24</v>
+        <v>100</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>24</v>
+        <v>101</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="B23" s="1" t="s">
-        <v>129</v>
+        <v>224</v>
+      </c>
+      <c r="B23" t="s">
+        <v>126</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>140</v>
+      <c r="A24" s="1" t="s">
+        <v>63</v>
       </c>
       <c r="B24" t="s">
-        <v>146</v>
+        <v>75</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="B25" t="s">
-        <v>85</v>
+        <v>108</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>109</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="B26" t="s">
-        <v>84</v>
+        <v>200</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>201</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>1</v>
+        <v>24</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>10</v>
+        <v>24</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="B28" t="s">
-        <v>87</v>
+        <v>116</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>129</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="B29" s="1" t="s">
-        <v>37</v>
+        <v>236</v>
+      </c>
+      <c r="B29" t="s">
+        <v>237</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A30" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="B30" s="1" t="s">
-        <v>128</v>
+      <c r="A30" t="s">
+        <v>140</v>
+      </c>
+      <c r="B30" t="s">
+        <v>146</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>142</v>
+      <c r="A31" s="1" t="s">
+        <v>70</v>
       </c>
       <c r="B31" t="s">
-        <v>148</v>
+        <v>85</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
-        <v>194</v>
+      <c r="A32" s="1" t="s">
+        <v>69</v>
       </c>
       <c r="B32" t="s">
-        <v>195</v>
+        <v>84</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
-        <v>34</v>
+        <v>1</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>35</v>
+        <v>10</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
-        <v>141</v>
+      <c r="A34" s="1" t="s">
+        <v>71</v>
       </c>
       <c r="B34" t="s">
-        <v>147</v>
+        <v>87</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
-        <v>2</v>
+        <v>36</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>11</v>
+        <v>37</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
-        <v>154</v>
+        <v>114</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>156</v>
+        <v>128</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A37" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B37" s="1" t="s">
-        <v>12</v>
+      <c r="A37" t="s">
+        <v>142</v>
+      </c>
+      <c r="B37" t="s">
+        <v>148</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>162</v>
+        <v>202</v>
       </c>
       <c r="B38" t="s">
-        <v>187</v>
+        <v>204</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>164</v>
+        <v>194</v>
       </c>
       <c r="B39" t="s">
-        <v>175</v>
+        <v>195</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
-        <v>167</v>
+      <c r="A40" s="1" t="s">
+        <v>214</v>
       </c>
       <c r="B40" t="s">
-        <v>176</v>
+        <v>211</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
-        <v>27</v>
-      </c>
-      <c r="B41" s="1" t="s">
-        <v>31</v>
+      <c r="A41" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="B41" t="s">
+        <v>210</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="B42" s="1" t="s">
-        <v>38</v>
+        <v>220</v>
+      </c>
+      <c r="B42" t="s">
+        <v>212</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="B43" s="1" t="s">
-        <v>39</v>
+        <v>221</v>
+      </c>
+      <c r="B43" t="s">
+        <v>213</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
-        <v>149</v>
+      <c r="A44" s="1" t="s">
+        <v>34</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>150</v>
+        <v>35</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>132</v>
-      </c>
-      <c r="B45" s="1" t="s">
-        <v>133</v>
+        <v>141</v>
+      </c>
+      <c r="B45" t="s">
+        <v>147</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
-        <v>98</v>
+        <v>2</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>99</v>
+        <v>11</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A47" t="s">
-        <v>168</v>
-      </c>
-      <c r="B47" t="s">
-        <v>190</v>
+      <c r="A47" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>156</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A48" t="s">
-        <v>169</v>
-      </c>
-      <c r="B48" t="s">
-        <v>177</v>
+      <c r="A48" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>170</v>
+        <v>162</v>
       </c>
       <c r="B49" t="s">
-        <v>178</v>
+        <v>187</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A50" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="B50" s="1" t="s">
-        <v>95</v>
+      <c r="A50" t="s">
+        <v>164</v>
+      </c>
+      <c r="B50" t="s">
+        <v>175</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A51" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="B51" s="1" t="s">
-        <v>82</v>
+      <c r="A51" t="s">
+        <v>167</v>
+      </c>
+      <c r="B51" t="s">
+        <v>176</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A52" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="B52" t="s">
-        <v>89</v>
+      <c r="A52" t="s">
+        <v>27</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
-        <v>136</v>
+        <v>43</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>47</v>
+        <v>38</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
-        <v>138</v>
+        <v>40</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>145</v>
+        <v>39</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A55" s="1" t="s">
-        <v>46</v>
+      <c r="A55" t="s">
+        <v>149</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>47</v>
+        <v>150</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A56" t="s">
-        <v>29</v>
-      </c>
-      <c r="B56" s="1" t="s">
-        <v>32</v>
+      <c r="A56" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B56" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A57" s="1" t="s">
-        <v>103</v>
+      <c r="A57" t="s">
+        <v>205</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>104</v>
+        <v>206</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A58" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="B58" t="s">
-        <v>86</v>
+      <c r="A58" t="s">
+        <v>132</v>
+      </c>
+      <c r="B58" s="1" t="s">
+        <v>133</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
-        <v>157</v>
+        <v>98</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>159</v>
+        <v>99</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A60" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="B60" s="1" t="s">
-        <v>135</v>
+      <c r="A60" t="s">
+        <v>168</v>
+      </c>
+      <c r="B60" t="s">
+        <v>190</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A61" s="1" t="s">
-        <v>77</v>
+      <c r="A61" t="s">
+        <v>169</v>
       </c>
       <c r="B61" t="s">
-        <v>76</v>
+        <v>177</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A62" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="B62" s="1" t="s">
-        <v>56</v>
+      <c r="A62" t="s">
+        <v>170</v>
+      </c>
+      <c r="B62" t="s">
+        <v>178</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
-        <v>48</v>
+        <v>95</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>50</v>
+        <v>95</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
-        <v>57</v>
+        <v>65</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>58</v>
+        <v>82</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="B65" s="1" t="s">
-        <v>126</v>
+        <v>68</v>
+      </c>
+      <c r="B65" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
-        <v>4</v>
+        <v>136</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>13</v>
+        <v>47</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
-        <v>110</v>
+        <v>138</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>121</v>
+        <v>145</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
-        <v>25</v>
+        <v>46</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>26</v>
+        <v>47</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
-        <v>115</v>
+        <v>103</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>115</v>
+        <v>104</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B71" s="1" t="s">
-        <v>14</v>
+        <v>80</v>
+      </c>
+      <c r="B71" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
-        <v>6</v>
+        <v>157</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>15</v>
+        <v>159</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
-        <v>7</v>
+        <v>207</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>16</v>
+        <v>208</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A74" s="1" t="s">
-        <v>112</v>
+        <v>134</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>125</v>
+        <v>135</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A75" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="B75" s="1" t="s">
-        <v>124</v>
+        <v>77</v>
+      </c>
+      <c r="B75" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A76" t="s">
-        <v>165</v>
-      </c>
-      <c r="B76" t="s">
-        <v>189</v>
+      <c r="A76" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B76" s="1" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A77" t="s">
-        <v>191</v>
-      </c>
-      <c r="B77" t="s">
-        <v>193</v>
+      <c r="A77" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B77" s="1" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A78" s="1" t="s">
-        <v>122</v>
+        <v>57</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>118</v>
+        <v>58</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A79" t="s">
-        <v>160</v>
-      </c>
-      <c r="B79" t="s">
-        <v>185</v>
+      <c r="A79" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="B79" s="1" t="s">
+        <v>126</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A80" t="s">
-        <v>161</v>
-      </c>
-      <c r="B80" t="s">
-        <v>186</v>
+      <c r="A80" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B80" s="1" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A81" t="s">
-        <v>166</v>
-      </c>
-      <c r="B81" t="s">
-        <v>185</v>
+      <c r="A81" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="B81" s="1" t="s">
+        <v>121</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A82" s="1" t="s">
-        <v>90</v>
+        <v>25</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>91</v>
+        <v>26</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A83" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="B83" s="1" t="s">
-        <v>97</v>
+        <v>231</v>
+      </c>
+      <c r="B83" t="s">
+        <v>231</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A84" s="1" t="s">
-        <v>8</v>
+        <v>234</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>41</v>
+        <v>235</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A85" s="1" t="s">
-        <v>200</v>
+      <c r="A85" t="s">
+        <v>28</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>201</v>
+        <v>28</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A86" t="s">
-        <v>202</v>
-      </c>
-      <c r="B86" t="s">
-        <v>204</v>
+      <c r="A86" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="B86" s="1" t="s">
+        <v>115</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A87" t="s">
-        <v>205</v>
+      <c r="A87" s="1" t="s">
+        <v>5</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>206</v>
+        <v>14</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A88" s="1" t="s">
-        <v>207</v>
+        <v>6</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>208</v>
+        <v>15</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A89" s="1" t="s">
-        <v>214</v>
-      </c>
-      <c r="B89" t="s">
-        <v>211</v>
+        <v>7</v>
+      </c>
+      <c r="B89" s="1" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A90" s="1" t="s">
-        <v>215</v>
-      </c>
-      <c r="B90" t="s">
-        <v>210</v>
+        <v>112</v>
+      </c>
+      <c r="B90" s="1" t="s">
+        <v>125</v>
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A91" s="1" t="s">
-        <v>220</v>
-      </c>
-      <c r="B91" t="s">
-        <v>212</v>
+        <v>111</v>
+      </c>
+      <c r="B91" s="1" t="s">
+        <v>124</v>
       </c>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A92" s="1" t="s">
-        <v>221</v>
+      <c r="A92" t="s">
+        <v>165</v>
       </c>
       <c r="B92" t="s">
-        <v>213</v>
+        <v>189</v>
       </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A93" s="1" t="s">
-        <v>20</v>
+      <c r="A93" t="s">
+        <v>191</v>
       </c>
       <c r="B93" t="s">
-        <v>20</v>
+        <v>193</v>
       </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A94" s="1" t="s">
-        <v>224</v>
-      </c>
-      <c r="B94" t="s">
-        <v>126</v>
+        <v>122</v>
+      </c>
+      <c r="B94" s="1" t="s">
+        <v>118</v>
       </c>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A95" s="1" t="s">
-        <v>225</v>
+      <c r="A95" t="s">
+        <v>160</v>
       </c>
       <c r="B95" t="s">
-        <v>229</v>
+        <v>185</v>
       </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A96" s="1" t="s">
-        <v>227</v>
+      <c r="A96" t="s">
+        <v>161</v>
       </c>
       <c r="B96" t="s">
-        <v>230</v>
+        <v>186</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A97" t="s">
+        <v>166</v>
+      </c>
+      <c r="B97" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A98" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="B98" s="1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A99" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="B99" s="1" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A100" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B100" s="1" t="s">
+        <v>41</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:B24">
-    <sortState ref="A2:B84">
+    <sortState ref="A2:B100">
       <sortCondition ref="A1:A24"/>
     </sortState>
   </autoFilter>

</xml_diff>

<commit_message>
Pretty checkbox library added
</commit_message>
<xml_diff>
--- a/Vitae/Library/Resources/SharedResource.xlsx
+++ b/Vitae/Library/Resources/SharedResource.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\Vitae\Library\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B118CFB1-0DE7-4C70-ADCC-04354D9650F1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E108BCC-9DC2-4AC6-B32F-4B558B40C9CC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4270" yWindow="880" windowWidth="22500" windowHeight="14260" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="432" uniqueCount="260">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="460" uniqueCount="280">
   <si>
     <t>City</t>
   </si>
@@ -810,6 +810,66 @@
   </si>
   <si>
     <t>Create an account</t>
+  </si>
+  <si>
+    <t>CreateAccount</t>
+  </si>
+  <si>
+    <t>Create a new account.</t>
+  </si>
+  <si>
+    <t>Password</t>
+  </si>
+  <si>
+    <t>Passwort</t>
+  </si>
+  <si>
+    <t>Ein neues Konto eröffnen.</t>
+  </si>
+  <si>
+    <t>The {0} must be at least {2} and at max {1} characters long.</t>
+  </si>
+  <si>
+    <t>PasswordErrorLength</t>
+  </si>
+  <si>
+    <t>Das {0} muss mindestens {2} und höchstens {1} Zeichen lang sein.</t>
+  </si>
+  <si>
+    <t>ConfirmPassword</t>
+  </si>
+  <si>
+    <t>Passwort bestätigen</t>
+  </si>
+  <si>
+    <t>Confirm password</t>
+  </si>
+  <si>
+    <t>CompareFailed</t>
+  </si>
+  <si>
+    <t>The password and confirmation password do not match.</t>
+  </si>
+  <si>
+    <t>Die Passwörter stimmen nicht überein</t>
+  </si>
+  <si>
+    <t>LoginTitle</t>
+  </si>
+  <si>
+    <t>Use a local account to log in.</t>
+  </si>
+  <si>
+    <t>Melden Sie sich mit einem Konto an.</t>
+  </si>
+  <si>
+    <t>Remember me?</t>
+  </si>
+  <si>
+    <t>Eingeloggt bleiben</t>
+  </si>
+  <si>
+    <t>RememberMe</t>
   </si>
 </sst>
 </file>
@@ -1187,10 +1247,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B108"/>
+  <dimension ref="A1:B115"/>
   <sheetViews>
-    <sheetView topLeftCell="A85" workbookViewId="0">
-      <selection activeCell="A109" sqref="A109:XFD109"/>
+    <sheetView topLeftCell="A94" workbookViewId="0">
+      <selection activeCell="A115" sqref="A115:B115"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2061,6 +2121,62 @@
       </c>
       <c r="B108" s="1" t="s">
         <v>254</v>
+      </c>
+    </row>
+    <row r="109" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A109" s="1" t="s">
+        <v>260</v>
+      </c>
+      <c r="B109" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="110" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A110" s="1" t="s">
+        <v>262</v>
+      </c>
+      <c r="B110" s="1" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="111" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A111" s="1" t="s">
+        <v>266</v>
+      </c>
+      <c r="B111" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="112" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A112" t="s">
+        <v>268</v>
+      </c>
+      <c r="B112" s="1" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="113" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A113" s="1" t="s">
+        <v>271</v>
+      </c>
+      <c r="B113" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="114" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A114" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="B114" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="115" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A115" s="1" t="s">
+        <v>279</v>
+      </c>
+      <c r="B115" s="1" t="s">
+        <v>277</v>
       </c>
     </row>
   </sheetData>
@@ -2076,10 +2192,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:B109"/>
+  <dimension ref="A1:B115"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A85" workbookViewId="0">
-      <selection activeCell="B107" sqref="B107"/>
+    <sheetView tabSelected="1" topLeftCell="A94" workbookViewId="0">
+      <selection activeCell="A115" sqref="A115:B115"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2953,7 +3069,60 @@
       </c>
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="B109" s="1"/>
+      <c r="A109" s="1" t="s">
+        <v>260</v>
+      </c>
+      <c r="B109" s="1" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="110" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A110" s="1" t="s">
+        <v>262</v>
+      </c>
+      <c r="B110" s="1" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="111" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A111" s="1" t="s">
+        <v>266</v>
+      </c>
+      <c r="B111" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="112" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A112" t="s">
+        <v>268</v>
+      </c>
+      <c r="B112" s="1" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="113" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A113" s="1" t="s">
+        <v>271</v>
+      </c>
+      <c r="B113" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="114" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A114" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="B114" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="115" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A115" s="1" t="s">
+        <v>279</v>
+      </c>
+      <c r="B115" t="s">
+        <v>278</v>
+      </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:B23" xr:uid="{00000000-0009-0000-0000-000001000000}">

</xml_diff>

<commit_message>
Mailing with html template included
</commit_message>
<xml_diff>
--- a/Vitae/Library/Resources/SharedResource.xlsx
+++ b/Vitae/Library/Resources/SharedResource.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22430"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\Various\Vitae\Library\Resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\Vitae\Library\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2F757CC-EDC2-47A4-8282-03D3511C6F72}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4275" yWindow="885" windowWidth="22500" windowHeight="14265"/>
+    <workbookView xWindow="7000" yWindow="2330" windowWidth="22500" windowHeight="14260" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="en" sheetId="3" r:id="rId1"/>
@@ -29,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="592" uniqueCount="378">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="640" uniqueCount="413">
   <si>
     <t>City</t>
   </si>
@@ -1163,12 +1164,117 @@
   </si>
   <si>
     <t>Fehler bei der Bestätigung Ihrer E-Mail.</t>
+  </si>
+  <si>
+    <t>ResetPassword</t>
+  </si>
+  <si>
+    <t>Reset password</t>
+  </si>
+  <si>
+    <t>ResetYourPassword</t>
+  </si>
+  <si>
+    <t>Reset your password</t>
+  </si>
+  <si>
+    <t>Passwort zurücksetzen</t>
+  </si>
+  <si>
+    <t>Setzen Sie ihr Passwort zurück</t>
+  </si>
+  <si>
+    <t>Reset</t>
+  </si>
+  <si>
+    <t>Zurücksetzen</t>
+  </si>
+  <si>
+    <t>ResetPasswordConfirmation</t>
+  </si>
+  <si>
+    <t>Reset password confirmation</t>
+  </si>
+  <si>
+    <t>Your password has been reset. Please</t>
+  </si>
+  <si>
+    <t>ResetPasswordText2</t>
+  </si>
+  <si>
+    <t>click here to log in.</t>
+  </si>
+  <si>
+    <t>Passwort erfolgreich zurückgesetzt</t>
+  </si>
+  <si>
+    <t>Ihr Passwort wurde zurückgesetzt. Bitte</t>
+  </si>
+  <si>
+    <t>klicken Sie hier um sich anzumelden.</t>
+  </si>
+  <si>
+    <t>ResetPasswordText1</t>
+  </si>
+  <si>
+    <t>SupplyCode</t>
+  </si>
+  <si>
+    <t>A code must be supplied for password reset.</t>
+  </si>
+  <si>
+    <t>Für das Zurücksetzen des Passworts muss ein Code angegeben werden.</t>
+  </si>
+  <si>
+    <t>User created a new account with password.</t>
+  </si>
+  <si>
+    <t>UserCreatedWithPassword</t>
+  </si>
+  <si>
+    <t>Ein neues Benutzerkonto wurde erstellt</t>
+  </si>
+  <si>
+    <t>WelcomeToVitae</t>
+  </si>
+  <si>
+    <t>Welcome to VITAE</t>
+  </si>
+  <si>
+    <t>PleaseClickHereToConfirm</t>
+  </si>
+  <si>
+    <t>Willkommen bei VITAE</t>
+  </si>
+  <si>
+    <t>ClickHere</t>
+  </si>
+  <si>
+    <t>Please confirm your email account by</t>
+  </si>
+  <si>
+    <t>clicking here</t>
+  </si>
+  <si>
+    <t>Bitte bestätigen Sie ihr Benutzerkonto in dem Sie</t>
+  </si>
+  <si>
+    <t>hier klicken</t>
+  </si>
+  <si>
+    <t>ConfirmEmail</t>
+  </si>
+  <si>
+    <t>Confirm your email</t>
+  </si>
+  <si>
+    <t>Bestätigen Sie Ihr E-Mail</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1228,7 +1334,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1539,20 +1645,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B148"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:B160"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A136" workbookViewId="0">
-      <selection activeCell="A146" sqref="A146:B148"/>
+    <sheetView topLeftCell="A142" workbookViewId="0">
+      <selection activeCell="A160" sqref="A160:B160"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="37.28515625" customWidth="1"/>
-    <col min="2" max="2" width="118.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="37.26953125" customWidth="1"/>
+    <col min="2" max="2" width="118.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>20</v>
       </c>
@@ -1560,7 +1666,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>50</v>
       </c>
@@ -1568,1178 +1674,1274 @@
         <v>222</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>364</v>
+      </c>
+      <c r="B3" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A4" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B4" s="1" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A5" s="1" t="s">
+        <v>249</v>
+      </c>
+      <c r="B5" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A6" s="1" t="s">
+        <v>248</v>
+      </c>
+      <c r="B6" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A7" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B7" s="1" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
         <v>162</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B8" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A9" s="1" t="s">
         <v>224</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B9" t="s">
         <v>225</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A10" s="1" t="s">
         <v>226</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B10" t="s">
         <v>227</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A11" s="1" t="s">
         <v>151</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B11" s="1" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A12" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="B12" s="1" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A13" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="B13" s="1" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A14" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="B14" s="1" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A15" s="1" t="s">
         <v>231</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B15" t="s">
         <v>231</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A16" s="1" t="s">
+        <v>288</v>
+      </c>
+      <c r="B16" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A17" s="1" t="s">
+        <v>297</v>
+      </c>
+      <c r="B17" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A18" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="B13" s="1" t="s">
+      <c r="B18" s="1" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="s">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A19" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="B19" s="1" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" s="1" t="s">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A20" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B15" s="1" t="s">
+      <c r="B20" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
         <v>196</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B21" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" s="1" t="s">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A22" s="1" t="s">
+        <v>271</v>
+      </c>
+      <c r="B22" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A23" t="s">
+        <v>300</v>
+      </c>
+      <c r="B23" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A24" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="B17" s="1" t="s">
+      <c r="B24" s="1" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" s="1" t="s">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A25" t="s">
+        <v>369</v>
+      </c>
+      <c r="B25" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A26" t="s">
+        <v>373</v>
+      </c>
+      <c r="B26" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A27" t="s">
+        <v>268</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A28" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B18" s="1" t="s">
+      <c r="B28" s="1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" s="1" t="s">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A29" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B19" s="1" t="s">
+      <c r="B29" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A30" s="1" t="s">
+        <v>260</v>
+      </c>
+      <c r="B30" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A31" t="s">
         <v>142</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B31" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" s="1" t="s">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A32" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="B21" s="1" t="s">
+      <c r="B32" s="1" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" s="1" t="s">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A33" s="1" t="s">
+        <v>245</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A34" t="s">
+        <v>299</v>
+      </c>
+      <c r="B34" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A35" s="1" t="s">
         <v>223</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B35" t="s">
         <v>223</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" s="1" t="s">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A36" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="B23" t="s">
+      <c r="B36" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24" s="1" t="s">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A37" t="s">
+        <v>307</v>
+      </c>
+      <c r="B37" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A38" t="s">
+        <v>309</v>
+      </c>
+      <c r="B38" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A39" t="s">
+        <v>306</v>
+      </c>
+      <c r="B39" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A40" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="B24" s="1" t="s">
+      <c r="B40" s="1" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25" s="1" t="s">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A41" s="1" t="s">
         <v>199</v>
       </c>
-      <c r="B25" s="1" t="s">
+      <c r="B41" s="1" t="s">
         <v>199</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A26" s="1" t="s">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A42" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B26" s="1" t="s">
+      <c r="B42" s="1" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A27" s="1" t="s">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A43" s="1" t="s">
+        <v>291</v>
+      </c>
+      <c r="B43" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A44" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="B27" s="1" t="s">
+      <c r="B44" s="1" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A28" s="1" t="s">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A45" t="s">
+        <v>376</v>
+      </c>
+      <c r="B45" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A46" s="1" t="s">
         <v>234</v>
       </c>
-      <c r="B28" t="s">
+      <c r="B46" t="s">
         <v>235</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A47" t="s">
         <v>139</v>
       </c>
-      <c r="B29" t="s">
+      <c r="B47" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A30" s="1" t="s">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A48" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="B30" t="s">
+      <c r="B48" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A31" s="1" t="s">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A49" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="B31" t="s">
+      <c r="B49" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A32" s="1" t="s">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A50" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B32" s="1" t="s">
+      <c r="B50" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A33" s="1" t="s">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A51" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="B33" t="s">
+      <c r="B51" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A34" s="1" t="s">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A52" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A53" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="B34" s="1" t="s">
+      <c r="B53" s="1" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A35" s="1" t="s">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A54" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="B35" s="1" t="s">
+      <c r="B54" s="1" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A55" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="B55" s="1" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A56" t="s">
         <v>141</v>
       </c>
-      <c r="B36" t="s">
+      <c r="B56" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A57" t="s">
+        <v>305</v>
+      </c>
+      <c r="B57" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A58" t="s">
+        <v>360</v>
+      </c>
+      <c r="B58" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A59" t="s">
+        <v>308</v>
+      </c>
+      <c r="B59" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A60" t="s">
+        <v>302</v>
+      </c>
+      <c r="B60" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A61" t="s">
+        <v>304</v>
+      </c>
+      <c r="B61" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A62" t="s">
         <v>201</v>
       </c>
-      <c r="B37" s="1" t="s">
+      <c r="B62" s="1" t="s">
         <v>202</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
+    <row r="63" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A63" t="s">
         <v>193</v>
       </c>
-      <c r="B38" t="s">
+      <c r="B63" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A39" s="1" t="s">
+    <row r="64" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A64" s="1" t="s">
         <v>213</v>
       </c>
-      <c r="B39" t="s">
+      <c r="B64" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A40" s="1" t="s">
+    <row r="65" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A65" s="1" t="s">
         <v>214</v>
       </c>
-      <c r="B40" t="s">
+      <c r="B65" t="s">
         <v>215</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A41" s="1" t="s">
+    <row r="66" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A66" s="1" t="s">
         <v>219</v>
       </c>
-      <c r="B41" t="s">
+      <c r="B66" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A42" s="1" t="s">
+    <row r="67" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A67" s="1" t="s">
         <v>220</v>
       </c>
-      <c r="B42" t="s">
+      <c r="B67" t="s">
         <v>217</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A43" s="1" t="s">
+    <row r="68" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A68" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B43" s="1" t="s">
+      <c r="B68" s="1" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
+    <row r="69" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A69" t="s">
         <v>140</v>
       </c>
-      <c r="B44" t="s">
+      <c r="B69" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A45" s="1" t="s">
+    <row r="70" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A70" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B45" s="1" t="s">
+      <c r="B70" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A46" s="1" t="s">
+    <row r="71" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A71" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="B46" s="1" t="s">
+      <c r="B71" s="1" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A47" s="1" t="s">
+    <row r="72" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A72" t="s">
+        <v>303</v>
+      </c>
+      <c r="B72" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A73" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="B73" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A74" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B47" s="1" t="s">
+      <c r="B74" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A48" t="s">
+    <row r="75" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A75" t="s">
         <v>161</v>
       </c>
-      <c r="B48" t="s">
+      <c r="B75" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A49" t="s">
+    <row r="76" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A76" t="s">
         <v>163</v>
       </c>
-      <c r="B49" t="s">
+      <c r="B76" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A50" t="s">
+    <row r="77" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A77" t="s">
         <v>166</v>
       </c>
-      <c r="B50" t="s">
+      <c r="B77" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A51" t="s">
+    <row r="78" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A78" t="s">
         <v>27</v>
       </c>
-      <c r="B51" s="1" t="s">
+      <c r="B78" s="1" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A52" s="1" t="s">
+    <row r="79" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A79" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="B52" s="1" t="s">
+      <c r="B79" s="1" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A53" s="1" t="s">
+    <row r="80" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A80" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="B53" s="1" t="s">
+      <c r="B80" s="1" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A54" t="s">
+    <row r="81" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A81" t="s">
         <v>148</v>
       </c>
-      <c r="B54" s="1" t="s">
+      <c r="B81" s="1" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A55" s="1" t="s">
+    <row r="82" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A82" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B55" t="s">
+      <c r="B82" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A56" t="s">
+    <row r="83" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A83" t="s">
         <v>204</v>
       </c>
-      <c r="B56" s="1" t="s">
+      <c r="B83" s="1" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A57" t="s">
+    <row r="84" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A84" t="s">
         <v>131</v>
       </c>
-      <c r="B57" t="s">
+      <c r="B84" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A58" s="1" t="s">
+    <row r="85" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A85" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="B58" s="1" t="s">
+      <c r="B85" s="1" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A59" t="s">
+    <row r="86" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A86" t="s">
         <v>167</v>
       </c>
-      <c r="B59" t="s">
+      <c r="B86" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A60" t="s">
+    <row r="87" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A87" t="s">
         <v>168</v>
       </c>
-      <c r="B60" t="s">
+      <c r="B87" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A61" t="s">
+    <row r="88" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A88" t="s">
         <v>169</v>
       </c>
-      <c r="B61" t="s">
+      <c r="B88" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A62" s="1" t="s">
+    <row r="89" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A89" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="B62" s="1" t="s">
+      <c r="B89" s="1" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A63" s="1" t="s">
+    <row r="90" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A90" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="B63" s="1" t="s">
+      <c r="B90" s="1" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A64" s="1" t="s">
+    <row r="91" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A91" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="B64" t="s">
+      <c r="B91" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A65" s="1" t="s">
+    <row r="92" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A92" s="1" t="s">
+        <v>262</v>
+      </c>
+      <c r="B92" s="1" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A93" s="1" t="s">
+        <v>266</v>
+      </c>
+      <c r="B93" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A94" s="1" t="s">
+        <v>280</v>
+      </c>
+      <c r="B94" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A95" t="s">
+        <v>301</v>
+      </c>
+      <c r="B95" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A96" t="s">
+        <v>316</v>
+      </c>
+      <c r="B96" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A97" t="s">
+        <v>317</v>
+      </c>
+      <c r="B97" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A98" t="s">
+        <v>315</v>
+      </c>
+      <c r="B98" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A99" t="s">
+        <v>318</v>
+      </c>
+      <c r="B99" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A100" t="s">
+        <v>314</v>
+      </c>
+      <c r="B100" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A101" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="B65" s="1" t="s">
+      <c r="B101" s="1" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A66" s="1" t="s">
+    <row r="102" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A102" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="B66" s="1" t="s">
+      <c r="B102" s="1" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A67" s="1" t="s">
+    <row r="103" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A103" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="B67" s="1" t="s">
+      <c r="B103" s="1" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A68" t="s">
+    <row r="104" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A104" t="s">
         <v>29</v>
       </c>
-      <c r="B68" s="1" t="s">
+      <c r="B104" s="1" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A69" s="1" t="s">
+    <row r="105" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A105" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="B69" s="1" t="s">
+      <c r="B105" s="1" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A70" s="1" t="s">
+    <row r="106" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A106" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="B70" t="s">
+      <c r="B106" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A71" s="1" t="s">
+    <row r="107" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A107" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="B71" s="1" t="s">
+      <c r="B107" s="1" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A72" s="1" t="s">
+    <row r="108" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A108" s="1" t="s">
         <v>206</v>
       </c>
-      <c r="B72" s="1" t="s">
+      <c r="B108" s="1" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A73" s="1" t="s">
+    <row r="109" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A109" s="1" t="s">
+        <v>252</v>
+      </c>
+      <c r="B109" s="1" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="110" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A110" s="1" t="s">
+        <v>281</v>
+      </c>
+      <c r="B110" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="111" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A111" s="1" t="s">
+        <v>294</v>
+      </c>
+      <c r="B111" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="112" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A112" s="1" t="s">
+        <v>279</v>
+      </c>
+      <c r="B112" s="1" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="113" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A113" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="B73" s="1" t="s">
+      <c r="B113" s="1" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A74" s="1" t="s">
+    <row r="114" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A114" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="B74" t="s">
+      <c r="B114" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A75" s="1" t="s">
+    <row r="115" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A115" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="B75" s="1" t="s">
+      <c r="B115" s="1" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A76" s="1" t="s">
+    <row r="116" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A116" s="1" t="s">
+        <v>286</v>
+      </c>
+      <c r="B116" s="1" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="117" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A117" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="B76" s="1" t="s">
+      <c r="B117" s="1" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A77" s="1" t="s">
+    <row r="118" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A118" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="B77" s="1" t="s">
+      <c r="B118" s="1" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A78" s="1" t="s">
+    <row r="119" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A119" t="s">
+        <v>384</v>
+      </c>
+      <c r="B119" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="120" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A120" t="s">
+        <v>378</v>
+      </c>
+      <c r="B120" t="s">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="121" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A121" t="s">
+        <v>386</v>
+      </c>
+      <c r="B121" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="122" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A122" t="s">
+        <v>394</v>
+      </c>
+      <c r="B122" t="s">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="123" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A123" t="s">
+        <v>389</v>
+      </c>
+      <c r="B123" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="124" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A124" t="s">
+        <v>380</v>
+      </c>
+      <c r="B124" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="125" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A125" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="B78" s="1" t="s">
+      <c r="B125" s="1" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A79" s="1" t="s">
+    <row r="126" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A126" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B79" s="1" t="s">
+      <c r="B126" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A80" s="1" t="s">
+    <row r="127" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A127" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="B80" s="3" t="s">
+      <c r="B127" s="3" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A81" s="1" t="s">
+    <row r="128" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A128" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B81" s="1" t="s">
+      <c r="B128" s="1" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A82" s="1" t="s">
+    <row r="129" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A129" s="1" t="s">
+        <v>253</v>
+      </c>
+      <c r="B129" s="1" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="130" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A130" s="1" t="s">
         <v>230</v>
       </c>
-      <c r="B82" t="s">
+      <c r="B130" t="s">
         <v>230</v>
       </c>
     </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A83" s="1" t="s">
+    <row r="131" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A131" s="1" t="s">
         <v>233</v>
       </c>
-      <c r="B83" t="s">
+      <c r="B131" t="s">
         <v>233</v>
       </c>
     </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A84" t="s">
+    <row r="132" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A132" t="s">
         <v>28</v>
       </c>
-      <c r="B84" s="1" t="s">
+      <c r="B132" s="1" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A85" s="1" t="s">
+    <row r="133" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A133" t="s">
+        <v>239</v>
+      </c>
+      <c r="B133" s="1" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="134" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A134" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="B134" s="1" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="135" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A135" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="B85" s="1" t="s">
+      <c r="B135" s="1" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A86" s="1" t="s">
+    <row r="136" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A136" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B86" s="1" t="s">
+      <c r="B136" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A87" s="1" t="s">
+    <row r="137" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A137" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B87" s="1" t="s">
+      <c r="B137" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A88" s="1" t="s">
+    <row r="138" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A138" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B88" s="1" t="s">
+      <c r="B138" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A89" s="1" t="s">
+    <row r="139" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A139" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="B89" s="1" t="s">
+      <c r="B139" s="1" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A90" s="1" t="s">
+    <row r="140" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A140" t="s">
+        <v>395</v>
+      </c>
+      <c r="B140" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="141" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A141" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="B90" s="1" t="s">
+      <c r="B141" s="1" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A91" t="s">
+    <row r="142" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A142" t="s">
         <v>164</v>
       </c>
-      <c r="B91" t="s">
+      <c r="B142" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A92" t="s">
+    <row r="143" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A143" t="s">
         <v>190</v>
       </c>
-      <c r="B92" t="s">
+      <c r="B143" t="s">
         <v>191</v>
       </c>
     </row>
-    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A93" s="1" t="s">
+    <row r="144" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A144" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="B93" s="1" t="s">
+      <c r="B144" s="1" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A94" t="s">
+    <row r="145" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A145" t="s">
+        <v>310</v>
+      </c>
+      <c r="B145" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="146" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A146" t="s">
+        <v>312</v>
+      </c>
+      <c r="B146" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="147" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A147" t="s">
+        <v>311</v>
+      </c>
+      <c r="B147" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="148" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A148" t="s">
+        <v>366</v>
+      </c>
+      <c r="B148" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="149" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A149" t="s">
+        <v>313</v>
+      </c>
+      <c r="B149" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="150" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A150" t="s">
         <v>159</v>
       </c>
-      <c r="B94" t="s">
+      <c r="B150" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A95" t="s">
+    <row r="151" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A151" t="s">
         <v>160</v>
       </c>
-      <c r="B95" t="s">
+      <c r="B151" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A96" t="s">
+    <row r="152" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A152" t="s">
         <v>165</v>
       </c>
-      <c r="B96" t="s">
+      <c r="B152" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A97" s="1" t="s">
+    <row r="153" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A153" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="B97" s="1" t="s">
+      <c r="B153" s="1" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A98" s="1" t="s">
+    <row r="154" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A154" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="B98" s="1" t="s">
+      <c r="B154" s="1" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A99" s="1" t="s">
+    <row r="155" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A155" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B99" s="1" t="s">
+      <c r="B155" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A100" t="s">
-        <v>239</v>
-      </c>
-      <c r="B100" s="1" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="101" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A101" s="1" t="s">
-        <v>240</v>
-      </c>
-      <c r="B101" s="1" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="102" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A102" s="1" t="s">
-        <v>243</v>
-      </c>
-      <c r="B102" s="1" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="103" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A103" s="1" t="s">
-        <v>245</v>
-      </c>
-      <c r="B103" s="1" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="104" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A104" s="1" t="s">
-        <v>246</v>
-      </c>
-      <c r="B104" s="1" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="105" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A105" s="1" t="s">
-        <v>249</v>
-      </c>
-      <c r="B105" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="106" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A106" s="1" t="s">
-        <v>248</v>
-      </c>
-      <c r="B106" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="107" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A107" s="1" t="s">
-        <v>252</v>
-      </c>
-      <c r="B107" s="1" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="108" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A108" s="1" t="s">
-        <v>253</v>
-      </c>
-      <c r="B108" s="1" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="109" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A109" s="1" t="s">
-        <v>260</v>
-      </c>
-      <c r="B109" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="110" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A110" s="1" t="s">
-        <v>262</v>
-      </c>
-      <c r="B110" s="1" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="111" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A111" s="1" t="s">
-        <v>266</v>
-      </c>
-      <c r="B111" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="112" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A112" t="s">
-        <v>268</v>
-      </c>
-      <c r="B112" s="1" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="113" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A113" s="1" t="s">
-        <v>271</v>
-      </c>
-      <c r="B113" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="114" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A114" s="1" t="s">
-        <v>274</v>
-      </c>
-      <c r="B114" t="s">
-        <v>275</v>
-      </c>
-    </row>
-    <row r="115" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A115" s="1" t="s">
-        <v>279</v>
-      </c>
-      <c r="B115" s="1" t="s">
-        <v>277</v>
-      </c>
-    </row>
-    <row r="116" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A116" s="1" t="s">
-        <v>280</v>
-      </c>
-      <c r="B116" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="117" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A117" s="1" t="s">
-        <v>281</v>
-      </c>
-      <c r="B117" t="s">
-        <v>284</v>
-      </c>
-    </row>
-    <row r="118" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A118" s="1" t="s">
-        <v>286</v>
-      </c>
-      <c r="B118" s="1" t="s">
-        <v>286</v>
-      </c>
-    </row>
-    <row r="119" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A119" s="1" t="s">
-        <v>288</v>
-      </c>
-      <c r="B119" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="120" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A120" s="1" t="s">
-        <v>291</v>
-      </c>
-      <c r="B120" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="121" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A121" s="1" t="s">
-        <v>294</v>
-      </c>
-      <c r="B121" t="s">
-        <v>295</v>
-      </c>
-    </row>
-    <row r="122" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A122" s="1" t="s">
-        <v>297</v>
-      </c>
-      <c r="B122" t="s">
-        <v>319</v>
-      </c>
-    </row>
-    <row r="123" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A123" t="s">
-        <v>299</v>
-      </c>
-      <c r="B123" t="s">
-        <v>320</v>
-      </c>
-    </row>
-    <row r="124" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A124" t="s">
-        <v>300</v>
-      </c>
-      <c r="B124" t="s">
-        <v>321</v>
-      </c>
-    </row>
-    <row r="125" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A125" t="s">
-        <v>301</v>
-      </c>
-      <c r="B125" t="s">
-        <v>322</v>
-      </c>
-    </row>
-    <row r="126" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A126" t="s">
-        <v>302</v>
-      </c>
-      <c r="B126" t="s">
-        <v>323</v>
-      </c>
-    </row>
-    <row r="127" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A127" t="s">
-        <v>303</v>
-      </c>
-      <c r="B127" t="s">
-        <v>324</v>
-      </c>
-    </row>
-    <row r="128" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A128" t="s">
-        <v>304</v>
-      </c>
-      <c r="B128" t="s">
-        <v>325</v>
-      </c>
-    </row>
-    <row r="129" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A129" t="s">
-        <v>305</v>
-      </c>
-      <c r="B129" t="s">
-        <v>326</v>
-      </c>
-    </row>
-    <row r="130" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A130" t="s">
-        <v>306</v>
-      </c>
-      <c r="B130" t="s">
-        <v>327</v>
-      </c>
-    </row>
-    <row r="131" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A131" t="s">
-        <v>307</v>
-      </c>
-      <c r="B131" t="s">
-        <v>328</v>
-      </c>
-    </row>
-    <row r="132" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A132" t="s">
-        <v>308</v>
-      </c>
-      <c r="B132" t="s">
-        <v>329</v>
-      </c>
-    </row>
-    <row r="133" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A133" t="s">
-        <v>309</v>
-      </c>
-      <c r="B133" t="s">
-        <v>330</v>
-      </c>
-    </row>
-    <row r="134" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A134" t="s">
-        <v>310</v>
-      </c>
-      <c r="B134" t="s">
-        <v>331</v>
-      </c>
-    </row>
-    <row r="135" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A135" t="s">
-        <v>311</v>
-      </c>
-      <c r="B135" t="s">
-        <v>332</v>
-      </c>
-    </row>
-    <row r="136" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A136" t="s">
-        <v>312</v>
-      </c>
-      <c r="B136" t="s">
-        <v>333</v>
-      </c>
-    </row>
-    <row r="137" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A137" t="s">
-        <v>313</v>
-      </c>
-      <c r="B137" t="s">
-        <v>334</v>
-      </c>
-    </row>
-    <row r="138" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A138" t="s">
-        <v>314</v>
-      </c>
-      <c r="B138" t="s">
-        <v>335</v>
-      </c>
-    </row>
-    <row r="139" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A139" t="s">
-        <v>315</v>
-      </c>
-      <c r="B139" t="s">
-        <v>336</v>
-      </c>
-    </row>
-    <row r="140" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A140" t="s">
-        <v>316</v>
-      </c>
-      <c r="B140" t="s">
-        <v>337</v>
-      </c>
-    </row>
-    <row r="141" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A141" t="s">
-        <v>317</v>
-      </c>
-      <c r="B141" t="s">
-        <v>338</v>
-      </c>
-    </row>
-    <row r="142" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A142" t="s">
-        <v>318</v>
-      </c>
-      <c r="B142" t="s">
-        <v>339</v>
-      </c>
-    </row>
-    <row r="143" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A143" t="s">
-        <v>360</v>
-      </c>
-      <c r="B143" t="s">
-        <v>361</v>
-      </c>
-    </row>
-    <row r="144" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A144" t="s">
-        <v>364</v>
-      </c>
-      <c r="B144" t="s">
-        <v>363</v>
-      </c>
-    </row>
-    <row r="145" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A145" t="s">
-        <v>366</v>
-      </c>
-      <c r="B145" t="s">
-        <v>365</v>
-      </c>
-    </row>
-    <row r="146" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A146" t="s">
-        <v>369</v>
-      </c>
-      <c r="B146" t="s">
-        <v>370</v>
-      </c>
-    </row>
-    <row r="147" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A147" t="s">
-        <v>373</v>
-      </c>
-      <c r="B147" t="s">
-        <v>372</v>
-      </c>
-    </row>
-    <row r="148" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A148" t="s">
-        <v>376</v>
-      </c>
-      <c r="B148" t="s">
-        <v>375</v>
+    <row r="156" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A156" s="1" t="s">
+        <v>399</v>
+      </c>
+      <c r="B156" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="157" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A157" s="1" t="s">
+        <v>401</v>
+      </c>
+      <c r="B157" s="1" t="s">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="158" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A158" s="1" t="s">
+        <v>403</v>
+      </c>
+      <c r="B158" s="1" t="s">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="159" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A159" s="1" t="s">
+        <v>405</v>
+      </c>
+      <c r="B159" s="1" t="s">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="160" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A160" s="1" t="s">
+        <v>410</v>
+      </c>
+      <c r="B160" t="s">
+        <v>411</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:B23">
-    <sortState ref="A2:B100">
-      <sortCondition ref="A1:A24"/>
+  <autoFilter ref="A1:B23" xr:uid="{00000000-0009-0000-0000-000000000000}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B155">
+      <sortCondition ref="A1:A23"/>
     </sortState>
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
@@ -2748,20 +2950,20 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B148"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:B160"/>
   <sheetViews>
-    <sheetView topLeftCell="A127" workbookViewId="0">
-      <selection activeCell="A146" sqref="A146:B148"/>
+    <sheetView tabSelected="1" topLeftCell="A142" workbookViewId="0">
+      <selection activeCell="B160" sqref="B160"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="31.5703125" customWidth="1"/>
-    <col min="2" max="2" width="57.5703125" customWidth="1"/>
+    <col min="1" max="1" width="31.54296875" customWidth="1"/>
+    <col min="2" max="2" width="57.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>20</v>
       </c>
@@ -2769,7 +2971,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>50</v>
       </c>
@@ -2777,1178 +2979,1274 @@
         <v>221</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>364</v>
+      </c>
+      <c r="B3" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A4" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B4" s="1" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A5" s="1" t="s">
+        <v>249</v>
+      </c>
+      <c r="B5" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A6" s="1" t="s">
+        <v>248</v>
+      </c>
+      <c r="B6" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A7" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B7" s="1" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
         <v>162</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B8" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A9" s="1" t="s">
         <v>224</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B9" t="s">
         <v>228</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A10" s="1" t="s">
         <v>226</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B10" t="s">
         <v>229</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A11" s="1" t="s">
         <v>151</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B11" s="1" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A12" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="B12" s="1" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A13" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="B13" s="1" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A14" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="B14" s="1" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A15" s="1" t="s">
         <v>231</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B15" t="s">
         <v>232</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A16" s="1" t="s">
+        <v>288</v>
+      </c>
+      <c r="B16" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A17" s="1" t="s">
+        <v>297</v>
+      </c>
+      <c r="B17" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A18" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="B13" s="1" t="s">
+      <c r="B18" s="1" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="s">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A19" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="B19" s="1" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" s="1" t="s">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A20" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B15" s="1" t="s">
+      <c r="B20" s="1" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
         <v>196</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B21" t="s">
         <v>198</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" s="1" t="s">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A22" s="1" t="s">
+        <v>271</v>
+      </c>
+      <c r="B22" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A23" t="s">
+        <v>300</v>
+      </c>
+      <c r="B23" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A24" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="B17" s="1" t="s">
+      <c r="B24" s="1" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" s="1" t="s">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A25" t="s">
+        <v>369</v>
+      </c>
+      <c r="B25" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A26" t="s">
+        <v>373</v>
+      </c>
+      <c r="B26" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A27" t="s">
+        <v>268</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A28" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B18" s="1" t="s">
+      <c r="B28" s="1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" s="1" t="s">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A29" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B19" s="1" t="s">
+      <c r="B29" s="1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A30" s="1" t="s">
+        <v>260</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A31" t="s">
         <v>142</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B31" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" s="1" t="s">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A32" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="B21" s="1" t="s">
+      <c r="B32" s="1" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" s="1" t="s">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A33" s="1" t="s">
+        <v>245</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A34" t="s">
+        <v>299</v>
+      </c>
+      <c r="B34" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A35" s="1" t="s">
         <v>223</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B35" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" s="1" t="s">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A36" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="B23" t="s">
+      <c r="B36" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24" s="1" t="s">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A37" t="s">
+        <v>307</v>
+      </c>
+      <c r="B37" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A38" t="s">
+        <v>309</v>
+      </c>
+      <c r="B38" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A39" t="s">
+        <v>306</v>
+      </c>
+      <c r="B39" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A40" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="B24" s="1" t="s">
+      <c r="B40" s="1" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25" s="1" t="s">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A41" s="1" t="s">
         <v>199</v>
       </c>
-      <c r="B25" s="1" t="s">
+      <c r="B41" s="1" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A26" s="1" t="s">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A42" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B26" s="1" t="s">
+      <c r="B42" s="1" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A27" s="1" t="s">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A43" s="1" t="s">
+        <v>291</v>
+      </c>
+      <c r="B43" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A44" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="B27" s="1" t="s">
+      <c r="B44" s="1" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A28" s="1" t="s">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A45" t="s">
+        <v>376</v>
+      </c>
+      <c r="B45" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A46" s="1" t="s">
         <v>234</v>
       </c>
-      <c r="B28" t="s">
+      <c r="B46" t="s">
         <v>235</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A47" t="s">
         <v>139</v>
       </c>
-      <c r="B29" t="s">
+      <c r="B47" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A30" s="1" t="s">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A48" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="B30" t="s">
+      <c r="B48" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A31" s="1" t="s">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A49" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="B31" t="s">
+      <c r="B49" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A32" s="1" t="s">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A50" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B32" s="1" t="s">
+      <c r="B50" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A33" s="1" t="s">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A51" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="B33" t="s">
+      <c r="B51" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A34" s="1" t="s">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A52" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A53" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="B34" s="1" t="s">
+      <c r="B53" s="1" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A35" s="1" t="s">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A54" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="B35" s="1" t="s">
+      <c r="B54" s="1" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A55" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="B55" s="1" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A56" t="s">
         <v>141</v>
       </c>
-      <c r="B36" t="s">
+      <c r="B56" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A57" t="s">
+        <v>305</v>
+      </c>
+      <c r="B57" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A58" t="s">
+        <v>360</v>
+      </c>
+      <c r="B58" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A59" t="s">
+        <v>308</v>
+      </c>
+      <c r="B59" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A60" t="s">
+        <v>302</v>
+      </c>
+      <c r="B60" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A61" t="s">
+        <v>304</v>
+      </c>
+      <c r="B61" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A62" t="s">
         <v>201</v>
       </c>
-      <c r="B37" t="s">
+      <c r="B62" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
+    <row r="63" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A63" t="s">
         <v>193</v>
       </c>
-      <c r="B38" t="s">
+      <c r="B63" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A39" s="1" t="s">
+    <row r="64" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A64" s="1" t="s">
         <v>213</v>
       </c>
-      <c r="B39" t="s">
+      <c r="B64" t="s">
         <v>210</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A40" s="1" t="s">
+    <row r="65" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A65" s="1" t="s">
         <v>214</v>
       </c>
-      <c r="B40" t="s">
+      <c r="B65" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A41" s="1" t="s">
+    <row r="66" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A66" s="1" t="s">
         <v>219</v>
       </c>
-      <c r="B41" t="s">
+      <c r="B66" t="s">
         <v>211</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A42" s="1" t="s">
+    <row r="67" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A67" s="1" t="s">
         <v>220</v>
       </c>
-      <c r="B42" t="s">
+      <c r="B67" t="s">
         <v>212</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A43" s="1" t="s">
+    <row r="68" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A68" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B43" s="1" t="s">
+      <c r="B68" s="1" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
+    <row r="69" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A69" t="s">
         <v>140</v>
       </c>
-      <c r="B44" t="s">
+      <c r="B69" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A45" s="1" t="s">
+    <row r="70" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A70" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B45" s="1" t="s">
+      <c r="B70" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A46" s="1" t="s">
+    <row r="71" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A71" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="B46" s="1" t="s">
+      <c r="B71" s="1" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A47" s="1" t="s">
+    <row r="72" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A72" t="s">
+        <v>303</v>
+      </c>
+      <c r="B72" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A73" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="B73" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A74" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B47" s="1" t="s">
+      <c r="B74" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A48" t="s">
+    <row r="75" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A75" t="s">
         <v>161</v>
       </c>
-      <c r="B48" t="s">
+      <c r="B75" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A49" t="s">
+    <row r="76" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A76" t="s">
         <v>163</v>
       </c>
-      <c r="B49" t="s">
+      <c r="B76" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A50" t="s">
+    <row r="77" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A77" t="s">
         <v>166</v>
       </c>
-      <c r="B50" t="s">
+      <c r="B77" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A51" t="s">
+    <row r="78" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A78" t="s">
         <v>27</v>
       </c>
-      <c r="B51" s="1" t="s">
+      <c r="B78" s="1" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A52" s="1" t="s">
+    <row r="79" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A79" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="B52" s="1" t="s">
+      <c r="B79" s="1" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A53" s="1" t="s">
+    <row r="80" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A80" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="B53" s="1" t="s">
+      <c r="B80" s="1" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A54" t="s">
+    <row r="81" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A81" t="s">
         <v>148</v>
       </c>
-      <c r="B54" s="1" t="s">
+      <c r="B81" s="1" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A55" s="1" t="s">
+    <row r="82" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A82" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B55" t="s">
+      <c r="B82" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A56" t="s">
+    <row r="83" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A83" t="s">
         <v>204</v>
       </c>
-      <c r="B56" s="1" t="s">
+      <c r="B83" s="1" t="s">
         <v>205</v>
       </c>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A57" t="s">
+    <row r="84" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A84" t="s">
         <v>131</v>
       </c>
-      <c r="B57" s="1" t="s">
+      <c r="B84" s="1" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A58" s="1" t="s">
+    <row r="85" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A85" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="B58" s="1" t="s">
+      <c r="B85" s="1" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A59" t="s">
+    <row r="86" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A86" t="s">
         <v>167</v>
       </c>
-      <c r="B59" t="s">
+      <c r="B86" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A60" t="s">
+    <row r="87" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A87" t="s">
         <v>168</v>
       </c>
-      <c r="B60" t="s">
+      <c r="B87" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A61" t="s">
+    <row r="88" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A88" t="s">
         <v>169</v>
       </c>
-      <c r="B61" t="s">
+      <c r="B88" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A62" s="1" t="s">
+    <row r="89" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A89" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="B62" s="1" t="s">
+      <c r="B89" s="1" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A63" s="1" t="s">
+    <row r="90" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A90" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="B63" s="1" t="s">
+      <c r="B90" s="1" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A64" s="1" t="s">
+    <row r="91" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A91" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="B64" t="s">
+      <c r="B91" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A65" s="1" t="s">
+    <row r="92" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A92" s="1" t="s">
+        <v>262</v>
+      </c>
+      <c r="B92" s="1" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A93" s="1" t="s">
+        <v>266</v>
+      </c>
+      <c r="B93" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A94" s="1" t="s">
+        <v>280</v>
+      </c>
+      <c r="B94" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A95" t="s">
+        <v>301</v>
+      </c>
+      <c r="B95" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A96" t="s">
+        <v>316</v>
+      </c>
+      <c r="B96" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A97" t="s">
+        <v>317</v>
+      </c>
+      <c r="B97" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A98" t="s">
+        <v>315</v>
+      </c>
+      <c r="B98" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A99" t="s">
+        <v>318</v>
+      </c>
+      <c r="B99" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A100" t="s">
+        <v>314</v>
+      </c>
+      <c r="B100" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A101" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="B65" s="1" t="s">
+      <c r="B101" s="1" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A66" s="1" t="s">
+    <row r="102" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A102" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="B66" s="1" t="s">
+      <c r="B102" s="1" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A67" s="1" t="s">
+    <row r="103" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A103" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="B67" s="1" t="s">
+      <c r="B103" s="1" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A68" t="s">
+    <row r="104" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A104" t="s">
         <v>29</v>
       </c>
-      <c r="B68" s="1" t="s">
+      <c r="B104" s="1" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A69" s="1" t="s">
+    <row r="105" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A105" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="B69" s="1" t="s">
+      <c r="B105" s="1" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A70" s="1" t="s">
+    <row r="106" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A106" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="B70" t="s">
+      <c r="B106" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A71" s="1" t="s">
+    <row r="107" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A107" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="B71" s="1" t="s">
+      <c r="B107" s="1" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A72" s="1" t="s">
+    <row r="108" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A108" s="1" t="s">
         <v>206</v>
       </c>
-      <c r="B72" s="1" t="s">
+      <c r="B108" s="1" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A73" s="1" t="s">
+    <row r="109" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A109" s="1" t="s">
+        <v>252</v>
+      </c>
+      <c r="B109" s="1" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="110" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A110" s="1" t="s">
+        <v>281</v>
+      </c>
+      <c r="B110" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="111" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A111" s="1" t="s">
+        <v>294</v>
+      </c>
+      <c r="B111" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="112" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A112" s="1" t="s">
+        <v>279</v>
+      </c>
+      <c r="B112" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="113" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A113" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="B73" s="1" t="s">
+      <c r="B113" s="1" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A74" s="1" t="s">
+    <row r="114" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A114" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="B74" t="s">
+      <c r="B114" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A75" s="1" t="s">
+    <row r="115" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A115" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="B75" s="1" t="s">
+      <c r="B115" s="1" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A76" s="1" t="s">
+    <row r="116" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A116" s="1" t="s">
+        <v>286</v>
+      </c>
+      <c r="B116" s="1" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="117" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A117" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="B76" s="1" t="s">
+      <c r="B117" s="1" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A77" s="1" t="s">
+    <row r="118" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A118" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="B77" s="1" t="s">
+      <c r="B118" s="1" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A78" s="1" t="s">
+    <row r="119" spans="1:2" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A119" t="s">
+        <v>384</v>
+      </c>
+      <c r="B119" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="120" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A120" t="s">
+        <v>378</v>
+      </c>
+      <c r="B120" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="121" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A121" t="s">
+        <v>386</v>
+      </c>
+      <c r="B121" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="122" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A122" t="s">
+        <v>394</v>
+      </c>
+      <c r="B122" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="123" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A123" t="s">
+        <v>389</v>
+      </c>
+      <c r="B123" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="124" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A124" t="s">
+        <v>380</v>
+      </c>
+      <c r="B124" t="s">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="125" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A125" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="B78" s="1" t="s">
+      <c r="B125" s="1" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A79" s="1" t="s">
+    <row r="126" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A126" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B79" s="1" t="s">
+      <c r="B126" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A80" s="1" t="s">
+    <row r="127" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A127" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="B80" s="1" t="s">
+      <c r="B127" s="1" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A81" s="1" t="s">
+    <row r="128" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A128" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B81" s="1" t="s">
+      <c r="B128" s="1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A82" s="1" t="s">
+    <row r="129" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A129" s="1" t="s">
+        <v>253</v>
+      </c>
+      <c r="B129" s="1" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="130" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A130" s="1" t="s">
         <v>230</v>
       </c>
-      <c r="B82" t="s">
+      <c r="B130" t="s">
         <v>230</v>
       </c>
     </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A83" s="1" t="s">
+    <row r="131" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A131" s="1" t="s">
         <v>233</v>
       </c>
-      <c r="B83" s="1" t="s">
+      <c r="B131" s="1" t="s">
         <v>236</v>
       </c>
     </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A84" t="s">
+    <row r="132" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A132" t="s">
         <v>28</v>
       </c>
-      <c r="B84" s="1" t="s">
+      <c r="B132" s="1" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A85" s="1" t="s">
+    <row r="133" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A133" t="s">
+        <v>239</v>
+      </c>
+      <c r="B133" s="1" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="134" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A134" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="B134" s="1" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="135" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A135" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="B85" s="1" t="s">
+      <c r="B135" s="1" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A86" s="1" t="s">
+    <row r="136" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A136" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B86" s="1" t="s">
+      <c r="B136" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A87" s="1" t="s">
+    <row r="137" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A137" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B87" s="1" t="s">
+      <c r="B137" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A88" s="1" t="s">
+    <row r="138" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A138" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B88" s="1" t="s">
+      <c r="B138" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A89" s="1" t="s">
+    <row r="139" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A139" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="B89" s="1" t="s">
+      <c r="B139" s="1" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A90" s="1" t="s">
+    <row r="140" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A140" t="s">
+        <v>395</v>
+      </c>
+      <c r="B140" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="141" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A141" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="B90" s="1" t="s">
+      <c r="B141" s="1" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A91" t="s">
+    <row r="142" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A142" t="s">
         <v>164</v>
       </c>
-      <c r="B91" t="s">
+      <c r="B142" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A92" t="s">
+    <row r="143" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A143" t="s">
         <v>190</v>
       </c>
-      <c r="B92" t="s">
+      <c r="B143" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A93" s="1" t="s">
+    <row r="144" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A144" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="B93" s="1" t="s">
+      <c r="B144" s="1" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A94" t="s">
+    <row r="145" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A145" t="s">
+        <v>310</v>
+      </c>
+      <c r="B145" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="146" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A146" t="s">
+        <v>312</v>
+      </c>
+      <c r="B146" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="147" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A147" t="s">
+        <v>311</v>
+      </c>
+      <c r="B147" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="148" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A148" t="s">
+        <v>366</v>
+      </c>
+      <c r="B148" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="149" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A149" t="s">
+        <v>313</v>
+      </c>
+      <c r="B149" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="150" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A150" t="s">
         <v>159</v>
       </c>
-      <c r="B94" t="s">
+      <c r="B150" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A95" t="s">
+    <row r="151" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A151" t="s">
         <v>160</v>
       </c>
-      <c r="B95" t="s">
+      <c r="B151" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A96" t="s">
+    <row r="152" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A152" t="s">
         <v>165</v>
       </c>
-      <c r="B96" t="s">
+      <c r="B152" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A97" s="1" t="s">
+    <row r="153" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A153" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="B97" s="1" t="s">
+      <c r="B153" s="1" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A98" s="1" t="s">
+    <row r="154" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A154" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="B98" s="1" t="s">
+      <c r="B154" s="1" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A99" s="1" t="s">
+    <row r="155" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A155" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B99" s="1" t="s">
+      <c r="B155" s="1" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A100" t="s">
-        <v>239</v>
-      </c>
-      <c r="B100" s="1" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="101" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A101" s="1" t="s">
-        <v>240</v>
-      </c>
-      <c r="B101" s="1" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="102" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A102" s="1" t="s">
-        <v>243</v>
-      </c>
-      <c r="B102" s="1" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="103" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A103" s="1" t="s">
-        <v>245</v>
-      </c>
-      <c r="B103" s="1" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="104" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A104" s="1" t="s">
-        <v>246</v>
-      </c>
-      <c r="B104" s="1" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="105" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A105" s="1" t="s">
-        <v>249</v>
-      </c>
-      <c r="B105" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="106" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A106" s="1" t="s">
-        <v>248</v>
-      </c>
-      <c r="B106" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="107" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A107" s="1" t="s">
-        <v>252</v>
-      </c>
-      <c r="B107" s="1" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="108" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A108" s="1" t="s">
-        <v>253</v>
-      </c>
-      <c r="B108" s="1" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="109" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A109" s="1" t="s">
-        <v>260</v>
-      </c>
-      <c r="B109" s="1" t="s">
-        <v>264</v>
-      </c>
-    </row>
-    <row r="110" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A110" s="1" t="s">
-        <v>262</v>
-      </c>
-      <c r="B110" s="1" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="111" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A111" s="1" t="s">
-        <v>266</v>
-      </c>
-      <c r="B111" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="112" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A112" t="s">
-        <v>268</v>
-      </c>
-      <c r="B112" s="1" t="s">
-        <v>269</v>
-      </c>
-    </row>
-    <row r="113" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A113" s="1" t="s">
-        <v>271</v>
-      </c>
-      <c r="B113" t="s">
-        <v>273</v>
-      </c>
-    </row>
-    <row r="114" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A114" s="1" t="s">
-        <v>274</v>
-      </c>
-      <c r="B114" t="s">
-        <v>276</v>
-      </c>
-    </row>
-    <row r="115" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A115" s="1" t="s">
-        <v>279</v>
-      </c>
-      <c r="B115" t="s">
-        <v>278</v>
-      </c>
-    </row>
-    <row r="116" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A116" s="1" t="s">
-        <v>280</v>
-      </c>
-      <c r="B116" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="117" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A117" s="1" t="s">
-        <v>281</v>
-      </c>
-      <c r="B117" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="118" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A118" s="1" t="s">
-        <v>286</v>
-      </c>
-      <c r="B118" s="1" t="s">
-        <v>287</v>
-      </c>
-    </row>
-    <row r="119" spans="1:2" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A119" s="1" t="s">
-        <v>288</v>
-      </c>
-      <c r="B119" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="120" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A120" s="1" t="s">
-        <v>291</v>
-      </c>
-      <c r="B120" t="s">
-        <v>293</v>
-      </c>
-    </row>
-    <row r="121" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A121" s="1" t="s">
-        <v>294</v>
-      </c>
-      <c r="B121" t="s">
-        <v>296</v>
-      </c>
-    </row>
-    <row r="122" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A122" s="1" t="s">
-        <v>297</v>
-      </c>
-      <c r="B122" t="s">
-        <v>298</v>
-      </c>
-    </row>
-    <row r="123" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A123" t="s">
-        <v>299</v>
-      </c>
-      <c r="B123" t="s">
-        <v>340</v>
-      </c>
-    </row>
-    <row r="124" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A124" t="s">
-        <v>300</v>
-      </c>
-      <c r="B124" t="s">
-        <v>341</v>
-      </c>
-    </row>
-    <row r="125" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A125" t="s">
-        <v>301</v>
-      </c>
-      <c r="B125" t="s">
-        <v>342</v>
-      </c>
-    </row>
-    <row r="126" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A126" t="s">
-        <v>302</v>
-      </c>
-      <c r="B126" t="s">
-        <v>343</v>
-      </c>
-    </row>
-    <row r="127" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A127" t="s">
-        <v>303</v>
-      </c>
-      <c r="B127" t="s">
-        <v>344</v>
-      </c>
-    </row>
-    <row r="128" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A128" t="s">
-        <v>304</v>
-      </c>
-      <c r="B128" t="s">
-        <v>345</v>
-      </c>
-    </row>
-    <row r="129" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A129" t="s">
-        <v>305</v>
-      </c>
-      <c r="B129" t="s">
-        <v>346</v>
-      </c>
-    </row>
-    <row r="130" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A130" t="s">
-        <v>306</v>
-      </c>
-      <c r="B130" t="s">
-        <v>347</v>
-      </c>
-    </row>
-    <row r="131" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A131" t="s">
-        <v>307</v>
-      </c>
-      <c r="B131" t="s">
-        <v>348</v>
-      </c>
-    </row>
-    <row r="132" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A132" t="s">
-        <v>308</v>
-      </c>
-      <c r="B132" t="s">
-        <v>351</v>
-      </c>
-    </row>
-    <row r="133" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A133" t="s">
-        <v>309</v>
-      </c>
-      <c r="B133" t="s">
-        <v>349</v>
-      </c>
-    </row>
-    <row r="134" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A134" t="s">
-        <v>310</v>
-      </c>
-      <c r="B134" t="s">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="135" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A135" t="s">
-        <v>311</v>
-      </c>
-      <c r="B135" t="s">
-        <v>352</v>
-      </c>
-    </row>
-    <row r="136" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A136" t="s">
-        <v>312</v>
-      </c>
-      <c r="B136" t="s">
-        <v>353</v>
-      </c>
-    </row>
-    <row r="137" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A137" t="s">
-        <v>313</v>
-      </c>
-      <c r="B137" t="s">
-        <v>354</v>
-      </c>
-    </row>
-    <row r="138" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A138" t="s">
-        <v>314</v>
-      </c>
-      <c r="B138" t="s">
-        <v>355</v>
-      </c>
-    </row>
-    <row r="139" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A139" t="s">
-        <v>315</v>
-      </c>
-      <c r="B139" t="s">
-        <v>356</v>
-      </c>
-    </row>
-    <row r="140" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A140" t="s">
-        <v>316</v>
-      </c>
-      <c r="B140" t="s">
-        <v>357</v>
-      </c>
-    </row>
-    <row r="141" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A141" t="s">
-        <v>317</v>
-      </c>
-      <c r="B141" t="s">
-        <v>358</v>
-      </c>
-    </row>
-    <row r="142" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A142" t="s">
-        <v>318</v>
-      </c>
-      <c r="B142" t="s">
-        <v>359</v>
-      </c>
-    </row>
-    <row r="143" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A143" t="s">
-        <v>360</v>
-      </c>
-      <c r="B143" t="s">
-        <v>362</v>
-      </c>
-    </row>
-    <row r="144" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A144" t="s">
-        <v>364</v>
-      </c>
-      <c r="B144" t="s">
-        <v>367</v>
-      </c>
-    </row>
-    <row r="145" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A145" t="s">
-        <v>366</v>
-      </c>
-      <c r="B145" t="s">
-        <v>368</v>
-      </c>
-    </row>
-    <row r="146" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A146" t="s">
-        <v>369</v>
-      </c>
-      <c r="B146" t="s">
-        <v>371</v>
-      </c>
-    </row>
-    <row r="147" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A147" t="s">
-        <v>373</v>
-      </c>
-      <c r="B147" t="s">
-        <v>374</v>
-      </c>
-    </row>
-    <row r="148" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A148" t="s">
-        <v>376</v>
-      </c>
-      <c r="B148" t="s">
-        <v>377</v>
+    <row r="156" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A156" s="1" t="s">
+        <v>399</v>
+      </c>
+      <c r="B156" t="s">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="157" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A157" s="1" t="s">
+        <v>401</v>
+      </c>
+      <c r="B157" s="1" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="158" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A158" s="1" t="s">
+        <v>403</v>
+      </c>
+      <c r="B158" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="159" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A159" s="1" t="s">
+        <v>405</v>
+      </c>
+      <c r="B159" s="1" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="160" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A160" s="1" t="s">
+        <v>410</v>
+      </c>
+      <c r="B160" t="s">
+        <v>412</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:B23">
-    <sortState ref="A2:B100">
-      <sortCondition ref="A1:A24"/>
+  <autoFilter ref="A1:B23" xr:uid="{00000000-0009-0000-0000-000001000000}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B155">
+      <sortCondition ref="A1:A23"/>
     </sortState>
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Error message popups added
</commit_message>
<xml_diff>
--- a/Vitae/Library/Resources/SharedResource.xlsx
+++ b/Vitae/Library/Resources/SharedResource.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\Vitae\Library\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0670FD9D-6760-4A8F-A6D8-510AE0BACF6D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{692201AF-4292-41FA-A46F-7D03068E348D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5590" yWindow="1810" windowWidth="22500" windowHeight="14260" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5590" yWindow="1810" windowWidth="22500" windowHeight="14260" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="en" sheetId="3" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="680" uniqueCount="440">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="688" uniqueCount="445">
   <si>
     <t>City</t>
   </si>
@@ -1109,9 +1109,6 @@
     <t>Passwörter müssen mindestens ein Kleinbuchstabe ('a'-'z') haben.</t>
   </si>
   <si>
-    <t>Passwörter müssen mindestens ein Großbuchstabenzeichen ('A'-'Z') haben.</t>
-  </si>
-  <si>
     <t>InvalidLoginAttempt</t>
   </si>
   <si>
@@ -1350,6 +1347,24 @@
   </si>
   <si>
     <t>Change</t>
+  </si>
+  <si>
+    <t>Passwörter müssen mindestens ein Grossbuchstabenzeichen ('A'-'Z') haben.</t>
+  </si>
+  <si>
+    <t>TheLogout</t>
+  </si>
+  <si>
+    <t>Abmeldung</t>
+  </si>
+  <si>
+    <t>ResetPasswordBy</t>
+  </si>
+  <si>
+    <t>Please reset your password by</t>
+  </si>
+  <si>
+    <t>Bitte setzen Sie ihr Passwort zurück in dem Sie</t>
   </si>
 </sst>
 </file>
@@ -1727,10 +1742,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B170"/>
+  <dimension ref="A1:B172"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A153" workbookViewId="0">
-      <selection activeCell="A170" sqref="A170:B170"/>
+    <sheetView topLeftCell="A153" workbookViewId="0">
+      <selection activeCell="A172" sqref="A172:B172"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1757,10 +1772,10 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="B3" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
@@ -1933,18 +1948,18 @@
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
+        <v>368</v>
+      </c>
+      <c r="B25" t="s">
         <v>369</v>
-      </c>
-      <c r="B25" t="s">
-        <v>370</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="B26" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.35">
@@ -2093,10 +2108,10 @@
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="B45" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.35">
@@ -2197,10 +2212,10 @@
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
+        <v>359</v>
+      </c>
+      <c r="B58" t="s">
         <v>360</v>
-      </c>
-      <c r="B58" t="s">
-        <v>361</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.35">
@@ -2685,50 +2700,50 @@
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A119" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="B119" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
     </row>
     <row r="120" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A120" t="s">
+        <v>377</v>
+      </c>
+      <c r="B120" t="s">
         <v>378</v>
-      </c>
-      <c r="B120" t="s">
-        <v>379</v>
       </c>
     </row>
     <row r="121" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A121" t="s">
+        <v>385</v>
+      </c>
+      <c r="B121" t="s">
         <v>386</v>
-      </c>
-      <c r="B121" t="s">
-        <v>387</v>
       </c>
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A122" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="B122" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
     </row>
     <row r="123" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A123" t="s">
+        <v>388</v>
+      </c>
+      <c r="B123" t="s">
         <v>389</v>
-      </c>
-      <c r="B123" t="s">
-        <v>390</v>
       </c>
     </row>
     <row r="124" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A124" t="s">
+        <v>379</v>
+      </c>
+      <c r="B124" t="s">
         <v>380</v>
-      </c>
-      <c r="B124" t="s">
-        <v>381</v>
       </c>
     </row>
     <row r="125" spans="1:2" x14ac:dyDescent="0.35">
@@ -2853,10 +2868,10 @@
     </row>
     <row r="140" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A140" t="s">
+        <v>394</v>
+      </c>
+      <c r="B140" t="s">
         <v>395</v>
-      </c>
-      <c r="B140" t="s">
-        <v>396</v>
       </c>
     </row>
     <row r="141" spans="1:2" x14ac:dyDescent="0.35">
@@ -2917,10 +2932,10 @@
     </row>
     <row r="148" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A148" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="B148" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
     </row>
     <row r="149" spans="1:2" x14ac:dyDescent="0.35">
@@ -2981,122 +2996,138 @@
     </row>
     <row r="156" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A156" s="1" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="B156" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
     </row>
     <row r="157" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A157" s="1" t="s">
+        <v>400</v>
+      </c>
+      <c r="B157" s="1" t="s">
         <v>401</v>
-      </c>
-      <c r="B157" s="1" t="s">
-        <v>402</v>
       </c>
     </row>
     <row r="158" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A158" s="1" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="B158" s="1" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
     </row>
     <row r="159" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A159" s="1" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="B159" s="1" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
     </row>
     <row r="160" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A160" s="1" t="s">
+        <v>409</v>
+      </c>
+      <c r="B160" t="s">
         <v>410</v>
-      </c>
-      <c r="B160" t="s">
-        <v>411</v>
       </c>
     </row>
     <row r="161" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A161" s="1" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="B161" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
     </row>
     <row r="162" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A162" s="1" t="s">
+        <v>415</v>
+      </c>
+      <c r="B162" t="s">
         <v>416</v>
-      </c>
-      <c r="B162" t="s">
-        <v>417</v>
       </c>
     </row>
     <row r="163" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A163" s="1" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="B163" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
     </row>
     <row r="164" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A164" s="1" t="s">
+        <v>420</v>
+      </c>
+      <c r="B164" t="s">
         <v>421</v>
-      </c>
-      <c r="B164" t="s">
-        <v>422</v>
       </c>
     </row>
     <row r="165" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A165" s="1" t="s">
+        <v>422</v>
+      </c>
+      <c r="B165" t="s">
         <v>423</v>
-      </c>
-      <c r="B165" t="s">
-        <v>424</v>
       </c>
     </row>
     <row r="166" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A166" s="1" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="B166" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="167" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A167" s="1" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="B167" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
     </row>
     <row r="168" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A168" s="1" t="s">
+        <v>432</v>
+      </c>
+      <c r="B168" t="s">
         <v>433</v>
-      </c>
-      <c r="B168" t="s">
-        <v>434</v>
       </c>
     </row>
     <row r="169" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A169" s="1" t="s">
+        <v>435</v>
+      </c>
+      <c r="B169" t="s">
         <v>436</v>
-      </c>
-      <c r="B169" t="s">
-        <v>437</v>
       </c>
     </row>
     <row r="170" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A170" s="1" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="B170" t="s">
-        <v>439</v>
+        <v>438</v>
+      </c>
+    </row>
+    <row r="171" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A171" s="1" t="s">
+        <v>440</v>
+      </c>
+      <c r="B171" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="172" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A172" s="1" t="s">
+        <v>442</v>
+      </c>
+      <c r="B172" t="s">
+        <v>443</v>
       </c>
     </row>
   </sheetData>
@@ -3112,10 +3143,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:B170"/>
+  <dimension ref="A1:B172"/>
   <sheetViews>
-    <sheetView topLeftCell="A174" workbookViewId="0">
-      <selection activeCell="B74" sqref="B74"/>
+    <sheetView tabSelected="1" topLeftCell="A154" workbookViewId="0">
+      <selection activeCell="A172" sqref="A172:B172"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3142,10 +3173,10 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="B3" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
@@ -3318,18 +3349,18 @@
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="B25" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
+        <v>372</v>
+      </c>
+      <c r="B26" t="s">
         <v>373</v>
-      </c>
-      <c r="B26" t="s">
-        <v>374</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.35">
@@ -3478,10 +3509,10 @@
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
+        <v>375</v>
+      </c>
+      <c r="B45" t="s">
         <v>376</v>
-      </c>
-      <c r="B45" t="s">
-        <v>377</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.35">
@@ -3582,10 +3613,10 @@
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="B58" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.35">
@@ -3913,7 +3944,7 @@
         <v>318</v>
       </c>
       <c r="B99" t="s">
-        <v>359</v>
+        <v>439</v>
       </c>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.35">
@@ -4070,50 +4101,50 @@
     </row>
     <row r="119" spans="1:2" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A119" t="s">
+        <v>383</v>
+      </c>
+      <c r="B119" t="s">
         <v>384</v>
-      </c>
-      <c r="B119" t="s">
-        <v>385</v>
       </c>
     </row>
     <row r="120" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A120" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="B120" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
     </row>
     <row r="121" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A121" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="B121" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A122" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="B122" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
     </row>
     <row r="123" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A123" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="B123" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
     </row>
     <row r="124" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A124" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="B124" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
     </row>
     <row r="125" spans="1:2" x14ac:dyDescent="0.35">
@@ -4238,10 +4269,10 @@
     </row>
     <row r="140" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A140" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="B140" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
     </row>
     <row r="141" spans="1:2" x14ac:dyDescent="0.35">
@@ -4302,10 +4333,10 @@
     </row>
     <row r="148" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A148" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="B148" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
     </row>
     <row r="149" spans="1:2" x14ac:dyDescent="0.35">
@@ -4366,122 +4397,138 @@
     </row>
     <row r="156" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A156" s="1" t="s">
+        <v>398</v>
+      </c>
+      <c r="B156" t="s">
         <v>399</v>
-      </c>
-      <c r="B156" t="s">
-        <v>400</v>
       </c>
     </row>
     <row r="157" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A157" s="1" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="B157" s="1" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
     </row>
     <row r="158" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A158" s="1" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="B158" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
     </row>
     <row r="159" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A159" s="1" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="B159" s="1" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
     </row>
     <row r="160" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A160" s="1" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="B160" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
     </row>
     <row r="161" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A161" s="1" t="s">
+        <v>413</v>
+      </c>
+      <c r="B161" t="s">
         <v>414</v>
-      </c>
-      <c r="B161" t="s">
-        <v>415</v>
       </c>
     </row>
     <row r="162" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A162" s="1" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="B162" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
     </row>
     <row r="163" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A163" s="1" t="s">
+        <v>418</v>
+      </c>
+      <c r="B163" t="s">
         <v>419</v>
-      </c>
-      <c r="B163" t="s">
-        <v>420</v>
       </c>
     </row>
     <row r="164" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A164" s="1" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="B164" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
     </row>
     <row r="165" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A165" s="1" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="B165" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
     </row>
     <row r="166" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A166" s="1" t="s">
+        <v>426</v>
+      </c>
+      <c r="B166" t="s">
         <v>427</v>
-      </c>
-      <c r="B166" t="s">
-        <v>428</v>
       </c>
     </row>
     <row r="167" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A167" s="1" t="s">
+        <v>429</v>
+      </c>
+      <c r="B167" t="s">
         <v>430</v>
-      </c>
-      <c r="B167" t="s">
-        <v>431</v>
       </c>
     </row>
     <row r="168" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A168" s="1" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B168" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
     </row>
     <row r="169" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A169" s="1" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B169" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
     </row>
     <row r="170" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A170" s="1" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="B170" t="s">
         <v>12</v>
+      </c>
+    </row>
+    <row r="171" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A171" s="1" t="s">
+        <v>440</v>
+      </c>
+      <c r="B171" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="172" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A172" s="1" t="s">
+        <v>442</v>
+      </c>
+      <c r="B172" t="s">
+        <v>444</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Access denied messages added
</commit_message>
<xml_diff>
--- a/Vitae/Library/Resources/SharedResource.xlsx
+++ b/Vitae/Library/Resources/SharedResource.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\Vitae\Library\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDB8142E-5CD3-43C3-934F-0BE0FD5A015A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B7AADFE-62C9-47C3-82D5-9C86C5AF5AD4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2070" yWindow="2520" windowWidth="22500" windowHeight="14260" tabRatio="406" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6700" yWindow="4980" windowWidth="22500" windowHeight="14260" tabRatio="406" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="en" sheetId="3" r:id="rId1"/>
@@ -20,17 +20,25 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">de!$A$1:$B$23</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">en!$A$1:$B$23</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="724" uniqueCount="470">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="752" uniqueCount="490">
   <si>
     <t>City</t>
   </si>
@@ -1440,6 +1448,66 @@
   </si>
   <si>
     <t>Übersicht</t>
+  </si>
+  <si>
+    <t>PasswordRules</t>
+  </si>
+  <si>
+    <t>Bitte wählen Sie ein Passwort, welches aus Klein- und Grossbuchstaben, Zahlen und mindestens einem Sonderzeichen besteht. Es muss aus mindestens 6 Zeichen bestehen.</t>
+  </si>
+  <si>
+    <t>Please choose a password consisting of lower and upper case letters, numbers and at least one special character. It must consist of at least 6 characters.</t>
+  </si>
+  <si>
+    <t>LockedOut</t>
+  </si>
+  <si>
+    <t>Locked out</t>
+  </si>
+  <si>
+    <t>Lockout</t>
+  </si>
+  <si>
+    <t>LockoutMessage</t>
+  </si>
+  <si>
+    <t>This account has been locked out, please try again later.</t>
+  </si>
+  <si>
+    <t>Ausgesperrt</t>
+  </si>
+  <si>
+    <t>Aussperrung</t>
+  </si>
+  <si>
+    <t>Dieses Konto wurde gesperrt, bitte versuchen Sie es später noch einmal.</t>
+  </si>
+  <si>
+    <t>Back</t>
+  </si>
+  <si>
+    <t>Zurück</t>
+  </si>
+  <si>
+    <t>Go back</t>
+  </si>
+  <si>
+    <t>AccessDenied</t>
+  </si>
+  <si>
+    <t>Access denied</t>
+  </si>
+  <si>
+    <t>Please fill out the Personal details first.</t>
+  </si>
+  <si>
+    <t>Zugang verweigert</t>
+  </si>
+  <si>
+    <t>Bitte füllen Sie zuerst die persönlichen Angaben aus.</t>
+  </si>
+  <si>
+    <t>AccessDeniedMessage</t>
   </si>
 </sst>
 </file>
@@ -1496,13 +1564,24 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -1817,23 +1896,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B181"/>
+  <dimension ref="A1:B188"/>
   <sheetViews>
-    <sheetView topLeftCell="A155" workbookViewId="0">
-      <selection activeCell="B181" sqref="B181"/>
+    <sheetView tabSelected="1" topLeftCell="A165" workbookViewId="0">
+      <selection activeCell="A188" sqref="A188"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="37.26953125" customWidth="1"/>
-    <col min="2" max="2" width="118.1796875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="80.08984375" style="5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="3" t="s">
         <v>22</v>
       </c>
     </row>
@@ -1841,7 +1920,7 @@
       <c r="A2" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="4" t="s">
         <v>222</v>
       </c>
     </row>
@@ -1849,7 +1928,7 @@
       <c r="A3" t="s">
         <v>362</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="5" t="s">
         <v>361</v>
       </c>
     </row>
@@ -1857,7 +1936,7 @@
       <c r="A4" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" s="4" t="s">
         <v>129</v>
       </c>
     </row>
@@ -1865,15 +1944,15 @@
       <c r="A5" s="1" t="s">
         <v>249</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="5" t="s">
         <v>251</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:2" ht="29" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>248</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="5" t="s">
         <v>250</v>
       </c>
     </row>
@@ -1881,7 +1960,7 @@
       <c r="A7" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B7" s="4" t="s">
         <v>66</v>
       </c>
     </row>
@@ -1889,7 +1968,7 @@
       <c r="A8" t="s">
         <v>162</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="5" t="s">
         <v>181</v>
       </c>
     </row>
@@ -1897,7 +1976,7 @@
       <c r="A9" s="1" t="s">
         <v>224</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="5" t="s">
         <v>225</v>
       </c>
     </row>
@@ -1905,7 +1984,7 @@
       <c r="A10" s="1" t="s">
         <v>226</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="5" t="s">
         <v>227</v>
       </c>
     </row>
@@ -1913,7 +1992,7 @@
       <c r="A11" s="1" t="s">
         <v>151</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="B11" s="4" t="s">
         <v>151</v>
       </c>
     </row>
@@ -1921,7 +2000,7 @@
       <c r="A12" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="B12" s="4" t="s">
         <v>43</v>
       </c>
     </row>
@@ -1929,7 +2008,7 @@
       <c r="A13" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="B13" s="1" t="s">
+      <c r="B13" s="4" t="s">
         <v>51</v>
       </c>
     </row>
@@ -1937,7 +2016,7 @@
       <c r="A14" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="B14" s="4" t="s">
         <v>93</v>
       </c>
     </row>
@@ -1945,7 +2024,7 @@
       <c r="A15" s="1" t="s">
         <v>231</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B15" s="5" t="s">
         <v>231</v>
       </c>
     </row>
@@ -1953,7 +2032,7 @@
       <c r="A16" s="1" t="s">
         <v>433</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B16" s="5" t="s">
         <v>433</v>
       </c>
     </row>
@@ -1961,7 +2040,7 @@
       <c r="A17" t="s">
         <v>440</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B17" s="5" t="s">
         <v>442</v>
       </c>
     </row>
@@ -1969,7 +2048,7 @@
       <c r="A18" s="1" t="s">
         <v>421</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B18" s="5" t="s">
         <v>423</v>
       </c>
     </row>
@@ -1977,7 +2056,7 @@
       <c r="A19" s="1" t="s">
         <v>287</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B19" s="5" t="s">
         <v>288</v>
       </c>
     </row>
@@ -1985,7 +2064,7 @@
       <c r="A20" s="1" t="s">
         <v>296</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B20" s="5" t="s">
         <v>318</v>
       </c>
     </row>
@@ -1993,7 +2072,7 @@
       <c r="A21" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="B21" s="1" t="s">
+      <c r="B21" s="4" t="s">
         <v>59</v>
       </c>
     </row>
@@ -2001,7 +2080,7 @@
       <c r="A22" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="B22" s="1" t="s">
+      <c r="B22" s="4" t="s">
         <v>105</v>
       </c>
     </row>
@@ -2009,7 +2088,7 @@
       <c r="A23" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B23" s="1" t="s">
+      <c r="B23" s="4" t="s">
         <v>0</v>
       </c>
     </row>
@@ -2017,7 +2096,7 @@
       <c r="A24" s="1" t="s">
         <v>453</v>
       </c>
-      <c r="B24" s="1" t="s">
+      <c r="B24" s="4" t="s">
         <v>401</v>
       </c>
     </row>
@@ -2025,7 +2104,7 @@
       <c r="A25" t="s">
         <v>196</v>
       </c>
-      <c r="B25" t="s">
+      <c r="B25" s="5" t="s">
         <v>197</v>
       </c>
     </row>
@@ -2033,7 +2112,7 @@
       <c r="A26" s="1" t="s">
         <v>270</v>
       </c>
-      <c r="B26" t="s">
+      <c r="B26" s="5" t="s">
         <v>271</v>
       </c>
     </row>
@@ -2041,7 +2120,7 @@
       <c r="A27" t="s">
         <v>299</v>
       </c>
-      <c r="B27" t="s">
+      <c r="B27" s="5" t="s">
         <v>320</v>
       </c>
     </row>
@@ -2049,7 +2128,7 @@
       <c r="A28" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="B28" s="1" t="s">
+      <c r="B28" s="4" t="s">
         <v>91</v>
       </c>
     </row>
@@ -2057,7 +2136,7 @@
       <c r="A29" s="1" t="s">
         <v>449</v>
       </c>
-      <c r="B29" t="s">
+      <c r="B29" s="5" t="s">
         <v>450</v>
       </c>
     </row>
@@ -2065,7 +2144,7 @@
       <c r="A30" t="s">
         <v>404</v>
       </c>
-      <c r="B30" t="s">
+      <c r="B30" s="5" t="s">
         <v>367</v>
       </c>
     </row>
@@ -2073,7 +2152,7 @@
       <c r="A31" s="1" t="s">
         <v>404</v>
       </c>
-      <c r="B31" t="s">
+      <c r="B31" s="5" t="s">
         <v>405</v>
       </c>
     </row>
@@ -2081,7 +2160,7 @@
       <c r="A32" t="s">
         <v>451</v>
       </c>
-      <c r="B32" t="s">
+      <c r="B32" s="5" t="s">
         <v>369</v>
       </c>
     </row>
@@ -2089,7 +2168,7 @@
       <c r="A33" t="s">
         <v>267</v>
       </c>
-      <c r="B33" s="1" t="s">
+      <c r="B33" s="4" t="s">
         <v>269</v>
       </c>
     </row>
@@ -2097,7 +2176,7 @@
       <c r="A34" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B34" s="1" t="s">
+      <c r="B34" s="4" t="s">
         <v>21</v>
       </c>
     </row>
@@ -2105,7 +2184,7 @@
       <c r="A35" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B35" s="1" t="s">
+      <c r="B35" s="4" t="s">
         <v>33</v>
       </c>
     </row>
@@ -2113,7 +2192,7 @@
       <c r="A36" s="1" t="s">
         <v>259</v>
       </c>
-      <c r="B36" t="s">
+      <c r="B36" s="5" t="s">
         <v>260</v>
       </c>
     </row>
@@ -2121,7 +2200,7 @@
       <c r="A37" s="1" t="s">
         <v>427</v>
       </c>
-      <c r="B37" t="s">
+      <c r="B37" s="5" t="s">
         <v>428</v>
       </c>
     </row>
@@ -2129,7 +2208,7 @@
       <c r="A38" t="s">
         <v>142</v>
       </c>
-      <c r="B38" t="s">
+      <c r="B38" s="5" t="s">
         <v>143</v>
       </c>
     </row>
@@ -2137,7 +2216,7 @@
       <c r="A39" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="B39" s="1" t="s">
+      <c r="B39" s="4" t="s">
         <v>99</v>
       </c>
     </row>
@@ -2145,7 +2224,7 @@
       <c r="A40" s="1" t="s">
         <v>245</v>
       </c>
-      <c r="B40" s="1" t="s">
+      <c r="B40" s="4" t="s">
         <v>245</v>
       </c>
     </row>
@@ -2153,7 +2232,7 @@
       <c r="A41" t="s">
         <v>298</v>
       </c>
-      <c r="B41" t="s">
+      <c r="B41" s="5" t="s">
         <v>319</v>
       </c>
     </row>
@@ -2161,7 +2240,7 @@
       <c r="A42" s="1" t="s">
         <v>223</v>
       </c>
-      <c r="B42" t="s">
+      <c r="B42" s="5" t="s">
         <v>223</v>
       </c>
     </row>
@@ -2169,7 +2248,7 @@
       <c r="A43" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="B43" t="s">
+      <c r="B43" s="5" t="s">
         <v>63</v>
       </c>
     </row>
@@ -2177,7 +2256,7 @@
       <c r="A44" t="s">
         <v>306</v>
       </c>
-      <c r="B44" t="s">
+      <c r="B44" s="5" t="s">
         <v>327</v>
       </c>
     </row>
@@ -2185,7 +2264,7 @@
       <c r="A45" t="s">
         <v>308</v>
       </c>
-      <c r="B45" t="s">
+      <c r="B45" s="5" t="s">
         <v>329</v>
       </c>
     </row>
@@ -2193,7 +2272,7 @@
       <c r="A46" t="s">
         <v>305</v>
       </c>
-      <c r="B46" t="s">
+      <c r="B46" s="5" t="s">
         <v>326</v>
       </c>
     </row>
@@ -2201,7 +2280,7 @@
       <c r="A47" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="B47" s="1" t="s">
+      <c r="B47" s="4" t="s">
         <v>107</v>
       </c>
     </row>
@@ -2209,7 +2288,7 @@
       <c r="A48" s="1" t="s">
         <v>199</v>
       </c>
-      <c r="B48" s="1" t="s">
+      <c r="B48" s="4" t="s">
         <v>199</v>
       </c>
     </row>
@@ -2217,7 +2296,7 @@
       <c r="A49" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B49" s="1" t="s">
+      <c r="B49" s="4" t="s">
         <v>24</v>
       </c>
     </row>
@@ -2225,7 +2304,7 @@
       <c r="A50" s="1" t="s">
         <v>290</v>
       </c>
-      <c r="B50" t="s">
+      <c r="B50" s="5" t="s">
         <v>291</v>
       </c>
     </row>
@@ -2233,7 +2312,7 @@
       <c r="A51" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="B51" s="1" t="s">
+      <c r="B51" s="4" t="s">
         <v>115</v>
       </c>
     </row>
@@ -2241,7 +2320,7 @@
       <c r="A52" t="s">
         <v>452</v>
       </c>
-      <c r="B52" t="s">
+      <c r="B52" s="5" t="s">
         <v>371</v>
       </c>
     </row>
@@ -2249,7 +2328,7 @@
       <c r="A53" s="1" t="s">
         <v>465</v>
       </c>
-      <c r="B53" s="1" t="s">
+      <c r="B53" s="4" t="s">
         <v>466</v>
       </c>
     </row>
@@ -2257,7 +2336,7 @@
       <c r="A54" s="1" t="s">
         <v>234</v>
       </c>
-      <c r="B54" t="s">
+      <c r="B54" s="5" t="s">
         <v>235</v>
       </c>
     </row>
@@ -2265,7 +2344,7 @@
       <c r="A55" t="s">
         <v>139</v>
       </c>
-      <c r="B55" t="s">
+      <c r="B55" s="5" t="s">
         <v>139</v>
       </c>
     </row>
@@ -2273,7 +2352,7 @@
       <c r="A56" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="B56" t="s">
+      <c r="B56" s="5" t="s">
         <v>78</v>
       </c>
     </row>
@@ -2281,7 +2360,7 @@
       <c r="A57" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="B57" t="s">
+      <c r="B57" s="5" t="s">
         <v>72</v>
       </c>
     </row>
@@ -2289,7 +2368,7 @@
       <c r="A58" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B58" s="1" t="s">
+      <c r="B58" s="4" t="s">
         <v>1</v>
       </c>
     </row>
@@ -2297,7 +2376,7 @@
       <c r="A59" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="B59" t="s">
+      <c r="B59" s="5" t="s">
         <v>71</v>
       </c>
     </row>
@@ -2305,7 +2384,7 @@
       <c r="A60" s="1" t="s">
         <v>243</v>
       </c>
-      <c r="B60" s="1" t="s">
+      <c r="B60" s="4" t="s">
         <v>243</v>
       </c>
     </row>
@@ -2313,7 +2392,7 @@
       <c r="A61" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="B61" s="1" t="s">
+      <c r="B61" s="4" t="s">
         <v>36</v>
       </c>
     </row>
@@ -2321,7 +2400,7 @@
       <c r="A62" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="B62" s="1" t="s">
+      <c r="B62" s="4" t="s">
         <v>113</v>
       </c>
     </row>
@@ -2329,7 +2408,7 @@
       <c r="A63" s="1" t="s">
         <v>246</v>
       </c>
-      <c r="B63" s="1" t="s">
+      <c r="B63" s="4" t="s">
         <v>246</v>
       </c>
     </row>
@@ -2337,7 +2416,7 @@
       <c r="A64" t="s">
         <v>141</v>
       </c>
-      <c r="B64" t="s">
+      <c r="B64" s="5" t="s">
         <v>141</v>
       </c>
     </row>
@@ -2345,7 +2424,7 @@
       <c r="A65" t="s">
         <v>304</v>
       </c>
-      <c r="B65" t="s">
+      <c r="B65" s="5" t="s">
         <v>325</v>
       </c>
     </row>
@@ -2353,7 +2432,7 @@
       <c r="A66" t="s">
         <v>358</v>
       </c>
-      <c r="B66" t="s">
+      <c r="B66" s="5" t="s">
         <v>359</v>
       </c>
     </row>
@@ -2361,7 +2440,7 @@
       <c r="A67" t="s">
         <v>307</v>
       </c>
-      <c r="B67" t="s">
+      <c r="B67" s="5" t="s">
         <v>328</v>
       </c>
     </row>
@@ -2369,7 +2448,7 @@
       <c r="A68" t="s">
         <v>301</v>
       </c>
-      <c r="B68" t="s">
+      <c r="B68" s="5" t="s">
         <v>322</v>
       </c>
     </row>
@@ -2377,7 +2456,7 @@
       <c r="A69" t="s">
         <v>303</v>
       </c>
-      <c r="B69" t="s">
+      <c r="B69" s="5" t="s">
         <v>324</v>
       </c>
     </row>
@@ -2385,7 +2464,7 @@
       <c r="A70" t="s">
         <v>201</v>
       </c>
-      <c r="B70" s="1" t="s">
+      <c r="B70" s="4" t="s">
         <v>202</v>
       </c>
     </row>
@@ -2393,7 +2472,7 @@
       <c r="A71" t="s">
         <v>193</v>
       </c>
-      <c r="B71" t="s">
+      <c r="B71" s="5" t="s">
         <v>195</v>
       </c>
     </row>
@@ -2401,7 +2480,7 @@
       <c r="A72" s="1" t="s">
         <v>213</v>
       </c>
-      <c r="B72" t="s">
+      <c r="B72" s="5" t="s">
         <v>218</v>
       </c>
     </row>
@@ -2409,7 +2488,7 @@
       <c r="A73" s="1" t="s">
         <v>214</v>
       </c>
-      <c r="B73" t="s">
+      <c r="B73" s="5" t="s">
         <v>215</v>
       </c>
     </row>
@@ -2417,7 +2496,7 @@
       <c r="A74" s="1" t="s">
         <v>219</v>
       </c>
-      <c r="B74" t="s">
+      <c r="B74" s="5" t="s">
         <v>216</v>
       </c>
     </row>
@@ -2425,7 +2504,7 @@
       <c r="A75" s="1" t="s">
         <v>220</v>
       </c>
-      <c r="B75" t="s">
+      <c r="B75" s="5" t="s">
         <v>217</v>
       </c>
     </row>
@@ -2433,7 +2512,7 @@
       <c r="A76" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B76" s="1" t="s">
+      <c r="B76" s="4" t="s">
         <v>34</v>
       </c>
     </row>
@@ -2441,7 +2520,7 @@
       <c r="A77" t="s">
         <v>140</v>
       </c>
-      <c r="B77" t="s">
+      <c r="B77" s="5" t="s">
         <v>140</v>
       </c>
     </row>
@@ -2449,7 +2528,7 @@
       <c r="A78" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B78" s="1" t="s">
+      <c r="B78" s="4" t="s">
         <v>2</v>
       </c>
     </row>
@@ -2457,7 +2536,7 @@
       <c r="A79" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="B79" s="1" t="s">
+      <c r="B79" s="4" t="s">
         <v>154</v>
       </c>
     </row>
@@ -2465,7 +2544,7 @@
       <c r="A80" s="1" t="s">
         <v>415</v>
       </c>
-      <c r="B80" t="s">
+      <c r="B80" s="5" t="s">
         <v>416</v>
       </c>
     </row>
@@ -2473,7 +2552,7 @@
       <c r="A81" s="1" t="s">
         <v>417</v>
       </c>
-      <c r="B81" t="s">
+      <c r="B81" s="5" t="s">
         <v>418</v>
       </c>
     </row>
@@ -2481,7 +2560,7 @@
       <c r="A82" t="s">
         <v>302</v>
       </c>
-      <c r="B82" t="s">
+      <c r="B82" s="5" t="s">
         <v>323</v>
       </c>
     </row>
@@ -2489,7 +2568,7 @@
       <c r="A83" s="1" t="s">
         <v>273</v>
       </c>
-      <c r="B83" t="s">
+      <c r="B83" s="5" t="s">
         <v>274</v>
       </c>
     </row>
@@ -2497,7 +2576,7 @@
       <c r="A84" s="1" t="s">
         <v>413</v>
       </c>
-      <c r="B84" t="s">
+      <c r="B84" s="5" t="s">
         <v>413</v>
       </c>
     </row>
@@ -2505,7 +2584,7 @@
       <c r="A85" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B85" s="1" t="s">
+      <c r="B85" s="4" t="s">
         <v>3</v>
       </c>
     </row>
@@ -2513,7 +2592,7 @@
       <c r="A86" t="s">
         <v>161</v>
       </c>
-      <c r="B86" t="s">
+      <c r="B86" s="5" t="s">
         <v>180</v>
       </c>
     </row>
@@ -2521,7 +2600,7 @@
       <c r="A87" t="s">
         <v>163</v>
       </c>
-      <c r="B87" t="s">
+      <c r="B87" s="5" t="s">
         <v>170</v>
       </c>
     </row>
@@ -2529,7 +2608,7 @@
       <c r="A88" t="s">
         <v>166</v>
       </c>
-      <c r="B88" t="s">
+      <c r="B88" s="5" t="s">
         <v>171</v>
       </c>
     </row>
@@ -2537,7 +2616,7 @@
       <c r="A89" t="s">
         <v>27</v>
       </c>
-      <c r="B89" s="1" t="s">
+      <c r="B89" s="4" t="s">
         <v>30</v>
       </c>
     </row>
@@ -2545,7 +2624,7 @@
       <c r="A90" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="B90" s="1" t="s">
+      <c r="B90" s="4" t="s">
         <v>42</v>
       </c>
     </row>
@@ -2553,7 +2632,7 @@
       <c r="A91" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="B91" s="1" t="s">
+      <c r="B91" s="4" t="s">
         <v>40</v>
       </c>
     </row>
@@ -2561,7 +2640,7 @@
       <c r="A92" t="s">
         <v>148</v>
       </c>
-      <c r="B92" s="1" t="s">
+      <c r="B92" s="4" t="s">
         <v>150</v>
       </c>
     </row>
@@ -2569,7 +2648,7 @@
       <c r="A93" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B93" t="s">
+      <c r="B93" s="5" t="s">
         <v>20</v>
       </c>
     </row>
@@ -2577,7 +2656,7 @@
       <c r="A94" t="s">
         <v>204</v>
       </c>
-      <c r="B94" s="1" t="s">
+      <c r="B94" s="4" t="s">
         <v>204</v>
       </c>
     </row>
@@ -2585,7 +2664,7 @@
       <c r="A95" t="s">
         <v>131</v>
       </c>
-      <c r="B95" t="s">
+      <c r="B95" s="5" t="s">
         <v>131</v>
       </c>
     </row>
@@ -2593,7 +2672,7 @@
       <c r="A96" s="1" t="s">
         <v>446</v>
       </c>
-      <c r="B96" t="s">
+      <c r="B96" s="5" t="s">
         <v>448</v>
       </c>
     </row>
@@ -2601,7 +2680,7 @@
       <c r="A97" s="1" t="s">
         <v>424</v>
       </c>
-      <c r="B97" t="s">
+      <c r="B97" s="5" t="s">
         <v>426</v>
       </c>
     </row>
@@ -2609,7 +2688,7 @@
       <c r="A98" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="B98" s="1" t="s">
+      <c r="B98" s="4" t="s">
         <v>97</v>
       </c>
     </row>
@@ -2617,7 +2696,7 @@
       <c r="A99" t="s">
         <v>167</v>
       </c>
-      <c r="B99" t="s">
+      <c r="B99" s="5" t="s">
         <v>183</v>
       </c>
     </row>
@@ -2625,7 +2704,7 @@
       <c r="A100" t="s">
         <v>168</v>
       </c>
-      <c r="B100" t="s">
+      <c r="B100" s="5" t="s">
         <v>172</v>
       </c>
     </row>
@@ -2633,7 +2712,7 @@
       <c r="A101" t="s">
         <v>169</v>
       </c>
-      <c r="B101" t="s">
+      <c r="B101" s="5" t="s">
         <v>173</v>
       </c>
     </row>
@@ -2641,7 +2720,7 @@
       <c r="A102" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="B102" s="1" t="s">
+      <c r="B102" s="4" t="s">
         <v>94</v>
       </c>
     </row>
@@ -2649,7 +2728,7 @@
       <c r="A103" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="B103" s="1" t="s">
+      <c r="B103" s="4" t="s">
         <v>64</v>
       </c>
     </row>
@@ -2657,7 +2736,7 @@
       <c r="A104" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="B104" t="s">
+      <c r="B104" s="5" t="s">
         <v>87</v>
       </c>
     </row>
@@ -2665,7 +2744,7 @@
       <c r="A105" s="1" t="s">
         <v>261</v>
       </c>
-      <c r="B105" s="1" t="s">
+      <c r="B105" s="4" t="s">
         <v>261</v>
       </c>
     </row>
@@ -2673,7 +2752,7 @@
       <c r="A106" s="1" t="s">
         <v>430</v>
       </c>
-      <c r="B106" t="s">
+      <c r="B106" s="5" t="s">
         <v>431</v>
       </c>
     </row>
@@ -2681,7 +2760,7 @@
       <c r="A107" s="1" t="s">
         <v>265</v>
       </c>
-      <c r="B107" t="s">
+      <c r="B107" s="5" t="s">
         <v>264</v>
       </c>
     </row>
@@ -2689,7 +2768,7 @@
       <c r="A108" s="1" t="s">
         <v>279</v>
       </c>
-      <c r="B108" t="s">
+      <c r="B108" s="5" t="s">
         <v>282</v>
       </c>
     </row>
@@ -2697,7 +2776,7 @@
       <c r="A109" t="s">
         <v>300</v>
       </c>
-      <c r="B109" t="s">
+      <c r="B109" s="5" t="s">
         <v>321</v>
       </c>
     </row>
@@ -2705,7 +2784,7 @@
       <c r="A110" t="s">
         <v>315</v>
       </c>
-      <c r="B110" t="s">
+      <c r="B110" s="5" t="s">
         <v>336</v>
       </c>
     </row>
@@ -2713,7 +2792,7 @@
       <c r="A111" t="s">
         <v>316</v>
       </c>
-      <c r="B111" t="s">
+      <c r="B111" s="5" t="s">
         <v>337</v>
       </c>
     </row>
@@ -2721,7 +2800,7 @@
       <c r="A112" t="s">
         <v>314</v>
       </c>
-      <c r="B112" t="s">
+      <c r="B112" s="5" t="s">
         <v>335</v>
       </c>
     </row>
@@ -2729,7 +2808,7 @@
       <c r="A113" t="s">
         <v>317</v>
       </c>
-      <c r="B113" t="s">
+      <c r="B113" s="5" t="s">
         <v>338</v>
       </c>
     </row>
@@ -2737,7 +2816,7 @@
       <c r="A114" t="s">
         <v>313</v>
       </c>
-      <c r="B114" t="s">
+      <c r="B114" s="5" t="s">
         <v>334</v>
       </c>
     </row>
@@ -2745,7 +2824,7 @@
       <c r="A115" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="B115" s="1" t="s">
+      <c r="B115" s="4" t="s">
         <v>136</v>
       </c>
     </row>
@@ -2753,7 +2832,7 @@
       <c r="A116" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="B116" s="1" t="s">
+      <c r="B116" s="4" t="s">
         <v>138</v>
       </c>
     </row>
@@ -2761,7 +2840,7 @@
       <c r="A117" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="B117" s="1" t="s">
+      <c r="B117" s="4" t="s">
         <v>45</v>
       </c>
     </row>
@@ -2769,7 +2848,7 @@
       <c r="A118" t="s">
         <v>29</v>
       </c>
-      <c r="B118" s="1" t="s">
+      <c r="B118" s="4" t="s">
         <v>29</v>
       </c>
     </row>
@@ -2777,7 +2856,7 @@
       <c r="A119" s="1" t="s">
         <v>455</v>
       </c>
-      <c r="B119" t="s">
+      <c r="B119" s="5" t="s">
         <v>459</v>
       </c>
     </row>
@@ -2785,7 +2864,7 @@
       <c r="A120" s="1" t="s">
         <v>398</v>
       </c>
-      <c r="B120" s="1" t="s">
+      <c r="B120" s="4" t="s">
         <v>400</v>
       </c>
     </row>
@@ -2793,7 +2872,7 @@
       <c r="A121" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="B121" s="1" t="s">
+      <c r="B121" s="4" t="s">
         <v>104</v>
       </c>
     </row>
@@ -2801,7 +2880,7 @@
       <c r="A122" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="B122" t="s">
+      <c r="B122" s="5" t="s">
         <v>80</v>
       </c>
     </row>
@@ -2809,7 +2888,7 @@
       <c r="A123" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="B123" s="1" t="s">
+      <c r="B123" s="4" t="s">
         <v>157</v>
       </c>
     </row>
@@ -2817,7 +2896,7 @@
       <c r="A124" s="1" t="s">
         <v>206</v>
       </c>
-      <c r="B124" s="1" t="s">
+      <c r="B124" s="4" t="s">
         <v>208</v>
       </c>
     </row>
@@ -2825,7 +2904,7 @@
       <c r="A125" s="1" t="s">
         <v>252</v>
       </c>
-      <c r="B125" s="1" t="s">
+      <c r="B125" s="4" t="s">
         <v>258</v>
       </c>
     </row>
@@ -2833,7 +2912,7 @@
       <c r="A126" s="1" t="s">
         <v>280</v>
       </c>
-      <c r="B126" t="s">
+      <c r="B126" s="5" t="s">
         <v>283</v>
       </c>
     </row>
@@ -2841,7 +2920,7 @@
       <c r="A127" s="1" t="s">
         <v>293</v>
       </c>
-      <c r="B127" t="s">
+      <c r="B127" s="5" t="s">
         <v>294</v>
       </c>
     </row>
@@ -2849,7 +2928,7 @@
       <c r="A128" s="1" t="s">
         <v>278</v>
       </c>
-      <c r="B128" s="1" t="s">
+      <c r="B128" s="4" t="s">
         <v>276</v>
       </c>
     </row>
@@ -2857,7 +2936,7 @@
       <c r="A129" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="B129" s="1" t="s">
+      <c r="B129" s="4" t="s">
         <v>133</v>
       </c>
     </row>
@@ -2865,7 +2944,7 @@
       <c r="A130" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="B130" t="s">
+      <c r="B130" s="5" t="s">
         <v>77</v>
       </c>
     </row>
@@ -2873,7 +2952,7 @@
       <c r="A131" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="B131" s="1" t="s">
+      <c r="B131" s="4" t="s">
         <v>54</v>
       </c>
     </row>
@@ -2881,7 +2960,7 @@
       <c r="A132" s="1" t="s">
         <v>285</v>
       </c>
-      <c r="B132" s="1" t="s">
+      <c r="B132" s="4" t="s">
         <v>285</v>
       </c>
     </row>
@@ -2889,7 +2968,7 @@
       <c r="A133" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="B133" s="1" t="s">
+      <c r="B133" s="4" t="s">
         <v>48</v>
       </c>
     </row>
@@ -2897,7 +2976,7 @@
       <c r="A134" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="B134" s="1" t="s">
+      <c r="B134" s="4" t="s">
         <v>58</v>
       </c>
     </row>
@@ -2905,7 +2984,7 @@
       <c r="A135" t="s">
         <v>379</v>
       </c>
-      <c r="B135" t="s">
+      <c r="B135" s="5" t="s">
         <v>379</v>
       </c>
     </row>
@@ -2913,7 +2992,7 @@
       <c r="A136" t="s">
         <v>373</v>
       </c>
-      <c r="B136" t="s">
+      <c r="B136" s="5" t="s">
         <v>374</v>
       </c>
     </row>
@@ -2921,7 +3000,7 @@
       <c r="A137" s="1" t="s">
         <v>437</v>
       </c>
-      <c r="B137" t="s">
+      <c r="B137" s="5" t="s">
         <v>438</v>
       </c>
     </row>
@@ -2929,7 +3008,7 @@
       <c r="A138" t="s">
         <v>381</v>
       </c>
-      <c r="B138" t="s">
+      <c r="B138" s="5" t="s">
         <v>382</v>
       </c>
     </row>
@@ -2937,7 +3016,7 @@
       <c r="A139" t="s">
         <v>389</v>
       </c>
-      <c r="B139" t="s">
+      <c r="B139" s="5" t="s">
         <v>383</v>
       </c>
     </row>
@@ -2945,7 +3024,7 @@
       <c r="A140" t="s">
         <v>384</v>
       </c>
-      <c r="B140" t="s">
+      <c r="B140" s="5" t="s">
         <v>385</v>
       </c>
     </row>
@@ -2953,7 +3032,7 @@
       <c r="A141" t="s">
         <v>375</v>
       </c>
-      <c r="B141" t="s">
+      <c r="B141" s="5" t="s">
         <v>376</v>
       </c>
     </row>
@@ -2961,7 +3040,7 @@
       <c r="A142" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="B142" s="1" t="s">
+      <c r="B142" s="4" t="s">
         <v>126</v>
       </c>
     </row>
@@ -2969,7 +3048,7 @@
       <c r="A143" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B143" s="1" t="s">
+      <c r="B143" s="4" t="s">
         <v>4</v>
       </c>
     </row>
@@ -2977,7 +3056,7 @@
       <c r="A144" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="B144" s="3" t="s">
+      <c r="B144" s="6" t="s">
         <v>116</v>
       </c>
     </row>
@@ -2985,7 +3064,7 @@
       <c r="A145" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B145" s="1" t="s">
+      <c r="B145" s="4" t="s">
         <v>25</v>
       </c>
     </row>
@@ -2993,7 +3072,7 @@
       <c r="A146" s="1" t="s">
         <v>443</v>
       </c>
-      <c r="B146" t="s">
+      <c r="B146" s="5" t="s">
         <v>444</v>
       </c>
     </row>
@@ -3001,7 +3080,7 @@
       <c r="A147" s="1" t="s">
         <v>253</v>
       </c>
-      <c r="B147" s="1" t="s">
+      <c r="B147" s="4" t="s">
         <v>254</v>
       </c>
     </row>
@@ -3009,7 +3088,7 @@
       <c r="A148" s="1" t="s">
         <v>230</v>
       </c>
-      <c r="B148" t="s">
+      <c r="B148" s="5" t="s">
         <v>230</v>
       </c>
     </row>
@@ -3017,7 +3096,7 @@
       <c r="A149" s="1" t="s">
         <v>233</v>
       </c>
-      <c r="B149" t="s">
+      <c r="B149" s="5" t="s">
         <v>233</v>
       </c>
     </row>
@@ -3025,7 +3104,7 @@
       <c r="A150" t="s">
         <v>28</v>
       </c>
-      <c r="B150" s="1" t="s">
+      <c r="B150" s="4" t="s">
         <v>28</v>
       </c>
     </row>
@@ -3033,7 +3112,7 @@
       <c r="A151" t="s">
         <v>239</v>
       </c>
-      <c r="B151" s="1" t="s">
+      <c r="B151" s="4" t="s">
         <v>237</v>
       </c>
     </row>
@@ -3041,7 +3120,7 @@
       <c r="A152" s="1" t="s">
         <v>240</v>
       </c>
-      <c r="B152" s="1" t="s">
+      <c r="B152" s="4" t="s">
         <v>241</v>
       </c>
     </row>
@@ -3049,7 +3128,7 @@
       <c r="A153" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="B153" s="1" t="s">
+      <c r="B153" s="4" t="s">
         <v>114</v>
       </c>
     </row>
@@ -3057,7 +3136,7 @@
       <c r="A154" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B154" s="1" t="s">
+      <c r="B154" s="4" t="s">
         <v>5</v>
       </c>
     </row>
@@ -3065,7 +3144,7 @@
       <c r="A155" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B155" s="1" t="s">
+      <c r="B155" s="4" t="s">
         <v>6</v>
       </c>
     </row>
@@ -3073,7 +3152,7 @@
       <c r="A156" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B156" s="1" t="s">
+      <c r="B156" s="4" t="s">
         <v>23</v>
       </c>
     </row>
@@ -3081,7 +3160,7 @@
       <c r="A157" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="B157" s="1" t="s">
+      <c r="B157" s="4" t="s">
         <v>119</v>
       </c>
     </row>
@@ -3089,7 +3168,7 @@
       <c r="A158" t="s">
         <v>390</v>
       </c>
-      <c r="B158" t="s">
+      <c r="B158" s="5" t="s">
         <v>391</v>
       </c>
     </row>
@@ -3097,7 +3176,7 @@
       <c r="A159" s="1" t="s">
         <v>435</v>
       </c>
-      <c r="B159" t="s">
+      <c r="B159" s="5" t="s">
         <v>413</v>
       </c>
     </row>
@@ -3105,7 +3184,7 @@
       <c r="A160" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="B160" s="1" t="s">
+      <c r="B160" s="4" t="s">
         <v>118</v>
       </c>
     </row>
@@ -3113,7 +3192,7 @@
       <c r="A161" s="1" t="s">
         <v>408</v>
       </c>
-      <c r="B161" t="s">
+      <c r="B161" s="5" t="s">
         <v>407</v>
       </c>
     </row>
@@ -3121,7 +3200,7 @@
       <c r="A162" s="1" t="s">
         <v>410</v>
       </c>
-      <c r="B162" t="s">
+      <c r="B162" s="5" t="s">
         <v>411</v>
       </c>
     </row>
@@ -3129,7 +3208,7 @@
       <c r="A163" t="s">
         <v>164</v>
       </c>
-      <c r="B163" t="s">
+      <c r="B163" s="5" t="s">
         <v>182</v>
       </c>
     </row>
@@ -3137,7 +3216,7 @@
       <c r="A164" t="s">
         <v>190</v>
       </c>
-      <c r="B164" t="s">
+      <c r="B164" s="5" t="s">
         <v>191</v>
       </c>
     </row>
@@ -3145,7 +3224,7 @@
       <c r="A165" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="B165" s="1" t="s">
+      <c r="B165" s="4" t="s">
         <v>117</v>
       </c>
     </row>
@@ -3153,7 +3232,7 @@
       <c r="A166" t="s">
         <v>309</v>
       </c>
-      <c r="B166" t="s">
+      <c r="B166" s="5" t="s">
         <v>330</v>
       </c>
     </row>
@@ -3161,7 +3240,7 @@
       <c r="A167" t="s">
         <v>311</v>
       </c>
-      <c r="B167" t="s">
+      <c r="B167" s="5" t="s">
         <v>332</v>
       </c>
     </row>
@@ -3169,7 +3248,7 @@
       <c r="A168" s="1" t="s">
         <v>394</v>
       </c>
-      <c r="B168" t="s">
+      <c r="B168" s="5" t="s">
         <v>393</v>
       </c>
     </row>
@@ -3177,7 +3256,7 @@
       <c r="A169" t="s">
         <v>310</v>
       </c>
-      <c r="B169" t="s">
+      <c r="B169" s="5" t="s">
         <v>331</v>
       </c>
     </row>
@@ -3185,7 +3264,7 @@
       <c r="A170" t="s">
         <v>364</v>
       </c>
-      <c r="B170" t="s">
+      <c r="B170" s="5" t="s">
         <v>363</v>
       </c>
     </row>
@@ -3193,7 +3272,7 @@
       <c r="A171" t="s">
         <v>312</v>
       </c>
-      <c r="B171" t="s">
+      <c r="B171" s="5" t="s">
         <v>333</v>
       </c>
     </row>
@@ -3201,7 +3280,7 @@
       <c r="A172" t="s">
         <v>159</v>
       </c>
-      <c r="B172" t="s">
+      <c r="B172" s="5" t="s">
         <v>178</v>
       </c>
     </row>
@@ -3209,7 +3288,7 @@
       <c r="A173" t="s">
         <v>160</v>
       </c>
-      <c r="B173" t="s">
+      <c r="B173" s="5" t="s">
         <v>179</v>
       </c>
     </row>
@@ -3217,7 +3296,7 @@
       <c r="A174" t="s">
         <v>165</v>
       </c>
-      <c r="B174" t="s">
+      <c r="B174" s="5" t="s">
         <v>178</v>
       </c>
     </row>
@@ -3225,7 +3304,7 @@
       <c r="A175" s="1" t="s">
         <v>454</v>
       </c>
-      <c r="B175" t="s">
+      <c r="B175" s="5" t="s">
         <v>460</v>
       </c>
     </row>
@@ -3233,7 +3312,7 @@
       <c r="A176" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="B176" s="1" t="s">
+      <c r="B176" s="4" t="s">
         <v>89</v>
       </c>
     </row>
@@ -3241,7 +3320,7 @@
       <c r="A177" s="1" t="s">
         <v>396</v>
       </c>
-      <c r="B177" s="1" t="s">
+      <c r="B177" s="4" t="s">
         <v>397</v>
       </c>
     </row>
@@ -3249,7 +3328,7 @@
       <c r="A178" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="B178" s="1" t="s">
+      <c r="B178" s="4" t="s">
         <v>95</v>
       </c>
     </row>
@@ -3257,7 +3336,7 @@
       <c r="A179" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B179" s="1" t="s">
+      <c r="B179" s="4" t="s">
         <v>9</v>
       </c>
     </row>
@@ -3265,7 +3344,7 @@
       <c r="A180" s="1" t="s">
         <v>461</v>
       </c>
-      <c r="B180" t="s">
+      <c r="B180" s="5" t="s">
         <v>462</v>
       </c>
     </row>
@@ -3273,8 +3352,64 @@
       <c r="A181" s="1" t="s">
         <v>468</v>
       </c>
-      <c r="B181" s="1" t="s">
+      <c r="B181" s="4" t="s">
         <v>468</v>
+      </c>
+    </row>
+    <row r="182" spans="1:2" ht="29" x14ac:dyDescent="0.35">
+      <c r="A182" s="1" t="s">
+        <v>470</v>
+      </c>
+      <c r="B182" s="4" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="183" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A183" s="1" t="s">
+        <v>473</v>
+      </c>
+      <c r="B183" s="5" t="s">
+        <v>474</v>
+      </c>
+    </row>
+    <row r="184" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A184" s="1" t="s">
+        <v>475</v>
+      </c>
+      <c r="B184" s="5" t="s">
+        <v>475</v>
+      </c>
+    </row>
+    <row r="185" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A185" s="1" t="s">
+        <v>476</v>
+      </c>
+      <c r="B185" s="5" t="s">
+        <v>477</v>
+      </c>
+    </row>
+    <row r="186" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A186" s="1" t="s">
+        <v>481</v>
+      </c>
+      <c r="B186" s="5" t="s">
+        <v>483</v>
+      </c>
+    </row>
+    <row r="187" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A187" s="1" t="s">
+        <v>484</v>
+      </c>
+      <c r="B187" s="5" t="s">
+        <v>485</v>
+      </c>
+    </row>
+    <row r="188" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A188" s="1" t="s">
+        <v>489</v>
+      </c>
+      <c r="B188" s="5" t="s">
+        <v>486</v>
       </c>
     </row>
   </sheetData>
@@ -3290,16 +3425,16 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:B181"/>
+  <dimension ref="A1:B188"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A169" workbookViewId="0">
-      <selection activeCell="B181" sqref="B181"/>
+    <sheetView topLeftCell="A184" workbookViewId="0">
+      <selection activeCell="A188" sqref="A188"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="31.54296875" customWidth="1"/>
-    <col min="2" max="2" width="57.54296875" customWidth="1"/>
+    <col min="2" max="2" width="62.54296875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
@@ -4748,6 +4883,62 @@
       </c>
       <c r="B181" s="1" t="s">
         <v>469</v>
+      </c>
+    </row>
+    <row r="182" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A182" s="1" t="s">
+        <v>470</v>
+      </c>
+      <c r="B182" s="1" t="s">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="183" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A183" s="1" t="s">
+        <v>473</v>
+      </c>
+      <c r="B183" s="5" t="s">
+        <v>478</v>
+      </c>
+    </row>
+    <row r="184" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A184" s="1" t="s">
+        <v>475</v>
+      </c>
+      <c r="B184" s="5" t="s">
+        <v>479</v>
+      </c>
+    </row>
+    <row r="185" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A185" s="1" t="s">
+        <v>476</v>
+      </c>
+      <c r="B185" s="5" t="s">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="186" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A186" s="1" t="s">
+        <v>481</v>
+      </c>
+      <c r="B186" s="5" t="s">
+        <v>482</v>
+      </c>
+    </row>
+    <row r="187" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A187" s="1" t="s">
+        <v>484</v>
+      </c>
+      <c r="B187" s="5" t="s">
+        <v>487</v>
+      </c>
+    </row>
+    <row r="188" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A188" s="1" t="s">
+        <v>489</v>
+      </c>
+      <c r="B188" s="5" t="s">
+        <v>488</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
New select picker added
</commit_message>
<xml_diff>
--- a/Vitae/Library/Resources/SharedResource.xlsx
+++ b/Vitae/Library/Resources/SharedResource.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\Vitae\Library\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FC0717E-F7CF-40ED-A434-A541033D3C6E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DD66890-5525-4C5B-AE08-4AD829532EBA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2890" yWindow="2090" windowWidth="22500" windowHeight="14260" tabRatio="406" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2890" yWindow="2090" windowWidth="22500" windowHeight="14260" tabRatio="406" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="en" sheetId="3" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="752" uniqueCount="489">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="756" uniqueCount="492">
   <si>
     <t>City</t>
   </si>
@@ -1505,6 +1505,15 @@
   </si>
   <si>
     <t>Über</t>
+  </si>
+  <si>
+    <t>NoResults</t>
+  </si>
+  <si>
+    <t>Keine Suchergebnisse für {0}</t>
+  </si>
+  <si>
+    <t>No results for {0}</t>
   </si>
 </sst>
 </file>
@@ -1893,10 +1902,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B188"/>
+  <dimension ref="A1:B189"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" topLeftCell="A185" workbookViewId="0">
+      <selection activeCell="B190" sqref="B190"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3407,6 +3416,14 @@
       </c>
       <c r="B188" s="5" t="s">
         <v>482</v>
+      </c>
+    </row>
+    <row r="189" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A189" s="1" t="s">
+        <v>489</v>
+      </c>
+      <c r="B189" s="5" t="s">
+        <v>491</v>
       </c>
     </row>
   </sheetData>
@@ -3422,10 +3439,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:B188"/>
+  <dimension ref="A1:B189"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView topLeftCell="A166" workbookViewId="0">
+      <selection activeCell="B190" sqref="B190"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4938,6 +4955,14 @@
         <v>484</v>
       </c>
     </row>
+    <row r="189" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A189" s="1" t="s">
+        <v>489</v>
+      </c>
+      <c r="B189" s="5" t="s">
+        <v>490</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:B23" xr:uid="{00000000-0009-0000-0000-000001000000}">
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B178">

</xml_diff>

<commit_message>
Bugfix: Checkbox hidden field problem
</commit_message>
<xml_diff>
--- a/Vitae/Library/Resources/SharedResource.xlsx
+++ b/Vitae/Library/Resources/SharedResource.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\Vitae\Library\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49A4A028-562C-41A4-A962-38D33A9E567B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DC2B332-26E4-43B4-9D94-42A4E8CE4AB0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2890" yWindow="2090" windowWidth="22500" windowHeight="14260" tabRatio="406" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="812" uniqueCount="525">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="824" uniqueCount="534">
   <si>
     <t>City</t>
   </si>
@@ -1605,6 +1605,33 @@
   </si>
   <si>
     <t>Telefonnummer</t>
+  </si>
+  <si>
+    <t>EnterSkill</t>
+  </si>
+  <si>
+    <t>Bitte drücken Sie die Enter-Taste um einen neuen Skill einzufügen</t>
+  </si>
+  <si>
+    <t>Please press Enter to insert a new Skill</t>
+  </si>
+  <si>
+    <t>Abroad</t>
+  </si>
+  <si>
+    <t>Abroad stay</t>
+  </si>
+  <si>
+    <t>Auslandaufenthalt</t>
+  </si>
+  <si>
+    <t>Reference</t>
+  </si>
+  <si>
+    <t>References</t>
+  </si>
+  <si>
+    <t>Referenzen</t>
   </si>
 </sst>
 </file>
@@ -1993,10 +2020,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B203"/>
+  <dimension ref="A1:B206"/>
   <sheetViews>
-    <sheetView topLeftCell="A172" workbookViewId="0">
-      <selection activeCell="B204" sqref="B204"/>
+    <sheetView topLeftCell="A187" workbookViewId="0">
+      <selection activeCell="A206" sqref="A206:B206"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3627,6 +3654,30 @@
       </c>
       <c r="B203" s="5" t="s">
         <v>523</v>
+      </c>
+    </row>
+    <row r="204" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A204" s="1" t="s">
+        <v>525</v>
+      </c>
+      <c r="B204" s="5" t="s">
+        <v>527</v>
+      </c>
+    </row>
+    <row r="205" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A205" t="s">
+        <v>528</v>
+      </c>
+      <c r="B205" s="5" t="s">
+        <v>529</v>
+      </c>
+    </row>
+    <row r="206" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A206" s="1" t="s">
+        <v>531</v>
+      </c>
+      <c r="B206" s="5" t="s">
+        <v>532</v>
       </c>
     </row>
   </sheetData>
@@ -3642,10 +3693,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:B203"/>
+  <dimension ref="A1:B206"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A178" workbookViewId="0">
-      <selection activeCell="B204" sqref="B204"/>
+    <sheetView tabSelected="1" topLeftCell="A190" workbookViewId="0">
+      <selection activeCell="A206" sqref="A206:B206"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -5278,6 +5329,30 @@
         <v>524</v>
       </c>
     </row>
+    <row r="204" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A204" s="1" t="s">
+        <v>525</v>
+      </c>
+      <c r="B204" t="s">
+        <v>526</v>
+      </c>
+    </row>
+    <row r="205" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A205" t="s">
+        <v>528</v>
+      </c>
+      <c r="B205" s="5" t="s">
+        <v>530</v>
+      </c>
+    </row>
+    <row r="206" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A206" s="1" t="s">
+        <v>531</v>
+      </c>
+      <c r="B206" s="5" t="s">
+        <v>533</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:B23" xr:uid="{00000000-0009-0000-0000-000001000000}">
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B198">

</xml_diff>

<commit_message>
Implemented Courses (removed LanguageCourse)
</commit_message>
<xml_diff>
--- a/Vitae/Library/Resources/SharedResource.xlsx
+++ b/Vitae/Library/Resources/SharedResource.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="844" uniqueCount="546">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="860" uniqueCount="553">
   <si>
     <t>City</t>
   </si>
@@ -1667,6 +1667,27 @@
   </si>
   <si>
     <t>Aussteller</t>
+  </si>
+  <si>
+    <t>Level</t>
+  </si>
+  <si>
+    <t>Niveau</t>
+  </si>
+  <si>
+    <t>Referenz</t>
+  </si>
+  <si>
+    <t>Courses</t>
+  </si>
+  <si>
+    <t>Kurse</t>
+  </si>
+  <si>
+    <t>Course</t>
+  </si>
+  <si>
+    <t>Kurs</t>
   </si>
 </sst>
 </file>
@@ -2055,10 +2076,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B211"/>
+  <dimension ref="A1:B215"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A187" workbookViewId="0">
-      <selection activeCell="A212" sqref="A212"/>
+      <selection activeCell="B214" sqref="B214:B215"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3712,7 +3733,7 @@
         <v>531</v>
       </c>
       <c r="B206" s="5" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
     </row>
     <row r="207" spans="1:2" x14ac:dyDescent="0.25">
@@ -3753,6 +3774,38 @@
       </c>
       <c r="B211" s="5" t="s">
         <v>544</v>
+      </c>
+    </row>
+    <row r="212" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A212" t="s">
+        <v>546</v>
+      </c>
+      <c r="B212" s="5" t="s">
+        <v>546</v>
+      </c>
+    </row>
+    <row r="213" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A213" s="1" t="s">
+        <v>532</v>
+      </c>
+      <c r="B213" s="1" t="s">
+        <v>532</v>
+      </c>
+    </row>
+    <row r="214" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A214" t="s">
+        <v>551</v>
+      </c>
+      <c r="B214" t="s">
+        <v>551</v>
+      </c>
+    </row>
+    <row r="215" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A215" t="s">
+        <v>549</v>
+      </c>
+      <c r="B215" t="s">
+        <v>549</v>
       </c>
     </row>
   </sheetData>
@@ -3768,10 +3821,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B211"/>
+  <dimension ref="A1:B215"/>
   <sheetViews>
-    <sheetView topLeftCell="A190" workbookViewId="0">
-      <selection activeCell="A212" sqref="A212"/>
+    <sheetView topLeftCell="A185" workbookViewId="0">
+      <selection activeCell="B215" sqref="A214:B215"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5425,7 +5478,7 @@
         <v>531</v>
       </c>
       <c r="B206" s="5" t="s">
-        <v>533</v>
+        <v>548</v>
       </c>
     </row>
     <row r="207" spans="1:2" x14ac:dyDescent="0.25">
@@ -5466,6 +5519,38 @@
       </c>
       <c r="B211" s="5" t="s">
         <v>545</v>
+      </c>
+    </row>
+    <row r="212" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A212" t="s">
+        <v>546</v>
+      </c>
+      <c r="B212" s="5" t="s">
+        <v>547</v>
+      </c>
+    </row>
+    <row r="213" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A213" s="1" t="s">
+        <v>532</v>
+      </c>
+      <c r="B213" s="5" t="s">
+        <v>533</v>
+      </c>
+    </row>
+    <row r="214" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A214" t="s">
+        <v>551</v>
+      </c>
+      <c r="B214" s="5" t="s">
+        <v>552</v>
+      </c>
+    </row>
+    <row r="215" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A215" t="s">
+        <v>549</v>
+      </c>
+      <c r="B215" s="5" t="s">
+        <v>550</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Included CV of ATH
</commit_message>
<xml_diff>
--- a/Vitae/Library/Resources/SharedResource.xlsx
+++ b/Vitae/Library/Resources/SharedResource.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\Vitae\Library\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3926E878-0B91-464D-9201-B98C95FF2EE4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32259D83-D5C4-4B74-9EEE-4682E0C1C0D3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3456" yWindow="3456" windowWidth="27000" windowHeight="17244" tabRatio="406" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3040" yWindow="3040" windowWidth="22500" windowHeight="14300" tabRatio="406" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="en" sheetId="3" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="868" uniqueCount="558">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="872" uniqueCount="561">
   <si>
     <t>City</t>
   </si>
@@ -1704,6 +1704,15 @@
   </si>
   <si>
     <t>Einzeltag</t>
+  </si>
+  <si>
+    <t>AcademicTitle</t>
+  </si>
+  <si>
+    <t>Academic title</t>
+  </si>
+  <si>
+    <t>Akademischer Titel</t>
   </si>
 </sst>
 </file>
@@ -2094,17 +2103,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B218"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A187" workbookViewId="0">
-      <selection activeCell="B218" sqref="B218"/>
+    <sheetView tabSelected="1" topLeftCell="A193" workbookViewId="0">
+      <selection activeCell="A218" sqref="A218:B218"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="37.33203125" customWidth="1"/>
-    <col min="2" max="2" width="80.33203125" style="5" customWidth="1"/>
+    <col min="1" max="1" width="37.36328125" customWidth="1"/>
+    <col min="2" max="2" width="80.36328125" style="5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>20</v>
       </c>
@@ -2112,7 +2121,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>50</v>
       </c>
@@ -2120,7 +2129,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>479</v>
       </c>
@@ -2128,7 +2137,7 @@
         <v>480</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>484</v>
       </c>
@@ -2136,7 +2145,7 @@
         <v>481</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>357</v>
       </c>
@@ -2144,7 +2153,7 @@
         <v>356</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>129</v>
       </c>
@@ -2152,7 +2161,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
         <v>494</v>
       </c>
@@ -2160,7 +2169,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>491</v>
       </c>
@@ -2168,7 +2177,7 @@
         <v>493</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2" ht="29" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
         <v>246</v>
       </c>
@@ -2176,7 +2185,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
         <v>65</v>
       </c>
@@ -2184,7 +2193,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>162</v>
       </c>
@@ -2192,7 +2201,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
         <v>222</v>
       </c>
@@ -2200,7 +2209,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
         <v>224</v>
       </c>
@@ -2208,7 +2217,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
         <v>151</v>
       </c>
@@ -2216,7 +2225,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
         <v>476</v>
       </c>
@@ -2224,7 +2233,7 @@
         <v>478</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
         <v>43</v>
       </c>
@@ -2232,7 +2241,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
         <v>51</v>
       </c>
@@ -2240,7 +2249,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A18" s="1" t="s">
         <v>93</v>
       </c>
@@ -2248,7 +2257,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A19" s="1" t="s">
         <v>229</v>
       </c>
@@ -2256,7 +2265,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A20" s="1" t="s">
         <v>428</v>
       </c>
@@ -2264,7 +2273,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>435</v>
       </c>
@@ -2272,7 +2281,7 @@
         <v>437</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A22" s="1" t="s">
         <v>416</v>
       </c>
@@ -2280,7 +2289,7 @@
         <v>418</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A23" s="1" t="s">
         <v>282</v>
       </c>
@@ -2288,7 +2297,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A24" s="1" t="s">
         <v>291</v>
       </c>
@@ -2296,7 +2305,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A25" s="1" t="s">
         <v>495</v>
       </c>
@@ -2304,7 +2313,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A26" s="1" t="s">
         <v>497</v>
       </c>
@@ -2312,7 +2321,7 @@
         <v>497</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A27" s="1" t="s">
         <v>60</v>
       </c>
@@ -2320,7 +2329,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A28" s="1" t="s">
         <v>61</v>
       </c>
@@ -2328,7 +2337,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A29" s="1" t="s">
         <v>0</v>
       </c>
@@ -2336,7 +2345,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A30" s="1" t="s">
         <v>448</v>
       </c>
@@ -2344,7 +2353,7 @@
         <v>396</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>196</v>
       </c>
@@ -2352,7 +2361,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A32" s="1" t="s">
         <v>267</v>
       </c>
@@ -2360,7 +2369,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>501</v>
       </c>
@@ -2368,7 +2377,7 @@
         <v>501</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>294</v>
       </c>
@@ -2376,7 +2385,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A35" s="1" t="s">
         <v>91</v>
       </c>
@@ -2384,7 +2393,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A36" s="1" t="s">
         <v>444</v>
       </c>
@@ -2392,7 +2401,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>399</v>
       </c>
@@ -2400,7 +2409,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A38" s="1" t="s">
         <v>399</v>
       </c>
@@ -2408,7 +2417,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>446</v>
       </c>
@@ -2416,7 +2425,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>264</v>
       </c>
@@ -2424,7 +2433,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A41" s="1" t="s">
         <v>17</v>
       </c>
@@ -2432,7 +2441,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A42" s="1" t="s">
         <v>18</v>
       </c>
@@ -2440,7 +2449,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A43" s="1" t="s">
         <v>256</v>
       </c>
@@ -2448,7 +2457,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A44" s="1" t="s">
         <v>422</v>
       </c>
@@ -2456,7 +2465,7 @@
         <v>423</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
         <v>142</v>
       </c>
@@ -2464,7 +2473,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A46" s="1" t="s">
         <v>99</v>
       </c>
@@ -2472,7 +2481,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A47" s="1" t="s">
         <v>243</v>
       </c>
@@ -2480,7 +2489,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
         <v>293</v>
       </c>
@@ -2488,7 +2497,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A49" s="1" t="s">
         <v>221</v>
       </c>
@@ -2496,7 +2505,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
         <v>502</v>
       </c>
@@ -2504,7 +2513,7 @@
         <v>502</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A51" s="1" t="s">
         <v>62</v>
       </c>
@@ -2512,7 +2521,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
         <v>301</v>
       </c>
@@ -2520,7 +2529,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
         <v>303</v>
       </c>
@@ -2528,7 +2537,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
         <v>300</v>
       </c>
@@ -2536,7 +2545,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A55" s="1" t="s">
         <v>107</v>
       </c>
@@ -2544,7 +2553,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A56" s="1" t="s">
         <v>199</v>
       </c>
@@ -2552,7 +2561,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A57" s="1" t="s">
         <v>24</v>
       </c>
@@ -2560,7 +2569,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A58" s="1" t="s">
         <v>460</v>
       </c>
@@ -2568,7 +2577,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A59" s="1" t="s">
         <v>285</v>
       </c>
@@ -2576,7 +2585,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A60" s="1" t="s">
         <v>456</v>
       </c>
@@ -2584,7 +2593,7 @@
         <v>457</v>
       </c>
     </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A61" s="1" t="s">
         <v>115</v>
       </c>
@@ -2592,7 +2601,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
         <v>447</v>
       </c>
@@ -2600,7 +2609,7 @@
         <v>366</v>
       </c>
     </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A63" s="1" t="s">
         <v>232</v>
       </c>
@@ -2608,7 +2617,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
         <v>139</v>
       </c>
@@ -2616,7 +2625,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A65" s="1" t="s">
         <v>69</v>
       </c>
@@ -2624,7 +2633,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A66" s="1" t="s">
         <v>68</v>
       </c>
@@ -2632,7 +2641,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A67" s="1" t="s">
         <v>1</v>
       </c>
@@ -2640,7 +2649,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A68" s="1" t="s">
         <v>70</v>
       </c>
@@ -2648,7 +2657,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A69" s="1" t="s">
         <v>241</v>
       </c>
@@ -2656,7 +2665,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A70" s="1" t="s">
         <v>36</v>
       </c>
@@ -2664,7 +2673,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A71" s="1" t="s">
         <v>113</v>
       </c>
@@ -2672,7 +2681,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A72" s="1" t="s">
         <v>244</v>
       </c>
@@ -2680,7 +2689,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
         <v>141</v>
       </c>
@@ -2688,7 +2697,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A74" t="s">
         <v>299</v>
       </c>
@@ -2696,7 +2705,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A75" t="s">
         <v>353</v>
       </c>
@@ -2704,7 +2713,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A76" t="s">
         <v>302</v>
       </c>
@@ -2712,7 +2721,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A77" t="s">
         <v>296</v>
       </c>
@@ -2720,7 +2729,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A78" t="s">
         <v>298</v>
       </c>
@@ -2728,7 +2737,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A79" t="s">
         <v>201</v>
       </c>
@@ -2736,7 +2745,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A80" t="s">
         <v>193</v>
       </c>
@@ -2744,7 +2753,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A81" s="1" t="s">
         <v>213</v>
       </c>
@@ -2752,7 +2761,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A82" s="1" t="s">
         <v>214</v>
       </c>
@@ -2760,7 +2769,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A83" s="1" t="s">
         <v>219</v>
       </c>
@@ -2768,7 +2777,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A84" s="1" t="s">
         <v>220</v>
       </c>
@@ -2776,7 +2785,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A85" s="1" t="s">
         <v>34</v>
       </c>
@@ -2784,7 +2793,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A86" t="s">
         <v>140</v>
       </c>
@@ -2792,7 +2801,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A87" s="1" t="s">
         <v>2</v>
       </c>
@@ -2800,7 +2809,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A88" s="1" t="s">
         <v>468</v>
       </c>
@@ -2808,7 +2817,7 @@
         <v>469</v>
       </c>
     </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A89" s="1" t="s">
         <v>470</v>
       </c>
@@ -2816,7 +2825,7 @@
         <v>470</v>
       </c>
     </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A90" s="1" t="s">
         <v>471</v>
       </c>
@@ -2824,7 +2833,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A91" s="1" t="s">
         <v>153</v>
       </c>
@@ -2832,7 +2841,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A92" s="1" t="s">
         <v>410</v>
       </c>
@@ -2840,7 +2849,7 @@
         <v>411</v>
       </c>
     </row>
-    <row r="93" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A93" s="1" t="s">
         <v>412</v>
       </c>
@@ -2848,7 +2857,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A94" t="s">
         <v>297</v>
       </c>
@@ -2856,7 +2865,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="95" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A95" s="1" t="s">
         <v>270</v>
       </c>
@@ -2864,7 +2873,7 @@
         <v>486</v>
       </c>
     </row>
-    <row r="96" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A96" s="1" t="s">
         <v>408</v>
       </c>
@@ -2872,7 +2881,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A97" s="1" t="s">
         <v>3</v>
       </c>
@@ -2880,7 +2889,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A98" t="s">
         <v>500</v>
       </c>
@@ -2888,7 +2897,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A99" t="s">
         <v>161</v>
       </c>
@@ -2896,7 +2905,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="100" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A100" t="s">
         <v>163</v>
       </c>
@@ -2904,7 +2913,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="101" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A101" t="s">
         <v>166</v>
       </c>
@@ -2912,7 +2921,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="102" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A102" t="s">
         <v>27</v>
       </c>
@@ -2920,7 +2929,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="103" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A103" s="1" t="s">
         <v>42</v>
       </c>
@@ -2928,7 +2937,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="104" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A104" s="1" t="s">
         <v>40</v>
       </c>
@@ -2936,7 +2945,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="105" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A105" t="s">
         <v>148</v>
       </c>
@@ -2944,7 +2953,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="106" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A106" s="1" t="s">
         <v>20</v>
       </c>
@@ -2952,7 +2961,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="107" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A107" t="s">
         <v>204</v>
       </c>
@@ -2960,7 +2969,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="108" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A108" t="s">
         <v>131</v>
       </c>
@@ -2968,7 +2977,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="109" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A109" s="1" t="s">
         <v>441</v>
       </c>
@@ -2976,7 +2985,7 @@
         <v>443</v>
       </c>
     </row>
-    <row r="110" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A110" s="1" t="s">
         <v>419</v>
       </c>
@@ -2984,7 +2993,7 @@
         <v>421</v>
       </c>
     </row>
-    <row r="111" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A111" s="1" t="s">
         <v>97</v>
       </c>
@@ -2992,7 +3001,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="112" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A112" t="s">
         <v>510</v>
       </c>
@@ -3000,7 +3009,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="113" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A113" t="s">
         <v>167</v>
       </c>
@@ -3008,7 +3017,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="114" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A114" t="s">
         <v>168</v>
       </c>
@@ -3016,7 +3025,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="115" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A115" t="s">
         <v>169</v>
       </c>
@@ -3024,7 +3033,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="116" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A116" s="1" t="s">
         <v>488</v>
       </c>
@@ -3032,7 +3041,7 @@
         <v>490</v>
       </c>
     </row>
-    <row r="117" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A117" s="1" t="s">
         <v>94</v>
       </c>
@@ -3040,7 +3049,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="118" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A118" s="1" t="s">
         <v>64</v>
       </c>
@@ -3048,7 +3057,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="119" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A119" s="1" t="s">
         <v>67</v>
       </c>
@@ -3056,7 +3065,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="120" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A120" s="1" t="s">
         <v>463</v>
       </c>
@@ -3064,7 +3073,7 @@
         <v>463</v>
       </c>
     </row>
-    <row r="121" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A121" s="1" t="s">
         <v>258</v>
       </c>
@@ -3072,7 +3081,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="122" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A122" s="1" t="s">
         <v>425</v>
       </c>
@@ -3080,7 +3089,7 @@
         <v>426</v>
       </c>
     </row>
-    <row r="123" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A123" s="1" t="s">
         <v>262</v>
       </c>
@@ -3088,7 +3097,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="124" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A124" s="1" t="s">
         <v>274</v>
       </c>
@@ -3096,7 +3105,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="125" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A125" t="s">
         <v>295</v>
       </c>
@@ -3104,7 +3113,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="126" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A126" t="s">
         <v>310</v>
       </c>
@@ -3112,7 +3121,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="127" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A127" t="s">
         <v>311</v>
       </c>
@@ -3120,7 +3129,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="128" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A128" t="s">
         <v>309</v>
       </c>
@@ -3128,7 +3137,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="129" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A129" t="s">
         <v>312</v>
       </c>
@@ -3136,7 +3145,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="130" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:2" ht="29" x14ac:dyDescent="0.35">
       <c r="A130" s="1" t="s">
         <v>465</v>
       </c>
@@ -3144,7 +3153,7 @@
         <v>467</v>
       </c>
     </row>
-    <row r="131" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A131" t="s">
         <v>308</v>
       </c>
@@ -3152,7 +3161,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="132" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A132" s="1" t="s">
         <v>135</v>
       </c>
@@ -3160,7 +3169,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="133" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A133" s="1" t="s">
         <v>137</v>
       </c>
@@ -3168,7 +3177,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="134" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A134" s="1" t="s">
         <v>45</v>
       </c>
@@ -3176,7 +3185,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="135" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A135" t="s">
         <v>29</v>
       </c>
@@ -3184,7 +3193,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="136" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A136" s="1" t="s">
         <v>450</v>
       </c>
@@ -3192,7 +3201,7 @@
         <v>454</v>
       </c>
     </row>
-    <row r="137" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A137" s="1" t="s">
         <v>393</v>
       </c>
@@ -3200,7 +3209,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="138" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A138" s="1" t="s">
         <v>102</v>
       </c>
@@ -3208,7 +3217,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="139" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A139" s="1" t="s">
         <v>79</v>
       </c>
@@ -3216,7 +3225,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="140" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A140" s="1" t="s">
         <v>156</v>
       </c>
@@ -3224,7 +3233,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="141" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A141" s="1" t="s">
         <v>206</v>
       </c>
@@ -3232,7 +3241,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="142" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A142" s="1" t="s">
         <v>249</v>
       </c>
@@ -3240,7 +3249,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="143" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A143" s="1" t="s">
         <v>275</v>
       </c>
@@ -3248,7 +3257,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="144" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A144" s="1" t="s">
         <v>288</v>
       </c>
@@ -3256,7 +3265,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="145" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A145" s="1" t="s">
         <v>273</v>
       </c>
@@ -3264,7 +3273,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="146" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A146" s="1" t="s">
         <v>133</v>
       </c>
@@ -3272,7 +3281,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="147" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A147" s="1" t="s">
         <v>76</v>
       </c>
@@ -3280,7 +3289,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="148" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A148" s="1" t="s">
         <v>53</v>
       </c>
@@ -3288,7 +3297,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="149" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A149" s="1" t="s">
         <v>280</v>
       </c>
@@ -3296,7 +3305,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="150" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A150" s="1" t="s">
         <v>47</v>
       </c>
@@ -3304,7 +3313,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="151" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A151" s="1" t="s">
         <v>56</v>
       </c>
@@ -3312,7 +3321,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="152" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A152" t="s">
         <v>374</v>
       </c>
@@ -3320,7 +3329,7 @@
         <v>374</v>
       </c>
     </row>
-    <row r="153" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A153" t="s">
         <v>368</v>
       </c>
@@ -3328,7 +3337,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="154" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A154" s="1" t="s">
         <v>432</v>
       </c>
@@ -3336,7 +3345,7 @@
         <v>433</v>
       </c>
     </row>
-    <row r="155" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A155" t="s">
         <v>376</v>
       </c>
@@ -3344,7 +3353,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="156" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A156" t="s">
         <v>384</v>
       </c>
@@ -3352,7 +3361,7 @@
         <v>378</v>
       </c>
     </row>
-    <row r="157" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A157" t="s">
         <v>379</v>
       </c>
@@ -3360,7 +3369,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="158" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A158" t="s">
         <v>370</v>
       </c>
@@ -3368,7 +3377,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="159" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A159" s="1" t="s">
         <v>112</v>
       </c>
@@ -3376,7 +3385,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="160" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A160" s="1" t="s">
         <v>4</v>
       </c>
@@ -3384,7 +3393,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="161" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A161" s="1" t="s">
         <v>109</v>
       </c>
@@ -3392,7 +3401,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="162" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A162" s="1" t="s">
         <v>25</v>
       </c>
@@ -3400,7 +3409,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="163" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A163" s="1" t="s">
         <v>438</v>
       </c>
@@ -3408,7 +3417,7 @@
         <v>439</v>
       </c>
     </row>
-    <row r="164" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="164" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A164" s="1" t="s">
         <v>250</v>
       </c>
@@ -3416,7 +3425,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="165" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="165" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A165" t="s">
         <v>499</v>
       </c>
@@ -3424,7 +3433,7 @@
         <v>499</v>
       </c>
     </row>
-    <row r="166" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="166" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A166" s="1" t="s">
         <v>228</v>
       </c>
@@ -3432,7 +3441,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="167" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="167" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A167" s="1" t="s">
         <v>231</v>
       </c>
@@ -3440,7 +3449,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="168" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="168" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A168" t="s">
         <v>28</v>
       </c>
@@ -3448,7 +3457,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="169" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="169" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A169" t="s">
         <v>237</v>
       </c>
@@ -3456,7 +3465,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="170" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="170" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A170" s="1" t="s">
         <v>238</v>
       </c>
@@ -3464,7 +3473,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="171" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="171" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A171" s="1" t="s">
         <v>114</v>
       </c>
@@ -3472,7 +3481,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="172" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="172" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A172" s="1" t="s">
         <v>5</v>
       </c>
@@ -3480,7 +3489,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="173" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="173" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A173" s="1" t="s">
         <v>6</v>
       </c>
@@ -3488,7 +3497,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="174" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="174" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A174" s="1" t="s">
         <v>7</v>
       </c>
@@ -3496,7 +3505,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="175" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="175" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A175" s="1" t="s">
         <v>111</v>
       </c>
@@ -3504,7 +3513,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="176" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="176" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A176" t="s">
         <v>385</v>
       </c>
@@ -3512,7 +3521,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="177" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="177" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A177" s="1" t="s">
         <v>430</v>
       </c>
@@ -3520,7 +3529,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="178" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="178" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A178" s="1" t="s">
         <v>110</v>
       </c>
@@ -3528,7 +3537,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="179" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="179" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A179" s="1" t="s">
         <v>403</v>
       </c>
@@ -3536,7 +3545,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="180" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="180" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A180" s="1" t="s">
         <v>405</v>
       </c>
@@ -3544,7 +3553,7 @@
         <v>406</v>
       </c>
     </row>
-    <row r="181" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="181" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A181" t="s">
         <v>164</v>
       </c>
@@ -3552,7 +3561,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="182" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="182" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A182" t="s">
         <v>190</v>
       </c>
@@ -3560,7 +3569,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="183" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="183" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A183" s="1" t="s">
         <v>121</v>
       </c>
@@ -3568,7 +3577,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="184" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="184" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A184" t="s">
         <v>304</v>
       </c>
@@ -3576,7 +3585,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="185" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="185" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A185" t="s">
         <v>306</v>
       </c>
@@ -3584,7 +3593,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="186" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="186" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A186" s="1" t="s">
         <v>389</v>
       </c>
@@ -3592,7 +3601,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="187" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="187" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A187" t="s">
         <v>305</v>
       </c>
@@ -3600,7 +3609,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="188" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="188" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A188" t="s">
         <v>359</v>
       </c>
@@ -3608,7 +3617,7 @@
         <v>358</v>
       </c>
     </row>
-    <row r="189" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="189" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A189" t="s">
         <v>307</v>
       </c>
@@ -3616,7 +3625,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="190" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="190" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A190" t="s">
         <v>159</v>
       </c>
@@ -3624,7 +3633,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="191" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="191" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A191" t="s">
         <v>160</v>
       </c>
@@ -3632,7 +3641,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="192" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="192" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A192" t="s">
         <v>165</v>
       </c>
@@ -3640,7 +3649,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="193" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="193" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A193" s="1" t="s">
         <v>449</v>
       </c>
@@ -3648,7 +3657,7 @@
         <v>455</v>
       </c>
     </row>
-    <row r="194" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="194" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A194" s="1" t="s">
         <v>89</v>
       </c>
@@ -3656,7 +3665,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="195" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="195" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A195" s="1" t="s">
         <v>391</v>
       </c>
@@ -3664,7 +3673,7 @@
         <v>392</v>
       </c>
     </row>
-    <row r="196" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="196" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A196" t="s">
         <v>503</v>
       </c>
@@ -3672,7 +3681,7 @@
         <v>503</v>
       </c>
     </row>
-    <row r="197" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="197" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A197" s="1" t="s">
         <v>95</v>
       </c>
@@ -3680,7 +3689,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="198" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="198" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A198" s="1" t="s">
         <v>8</v>
       </c>
@@ -3688,7 +3697,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="199" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="199" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A199" s="1" t="s">
         <v>511</v>
       </c>
@@ -3696,7 +3705,7 @@
         <v>513</v>
       </c>
     </row>
-    <row r="200" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="200" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A200" s="1" t="s">
         <v>512</v>
       </c>
@@ -3704,7 +3713,7 @@
         <v>514</v>
       </c>
     </row>
-    <row r="201" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="201" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A201" t="s">
         <v>517</v>
       </c>
@@ -3712,7 +3721,7 @@
         <v>518</v>
       </c>
     </row>
-    <row r="202" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="202" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A202" s="1" t="s">
         <v>520</v>
       </c>
@@ -3720,7 +3729,7 @@
         <v>521</v>
       </c>
     </row>
-    <row r="203" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="203" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A203" s="1" t="s">
         <v>522</v>
       </c>
@@ -3728,7 +3737,7 @@
         <v>523</v>
       </c>
     </row>
-    <row r="204" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="204" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A204" s="1" t="s">
         <v>525</v>
       </c>
@@ -3736,7 +3745,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="205" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="205" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A205" t="s">
         <v>528</v>
       </c>
@@ -3744,7 +3753,7 @@
         <v>529</v>
       </c>
     </row>
-    <row r="206" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="206" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A206" s="1" t="s">
         <v>531</v>
       </c>
@@ -3752,7 +3761,7 @@
         <v>531</v>
       </c>
     </row>
-    <row r="207" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="207" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A207" t="s">
         <v>536</v>
       </c>
@@ -3760,7 +3769,7 @@
         <v>535</v>
       </c>
     </row>
-    <row r="208" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="208" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A208" s="1" t="s">
         <v>537</v>
       </c>
@@ -3768,7 +3777,7 @@
         <v>539</v>
       </c>
     </row>
-    <row r="209" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="209" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A209" t="s">
         <v>540</v>
       </c>
@@ -3776,7 +3785,7 @@
         <v>540</v>
       </c>
     </row>
-    <row r="210" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="210" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A210" t="s">
         <v>542</v>
       </c>
@@ -3784,7 +3793,7 @@
         <v>542</v>
       </c>
     </row>
-    <row r="211" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="211" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A211" t="s">
         <v>544</v>
       </c>
@@ -3792,7 +3801,7 @@
         <v>544</v>
       </c>
     </row>
-    <row r="212" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="212" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A212" t="s">
         <v>546</v>
       </c>
@@ -3800,7 +3809,7 @@
         <v>546</v>
       </c>
     </row>
-    <row r="213" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="213" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A213" s="1" t="s">
         <v>532</v>
       </c>
@@ -3808,7 +3817,7 @@
         <v>532</v>
       </c>
     </row>
-    <row r="214" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="214" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A214" t="s">
         <v>551</v>
       </c>
@@ -3816,7 +3825,7 @@
         <v>551</v>
       </c>
     </row>
-    <row r="215" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="215" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A215" t="s">
         <v>549</v>
       </c>
@@ -3824,7 +3833,7 @@
         <v>549</v>
       </c>
     </row>
-    <row r="216" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="216" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A216" t="s">
         <v>553</v>
       </c>
@@ -3832,7 +3841,7 @@
         <v>553</v>
       </c>
     </row>
-    <row r="217" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="217" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A217" t="s">
         <v>555</v>
       </c>
@@ -3840,9 +3849,12 @@
         <v>556</v>
       </c>
     </row>
-    <row r="218" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="218" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A218" t="s">
+        <v>558</v>
+      </c>
       <c r="B218" s="5" t="s">
-        <v>557</v>
+        <v>559</v>
       </c>
     </row>
   </sheetData>
@@ -3858,19 +3870,19 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:B217"/>
+  <dimension ref="A1:B218"/>
   <sheetViews>
-    <sheetView topLeftCell="A185" workbookViewId="0">
-      <selection activeCell="B217" sqref="B217"/>
+    <sheetView topLeftCell="A191" workbookViewId="0">
+      <selection activeCell="B218" sqref="B218"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="31.5546875" customWidth="1"/>
-    <col min="2" max="2" width="62.5546875" customWidth="1"/>
+    <col min="1" max="1" width="31.54296875" customWidth="1"/>
+    <col min="2" max="2" width="62.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>20</v>
       </c>
@@ -3878,7 +3890,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>50</v>
       </c>
@@ -3886,7 +3898,7 @@
         <v>487</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>479</v>
       </c>
@@ -3894,7 +3906,7 @@
         <v>482</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>484</v>
       </c>
@@ -3902,7 +3914,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>357</v>
       </c>
@@ -3910,7 +3922,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>129</v>
       </c>
@@ -3918,7 +3930,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
         <v>494</v>
       </c>
@@ -3926,7 +3938,7 @@
         <v>459</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>491</v>
       </c>
@@ -3934,7 +3946,7 @@
         <v>492</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
         <v>246</v>
       </c>
@@ -3942,7 +3954,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
         <v>65</v>
       </c>
@@ -3950,7 +3962,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>162</v>
       </c>
@@ -3958,7 +3970,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
         <v>222</v>
       </c>
@@ -3966,7 +3978,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
         <v>224</v>
       </c>
@@ -3974,7 +3986,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
         <v>151</v>
       </c>
@@ -3982,7 +3994,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
         <v>476</v>
       </c>
@@ -3990,7 +4002,7 @@
         <v>477</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
         <v>43</v>
       </c>
@@ -3998,7 +4010,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
         <v>51</v>
       </c>
@@ -4006,7 +4018,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A18" s="1" t="s">
         <v>93</v>
       </c>
@@ -4014,7 +4026,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A19" s="1" t="s">
         <v>229</v>
       </c>
@@ -4022,7 +4034,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A20" s="1" t="s">
         <v>428</v>
       </c>
@@ -4030,7 +4042,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>435</v>
       </c>
@@ -4038,7 +4050,7 @@
         <v>436</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A22" s="1" t="s">
         <v>416</v>
       </c>
@@ -4046,7 +4058,7 @@
         <v>417</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A23" s="1" t="s">
         <v>282</v>
       </c>
@@ -4054,7 +4066,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A24" s="1" t="s">
         <v>291</v>
       </c>
@@ -4062,7 +4074,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A25" s="1" t="s">
         <v>495</v>
       </c>
@@ -4070,7 +4082,7 @@
         <v>496</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A26" s="1" t="s">
         <v>497</v>
       </c>
@@ -4078,7 +4090,7 @@
         <v>498</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A27" s="1" t="s">
         <v>60</v>
       </c>
@@ -4086,7 +4098,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A28" s="1" t="s">
         <v>61</v>
       </c>
@@ -4094,7 +4106,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A29" s="1" t="s">
         <v>0</v>
       </c>
@@ -4102,7 +4114,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A30" s="1" t="s">
         <v>448</v>
       </c>
@@ -4110,7 +4122,7 @@
         <v>398</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>196</v>
       </c>
@@ -4118,7 +4130,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A32" s="1" t="s">
         <v>267</v>
       </c>
@@ -4126,7 +4138,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>501</v>
       </c>
@@ -4134,7 +4146,7 @@
         <v>507</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>294</v>
       </c>
@@ -4142,7 +4154,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A35" s="1" t="s">
         <v>91</v>
       </c>
@@ -4150,7 +4162,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A36" s="1" t="s">
         <v>444</v>
       </c>
@@ -4158,7 +4170,7 @@
         <v>451</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>399</v>
       </c>
@@ -4166,7 +4178,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A38" s="1" t="s">
         <v>399</v>
       </c>
@@ -4174,7 +4186,7 @@
         <v>401</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>446</v>
       </c>
@@ -4182,7 +4194,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>264</v>
       </c>
@@ -4190,7 +4202,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A41" s="1" t="s">
         <v>17</v>
       </c>
@@ -4198,7 +4210,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A42" s="1" t="s">
         <v>18</v>
       </c>
@@ -4206,7 +4218,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A43" s="1" t="s">
         <v>256</v>
       </c>
@@ -4214,7 +4226,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A44" s="1" t="s">
         <v>422</v>
       </c>
@@ -4222,7 +4234,7 @@
         <v>424</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
         <v>142</v>
       </c>
@@ -4230,7 +4242,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A46" s="1" t="s">
         <v>99</v>
       </c>
@@ -4238,7 +4250,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A47" s="1" t="s">
         <v>243</v>
       </c>
@@ -4246,7 +4258,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
         <v>293</v>
       </c>
@@ -4254,7 +4266,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A49" s="1" t="s">
         <v>221</v>
       </c>
@@ -4262,7 +4274,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
         <v>502</v>
       </c>
@@ -4270,7 +4282,7 @@
         <v>508</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A51" s="1" t="s">
         <v>62</v>
       </c>
@@ -4278,7 +4290,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
         <v>301</v>
       </c>
@@ -4286,7 +4298,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
         <v>303</v>
       </c>
@@ -4294,7 +4306,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
         <v>300</v>
       </c>
@@ -4302,7 +4314,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A55" s="1" t="s">
         <v>107</v>
       </c>
@@ -4310,7 +4322,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A56" s="1" t="s">
         <v>199</v>
       </c>
@@ -4318,7 +4330,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A57" s="1" t="s">
         <v>24</v>
       </c>
@@ -4326,7 +4338,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A58" s="1" t="s">
         <v>460</v>
       </c>
@@ -4334,7 +4346,7 @@
         <v>462</v>
       </c>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A59" s="1" t="s">
         <v>285</v>
       </c>
@@ -4342,7 +4354,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A60" s="1" t="s">
         <v>456</v>
       </c>
@@ -4350,7 +4362,7 @@
         <v>458</v>
       </c>
     </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A61" s="1" t="s">
         <v>115</v>
       </c>
@@ -4358,7 +4370,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
         <v>447</v>
       </c>
@@ -4366,7 +4378,7 @@
         <v>367</v>
       </c>
     </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A63" s="1" t="s">
         <v>232</v>
       </c>
@@ -4374,7 +4386,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
         <v>139</v>
       </c>
@@ -4382,7 +4394,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A65" s="1" t="s">
         <v>69</v>
       </c>
@@ -4390,7 +4402,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A66" s="1" t="s">
         <v>68</v>
       </c>
@@ -4398,7 +4410,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A67" s="1" t="s">
         <v>1</v>
       </c>
@@ -4406,7 +4418,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A68" s="1" t="s">
         <v>70</v>
       </c>
@@ -4414,7 +4426,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A69" s="1" t="s">
         <v>241</v>
       </c>
@@ -4422,7 +4434,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A70" s="1" t="s">
         <v>36</v>
       </c>
@@ -4430,7 +4442,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A71" s="1" t="s">
         <v>113</v>
       </c>
@@ -4438,7 +4450,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A72" s="1" t="s">
         <v>244</v>
       </c>
@@ -4446,7 +4458,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
         <v>141</v>
       </c>
@@ -4454,7 +4466,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A74" t="s">
         <v>299</v>
       </c>
@@ -4462,7 +4474,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A75" t="s">
         <v>353</v>
       </c>
@@ -4470,7 +4482,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A76" t="s">
         <v>302</v>
       </c>
@@ -4478,7 +4490,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A77" t="s">
         <v>296</v>
       </c>
@@ -4486,7 +4498,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A78" t="s">
         <v>298</v>
       </c>
@@ -4494,7 +4506,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A79" t="s">
         <v>201</v>
       </c>
@@ -4502,7 +4514,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A80" t="s">
         <v>193</v>
       </c>
@@ -4510,7 +4522,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A81" s="1" t="s">
         <v>213</v>
       </c>
@@ -4518,7 +4530,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A82" s="1" t="s">
         <v>214</v>
       </c>
@@ -4526,7 +4538,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A83" s="1" t="s">
         <v>219</v>
       </c>
@@ -4534,7 +4546,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A84" s="1" t="s">
         <v>220</v>
       </c>
@@ -4542,7 +4554,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A85" s="1" t="s">
         <v>34</v>
       </c>
@@ -4550,7 +4562,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A86" t="s">
         <v>140</v>
       </c>
@@ -4558,7 +4570,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A87" s="1" t="s">
         <v>2</v>
       </c>
@@ -4566,7 +4578,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A88" s="1" t="s">
         <v>468</v>
       </c>
@@ -4574,7 +4586,7 @@
         <v>473</v>
       </c>
     </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A89" s="1" t="s">
         <v>470</v>
       </c>
@@ -4582,7 +4594,7 @@
         <v>474</v>
       </c>
     </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A90" s="1" t="s">
         <v>471</v>
       </c>
@@ -4590,7 +4602,7 @@
         <v>475</v>
       </c>
     </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A91" s="1" t="s">
         <v>153</v>
       </c>
@@ -4598,7 +4610,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A92" s="1" t="s">
         <v>410</v>
       </c>
@@ -4606,7 +4618,7 @@
         <v>415</v>
       </c>
     </row>
-    <row r="93" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A93" s="1" t="s">
         <v>412</v>
       </c>
@@ -4614,7 +4626,7 @@
         <v>414</v>
       </c>
     </row>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A94" t="s">
         <v>297</v>
       </c>
@@ -4622,7 +4634,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="95" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A95" s="1" t="s">
         <v>270</v>
       </c>
@@ -4630,7 +4642,7 @@
         <v>485</v>
       </c>
     </row>
-    <row r="96" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A96" s="1" t="s">
         <v>408</v>
       </c>
@@ -4638,7 +4650,7 @@
         <v>409</v>
       </c>
     </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A97" s="1" t="s">
         <v>3</v>
       </c>
@@ -4646,7 +4658,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A98" t="s">
         <v>500</v>
       </c>
@@ -4654,7 +4666,7 @@
         <v>506</v>
       </c>
     </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A99" t="s">
         <v>161</v>
       </c>
@@ -4662,7 +4674,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="100" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A100" t="s">
         <v>163</v>
       </c>
@@ -4670,7 +4682,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="101" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A101" t="s">
         <v>166</v>
       </c>
@@ -4678,7 +4690,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="102" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A102" t="s">
         <v>27</v>
       </c>
@@ -4686,7 +4698,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="103" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A103" s="1" t="s">
         <v>42</v>
       </c>
@@ -4694,7 +4706,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="104" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A104" s="1" t="s">
         <v>40</v>
       </c>
@@ -4702,7 +4714,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="105" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A105" t="s">
         <v>148</v>
       </c>
@@ -4710,7 +4722,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="106" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A106" s="1" t="s">
         <v>20</v>
       </c>
@@ -4718,7 +4730,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="107" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A107" t="s">
         <v>204</v>
       </c>
@@ -4726,7 +4738,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="108" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A108" t="s">
         <v>131</v>
       </c>
@@ -4734,7 +4746,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="109" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A109" s="1" t="s">
         <v>441</v>
       </c>
@@ -4742,7 +4754,7 @@
         <v>442</v>
       </c>
     </row>
-    <row r="110" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A110" s="1" t="s">
         <v>419</v>
       </c>
@@ -4750,7 +4762,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="111" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A111" s="1" t="s">
         <v>97</v>
       </c>
@@ -4758,7 +4770,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="112" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A112" t="s">
         <v>510</v>
       </c>
@@ -4766,7 +4778,7 @@
         <v>505</v>
       </c>
     </row>
-    <row r="113" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A113" t="s">
         <v>167</v>
       </c>
@@ -4774,7 +4786,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="114" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A114" t="s">
         <v>168</v>
       </c>
@@ -4782,7 +4794,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="115" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A115" t="s">
         <v>169</v>
       </c>
@@ -4790,7 +4802,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="116" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A116" s="1" t="s">
         <v>488</v>
       </c>
@@ -4798,7 +4810,7 @@
         <v>489</v>
       </c>
     </row>
-    <row r="117" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A117" s="1" t="s">
         <v>94</v>
       </c>
@@ -4806,7 +4818,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="118" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A118" s="1" t="s">
         <v>64</v>
       </c>
@@ -4814,7 +4826,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="119" spans="1:2" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:2" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A119" s="1" t="s">
         <v>67</v>
       </c>
@@ -4822,7 +4834,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="120" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A120" s="1" t="s">
         <v>463</v>
       </c>
@@ -4830,7 +4842,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="121" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A121" s="1" t="s">
         <v>258</v>
       </c>
@@ -4838,7 +4850,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="122" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A122" s="1" t="s">
         <v>425</v>
       </c>
@@ -4846,7 +4858,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="123" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A123" s="1" t="s">
         <v>262</v>
       </c>
@@ -4854,7 +4866,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="124" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A124" s="1" t="s">
         <v>274</v>
       </c>
@@ -4862,7 +4874,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="125" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A125" t="s">
         <v>295</v>
       </c>
@@ -4870,7 +4882,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="126" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A126" t="s">
         <v>310</v>
       </c>
@@ -4878,7 +4890,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="127" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A127" t="s">
         <v>311</v>
       </c>
@@ -4886,7 +4898,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="128" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A128" t="s">
         <v>309</v>
       </c>
@@ -4894,7 +4906,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="129" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A129" t="s">
         <v>312</v>
       </c>
@@ -4902,7 +4914,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="130" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A130" s="1" t="s">
         <v>465</v>
       </c>
@@ -4910,7 +4922,7 @@
         <v>466</v>
       </c>
     </row>
-    <row r="131" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A131" t="s">
         <v>308</v>
       </c>
@@ -4918,7 +4930,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="132" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A132" s="1" t="s">
         <v>135</v>
       </c>
@@ -4926,7 +4938,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="133" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A133" s="1" t="s">
         <v>137</v>
       </c>
@@ -4934,7 +4946,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="134" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A134" s="1" t="s">
         <v>45</v>
       </c>
@@ -4942,7 +4954,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="135" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A135" t="s">
         <v>29</v>
       </c>
@@ -4950,7 +4962,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="136" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A136" s="1" t="s">
         <v>450</v>
       </c>
@@ -4958,7 +4970,7 @@
         <v>452</v>
       </c>
     </row>
-    <row r="137" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A137" s="1" t="s">
         <v>393</v>
       </c>
@@ -4966,7 +4978,7 @@
         <v>397</v>
       </c>
     </row>
-    <row r="138" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A138" s="1" t="s">
         <v>102</v>
       </c>
@@ -4974,7 +4986,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="139" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A139" s="1" t="s">
         <v>79</v>
       </c>
@@ -4982,7 +4994,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="140" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A140" s="1" t="s">
         <v>156</v>
       </c>
@@ -4990,7 +5002,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="141" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A141" s="1" t="s">
         <v>206</v>
       </c>
@@ -4998,7 +5010,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="142" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A142" s="1" t="s">
         <v>249</v>
       </c>
@@ -5006,7 +5018,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="143" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A143" s="1" t="s">
         <v>275</v>
       </c>
@@ -5014,7 +5026,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="144" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A144" s="1" t="s">
         <v>288</v>
       </c>
@@ -5022,7 +5034,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="145" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A145" s="1" t="s">
         <v>273</v>
       </c>
@@ -5030,7 +5042,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="146" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A146" s="1" t="s">
         <v>133</v>
       </c>
@@ -5038,7 +5050,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="147" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A147" s="1" t="s">
         <v>76</v>
       </c>
@@ -5046,7 +5058,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="148" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A148" s="1" t="s">
         <v>53</v>
       </c>
@@ -5054,7 +5066,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="149" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A149" s="1" t="s">
         <v>280</v>
       </c>
@@ -5062,7 +5074,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="150" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A150" s="1" t="s">
         <v>47</v>
       </c>
@@ -5070,7 +5082,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="151" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A151" s="1" t="s">
         <v>56</v>
       </c>
@@ -5078,7 +5090,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="152" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A152" t="s">
         <v>374</v>
       </c>
@@ -5086,7 +5098,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="153" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A153" t="s">
         <v>368</v>
       </c>
@@ -5094,7 +5106,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="154" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A154" s="1" t="s">
         <v>432</v>
       </c>
@@ -5102,7 +5114,7 @@
         <v>434</v>
       </c>
     </row>
-    <row r="155" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A155" t="s">
         <v>376</v>
       </c>
@@ -5110,7 +5122,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="156" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A156" t="s">
         <v>384</v>
       </c>
@@ -5118,7 +5130,7 @@
         <v>382</v>
       </c>
     </row>
-    <row r="157" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A157" t="s">
         <v>379</v>
       </c>
@@ -5126,7 +5138,7 @@
         <v>383</v>
       </c>
     </row>
-    <row r="158" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A158" t="s">
         <v>370</v>
       </c>
@@ -5134,7 +5146,7 @@
         <v>373</v>
       </c>
     </row>
-    <row r="159" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A159" s="1" t="s">
         <v>112</v>
       </c>
@@ -5142,7 +5154,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="160" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A160" s="1" t="s">
         <v>4</v>
       </c>
@@ -5150,7 +5162,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="161" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A161" s="1" t="s">
         <v>109</v>
       </c>
@@ -5158,7 +5170,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="162" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A162" s="1" t="s">
         <v>25</v>
       </c>
@@ -5166,7 +5178,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="163" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A163" s="1" t="s">
         <v>438</v>
       </c>
@@ -5174,7 +5186,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="164" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="164" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A164" s="1" t="s">
         <v>250</v>
       </c>
@@ -5182,7 +5194,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="165" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="165" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A165" t="s">
         <v>499</v>
       </c>
@@ -5190,7 +5202,7 @@
         <v>499</v>
       </c>
     </row>
-    <row r="166" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="166" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A166" s="1" t="s">
         <v>228</v>
       </c>
@@ -5198,7 +5210,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="167" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="167" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A167" s="1" t="s">
         <v>231</v>
       </c>
@@ -5206,7 +5218,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="168" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="168" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A168" t="s">
         <v>28</v>
       </c>
@@ -5214,7 +5226,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="169" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="169" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A169" t="s">
         <v>237</v>
       </c>
@@ -5222,7 +5234,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="170" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="170" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A170" s="1" t="s">
         <v>238</v>
       </c>
@@ -5230,7 +5242,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="171" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="171" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A171" s="1" t="s">
         <v>114</v>
       </c>
@@ -5238,7 +5250,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="172" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="172" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A172" s="1" t="s">
         <v>5</v>
       </c>
@@ -5246,7 +5258,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="173" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="173" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A173" s="1" t="s">
         <v>6</v>
       </c>
@@ -5254,7 +5266,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="174" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="174" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A174" s="1" t="s">
         <v>7</v>
       </c>
@@ -5262,7 +5274,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="175" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="175" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A175" s="1" t="s">
         <v>111</v>
       </c>
@@ -5270,7 +5282,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="176" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="176" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A176" t="s">
         <v>385</v>
       </c>
@@ -5278,7 +5290,7 @@
         <v>387</v>
       </c>
     </row>
-    <row r="177" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="177" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A177" s="1" t="s">
         <v>430</v>
       </c>
@@ -5286,7 +5298,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="178" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="178" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A178" s="1" t="s">
         <v>110</v>
       </c>
@@ -5294,7 +5306,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="179" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="179" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A179" s="1" t="s">
         <v>403</v>
       </c>
@@ -5302,7 +5314,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="180" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="180" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A180" s="1" t="s">
         <v>405</v>
       </c>
@@ -5310,7 +5322,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="181" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="181" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A181" t="s">
         <v>164</v>
       </c>
@@ -5318,7 +5330,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="182" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="182" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A182" t="s">
         <v>190</v>
       </c>
@@ -5326,7 +5338,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="183" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="183" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A183" s="1" t="s">
         <v>121</v>
       </c>
@@ -5334,7 +5346,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="184" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="184" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A184" t="s">
         <v>304</v>
       </c>
@@ -5342,7 +5354,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="185" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="185" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A185" t="s">
         <v>306</v>
       </c>
@@ -5350,7 +5362,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="186" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="186" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A186" s="1" t="s">
         <v>389</v>
       </c>
@@ -5358,7 +5370,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="187" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="187" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A187" t="s">
         <v>305</v>
       </c>
@@ -5366,7 +5378,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="188" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="188" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A188" t="s">
         <v>359</v>
       </c>
@@ -5374,7 +5386,7 @@
         <v>361</v>
       </c>
     </row>
-    <row r="189" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="189" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A189" t="s">
         <v>307</v>
       </c>
@@ -5382,7 +5394,7 @@
         <v>348</v>
       </c>
     </row>
-    <row r="190" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="190" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A190" t="s">
         <v>159</v>
       </c>
@@ -5390,7 +5402,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="191" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="191" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A191" t="s">
         <v>160</v>
       </c>
@@ -5398,7 +5410,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="192" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="192" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A192" t="s">
         <v>165</v>
       </c>
@@ -5406,7 +5418,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="193" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="193" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A193" s="1" t="s">
         <v>449</v>
       </c>
@@ -5414,7 +5426,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="194" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="194" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A194" s="1" t="s">
         <v>89</v>
       </c>
@@ -5422,7 +5434,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="195" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="195" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A195" s="1" t="s">
         <v>391</v>
       </c>
@@ -5430,7 +5442,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="196" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="196" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A196" t="s">
         <v>503</v>
       </c>
@@ -5438,7 +5450,7 @@
         <v>509</v>
       </c>
     </row>
-    <row r="197" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="197" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A197" s="1" t="s">
         <v>95</v>
       </c>
@@ -5446,7 +5458,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="198" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="198" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A198" s="1" t="s">
         <v>8</v>
       </c>
@@ -5454,7 +5466,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="199" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="199" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A199" s="1" t="s">
         <v>511</v>
       </c>
@@ -5462,7 +5474,7 @@
         <v>515</v>
       </c>
     </row>
-    <row r="200" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="200" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A200" s="1" t="s">
         <v>512</v>
       </c>
@@ -5470,7 +5482,7 @@
         <v>516</v>
       </c>
     </row>
-    <row r="201" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="201" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A201" t="s">
         <v>517</v>
       </c>
@@ -5478,7 +5490,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="202" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="202" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A202" s="1" t="s">
         <v>520</v>
       </c>
@@ -5486,7 +5498,7 @@
         <v>521</v>
       </c>
     </row>
-    <row r="203" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="203" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A203" t="s">
         <v>522</v>
       </c>
@@ -5494,7 +5506,7 @@
         <v>524</v>
       </c>
     </row>
-    <row r="204" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="204" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A204" s="1" t="s">
         <v>525</v>
       </c>
@@ -5502,7 +5514,7 @@
         <v>526</v>
       </c>
     </row>
-    <row r="205" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="205" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A205" t="s">
         <v>528</v>
       </c>
@@ -5510,7 +5522,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="206" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="206" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A206" s="1" t="s">
         <v>531</v>
       </c>
@@ -5518,7 +5530,7 @@
         <v>548</v>
       </c>
     </row>
-    <row r="207" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="207" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A207" t="s">
         <v>536</v>
       </c>
@@ -5526,7 +5538,7 @@
         <v>534</v>
       </c>
     </row>
-    <row r="208" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="208" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A208" s="1" t="s">
         <v>537</v>
       </c>
@@ -5534,7 +5546,7 @@
         <v>538</v>
       </c>
     </row>
-    <row r="209" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="209" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A209" t="s">
         <v>540</v>
       </c>
@@ -5542,7 +5554,7 @@
         <v>541</v>
       </c>
     </row>
-    <row r="210" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="210" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A210" t="s">
         <v>542</v>
       </c>
@@ -5550,7 +5562,7 @@
         <v>543</v>
       </c>
     </row>
-    <row r="211" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="211" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A211" t="s">
         <v>544</v>
       </c>
@@ -5558,7 +5570,7 @@
         <v>545</v>
       </c>
     </row>
-    <row r="212" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="212" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A212" t="s">
         <v>546</v>
       </c>
@@ -5566,7 +5578,7 @@
         <v>547</v>
       </c>
     </row>
-    <row r="213" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="213" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A213" s="1" t="s">
         <v>532</v>
       </c>
@@ -5574,7 +5586,7 @@
         <v>533</v>
       </c>
     </row>
-    <row r="214" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="214" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A214" t="s">
         <v>551</v>
       </c>
@@ -5582,7 +5594,7 @@
         <v>552</v>
       </c>
     </row>
-    <row r="215" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="215" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A215" t="s">
         <v>549</v>
       </c>
@@ -5590,7 +5602,7 @@
         <v>550</v>
       </c>
     </row>
-    <row r="216" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="216" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A216" t="s">
         <v>553</v>
       </c>
@@ -5598,9 +5610,20 @@
         <v>554</v>
       </c>
     </row>
-    <row r="217" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="217" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A217" t="s">
         <v>555</v>
+      </c>
+      <c r="B217" s="5" t="s">
+        <v>557</v>
+      </c>
+    </row>
+    <row r="218" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A218" t="s">
+        <v>558</v>
+      </c>
+      <c r="B218" s="5" t="s">
+        <v>560</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
CV page About enhanced
</commit_message>
<xml_diff>
--- a/Vitae/Library/Resources/SharedResource.xlsx
+++ b/Vitae/Library/Resources/SharedResource.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\Vitae\Library\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D13BB17F-C59A-4437-BBEF-2F93D0B12EB0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE754FB5-EF1D-4991-9BC3-791CD67D7F37}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="650" yWindow="1560" windowWidth="22500" windowHeight="14300" tabRatio="406" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="892" uniqueCount="577">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="900" uniqueCount="582">
   <si>
     <t>City</t>
   </si>
@@ -1761,6 +1761,21 @@
   </si>
   <si>
     <t>SumOfCVHits</t>
+  </si>
+  <si>
+    <t>YearsOld</t>
+  </si>
+  <si>
+    <t>years old</t>
+  </si>
+  <si>
+    <t>Jahre alt</t>
+  </si>
+  <si>
+    <t>From</t>
+  </si>
+  <si>
+    <t>Aus</t>
   </si>
 </sst>
 </file>
@@ -2149,10 +2164,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B223"/>
+  <dimension ref="A1:B225"/>
   <sheetViews>
     <sheetView topLeftCell="A201" workbookViewId="0">
-      <selection activeCell="A223" sqref="A223:B223"/>
+      <selection activeCell="B225" sqref="B225"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3943,6 +3958,22 @@
       </c>
       <c r="B223" s="1" t="s">
         <v>574</v>
+      </c>
+    </row>
+    <row r="224" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A224" s="1" t="s">
+        <v>577</v>
+      </c>
+      <c r="B224" s="5" t="s">
+        <v>578</v>
+      </c>
+    </row>
+    <row r="225" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A225" s="1" t="s">
+        <v>580</v>
+      </c>
+      <c r="B225" s="5" t="s">
+        <v>580</v>
       </c>
     </row>
   </sheetData>
@@ -3958,10 +3989,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:B223"/>
+  <dimension ref="A1:B225"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A213" workbookViewId="0">
-      <selection activeCell="A223" sqref="A223"/>
+      <selection activeCell="B225" sqref="B225"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -5754,6 +5785,22 @@
         <v>575</v>
       </c>
     </row>
+    <row r="224" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A224" s="1" t="s">
+        <v>577</v>
+      </c>
+      <c r="B224" s="1" t="s">
+        <v>579</v>
+      </c>
+    </row>
+    <row r="225" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A225" s="1" t="s">
+        <v>580</v>
+      </c>
+      <c r="B225" s="1" t="s">
+        <v>581</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:B23" xr:uid="{00000000-0009-0000-0000-000001000000}">
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B222">

</xml_diff>

<commit_message>
Restructuring Manage view: 50% done
</commit_message>
<xml_diff>
--- a/Vitae/Library/Resources/SharedResource.xlsx
+++ b/Vitae/Library/Resources/SharedResource.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\Vitae\Library\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE754FB5-EF1D-4991-9BC3-791CD67D7F37}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E642C5E-399D-4E96-A4A6-15A45F98B932}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="650" yWindow="1560" windowWidth="22500" windowHeight="14300" tabRatio="406" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="900" uniqueCount="582">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="912" uniqueCount="589">
   <si>
     <t>City</t>
   </si>
@@ -1776,6 +1776,27 @@
   </si>
   <si>
     <t>Aus</t>
+  </si>
+  <si>
+    <t>Day</t>
+  </si>
+  <si>
+    <t>Tag</t>
+  </si>
+  <si>
+    <t>Days</t>
+  </si>
+  <si>
+    <t>Tage</t>
+  </si>
+  <si>
+    <t>AddToTop</t>
+  </si>
+  <si>
+    <t>Add to top</t>
+  </si>
+  <si>
+    <t>Nach oben erweitern</t>
   </si>
 </sst>
 </file>
@@ -2164,10 +2185,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B225"/>
+  <dimension ref="A1:B228"/>
   <sheetViews>
     <sheetView topLeftCell="A201" workbookViewId="0">
-      <selection activeCell="B225" sqref="B225"/>
+      <selection activeCell="A228" sqref="A228"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3974,6 +3995,30 @@
       </c>
       <c r="B225" s="5" t="s">
         <v>580</v>
+      </c>
+    </row>
+    <row r="226" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A226" s="1" t="s">
+        <v>582</v>
+      </c>
+      <c r="B226" s="5" t="s">
+        <v>582</v>
+      </c>
+    </row>
+    <row r="227" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A227" s="1" t="s">
+        <v>584</v>
+      </c>
+      <c r="B227" s="5" t="s">
+        <v>584</v>
+      </c>
+    </row>
+    <row r="228" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A228" s="1" t="s">
+        <v>586</v>
+      </c>
+      <c r="B228" s="5" t="s">
+        <v>587</v>
       </c>
     </row>
   </sheetData>
@@ -3989,10 +4034,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:B225"/>
+  <dimension ref="A1:B228"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A213" workbookViewId="0">
-      <selection activeCell="B225" sqref="B225"/>
+      <selection activeCell="B229" sqref="B229"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -5801,6 +5846,30 @@
         <v>581</v>
       </c>
     </row>
+    <row r="226" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A226" s="1" t="s">
+        <v>582</v>
+      </c>
+      <c r="B226" s="1" t="s">
+        <v>583</v>
+      </c>
+    </row>
+    <row r="227" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A227" s="1" t="s">
+        <v>584</v>
+      </c>
+      <c r="B227" s="1" t="s">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="228" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A228" s="1" t="s">
+        <v>586</v>
+      </c>
+      <c r="B228" s="1" t="s">
+        <v>588</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:B23" xr:uid="{00000000-0009-0000-0000-000001000000}">
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B222">

</xml_diff>

<commit_message>
Refactoring of Manage page
</commit_message>
<xml_diff>
--- a/Vitae/Library/Resources/SharedResource.xlsx
+++ b/Vitae/Library/Resources/SharedResource.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\Vitae\Library\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E642C5E-399D-4E96-A4A6-15A45F98B932}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3BC2359-5717-4AAA-983C-89ED745A5B90}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="650" yWindow="1560" windowWidth="22500" windowHeight="14300" tabRatio="406" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="912" uniqueCount="589">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="924" uniqueCount="597">
   <si>
     <t>City</t>
   </si>
@@ -1607,9 +1607,6 @@
     <t>EnterSkill</t>
   </si>
   <si>
-    <t>Bitte drücken Sie die Enter-Taste um einen neuen Skill einzufügen</t>
-  </si>
-  <si>
     <t>Please press Enter to insert a new Skill</t>
   </si>
   <si>
@@ -1796,7 +1793,34 @@
     <t>Add to top</t>
   </si>
   <si>
-    <t>Nach oben erweitern</t>
+    <t>Award</t>
+  </si>
+  <si>
+    <t>Errungenschaft</t>
+  </si>
+  <si>
+    <t>Skill</t>
+  </si>
+  <si>
+    <t>Kompetenzen</t>
+  </si>
+  <si>
+    <t>Kompetenz</t>
+  </si>
+  <si>
+    <t>SocialLink</t>
+  </si>
+  <si>
+    <t>Social link</t>
+  </si>
+  <si>
+    <t>Soziale Verbindung</t>
+  </si>
+  <si>
+    <t>Bitte drücken Sie die Enter-Taste um eine neue Kompetenz einzufügen</t>
+  </si>
+  <si>
+    <t>Oben erweitern</t>
   </si>
 </sst>
 </file>
@@ -2185,10 +2209,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B228"/>
+  <dimension ref="A1:B231"/>
   <sheetViews>
-    <sheetView topLeftCell="A201" workbookViewId="0">
-      <selection activeCell="A228" sqref="A228"/>
+    <sheetView topLeftCell="A220" workbookViewId="0">
+      <selection activeCell="B232" sqref="B232"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2215,26 +2239,26 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
+        <v>526</v>
+      </c>
+      <c r="B3" s="5" t="s">
         <v>527</v>
-      </c>
-      <c r="B3" s="5" t="s">
-        <v>528</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
+        <v>559</v>
+      </c>
+      <c r="B4" s="5" t="s">
         <v>560</v>
-      </c>
-      <c r="B4" s="5" t="s">
-        <v>561</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
+        <v>556</v>
+      </c>
+      <c r="B5" s="5" t="s">
         <v>557</v>
-      </c>
-      <c r="B5" s="5" t="s">
-        <v>558</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.35">
@@ -2375,18 +2399,18 @@
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.35">
@@ -2583,18 +2607,18 @@
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="B49" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="B50" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.35">
@@ -2754,7 +2778,7 @@
         <v>524</v>
       </c>
       <c r="B70" s="5" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.35">
@@ -2783,10 +2807,10 @@
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A74" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="B74" s="5" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.35">
@@ -2863,10 +2887,10 @@
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A84" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="B84" s="5" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.35">
@@ -2927,10 +2951,10 @@
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A92" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
       <c r="B92" s="5" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.35">
@@ -3007,10 +3031,10 @@
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A102" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="B102" s="5" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.35">
@@ -3191,10 +3215,10 @@
     </row>
     <row r="125" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A125" s="1" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="B125" s="5" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
     </row>
     <row r="126" spans="1:2" x14ac:dyDescent="0.35">
@@ -3263,18 +3287,18 @@
     </row>
     <row r="134" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A134" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="B134" s="5" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
     </row>
     <row r="135" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A135" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="B135" s="5" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
     </row>
     <row r="136" spans="1:2" x14ac:dyDescent="0.35">
@@ -3463,10 +3487,10 @@
     </row>
     <row r="159" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A159" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="B159" s="5" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
     </row>
     <row r="160" spans="1:2" x14ac:dyDescent="0.35">
@@ -3487,18 +3511,18 @@
     </row>
     <row r="162" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A162" s="1" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="B162" s="5" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
     </row>
     <row r="163" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A163" s="1" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="B163" s="1" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
     </row>
     <row r="164" spans="1:2" x14ac:dyDescent="0.35">
@@ -3695,10 +3719,10 @@
     </row>
     <row r="188" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A188" t="s">
+        <v>553</v>
+      </c>
+      <c r="B188" s="5" t="s">
         <v>554</v>
-      </c>
-      <c r="B188" s="5" t="s">
-        <v>555</v>
       </c>
     </row>
     <row r="189" spans="1:2" x14ac:dyDescent="0.35">
@@ -3919,10 +3943,10 @@
     </row>
     <row r="216" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A216" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="B216" s="5" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
     </row>
     <row r="217" spans="1:2" x14ac:dyDescent="0.35">
@@ -3975,50 +3999,74 @@
     </row>
     <row r="223" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A223" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
       <c r="B223" s="1" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
     </row>
     <row r="224" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A224" s="1" t="s">
+        <v>576</v>
+      </c>
+      <c r="B224" s="5" t="s">
         <v>577</v>
-      </c>
-      <c r="B224" s="5" t="s">
-        <v>578</v>
       </c>
     </row>
     <row r="225" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A225" s="1" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="B225" s="5" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
     </row>
     <row r="226" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A226" s="1" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="B226" s="5" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
     </row>
     <row r="227" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A227" s="1" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="B227" s="5" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
     </row>
     <row r="228" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A228" s="1" t="s">
+        <v>585</v>
+      </c>
+      <c r="B228" s="5" t="s">
         <v>586</v>
       </c>
-      <c r="B228" s="5" t="s">
+    </row>
+    <row r="229" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A229" s="1" t="s">
         <v>587</v>
+      </c>
+      <c r="B229" s="5" t="s">
+        <v>587</v>
+      </c>
+    </row>
+    <row r="230" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A230" s="1" t="s">
+        <v>589</v>
+      </c>
+      <c r="B230" s="5" t="s">
+        <v>589</v>
+      </c>
+    </row>
+    <row r="231" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A231" s="1" t="s">
+        <v>592</v>
+      </c>
+      <c r="B231" s="5" t="s">
+        <v>593</v>
       </c>
     </row>
   </sheetData>
@@ -4034,9 +4082,9 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:B228"/>
+  <dimension ref="A1:B231"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A213" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A211" workbookViewId="0">
       <selection activeCell="B229" sqref="B229"/>
     </sheetView>
   </sheetViews>
@@ -4064,26 +4112,26 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.35">
@@ -4224,18 +4272,18 @@
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
+        <v>538</v>
+      </c>
+      <c r="B23" s="5" t="s">
         <v>539</v>
-      </c>
-      <c r="B23" s="5" t="s">
-        <v>540</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
+        <v>540</v>
+      </c>
+      <c r="B24" s="5" t="s">
         <v>541</v>
-      </c>
-      <c r="B24" s="5" t="s">
-        <v>542</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.35">
@@ -4432,18 +4480,18 @@
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
+        <v>549</v>
+      </c>
+      <c r="B49" s="5" t="s">
         <v>550</v>
-      </c>
-      <c r="B49" s="5" t="s">
-        <v>551</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
+        <v>547</v>
+      </c>
+      <c r="B50" s="5" t="s">
         <v>548</v>
-      </c>
-      <c r="B50" s="5" t="s">
-        <v>549</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.35">
@@ -4603,7 +4651,7 @@
         <v>524</v>
       </c>
       <c r="B70" t="s">
-        <v>525</v>
+        <v>595</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.35">
@@ -4632,10 +4680,10 @@
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A74" t="s">
+        <v>551</v>
+      </c>
+      <c r="B74" s="5" t="s">
         <v>552</v>
-      </c>
-      <c r="B74" s="5" t="s">
-        <v>553</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.35">
@@ -4712,10 +4760,10 @@
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A84" t="s">
+        <v>562</v>
+      </c>
+      <c r="B84" s="5" t="s">
         <v>563</v>
-      </c>
-      <c r="B84" s="5" t="s">
-        <v>564</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.35">
@@ -4776,10 +4824,10 @@
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A92" t="s">
+        <v>542</v>
+      </c>
+      <c r="B92" s="5" t="s">
         <v>543</v>
-      </c>
-      <c r="B92" s="5" t="s">
-        <v>544</v>
       </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.35">
@@ -4856,10 +4904,10 @@
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A102" t="s">
+        <v>544</v>
+      </c>
+      <c r="B102" s="5" t="s">
         <v>545</v>
-      </c>
-      <c r="B102" s="5" t="s">
-        <v>546</v>
       </c>
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.35">
@@ -5040,10 +5088,10 @@
     </row>
     <row r="125" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A125" s="1" t="s">
+        <v>535</v>
+      </c>
+      <c r="B125" s="5" t="s">
         <v>536</v>
-      </c>
-      <c r="B125" s="5" t="s">
-        <v>537</v>
       </c>
     </row>
     <row r="126" spans="1:2" x14ac:dyDescent="0.35">
@@ -5112,18 +5160,18 @@
     </row>
     <row r="134" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A134" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="B134" s="5" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
     </row>
     <row r="135" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A135" t="s">
+        <v>565</v>
+      </c>
+      <c r="B135" s="5" t="s">
         <v>566</v>
-      </c>
-      <c r="B135" s="5" t="s">
-        <v>567</v>
       </c>
     </row>
     <row r="136" spans="1:2" x14ac:dyDescent="0.35">
@@ -5312,10 +5360,10 @@
     </row>
     <row r="159" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A159" t="s">
+        <v>568</v>
+      </c>
+      <c r="B159" s="5" t="s">
         <v>569</v>
-      </c>
-      <c r="B159" s="5" t="s">
-        <v>570</v>
       </c>
     </row>
     <row r="160" spans="1:2" x14ac:dyDescent="0.35">
@@ -5336,18 +5384,18 @@
     </row>
     <row r="162" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A162" s="1" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="B162" s="5" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
     </row>
     <row r="163" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A163" s="1" t="s">
+        <v>530</v>
+      </c>
+      <c r="B163" s="5" t="s">
         <v>531</v>
-      </c>
-      <c r="B163" s="5" t="s">
-        <v>532</v>
       </c>
     </row>
     <row r="164" spans="1:2" x14ac:dyDescent="0.35">
@@ -5544,10 +5592,10 @@
     </row>
     <row r="188" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A188" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="B188" s="5" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
     </row>
     <row r="189" spans="1:2" x14ac:dyDescent="0.35">
@@ -5555,7 +5603,7 @@
         <v>227</v>
       </c>
       <c r="B189" t="s">
-        <v>227</v>
+        <v>590</v>
       </c>
     </row>
     <row r="190" spans="1:2" x14ac:dyDescent="0.35">
@@ -5768,10 +5816,10 @@
     </row>
     <row r="216" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A216" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="B216" s="5" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
     </row>
     <row r="217" spans="1:2" x14ac:dyDescent="0.35">
@@ -5824,50 +5872,74 @@
     </row>
     <row r="223" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A223" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
       <c r="B223" s="1" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
     </row>
     <row r="224" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A224" s="1" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="B224" s="1" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
     </row>
     <row r="225" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A225" s="1" t="s">
+        <v>579</v>
+      </c>
+      <c r="B225" s="1" t="s">
         <v>580</v>
-      </c>
-      <c r="B225" s="1" t="s">
-        <v>581</v>
       </c>
     </row>
     <row r="226" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A226" s="1" t="s">
+        <v>581</v>
+      </c>
+      <c r="B226" s="1" t="s">
         <v>582</v>
-      </c>
-      <c r="B226" s="1" t="s">
-        <v>583</v>
       </c>
     </row>
     <row r="227" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A227" s="1" t="s">
+        <v>583</v>
+      </c>
+      <c r="B227" s="1" t="s">
         <v>584</v>
-      </c>
-      <c r="B227" s="1" t="s">
-        <v>585</v>
       </c>
     </row>
     <row r="228" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A228" s="1" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="B228" s="1" t="s">
+        <v>596</v>
+      </c>
+    </row>
+    <row r="229" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A229" s="1" t="s">
+        <v>587</v>
+      </c>
+      <c r="B229" s="1" t="s">
         <v>588</v>
+      </c>
+    </row>
+    <row r="230" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A230" s="1" t="s">
+        <v>589</v>
+      </c>
+      <c r="B230" s="1" t="s">
+        <v>591</v>
+      </c>
+    </row>
+    <row r="231" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A231" s="1" t="s">
+        <v>592</v>
+      </c>
+      <c r="B231" s="1" t="s">
+        <v>594</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Read Advert text with reflexction
</commit_message>
<xml_diff>
--- a/Vitae/Library/Resources/SharedResource.xlsx
+++ b/Vitae/Library/Resources/SharedResource.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\Vitae\Library\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A624B46D-7405-420F-BB19-D45F96BD2238}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{727CB42F-13FB-47D2-8301-8A6EF8C2A723}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="650" yWindow="1560" windowWidth="22500" windowHeight="14300" tabRatio="406" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="924" uniqueCount="597">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="928" uniqueCount="601">
   <si>
     <t>City</t>
   </si>
@@ -767,9 +767,6 @@
     <t>Startseite</t>
   </si>
   <si>
-    <t>AdText2</t>
-  </si>
-  <si>
     <t>Want to improve your curriculum vitae? No problem - with VITAE you present yourself in the best possible light. Create a free account now!</t>
   </si>
   <si>
@@ -1502,18 +1499,12 @@
     <t>No results for {0}</t>
   </si>
   <si>
-    <t>AdText1b</t>
-  </si>
-  <si>
     <t>Präsentieren Sie sich im besten Licht</t>
   </si>
   <si>
     <t>Present yourself in the best light</t>
   </si>
   <si>
-    <t>AdText1a</t>
-  </si>
-  <si>
     <t>Child</t>
   </si>
   <si>
@@ -1821,6 +1812,27 @@
   </si>
   <si>
     <t>Nach oben erweitern</t>
+  </si>
+  <si>
+    <t>AdTextA1</t>
+  </si>
+  <si>
+    <t>AdTextA2</t>
+  </si>
+  <si>
+    <t>AdTextB1</t>
+  </si>
+  <si>
+    <t>AdTextA0</t>
+  </si>
+  <si>
+    <t>AdTextB0</t>
+  </si>
+  <si>
+    <t>Zeigen Sie Ihr Können</t>
+  </si>
+  <si>
+    <t>Show off your skills</t>
   </si>
 </sst>
 </file>
@@ -2209,10 +2221,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B231"/>
+  <dimension ref="A1:B232"/>
   <sheetViews>
-    <sheetView topLeftCell="A220" workbookViewId="0">
-      <selection activeCell="B232" sqref="B232"/>
+    <sheetView topLeftCell="A211" workbookViewId="0">
+      <selection activeCell="B232" sqref="A232:B232"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2239,50 +2251,50 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>526</v>
+        <v>523</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>527</v>
+        <v>524</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>559</v>
+        <v>556</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>560</v>
+        <v>557</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>556</v>
+        <v>553</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>557</v>
+        <v>554</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
+        <v>477</v>
+      </c>
+      <c r="B6" s="5" t="s">
         <v>478</v>
-      </c>
-      <c r="B6" s="5" t="s">
-        <v>479</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.35">
@@ -2295,26 +2307,26 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
-        <v>493</v>
+        <v>594</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
+        <v>595</v>
+      </c>
+      <c r="B11" s="5" t="s">
         <v>490</v>
-      </c>
-      <c r="B11" s="5" t="s">
-        <v>492</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="29" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
+        <v>596</v>
+      </c>
+      <c r="B12" s="5" t="s">
         <v>245</v>
-      </c>
-      <c r="B12" s="5" t="s">
-        <v>246</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.35">
@@ -2359,10 +2371,10 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A18" s="1" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.35">
@@ -2399,74 +2411,74 @@
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>538</v>
+        <v>535</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>538</v>
+        <v>535</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>540</v>
+        <v>537</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>540</v>
+        <v>537</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A25" s="1" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A27" s="1" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A28" s="1" t="s">
+        <v>280</v>
+      </c>
+      <c r="B28" s="5" t="s">
         <v>281</v>
-      </c>
-      <c r="B28" s="5" t="s">
-        <v>282</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A29" s="1" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A30" s="1" t="s">
-        <v>494</v>
+        <v>491</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>494</v>
+        <v>491</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A31" s="1" t="s">
-        <v>496</v>
+        <v>493</v>
       </c>
       <c r="B31" s="5" t="s">
-        <v>496</v>
+        <v>493</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.35">
@@ -2487,10 +2499,10 @@
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A34" s="1" t="s">
-        <v>519</v>
+        <v>516</v>
       </c>
       <c r="B34" s="5" t="s">
-        <v>520</v>
+        <v>517</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.35">
@@ -2503,10 +2515,10 @@
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A36" s="1" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="B36" s="4" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.35">
@@ -2519,26 +2531,26 @@
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A38" s="1" t="s">
+        <v>265</v>
+      </c>
+      <c r="B38" s="5" t="s">
         <v>266</v>
-      </c>
-      <c r="B38" s="5" t="s">
-        <v>267</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
-        <v>500</v>
+        <v>497</v>
       </c>
       <c r="B39" s="5" t="s">
-        <v>500</v>
+        <v>497</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="B40" s="5" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.35">
@@ -2551,42 +2563,42 @@
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A42" s="1" t="s">
+        <v>442</v>
+      </c>
+      <c r="B42" s="5" t="s">
         <v>443</v>
-      </c>
-      <c r="B42" s="5" t="s">
-        <v>444</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="B43" s="5" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A44" s="1" t="s">
+        <v>397</v>
+      </c>
+      <c r="B44" s="5" t="s">
         <v>398</v>
-      </c>
-      <c r="B44" s="5" t="s">
-        <v>399</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="B45" s="5" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="B46" s="4" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.35">
@@ -2607,34 +2619,34 @@
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
-        <v>549</v>
+        <v>546</v>
       </c>
       <c r="B49" t="s">
-        <v>549</v>
+        <v>546</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
-        <v>547</v>
+        <v>544</v>
       </c>
       <c r="B50" t="s">
-        <v>547</v>
+        <v>544</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A51" s="1" t="s">
+        <v>254</v>
+      </c>
+      <c r="B51" s="5" t="s">
         <v>255</v>
-      </c>
-      <c r="B51" s="5" t="s">
-        <v>256</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A52" s="1" t="s">
+        <v>420</v>
+      </c>
+      <c r="B52" s="5" t="s">
         <v>421</v>
-      </c>
-      <c r="B52" s="5" t="s">
-        <v>422</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.35">
@@ -2663,10 +2675,10 @@
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="B56" s="5" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.35">
@@ -2679,10 +2691,10 @@
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
-        <v>501</v>
+        <v>498</v>
       </c>
       <c r="B58" s="5" t="s">
-        <v>501</v>
+        <v>498</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.35">
@@ -2695,26 +2707,26 @@
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B60" s="5" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="B61" s="5" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="B62" s="5" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.35">
@@ -2743,26 +2755,26 @@
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A66" s="1" t="s">
+        <v>458</v>
+      </c>
+      <c r="B66" s="4" t="s">
         <v>459</v>
-      </c>
-      <c r="B66" s="4" t="s">
-        <v>460</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A67" s="1" t="s">
+        <v>283</v>
+      </c>
+      <c r="B67" s="5" t="s">
         <v>284</v>
-      </c>
-      <c r="B67" s="5" t="s">
-        <v>285</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A68" s="1" t="s">
+        <v>454</v>
+      </c>
+      <c r="B68" s="5" t="s">
         <v>455</v>
-      </c>
-      <c r="B68" s="5" t="s">
-        <v>456</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.35">
@@ -2775,18 +2787,18 @@
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A70" s="1" t="s">
-        <v>524</v>
+        <v>521</v>
       </c>
       <c r="B70" s="5" t="s">
-        <v>525</v>
+        <v>522</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="B71" s="5" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.35">
@@ -2807,18 +2819,18 @@
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A74" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="B74" s="5" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A75" s="1" t="s">
-        <v>511</v>
+        <v>508</v>
       </c>
       <c r="B75" s="5" t="s">
-        <v>513</v>
+        <v>510</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.35">
@@ -2887,10 +2899,10 @@
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A84" t="s">
-        <v>562</v>
+        <v>559</v>
       </c>
       <c r="B84" s="5" t="s">
-        <v>562</v>
+        <v>559</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.35">
@@ -2903,58 +2915,58 @@
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A86" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="B86" s="5" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A87" t="s">
+        <v>351</v>
+      </c>
+      <c r="B87" s="5" t="s">
         <v>352</v>
-      </c>
-      <c r="B87" s="5" t="s">
-        <v>353</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A88" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="B88" s="5" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A89" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="B89" s="5" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A90" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="B90" s="5" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A91" s="1" t="s">
-        <v>510</v>
+        <v>507</v>
       </c>
       <c r="B91" s="5" t="s">
-        <v>512</v>
+        <v>509</v>
       </c>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A92" t="s">
-        <v>542</v>
+        <v>539</v>
       </c>
       <c r="B92" s="5" t="s">
-        <v>542</v>
+        <v>539</v>
       </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.35">
@@ -3031,34 +3043,34 @@
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A102" t="s">
-        <v>544</v>
+        <v>541</v>
       </c>
       <c r="B102" s="5" t="s">
-        <v>544</v>
+        <v>541</v>
       </c>
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A103" s="1" t="s">
+        <v>466</v>
+      </c>
+      <c r="B103" s="5" t="s">
         <v>467</v>
-      </c>
-      <c r="B103" s="5" t="s">
-        <v>468</v>
       </c>
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A104" s="1" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="B104" s="5" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A105" s="1" t="s">
+        <v>469</v>
+      </c>
+      <c r="B105" s="5" t="s">
         <v>470</v>
-      </c>
-      <c r="B105" s="5" t="s">
-        <v>471</v>
       </c>
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.35">
@@ -3071,42 +3083,42 @@
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A107" s="1" t="s">
+        <v>408</v>
+      </c>
+      <c r="B107" s="5" t="s">
         <v>409</v>
-      </c>
-      <c r="B107" s="5" t="s">
-        <v>410</v>
       </c>
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A108" s="1" t="s">
+        <v>410</v>
+      </c>
+      <c r="B108" s="5" t="s">
         <v>411</v>
-      </c>
-      <c r="B108" s="5" t="s">
-        <v>412</v>
       </c>
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A109" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="B109" s="5" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A110" s="1" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="B110" s="5" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A111" s="1" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="B111" s="5" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.35">
@@ -3119,18 +3131,18 @@
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A113" t="s">
-        <v>516</v>
+        <v>513</v>
       </c>
       <c r="B113" s="5" t="s">
-        <v>517</v>
+        <v>514</v>
       </c>
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A114" t="s">
-        <v>499</v>
+        <v>496</v>
       </c>
       <c r="B114" s="5" t="s">
-        <v>499</v>
+        <v>496</v>
       </c>
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.35">
@@ -3215,26 +3227,26 @@
     </row>
     <row r="125" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A125" s="1" t="s">
-        <v>535</v>
+        <v>532</v>
       </c>
       <c r="B125" s="5" t="s">
-        <v>537</v>
+        <v>534</v>
       </c>
     </row>
     <row r="126" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A126" s="1" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="B126" s="5" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
     </row>
     <row r="127" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A127" s="1" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="B127" s="5" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
     </row>
     <row r="128" spans="1:2" x14ac:dyDescent="0.35">
@@ -3247,10 +3259,10 @@
     </row>
     <row r="129" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A129" t="s">
-        <v>509</v>
+        <v>506</v>
       </c>
       <c r="B129" s="5" t="s">
-        <v>503</v>
+        <v>500</v>
       </c>
     </row>
     <row r="130" spans="1:2" x14ac:dyDescent="0.35">
@@ -3279,26 +3291,26 @@
     </row>
     <row r="133" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A133" s="1" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="B133" s="5" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
     </row>
     <row r="134" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A134" t="s">
-        <v>564</v>
+        <v>561</v>
       </c>
       <c r="B134" s="5" t="s">
-        <v>572</v>
+        <v>569</v>
       </c>
     </row>
     <row r="135" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A135" t="s">
-        <v>565</v>
+        <v>562</v>
       </c>
       <c r="B135" s="5" t="s">
-        <v>567</v>
+        <v>564</v>
       </c>
     </row>
     <row r="136" spans="1:2" x14ac:dyDescent="0.35">
@@ -3327,98 +3339,98 @@
     </row>
     <row r="139" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A139" s="1" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="B139" s="4" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
     </row>
     <row r="140" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A140" s="1" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="B140" s="4" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="141" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A141" s="1" t="s">
+        <v>423</v>
+      </c>
+      <c r="B141" s="5" t="s">
         <v>424</v>
-      </c>
-      <c r="B141" s="5" t="s">
-        <v>425</v>
       </c>
     </row>
     <row r="142" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A142" s="1" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="B142" s="5" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="143" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A143" s="1" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="B143" s="5" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="144" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A144" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="B144" s="5" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
     </row>
     <row r="145" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A145" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="B145" s="5" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
     </row>
     <row r="146" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A146" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="B146" s="5" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
     </row>
     <row r="147" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A147" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="B147" s="5" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
     </row>
     <row r="148" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A148" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="B148" s="5" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
     </row>
     <row r="149" spans="1:2" ht="29" x14ac:dyDescent="0.35">
       <c r="A149" s="1" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="B149" s="4" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
     </row>
     <row r="150" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A150" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="B150" s="5" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="151" spans="1:2" x14ac:dyDescent="0.35">
@@ -3439,10 +3451,10 @@
     </row>
     <row r="153" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A153" s="1" t="s">
-        <v>521</v>
+        <v>518</v>
       </c>
       <c r="B153" s="5" t="s">
-        <v>522</v>
+        <v>519</v>
       </c>
     </row>
     <row r="154" spans="1:2" x14ac:dyDescent="0.35">
@@ -3455,18 +3467,18 @@
     </row>
     <row r="155" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A155" s="1" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="B155" s="5" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
     </row>
     <row r="156" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A156" s="1" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="B156" s="4" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
     </row>
     <row r="157" spans="1:2" x14ac:dyDescent="0.35">
@@ -3487,10 +3499,10 @@
     </row>
     <row r="159" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A159" t="s">
-        <v>568</v>
+        <v>565</v>
       </c>
       <c r="B159" s="5" t="s">
-        <v>570</v>
+        <v>567</v>
       </c>
     </row>
     <row r="160" spans="1:2" x14ac:dyDescent="0.35">
@@ -3511,50 +3523,50 @@
     </row>
     <row r="162" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A162" s="1" t="s">
-        <v>529</v>
+        <v>526</v>
       </c>
       <c r="B162" s="5" t="s">
-        <v>529</v>
+        <v>526</v>
       </c>
     </row>
     <row r="163" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A163" s="1" t="s">
-        <v>530</v>
+        <v>527</v>
       </c>
       <c r="B163" s="1" t="s">
-        <v>530</v>
+        <v>527</v>
       </c>
     </row>
     <row r="164" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A164" s="1" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B164" s="4" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="165" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A165" s="1" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="B165" s="5" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="166" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A166" s="1" t="s">
+        <v>286</v>
+      </c>
+      <c r="B166" s="5" t="s">
         <v>287</v>
-      </c>
-      <c r="B166" s="5" t="s">
-        <v>288</v>
       </c>
     </row>
     <row r="167" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A167" s="1" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="B167" s="4" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="168" spans="1:2" x14ac:dyDescent="0.35">
@@ -3583,10 +3595,10 @@
     </row>
     <row r="171" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A171" s="1" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="B171" s="4" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="172" spans="1:2" x14ac:dyDescent="0.35">
@@ -3607,58 +3619,58 @@
     </row>
     <row r="174" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A174" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="B174" s="5" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
     </row>
     <row r="175" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A175" t="s">
+        <v>366</v>
+      </c>
+      <c r="B175" s="5" t="s">
         <v>367</v>
-      </c>
-      <c r="B175" s="5" t="s">
-        <v>368</v>
       </c>
     </row>
     <row r="176" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A176" s="1" t="s">
+        <v>430</v>
+      </c>
+      <c r="B176" s="5" t="s">
         <v>431</v>
-      </c>
-      <c r="B176" s="5" t="s">
-        <v>432</v>
       </c>
     </row>
     <row r="177" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A177" t="s">
+        <v>374</v>
+      </c>
+      <c r="B177" s="5" t="s">
         <v>375</v>
-      </c>
-      <c r="B177" s="5" t="s">
-        <v>376</v>
       </c>
     </row>
     <row r="178" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A178" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="B178" s="5" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
     </row>
     <row r="179" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A179" t="s">
+        <v>377</v>
+      </c>
+      <c r="B179" s="5" t="s">
         <v>378</v>
-      </c>
-      <c r="B179" s="5" t="s">
-        <v>379</v>
       </c>
     </row>
     <row r="180" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A180" t="s">
+        <v>368</v>
+      </c>
+      <c r="B180" s="5" t="s">
         <v>369</v>
-      </c>
-      <c r="B180" s="5" t="s">
-        <v>370</v>
       </c>
     </row>
     <row r="181" spans="1:2" x14ac:dyDescent="0.35">
@@ -3695,34 +3707,34 @@
     </row>
     <row r="185" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A185" s="1" t="s">
+        <v>436</v>
+      </c>
+      <c r="B185" s="5" t="s">
         <v>437</v>
-      </c>
-      <c r="B185" s="5" t="s">
-        <v>438</v>
       </c>
     </row>
     <row r="186" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A186" s="1" t="s">
+        <v>248</v>
+      </c>
+      <c r="B186" s="4" t="s">
         <v>249</v>
-      </c>
-      <c r="B186" s="4" t="s">
-        <v>250</v>
       </c>
     </row>
     <row r="187" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A187" t="s">
-        <v>498</v>
+        <v>495</v>
       </c>
       <c r="B187" s="5" t="s">
-        <v>498</v>
+        <v>495</v>
       </c>
     </row>
     <row r="188" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A188" t="s">
-        <v>553</v>
+        <v>550</v>
       </c>
       <c r="B188" s="5" t="s">
-        <v>554</v>
+        <v>551</v>
       </c>
     </row>
     <row r="189" spans="1:2" x14ac:dyDescent="0.35">
@@ -3807,18 +3819,18 @@
     </row>
     <row r="199" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A199" t="s">
+        <v>383</v>
+      </c>
+      <c r="B199" s="5" t="s">
         <v>384</v>
-      </c>
-      <c r="B199" s="5" t="s">
-        <v>385</v>
       </c>
     </row>
     <row r="200" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A200" s="1" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="B200" s="5" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
     </row>
     <row r="201" spans="1:2" x14ac:dyDescent="0.35">
@@ -3831,18 +3843,18 @@
     </row>
     <row r="202" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A202" s="1" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="B202" s="5" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
     </row>
     <row r="203" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A203" s="1" t="s">
+        <v>403</v>
+      </c>
+      <c r="B203" s="5" t="s">
         <v>404</v>
-      </c>
-      <c r="B203" s="5" t="s">
-        <v>405</v>
       </c>
     </row>
     <row r="204" spans="1:2" x14ac:dyDescent="0.35">
@@ -3871,50 +3883,50 @@
     </row>
     <row r="207" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A207" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B207" s="5" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
     <row r="208" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A208" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="B208" s="5" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
     </row>
     <row r="209" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A209" s="1" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="B209" s="5" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
     </row>
     <row r="210" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A210" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="B210" s="5" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="211" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A211" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="B211" s="5" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
     </row>
     <row r="212" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A212" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="B212" s="5" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
     </row>
     <row r="213" spans="1:2" x14ac:dyDescent="0.35">
@@ -3943,18 +3955,18 @@
     </row>
     <row r="216" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A216" t="s">
-        <v>534</v>
+        <v>531</v>
       </c>
       <c r="B216" s="5" t="s">
-        <v>533</v>
+        <v>530</v>
       </c>
     </row>
     <row r="217" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A217" s="1" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="B217" s="5" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
     </row>
     <row r="218" spans="1:2" x14ac:dyDescent="0.35">
@@ -3967,18 +3979,18 @@
     </row>
     <row r="219" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A219" s="1" t="s">
+        <v>389</v>
+      </c>
+      <c r="B219" s="4" t="s">
         <v>390</v>
-      </c>
-      <c r="B219" s="4" t="s">
-        <v>391</v>
       </c>
     </row>
     <row r="220" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A220" t="s">
-        <v>502</v>
+        <v>499</v>
       </c>
       <c r="B220" s="5" t="s">
-        <v>502</v>
+        <v>499</v>
       </c>
     </row>
     <row r="221" spans="1:2" x14ac:dyDescent="0.35">
@@ -3999,74 +4011,82 @@
     </row>
     <row r="223" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A223" t="s">
-        <v>575</v>
+        <v>572</v>
       </c>
       <c r="B223" s="1" t="s">
-        <v>573</v>
+        <v>570</v>
       </c>
     </row>
     <row r="224" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A224" s="1" t="s">
-        <v>576</v>
+        <v>573</v>
       </c>
       <c r="B224" s="5" t="s">
-        <v>577</v>
+        <v>574</v>
       </c>
     </row>
     <row r="225" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A225" s="1" t="s">
-        <v>579</v>
+        <v>576</v>
       </c>
       <c r="B225" s="5" t="s">
-        <v>579</v>
+        <v>576</v>
       </c>
     </row>
     <row r="226" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A226" s="1" t="s">
-        <v>581</v>
+        <v>578</v>
       </c>
       <c r="B226" s="5" t="s">
-        <v>581</v>
+        <v>578</v>
       </c>
     </row>
     <row r="227" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A227" s="1" t="s">
-        <v>583</v>
+        <v>580</v>
       </c>
       <c r="B227" s="5" t="s">
-        <v>583</v>
+        <v>580</v>
       </c>
     </row>
     <row r="228" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A228" s="1" t="s">
-        <v>585</v>
+        <v>582</v>
       </c>
       <c r="B228" s="5" t="s">
-        <v>586</v>
+        <v>583</v>
       </c>
     </row>
     <row r="229" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A229" s="1" t="s">
-        <v>587</v>
+        <v>584</v>
       </c>
       <c r="B229" s="5" t="s">
-        <v>587</v>
+        <v>584</v>
       </c>
     </row>
     <row r="230" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A230" s="1" t="s">
-        <v>589</v>
+        <v>586</v>
       </c>
       <c r="B230" s="5" t="s">
-        <v>589</v>
+        <v>586</v>
       </c>
     </row>
     <row r="231" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A231" s="1" t="s">
-        <v>592</v>
+        <v>589</v>
       </c>
       <c r="B231" s="5" t="s">
-        <v>593</v>
+        <v>590</v>
+      </c>
+    </row>
+    <row r="232" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A232" s="1" t="s">
+        <v>595</v>
+      </c>
+      <c r="B232" t="s">
+        <v>600</v>
       </c>
     </row>
   </sheetData>
@@ -4082,10 +4102,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:B231"/>
+  <dimension ref="A1:B232"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A211" workbookViewId="0">
-      <selection activeCell="B229" sqref="B229"/>
+    <sheetView tabSelected="1" topLeftCell="A205" workbookViewId="0">
+      <selection activeCell="B223" sqref="B223"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4107,55 +4127,55 @@
         <v>49</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>526</v>
+        <v>523</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>528</v>
+        <v>525</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>559</v>
+        <v>556</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>561</v>
+        <v>558</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>556</v>
+        <v>553</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>558</v>
+        <v>555</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="B8" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.35">
@@ -4168,26 +4188,26 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
-        <v>493</v>
+        <v>597</v>
       </c>
       <c r="B10" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>490</v>
+        <v>594</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>491</v>
+        <v>489</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
-        <v>245</v>
+        <v>598</v>
       </c>
       <c r="B12" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.35">
@@ -4232,10 +4252,10 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A18" s="1" t="s">
+        <v>474</v>
+      </c>
+      <c r="B18" s="5" t="s">
         <v>475</v>
-      </c>
-      <c r="B18" s="5" t="s">
-        <v>476</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.35">
@@ -4272,23 +4292,23 @@
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>538</v>
+        <v>535</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>539</v>
+        <v>536</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>540</v>
+        <v>537</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>541</v>
+        <v>538</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A25" s="1" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="B25" t="s">
         <v>12</v>
@@ -4296,50 +4316,50 @@
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
+        <v>433</v>
+      </c>
+      <c r="B26" t="s">
         <v>434</v>
-      </c>
-      <c r="B26" t="s">
-        <v>435</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A27" s="1" t="s">
+        <v>414</v>
+      </c>
+      <c r="B27" t="s">
         <v>415</v>
-      </c>
-      <c r="B27" t="s">
-        <v>416</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A28" s="1" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="B28" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A29" s="1" t="s">
+        <v>289</v>
+      </c>
+      <c r="B29" t="s">
         <v>290</v>
-      </c>
-      <c r="B29" t="s">
-        <v>291</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A30" s="1" t="s">
-        <v>494</v>
+        <v>491</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>495</v>
+        <v>492</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A31" s="1" t="s">
-        <v>496</v>
+        <v>493</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>497</v>
+        <v>494</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.35">
@@ -4360,10 +4380,10 @@
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A34" s="1" t="s">
-        <v>519</v>
+        <v>516</v>
       </c>
       <c r="B34" s="5" t="s">
-        <v>520</v>
+        <v>517</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.35">
@@ -4376,10 +4396,10 @@
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A36" s="1" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.35">
@@ -4392,26 +4412,26 @@
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A38" s="1" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="B38" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
-        <v>500</v>
+        <v>497</v>
       </c>
       <c r="B39" s="5" t="s">
-        <v>506</v>
+        <v>503</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="B40" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.35">
@@ -4424,42 +4444,42 @@
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A42" s="1" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="B42" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="B43" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A44" s="1" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="B44" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="B45" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
+        <v>262</v>
+      </c>
+      <c r="B46" s="1" t="s">
         <v>263</v>
-      </c>
-      <c r="B46" s="1" t="s">
-        <v>264</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.35">
@@ -4480,34 +4500,34 @@
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
-        <v>549</v>
+        <v>546</v>
       </c>
       <c r="B49" s="5" t="s">
-        <v>550</v>
+        <v>547</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
-        <v>547</v>
+        <v>544</v>
       </c>
       <c r="B50" s="5" t="s">
-        <v>548</v>
+        <v>545</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A51" s="1" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A52" s="1" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="B52" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.35">
@@ -4536,10 +4556,10 @@
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="B56" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.35">
@@ -4552,10 +4572,10 @@
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
-        <v>501</v>
+        <v>498</v>
       </c>
       <c r="B58" s="5" t="s">
-        <v>507</v>
+        <v>504</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.35">
@@ -4568,26 +4588,26 @@
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B60" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="B61" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="B62" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.35">
@@ -4616,26 +4636,26 @@
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A66" s="1" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A67" s="1" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="B67" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A68" s="1" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="B68" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.35">
@@ -4648,18 +4668,18 @@
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A70" s="1" t="s">
-        <v>524</v>
+        <v>521</v>
       </c>
       <c r="B70" t="s">
-        <v>595</v>
+        <v>592</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="B71" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.35">
@@ -4680,18 +4700,18 @@
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A74" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="B74" s="5" t="s">
-        <v>552</v>
+        <v>549</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A75" s="1" t="s">
-        <v>511</v>
+        <v>508</v>
       </c>
       <c r="B75" s="5" t="s">
-        <v>515</v>
+        <v>512</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.35">
@@ -4760,10 +4780,10 @@
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A84" t="s">
-        <v>562</v>
+        <v>559</v>
       </c>
       <c r="B84" s="5" t="s">
-        <v>563</v>
+        <v>560</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.35">
@@ -4776,58 +4796,58 @@
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A86" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="B86" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A87" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="B87" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A88" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="B88" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A89" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="B89" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A90" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="B90" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A91" s="1" t="s">
-        <v>510</v>
+        <v>507</v>
       </c>
       <c r="B91" s="5" t="s">
-        <v>514</v>
+        <v>511</v>
       </c>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A92" t="s">
-        <v>542</v>
+        <v>539</v>
       </c>
       <c r="B92" s="5" t="s">
-        <v>543</v>
+        <v>540</v>
       </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.35">
@@ -4904,34 +4924,34 @@
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A102" t="s">
-        <v>544</v>
+        <v>541</v>
       </c>
       <c r="B102" s="5" t="s">
-        <v>545</v>
+        <v>542</v>
       </c>
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A103" s="1" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="B103" s="5" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A104" s="1" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="B104" s="5" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A105" s="1" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="B105" s="5" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.35">
@@ -4944,42 +4964,42 @@
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A107" s="1" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="B107" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A108" s="1" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="B108" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A109" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="B109" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A110" s="1" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="B110" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A111" s="1" t="s">
+        <v>406</v>
+      </c>
+      <c r="B111" t="s">
         <v>407</v>
-      </c>
-      <c r="B111" t="s">
-        <v>408</v>
       </c>
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.35">
@@ -4992,18 +5012,18 @@
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A113" t="s">
-        <v>516</v>
+        <v>513</v>
       </c>
       <c r="B113" s="5" t="s">
-        <v>518</v>
+        <v>515</v>
       </c>
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A114" t="s">
-        <v>499</v>
+        <v>496</v>
       </c>
       <c r="B114" s="5" t="s">
-        <v>505</v>
+        <v>502</v>
       </c>
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.35">
@@ -5088,26 +5108,26 @@
     </row>
     <row r="125" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A125" s="1" t="s">
-        <v>535</v>
+        <v>532</v>
       </c>
       <c r="B125" s="5" t="s">
-        <v>536</v>
+        <v>533</v>
       </c>
     </row>
     <row r="126" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A126" s="1" t="s">
+        <v>439</v>
+      </c>
+      <c r="B126" t="s">
         <v>440</v>
-      </c>
-      <c r="B126" t="s">
-        <v>441</v>
       </c>
     </row>
     <row r="127" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A127" s="1" t="s">
+        <v>417</v>
+      </c>
+      <c r="B127" t="s">
         <v>418</v>
-      </c>
-      <c r="B127" t="s">
-        <v>419</v>
       </c>
     </row>
     <row r="128" spans="1:2" x14ac:dyDescent="0.35">
@@ -5120,10 +5140,10 @@
     </row>
     <row r="129" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A129" t="s">
-        <v>509</v>
+        <v>506</v>
       </c>
       <c r="B129" s="5" t="s">
-        <v>504</v>
+        <v>501</v>
       </c>
     </row>
     <row r="130" spans="1:2" x14ac:dyDescent="0.35">
@@ -5152,26 +5172,26 @@
     </row>
     <row r="133" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A133" s="1" t="s">
+        <v>486</v>
+      </c>
+      <c r="B133" s="5" t="s">
         <v>487</v>
-      </c>
-      <c r="B133" s="5" t="s">
-        <v>488</v>
       </c>
     </row>
     <row r="134" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A134" t="s">
-        <v>564</v>
+        <v>561</v>
       </c>
       <c r="B134" s="5" t="s">
-        <v>571</v>
+        <v>568</v>
       </c>
     </row>
     <row r="135" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A135" t="s">
-        <v>565</v>
+        <v>562</v>
       </c>
       <c r="B135" s="5" t="s">
-        <v>566</v>
+        <v>563</v>
       </c>
     </row>
     <row r="136" spans="1:2" x14ac:dyDescent="0.35">
@@ -5200,98 +5220,98 @@
     </row>
     <row r="139" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A139" s="1" t="s">
+        <v>461</v>
+      </c>
+      <c r="B139" s="1" t="s">
         <v>462</v>
-      </c>
-      <c r="B139" s="1" t="s">
-        <v>463</v>
       </c>
     </row>
     <row r="140" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A140" s="1" t="s">
+        <v>256</v>
+      </c>
+      <c r="B140" s="1" t="s">
         <v>257</v>
-      </c>
-      <c r="B140" s="1" t="s">
-        <v>258</v>
       </c>
     </row>
     <row r="141" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A141" s="1" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="B141" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
     </row>
     <row r="142" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A142" s="1" t="s">
+        <v>260</v>
+      </c>
+      <c r="B142" t="s">
         <v>261</v>
-      </c>
-      <c r="B142" t="s">
-        <v>262</v>
       </c>
     </row>
     <row r="143" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A143" s="1" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="B143" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="144" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A144" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="B144" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
     </row>
     <row r="145" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A145" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="B145" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
     </row>
     <row r="146" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A146" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="B146" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
     </row>
     <row r="147" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A147" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="B147" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="148" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A148" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="B148" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
     </row>
     <row r="149" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A149" s="1" t="s">
+        <v>463</v>
+      </c>
+      <c r="B149" s="1" t="s">
         <v>464</v>
-      </c>
-      <c r="B149" s="1" t="s">
-        <v>465</v>
       </c>
     </row>
     <row r="150" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A150" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="B150" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
     </row>
     <row r="151" spans="1:2" x14ac:dyDescent="0.35">
@@ -5312,10 +5332,10 @@
     </row>
     <row r="153" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A153" t="s">
-        <v>521</v>
+        <v>518</v>
       </c>
       <c r="B153" s="5" t="s">
-        <v>523</v>
+        <v>520</v>
       </c>
     </row>
     <row r="154" spans="1:2" x14ac:dyDescent="0.35">
@@ -5328,18 +5348,18 @@
     </row>
     <row r="155" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A155" s="1" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="B155" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
     </row>
     <row r="156" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A156" s="1" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="B156" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
     </row>
     <row r="157" spans="1:2" x14ac:dyDescent="0.35">
@@ -5360,10 +5380,10 @@
     </row>
     <row r="159" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A159" t="s">
-        <v>568</v>
+        <v>565</v>
       </c>
       <c r="B159" s="5" t="s">
-        <v>569</v>
+        <v>566</v>
       </c>
     </row>
     <row r="160" spans="1:2" x14ac:dyDescent="0.35">
@@ -5384,50 +5404,50 @@
     </row>
     <row r="162" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A162" s="1" t="s">
-        <v>529</v>
+        <v>526</v>
       </c>
       <c r="B162" s="5" t="s">
-        <v>546</v>
+        <v>543</v>
       </c>
     </row>
     <row r="163" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A163" s="1" t="s">
-        <v>530</v>
+        <v>527</v>
       </c>
       <c r="B163" s="5" t="s">
-        <v>531</v>
+        <v>528</v>
       </c>
     </row>
     <row r="164" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A164" s="1" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B164" s="1" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="165" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A165" s="1" t="s">
+        <v>273</v>
+      </c>
+      <c r="B165" t="s">
         <v>274</v>
-      </c>
-      <c r="B165" t="s">
-        <v>275</v>
       </c>
     </row>
     <row r="166" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A166" s="1" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="B166" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
     </row>
     <row r="167" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A167" s="1" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="B167" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="168" spans="1:2" x14ac:dyDescent="0.35">
@@ -5456,10 +5476,10 @@
     </row>
     <row r="171" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A171" s="1" t="s">
+        <v>278</v>
+      </c>
+      <c r="B171" s="1" t="s">
         <v>279</v>
-      </c>
-      <c r="B171" s="1" t="s">
-        <v>280</v>
       </c>
     </row>
     <row r="172" spans="1:2" x14ac:dyDescent="0.35">
@@ -5480,58 +5500,58 @@
     </row>
     <row r="174" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A174" t="s">
+        <v>372</v>
+      </c>
+      <c r="B174" t="s">
         <v>373</v>
-      </c>
-      <c r="B174" t="s">
-        <v>374</v>
       </c>
     </row>
     <row r="175" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A175" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="B175" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
     </row>
     <row r="176" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A176" s="1" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="B176" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
     </row>
     <row r="177" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A177" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="B177" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
     </row>
     <row r="178" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A178" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="B178" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
     </row>
     <row r="179" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A179" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="B179" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
     </row>
     <row r="180" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A180" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="B180" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
     </row>
     <row r="181" spans="1:2" x14ac:dyDescent="0.35">
@@ -5568,34 +5588,34 @@
     </row>
     <row r="185" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A185" s="1" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="B185" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
     </row>
     <row r="186" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A186" s="1" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="B186" s="1" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="187" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A187" t="s">
-        <v>498</v>
+        <v>495</v>
       </c>
       <c r="B187" s="5" t="s">
-        <v>498</v>
+        <v>495</v>
       </c>
     </row>
     <row r="188" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A188" t="s">
-        <v>553</v>
+        <v>550</v>
       </c>
       <c r="B188" s="5" t="s">
-        <v>555</v>
+        <v>552</v>
       </c>
     </row>
     <row r="189" spans="1:2" x14ac:dyDescent="0.35">
@@ -5603,7 +5623,7 @@
         <v>227</v>
       </c>
       <c r="B189" t="s">
-        <v>590</v>
+        <v>587</v>
       </c>
     </row>
     <row r="190" spans="1:2" x14ac:dyDescent="0.35">
@@ -5680,18 +5700,18 @@
     </row>
     <row r="199" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A199" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="B199" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
     </row>
     <row r="200" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A200" s="1" t="s">
+        <v>428</v>
+      </c>
+      <c r="B200" t="s">
         <v>429</v>
-      </c>
-      <c r="B200" t="s">
-        <v>430</v>
       </c>
     </row>
     <row r="201" spans="1:2" x14ac:dyDescent="0.35">
@@ -5704,18 +5724,18 @@
     </row>
     <row r="202" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A202" s="1" t="s">
+        <v>401</v>
+      </c>
+      <c r="B202" t="s">
         <v>402</v>
-      </c>
-      <c r="B202" t="s">
-        <v>403</v>
       </c>
     </row>
     <row r="203" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A203" s="1" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="B203" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
     </row>
     <row r="204" spans="1:2" x14ac:dyDescent="0.35">
@@ -5744,50 +5764,50 @@
     </row>
     <row r="207" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A207" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B207" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
     </row>
     <row r="208" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A208" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="B208" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
     </row>
     <row r="209" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A209" s="1" t="s">
+        <v>387</v>
+      </c>
+      <c r="B209" t="s">
         <v>388</v>
-      </c>
-      <c r="B209" t="s">
-        <v>389</v>
       </c>
     </row>
     <row r="210" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A210" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="B210" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
     </row>
     <row r="211" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A211" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="B211" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
     </row>
     <row r="212" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A212" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="B212" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
     </row>
     <row r="213" spans="1:2" x14ac:dyDescent="0.35">
@@ -5816,18 +5836,18 @@
     </row>
     <row r="216" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A216" t="s">
-        <v>534</v>
+        <v>531</v>
       </c>
       <c r="B216" s="5" t="s">
-        <v>532</v>
+        <v>529</v>
       </c>
     </row>
     <row r="217" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A217" s="1" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="B217" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
     </row>
     <row r="218" spans="1:2" x14ac:dyDescent="0.35">
@@ -5840,18 +5860,18 @@
     </row>
     <row r="219" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A219" s="1" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="B219" s="1" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
     </row>
     <row r="220" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A220" t="s">
-        <v>502</v>
+        <v>499</v>
       </c>
       <c r="B220" s="5" t="s">
-        <v>508</v>
+        <v>505</v>
       </c>
     </row>
     <row r="221" spans="1:2" x14ac:dyDescent="0.35">
@@ -5872,74 +5892,82 @@
     </row>
     <row r="223" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A223" t="s">
-        <v>575</v>
+        <v>572</v>
       </c>
       <c r="B223" s="1" t="s">
-        <v>574</v>
+        <v>571</v>
       </c>
     </row>
     <row r="224" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A224" s="1" t="s">
-        <v>576</v>
+        <v>573</v>
       </c>
       <c r="B224" s="1" t="s">
-        <v>578</v>
+        <v>575</v>
       </c>
     </row>
     <row r="225" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A225" s="1" t="s">
-        <v>579</v>
+        <v>576</v>
       </c>
       <c r="B225" s="1" t="s">
-        <v>580</v>
+        <v>577</v>
       </c>
     </row>
     <row r="226" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A226" s="1" t="s">
-        <v>581</v>
+        <v>578</v>
       </c>
       <c r="B226" s="1" t="s">
-        <v>582</v>
+        <v>579</v>
       </c>
     </row>
     <row r="227" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A227" s="1" t="s">
-        <v>583</v>
+        <v>580</v>
       </c>
       <c r="B227" s="1" t="s">
-        <v>584</v>
+        <v>581</v>
       </c>
     </row>
     <row r="228" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A228" s="1" t="s">
-        <v>585</v>
+        <v>582</v>
       </c>
       <c r="B228" s="1" t="s">
-        <v>596</v>
+        <v>593</v>
       </c>
     </row>
     <row r="229" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A229" s="1" t="s">
-        <v>587</v>
+        <v>584</v>
       </c>
       <c r="B229" s="1" t="s">
-        <v>588</v>
+        <v>585</v>
       </c>
     </row>
     <row r="230" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A230" s="1" t="s">
-        <v>589</v>
+        <v>586</v>
       </c>
       <c r="B230" s="1" t="s">
-        <v>591</v>
+        <v>588</v>
       </c>
     </row>
     <row r="231" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A231" s="1" t="s">
-        <v>592</v>
+        <v>589</v>
       </c>
       <c r="B231" s="1" t="s">
-        <v>594</v>
+        <v>591</v>
+      </c>
+    </row>
+    <row r="232" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A232" s="1" t="s">
+        <v>595</v>
+      </c>
+      <c r="B232" t="s">
+        <v>599</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
New UnitTest project Serializable added
</commit_message>
<xml_diff>
--- a/Vitae/Library/Resources/SharedResource.xlsx
+++ b/Vitae/Library/Resources/SharedResource.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\Vitae\Library\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{458FD32F-F034-4176-93A8-45231D4FC647}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC877BF0-EA8E-4C26-ABD0-9C2433740655}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="650" yWindow="1560" windowWidth="22500" windowHeight="14300" tabRatio="406" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="650" yWindow="1560" windowWidth="22500" windowHeight="14300" tabRatio="406" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="en" sheetId="3" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="936" uniqueCount="607">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="956" uniqueCount="618">
   <si>
     <t>City</t>
   </si>
@@ -1851,6 +1851,39 @@
   </si>
   <si>
     <t>Year old</t>
+  </si>
+  <si>
+    <t>Year</t>
+  </si>
+  <si>
+    <t>Years</t>
+  </si>
+  <si>
+    <t>Jahr</t>
+  </si>
+  <si>
+    <t>Jahre</t>
+  </si>
+  <si>
+    <t>Month</t>
+  </si>
+  <si>
+    <t>Monat</t>
+  </si>
+  <si>
+    <t>Months</t>
+  </si>
+  <si>
+    <t>Monate</t>
+  </si>
+  <si>
+    <t>Additional info</t>
+  </si>
+  <si>
+    <t>Erweiterte Angaben</t>
+  </si>
+  <si>
+    <t>AboutInfo</t>
   </si>
 </sst>
 </file>
@@ -2239,10 +2272,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B234"/>
+  <dimension ref="A1:B239"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A217" workbookViewId="0">
-      <selection activeCell="B234" sqref="A234:B234"/>
+    <sheetView topLeftCell="A222" workbookViewId="0">
+      <selection activeCell="A239" sqref="A239"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2264,7 +2297,7 @@
         <v>49</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>49</v>
+        <v>615</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
@@ -4121,6 +4154,46 @@
       </c>
       <c r="B234" s="1" t="s">
         <v>606</v>
+      </c>
+    </row>
+    <row r="235" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A235" s="1" t="s">
+        <v>607</v>
+      </c>
+      <c r="B235" s="5" t="s">
+        <v>607</v>
+      </c>
+    </row>
+    <row r="236" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A236" s="1" t="s">
+        <v>608</v>
+      </c>
+      <c r="B236" s="5" t="s">
+        <v>608</v>
+      </c>
+    </row>
+    <row r="237" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A237" s="1" t="s">
+        <v>611</v>
+      </c>
+      <c r="B237" s="5" t="s">
+        <v>611</v>
+      </c>
+    </row>
+    <row r="238" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A238" s="1" t="s">
+        <v>613</v>
+      </c>
+      <c r="B238" s="5" t="s">
+        <v>613</v>
+      </c>
+    </row>
+    <row r="239" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A239" s="1" t="s">
+        <v>617</v>
+      </c>
+      <c r="B239" s="5" t="s">
+        <v>49</v>
       </c>
     </row>
   </sheetData>
@@ -4136,10 +4209,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:B234"/>
+  <dimension ref="A1:B239"/>
   <sheetViews>
-    <sheetView topLeftCell="A220" workbookViewId="0">
-      <selection activeCell="A234" sqref="A234:B234"/>
+    <sheetView tabSelected="1" topLeftCell="A232" workbookViewId="0">
+      <selection activeCell="B240" sqref="B240"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4161,7 +4234,7 @@
         <v>49</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>485</v>
+        <v>616</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
@@ -6018,6 +6091,46 @@
       </c>
       <c r="B234" s="1" t="s">
         <v>605</v>
+      </c>
+    </row>
+    <row r="235" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A235" s="1" t="s">
+        <v>607</v>
+      </c>
+      <c r="B235" s="5" t="s">
+        <v>609</v>
+      </c>
+    </row>
+    <row r="236" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A236" s="1" t="s">
+        <v>608</v>
+      </c>
+      <c r="B236" s="5" t="s">
+        <v>610</v>
+      </c>
+    </row>
+    <row r="237" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A237" s="1" t="s">
+        <v>611</v>
+      </c>
+      <c r="B237" s="5" t="s">
+        <v>612</v>
+      </c>
+    </row>
+    <row r="238" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A238" s="1" t="s">
+        <v>613</v>
+      </c>
+      <c r="B238" s="5" t="s">
+        <v>614</v>
+      </c>
+    </row>
+    <row r="239" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A239" s="1" t="s">
+        <v>617</v>
+      </c>
+      <c r="B239" s="5" t="s">
+        <v>485</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
CV enhanced - References left
</commit_message>
<xml_diff>
--- a/Vitae/Library/Resources/SharedResource.xlsx
+++ b/Vitae/Library/Resources/SharedResource.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\Vitae\Library\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C602BF4-CBCF-4893-8AA4-81D68E59D228}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2823E05-25F2-44D1-9421-C0EF8874F7E1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="650" yWindow="1560" windowWidth="22500" windowHeight="14300" tabRatio="406" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="960" uniqueCount="620">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="968" uniqueCount="625">
   <si>
     <t>City</t>
   </si>
@@ -1890,6 +1890,21 @@
   </si>
   <si>
     <t>Verein / Club</t>
+  </si>
+  <si>
+    <t>Hide</t>
+  </si>
+  <si>
+    <t>Verstecken</t>
+  </si>
+  <si>
+    <t>HideReference</t>
+  </si>
+  <si>
+    <t>Referenz verstecken</t>
+  </si>
+  <si>
+    <t>Hide reference</t>
   </si>
 </sst>
 </file>
@@ -2278,10 +2293,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B240"/>
+  <dimension ref="A1:B242"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A222" workbookViewId="0">
-      <selection activeCell="B240" sqref="B240"/>
+      <selection activeCell="B242" sqref="B242"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4208,6 +4223,22 @@
       </c>
       <c r="B240" s="5" t="s">
         <v>618</v>
+      </c>
+    </row>
+    <row r="241" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A241" s="1" t="s">
+        <v>620</v>
+      </c>
+      <c r="B241" s="5" t="s">
+        <v>620</v>
+      </c>
+    </row>
+    <row r="242" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A242" s="1" t="s">
+        <v>622</v>
+      </c>
+      <c r="B242" s="5" t="s">
+        <v>624</v>
       </c>
     </row>
   </sheetData>
@@ -4223,10 +4254,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:B240"/>
+  <dimension ref="A1:B242"/>
   <sheetViews>
     <sheetView topLeftCell="A232" workbookViewId="0">
-      <selection activeCell="B240" sqref="B240"/>
+      <selection activeCell="A242" sqref="A242"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -6155,6 +6186,22 @@
         <v>619</v>
       </c>
     </row>
+    <row r="241" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A241" s="1" t="s">
+        <v>620</v>
+      </c>
+      <c r="B241" s="5" t="s">
+        <v>621</v>
+      </c>
+    </row>
+    <row r="242" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A242" s="1" t="s">
+        <v>622</v>
+      </c>
+      <c r="B242" s="5" t="s">
+        <v>623</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:B23" xr:uid="{00000000-0009-0000-0000-000001000000}">
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B222">

</xml_diff>

<commit_message>
PersonalDetails and Abouts implemented
</commit_message>
<xml_diff>
--- a/Vitae/Library/Resources/SharedResource.xlsx
+++ b/Vitae/Library/Resources/SharedResource.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\Vitae\Library\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBB25BCB-1DD7-40C9-AE09-3A142512A651}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DD408A1-6C1B-44F5-99BA-AA55A1F1D849}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="650" yWindow="1560" windowWidth="22500" windowHeight="14300" tabRatio="406" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="988" uniqueCount="638">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1016" uniqueCount="657">
   <si>
     <t>City</t>
   </si>
@@ -1820,9 +1820,6 @@
     <t>AdTextA2</t>
   </si>
   <si>
-    <t>AdTextB1</t>
-  </si>
-  <si>
     <t>AdTextA0</t>
   </si>
   <si>
@@ -1944,6 +1941,66 @@
   </si>
   <si>
     <t>Short ID</t>
+  </si>
+  <si>
+    <t>LanguageVersions</t>
+  </si>
+  <si>
+    <t>Language versions</t>
+  </si>
+  <si>
+    <t>Sprachversionen</t>
+  </si>
+  <si>
+    <t>Import</t>
+  </si>
+  <si>
+    <t>Importieren</t>
+  </si>
+  <si>
+    <t>CopyValues</t>
+  </si>
+  <si>
+    <t>Copy values</t>
+  </si>
+  <si>
+    <t>Copy Values</t>
+  </si>
+  <si>
+    <t>Werte kopieren</t>
+  </si>
+  <si>
+    <t>Copy</t>
+  </si>
+  <si>
+    <t>Kopieren</t>
+  </si>
+  <si>
+    <t>CopyValuesDescription</t>
+  </si>
+  <si>
+    <t>Copies all values from the first language</t>
+  </si>
+  <si>
+    <t>Kopiert alle Werte von der ersten Sprache</t>
+  </si>
+  <si>
+    <t>CurriculumLanguage</t>
+  </si>
+  <si>
+    <t>Sprachversion</t>
+  </si>
+  <si>
+    <t>Curriculum language</t>
+  </si>
+  <si>
+    <t>CVLanguage</t>
+  </si>
+  <si>
+    <t>CV language</t>
+  </si>
+  <si>
+    <t>CV Sprache</t>
   </si>
 </sst>
 </file>
@@ -2332,10 +2389,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B247"/>
+  <dimension ref="A1:B254"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A222" workbookViewId="0">
-      <selection activeCell="A246" sqref="A246:B247"/>
+    <sheetView tabSelected="1" topLeftCell="A241" workbookViewId="0">
+      <selection activeCell="B255" sqref="B255"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2357,7 +2414,7 @@
         <v>49</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
@@ -2418,7 +2475,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
-        <v>594</v>
+        <v>596</v>
       </c>
       <c r="B10" s="5" t="s">
         <v>246</v>
@@ -2426,7 +2483,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
       <c r="B11" s="5" t="s">
         <v>490</v>
@@ -2434,7 +2491,7 @@
     </row>
     <row r="12" spans="1:2" ht="29" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
-        <v>596</v>
+        <v>597</v>
       </c>
       <c r="B12" s="5" t="s">
         <v>245</v>
@@ -4197,60 +4254,60 @@
         <v>595</v>
       </c>
       <c r="B232" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
     </row>
     <row r="233" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A233" s="1" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="B233" s="5" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
     </row>
     <row r="234" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A234" s="1" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="B234" s="1" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
     </row>
     <row r="235" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A235" s="1" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
       <c r="B235" s="5" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
     </row>
     <row r="236" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A236" s="1" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="B236" s="5" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
     </row>
     <row r="237" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A237" s="1" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
       <c r="B237" s="5" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
     </row>
     <row r="238" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A238" s="1" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
       <c r="B238" s="5" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
     </row>
     <row r="239" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A239" s="1" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
       <c r="B239" s="5" t="s">
         <v>49</v>
@@ -4258,66 +4315,122 @@
     </row>
     <row r="240" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A240" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
       <c r="B240" s="5" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
     </row>
     <row r="241" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A241" s="1" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
       <c r="B241" s="5" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
     </row>
     <row r="242" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A242" s="1" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
       <c r="B242" s="5" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
     </row>
     <row r="243" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A243" s="1" t="s">
+        <v>624</v>
+      </c>
+      <c r="B243" s="5" t="s">
         <v>625</v>
-      </c>
-      <c r="B243" s="5" t="s">
-        <v>626</v>
       </c>
     </row>
     <row r="244" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A244" s="1" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="B244" s="5" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
     </row>
     <row r="245" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A245" s="1" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
       <c r="B245" s="5" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
     </row>
     <row r="246" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A246" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
       <c r="B246" s="5" t="s">
-        <v>637</v>
+        <v>636</v>
       </c>
     </row>
     <row r="247" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A247" s="1" t="s">
+        <v>634</v>
+      </c>
+      <c r="B247" s="5" t="s">
         <v>635</v>
       </c>
-      <c r="B247" s="5" t="s">
-        <v>636</v>
+    </row>
+    <row r="248" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A248" s="1" t="s">
+        <v>637</v>
+      </c>
+      <c r="B248" s="5" t="s">
+        <v>638</v>
+      </c>
+    </row>
+    <row r="249" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A249" s="1" t="s">
+        <v>642</v>
+      </c>
+      <c r="B249" s="5" t="s">
+        <v>643</v>
+      </c>
+    </row>
+    <row r="250" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A250" s="1" t="s">
+        <v>640</v>
+      </c>
+      <c r="B250" s="5" t="s">
+        <v>640</v>
+      </c>
+    </row>
+    <row r="251" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A251" s="1" t="s">
+        <v>646</v>
+      </c>
+      <c r="B251" s="5" t="s">
+        <v>646</v>
+      </c>
+    </row>
+    <row r="252" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A252" s="1" t="s">
+        <v>648</v>
+      </c>
+      <c r="B252" s="5" t="s">
+        <v>649</v>
+      </c>
+    </row>
+    <row r="253" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A253" s="1" t="s">
+        <v>651</v>
+      </c>
+      <c r="B253" s="5" t="s">
+        <v>653</v>
+      </c>
+    </row>
+    <row r="254" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A254" s="1" t="s">
+        <v>654</v>
+      </c>
+      <c r="B254" s="5" t="s">
+        <v>655</v>
       </c>
     </row>
   </sheetData>
@@ -4333,10 +4446,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:B248"/>
+  <dimension ref="A1:B254"/>
   <sheetViews>
-    <sheetView topLeftCell="A224" workbookViewId="0">
-      <selection activeCell="A246" sqref="A246:B247"/>
+    <sheetView topLeftCell="A236" workbookViewId="0">
+      <selection activeCell="A254" sqref="A254:B254"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4358,7 +4471,7 @@
         <v>49</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
@@ -4419,7 +4532,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="B10" t="s">
         <v>457</v>
@@ -4435,7 +4548,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="B12" t="s">
         <v>252</v>
@@ -6198,60 +6311,60 @@
         <v>595</v>
       </c>
       <c r="B232" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
     </row>
     <row r="233" spans="1:2" ht="29" x14ac:dyDescent="0.35">
       <c r="A233" s="1" t="s">
+        <v>600</v>
+      </c>
+      <c r="B233" s="5" t="s">
         <v>601</v>
-      </c>
-      <c r="B233" s="5" t="s">
-        <v>602</v>
       </c>
     </row>
     <row r="234" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A234" s="1" t="s">
+        <v>603</v>
+      </c>
+      <c r="B234" s="1" t="s">
         <v>604</v>
-      </c>
-      <c r="B234" s="1" t="s">
-        <v>605</v>
       </c>
     </row>
     <row r="235" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A235" s="1" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
       <c r="B235" s="5" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
     </row>
     <row r="236" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A236" s="1" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="B236" s="5" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
     </row>
     <row r="237" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A237" s="1" t="s">
+        <v>610</v>
+      </c>
+      <c r="B237" s="5" t="s">
         <v>611</v>
-      </c>
-      <c r="B237" s="5" t="s">
-        <v>612</v>
       </c>
     </row>
     <row r="238" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A238" s="1" t="s">
+        <v>612</v>
+      </c>
+      <c r="B238" s="5" t="s">
         <v>613</v>
-      </c>
-      <c r="B238" s="5" t="s">
-        <v>614</v>
       </c>
     </row>
     <row r="239" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A239" s="1" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
       <c r="B239" s="5" t="s">
         <v>485</v>
@@ -6259,71 +6372,123 @@
     </row>
     <row r="240" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A240" t="s">
+        <v>617</v>
+      </c>
+      <c r="B240" s="5" t="s">
         <v>618</v>
-      </c>
-      <c r="B240" s="5" t="s">
-        <v>619</v>
       </c>
     </row>
     <row r="241" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A241" s="1" t="s">
+        <v>619</v>
+      </c>
+      <c r="B241" s="5" t="s">
         <v>620</v>
-      </c>
-      <c r="B241" s="5" t="s">
-        <v>621</v>
       </c>
     </row>
     <row r="242" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A242" s="1" t="s">
+        <v>621</v>
+      </c>
+      <c r="B242" s="5" t="s">
         <v>622</v>
-      </c>
-      <c r="B242" s="5" t="s">
-        <v>623</v>
       </c>
     </row>
     <row r="243" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A243" s="1" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
       <c r="B243" s="5" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
     </row>
     <row r="244" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A244" s="1" t="s">
+        <v>627</v>
+      </c>
+      <c r="B244" s="5" t="s">
         <v>628</v>
-      </c>
-      <c r="B244" s="5" t="s">
-        <v>629</v>
       </c>
     </row>
     <row r="245" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A245" s="1" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
       <c r="B245" s="5" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
     </row>
     <row r="246" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A246" t="s">
+        <v>632</v>
+      </c>
+      <c r="B246" s="5" t="s">
         <v>633</v>
-      </c>
-      <c r="B246" s="5" t="s">
-        <v>634</v>
       </c>
     </row>
     <row r="247" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A247" s="1" t="s">
+        <v>634</v>
+      </c>
+      <c r="B247" s="5" t="s">
         <v>635</v>
       </c>
-      <c r="B247" s="5" t="s">
-        <v>636</v>
-      </c>
     </row>
     <row r="248" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A248" s="1"/>
-      <c r="B248" s="5"/>
+      <c r="A248" s="1" t="s">
+        <v>637</v>
+      </c>
+      <c r="B248" s="5" t="s">
+        <v>639</v>
+      </c>
+    </row>
+    <row r="249" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A249" s="1" t="s">
+        <v>644</v>
+      </c>
+      <c r="B249" s="5" t="s">
+        <v>645</v>
+      </c>
+    </row>
+    <row r="250" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A250" s="1" t="s">
+        <v>640</v>
+      </c>
+      <c r="B250" s="5" t="s">
+        <v>641</v>
+      </c>
+    </row>
+    <row r="251" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A251" s="1" t="s">
+        <v>646</v>
+      </c>
+      <c r="B251" s="5" t="s">
+        <v>647</v>
+      </c>
+    </row>
+    <row r="252" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A252" s="1" t="s">
+        <v>648</v>
+      </c>
+      <c r="B252" s="5" t="s">
+        <v>650</v>
+      </c>
+    </row>
+    <row r="253" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A253" s="1" t="s">
+        <v>651</v>
+      </c>
+      <c r="B253" s="5" t="s">
+        <v>652</v>
+      </c>
+    </row>
+    <row r="254" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A254" s="1" t="s">
+        <v>654</v>
+      </c>
+      <c r="B254" s="5" t="s">
+        <v>656</v>
+      </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:B23" xr:uid="{00000000-0009-0000-0000-000001000000}">

</xml_diff>

<commit_message>
Level & Industry integrated
</commit_message>
<xml_diff>
--- a/Vitae/Library/Resources/SharedResource.xlsx
+++ b/Vitae/Library/Resources/SharedResource.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\Vitae\Library\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6AB2C55A-B824-43CC-ABE6-06C12BD00173}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0370D5AC-A4DF-4878-8EDD-67EA584834AE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="650" yWindow="1560" windowWidth="22500" windowHeight="14300" tabRatio="406" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1032" uniqueCount="669">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1048" uniqueCount="679">
   <si>
     <t>City</t>
   </si>
@@ -2037,6 +2037,36 @@
   </si>
   <si>
     <t>Das Start-Datum darf nicht grösser als das End-Datum sein</t>
+  </si>
+  <si>
+    <t>Industries</t>
+  </si>
+  <si>
+    <t>Industry</t>
+  </si>
+  <si>
+    <t>Industrie</t>
+  </si>
+  <si>
+    <t>Hierarchiestufe</t>
+  </si>
+  <si>
+    <t>Hierarchy level</t>
+  </si>
+  <si>
+    <t>HierarchyLevel</t>
+  </si>
+  <si>
+    <t>HierarchyLevels</t>
+  </si>
+  <si>
+    <t>Hierarchy levels</t>
+  </si>
+  <si>
+    <t>Industrien</t>
+  </si>
+  <si>
+    <t>Hierarchiestufen</t>
   </si>
 </sst>
 </file>
@@ -2425,15 +2455,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B258"/>
+  <dimension ref="A1:B262"/>
   <sheetViews>
     <sheetView topLeftCell="A237" workbookViewId="0">
-      <selection activeCell="B258" sqref="A258:B258"/>
+      <selection activeCell="A261" sqref="A261:B262"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="37.453125" customWidth="1"/>
+    <col min="1" max="1" width="35.1796875" customWidth="1"/>
     <col min="2" max="2" width="80.453125" style="5" customWidth="1"/>
   </cols>
   <sheetData>
@@ -4499,6 +4529,38 @@
       </c>
       <c r="B258" s="5" t="s">
         <v>667</v>
+      </c>
+    </row>
+    <row r="259" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A259" s="1" t="s">
+        <v>670</v>
+      </c>
+      <c r="B259" s="5" t="s">
+        <v>670</v>
+      </c>
+    </row>
+    <row r="260" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A260" s="1" t="s">
+        <v>674</v>
+      </c>
+      <c r="B260" s="5" t="s">
+        <v>673</v>
+      </c>
+    </row>
+    <row r="261" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A261" s="1" t="s">
+        <v>669</v>
+      </c>
+      <c r="B261" s="5" t="s">
+        <v>669</v>
+      </c>
+    </row>
+    <row r="262" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A262" s="1" t="s">
+        <v>675</v>
+      </c>
+      <c r="B262" s="5" t="s">
+        <v>676</v>
       </c>
     </row>
   </sheetData>
@@ -4514,15 +4576,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:B258"/>
+  <dimension ref="A1:B262"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A236" workbookViewId="0">
-      <selection activeCell="A258" sqref="A258:B258"/>
+    <sheetView tabSelected="1" topLeftCell="A247" workbookViewId="0">
+      <selection activeCell="A262" sqref="A261:B262"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="31.54296875" customWidth="1"/>
+    <col min="1" max="1" width="35.08984375" customWidth="1"/>
     <col min="2" max="2" width="62.54296875" customWidth="1"/>
   </cols>
   <sheetData>
@@ -6588,6 +6650,38 @@
       </c>
       <c r="B258" s="5" t="s">
         <v>668</v>
+      </c>
+    </row>
+    <row r="259" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A259" s="1" t="s">
+        <v>670</v>
+      </c>
+      <c r="B259" s="5" t="s">
+        <v>671</v>
+      </c>
+    </row>
+    <row r="260" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A260" s="1" t="s">
+        <v>541</v>
+      </c>
+      <c r="B260" s="5" t="s">
+        <v>672</v>
+      </c>
+    </row>
+    <row r="261" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A261" s="1" t="s">
+        <v>669</v>
+      </c>
+      <c r="B261" s="5" t="s">
+        <v>677</v>
+      </c>
+    </row>
+    <row r="262" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A262" s="1" t="s">
+        <v>675</v>
+      </c>
+      <c r="B262" s="5" t="s">
+        <v>678</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Personal details save bugfixes
</commit_message>
<xml_diff>
--- a/Vitae/Library/Resources/SharedResource.xlsx
+++ b/Vitae/Library/Resources/SharedResource.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\Vitae\Library\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0370D5AC-A4DF-4878-8EDD-67EA584834AE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F86DFC67-AD0D-4A5D-96AE-CAB674D18E4B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="650" yWindow="1560" windowWidth="22500" windowHeight="14300" tabRatio="406" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6260" yWindow="1450" windowWidth="22500" windowHeight="14300" tabRatio="406" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="en" sheetId="3" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1048" uniqueCount="679">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1052" uniqueCount="680">
   <si>
     <t>City</t>
   </si>
@@ -2067,6 +2067,9 @@
   </si>
   <si>
     <t>Hierarchiestufen</t>
+  </si>
+  <si>
+    <t>ShareIdentifier</t>
   </si>
 </sst>
 </file>
@@ -2455,10 +2458,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B262"/>
+  <dimension ref="A1:B263"/>
   <sheetViews>
     <sheetView topLeftCell="A237" workbookViewId="0">
-      <selection activeCell="A261" sqref="A261:B262"/>
+      <selection activeCell="A263" sqref="A263:B263"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4561,6 +4564,14 @@
       </c>
       <c r="B262" s="5" t="s">
         <v>676</v>
+      </c>
+    </row>
+    <row r="263" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A263" s="1" t="s">
+        <v>679</v>
+      </c>
+      <c r="B263" s="5" t="s">
+        <v>635</v>
       </c>
     </row>
   </sheetData>
@@ -4576,10 +4587,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:B262"/>
+  <dimension ref="A1:B263"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A247" workbookViewId="0">
-      <selection activeCell="A262" sqref="A261:B262"/>
+    <sheetView tabSelected="1" topLeftCell="A145" workbookViewId="0">
+      <selection activeCell="A160" sqref="A160"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -6684,6 +6695,14 @@
         <v>678</v>
       </c>
     </row>
+    <row r="263" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A263" s="1" t="s">
+        <v>679</v>
+      </c>
+      <c r="B263" s="5" t="s">
+        <v>635</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:B23" xr:uid="{00000000-0009-0000-0000-000001000000}">
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B222">

</xml_diff>

<commit_message>
Password dialog 50% implemented
</commit_message>
<xml_diff>
--- a/Vitae/Library/Resources/SharedResource.xlsx
+++ b/Vitae/Library/Resources/SharedResource.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\Vitae\Library\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{475B6D7A-64DB-4B80-A97F-889622C0AC2F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{048D6A28-D016-4E79-8645-63F9855963A0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="30220" windowHeight="19620" tabRatio="406" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="30220" windowHeight="19620" tabRatio="406" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="en" sheetId="3" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1140" uniqueCount="735">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1148" uniqueCount="740">
   <si>
     <t>City</t>
   </si>
@@ -2237,6 +2237,21 @@
   </si>
   <si>
     <t>Notes are invisible for visitors</t>
+  </si>
+  <si>
+    <t>Submit</t>
+  </si>
+  <si>
+    <t>Übermitteln</t>
+  </si>
+  <si>
+    <t>EnterPassword</t>
+  </si>
+  <si>
+    <t>Passwort eingeben</t>
+  </si>
+  <si>
+    <t>Enter password</t>
   </si>
 </sst>
 </file>
@@ -2631,10 +2646,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B285"/>
+  <dimension ref="A1:B287"/>
   <sheetViews>
-    <sheetView topLeftCell="A276" workbookViewId="0">
-      <selection activeCell="A285" sqref="A285:B285"/>
+    <sheetView tabSelected="1" topLeftCell="A270" workbookViewId="0">
+      <selection activeCell="A287" sqref="A287:B287"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4899,7 +4914,7 @@
         <v>725</v>
       </c>
     </row>
-    <row r="283" spans="1:2" ht="188.5" x14ac:dyDescent="0.35">
+    <row r="283" spans="1:2" ht="176" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A283" s="7" t="s">
         <v>727</v>
       </c>
@@ -4921,6 +4936,22 @@
       </c>
       <c r="B285" t="s">
         <v>734</v>
+      </c>
+    </row>
+    <row r="286" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A286" t="s">
+        <v>735</v>
+      </c>
+      <c r="B286" s="5" t="s">
+        <v>735</v>
+      </c>
+    </row>
+    <row r="287" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A287" t="s">
+        <v>737</v>
+      </c>
+      <c r="B287" s="5" t="s">
+        <v>739</v>
       </c>
     </row>
   </sheetData>
@@ -4936,10 +4967,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:B285"/>
+  <dimension ref="A1:B287"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A268" workbookViewId="0">
-      <selection activeCell="A285" sqref="A285:B285"/>
+    <sheetView topLeftCell="A268" workbookViewId="0">
+      <selection activeCell="A287" sqref="A287"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -7228,6 +7259,22 @@
         <v>733</v>
       </c>
     </row>
+    <row r="286" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A286" t="s">
+        <v>735</v>
+      </c>
+      <c r="B286" t="s">
+        <v>736</v>
+      </c>
+    </row>
+    <row r="287" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A287" t="s">
+        <v>737</v>
+      </c>
+      <c r="B287" t="s">
+        <v>738</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:B23" xr:uid="{00000000-0009-0000-0000-000001000000}">
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B265">

</xml_diff>

<commit_message>
Unused Identity pages moved to folder "unused"
</commit_message>
<xml_diff>
--- a/Vitae/Library/Resources/SharedResource.xlsx
+++ b/Vitae/Library/Resources/SharedResource.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\Vitae\Library\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACE0855E-AE3E-4F6F-BD24-BD49DDD01D3F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE7DC689-71B7-4E6B-AFCD-C66269D593A0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="6260" yWindow="1470" windowWidth="22500" windowHeight="14280" tabRatio="406" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1172" uniqueCount="756">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1176" uniqueCount="759">
   <si>
     <t>City</t>
   </si>
@@ -2300,6 +2300,15 @@
   </si>
   <si>
     <t>Möchten Sie diesen Eintrag wirklich löschen?</t>
+  </si>
+  <si>
+    <t>CVCompleteness</t>
+  </si>
+  <si>
+    <t>CV Completeness</t>
+  </si>
+  <si>
+    <t>CV Vollständigkeit</t>
   </si>
 </sst>
 </file>
@@ -2694,10 +2703,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B293"/>
+  <dimension ref="A1:B294"/>
   <sheetViews>
-    <sheetView topLeftCell="A283" workbookViewId="0">
-      <selection activeCell="A103" sqref="A103"/>
+    <sheetView topLeftCell="A284" workbookViewId="0">
+      <selection activeCell="A294" sqref="A294:B294"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -5048,6 +5057,14 @@
       </c>
       <c r="B293" s="4" t="s">
         <v>9</v>
+      </c>
+    </row>
+    <row r="294" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A294" s="1" t="s">
+        <v>756</v>
+      </c>
+      <c r="B294" s="5" t="s">
+        <v>757</v>
       </c>
     </row>
   </sheetData>
@@ -5063,10 +5080,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:B293"/>
+  <dimension ref="A1:B294"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B293" sqref="A2:B293"/>
+    <sheetView tabSelected="1" topLeftCell="A279" workbookViewId="0">
+      <selection activeCell="A294" sqref="A294:B294"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -7419,6 +7436,14 @@
         <v>41</v>
       </c>
     </row>
+    <row r="294" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A294" s="1" t="s">
+        <v>756</v>
+      </c>
+      <c r="B294" s="5" t="s">
+        <v>758</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:B23" xr:uid="{00000000-0009-0000-0000-000001000000}">
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B293">

</xml_diff>

<commit_message>
Mail sender (bye mail) modified Settings page changed
</commit_message>
<xml_diff>
--- a/Vitae/Library/Resources/SharedResource.xlsx
+++ b/Vitae/Library/Resources/SharedResource.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\Vitae\Library\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DD256CE-3840-45AB-A073-AE1C6B4BAA0A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E099448E-3267-4341-ABD7-24CDBC7576F3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="30220" windowHeight="19620" tabRatio="406" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="30220" windowHeight="19620" tabRatio="406" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="en" sheetId="3" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3550" uniqueCount="1901">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3570" uniqueCount="1913">
   <si>
     <t>City</t>
   </si>
@@ -5739,6 +5739,42 @@
   </si>
   <si>
     <t>Schweiz</t>
+  </si>
+  <si>
+    <t>MailBye3</t>
+  </si>
+  <si>
+    <t>Ihr Konto wurde erfolgreich gelöscht. Wir bedauern, dass Sie gegangen sind. Sie können sich jedoch jederzeit mit dieser E-Mail-Adresse wieder neu registrieren</t>
+  </si>
+  <si>
+    <t>Su cuenta fue eliminada con éxito. Lamentamos que te hayas ido. Sin embargo, puedes registrarte de nuevo en cualquier momento con esta dirección de correo electrónico</t>
+  </si>
+  <si>
+    <t>AccountDeleted</t>
+  </si>
+  <si>
+    <t>Account successfully deleted</t>
+  </si>
+  <si>
+    <t>Konto erfolgreich gelöscht</t>
+  </si>
+  <si>
+    <t>Compte supprimé avec succès</t>
+  </si>
+  <si>
+    <t>Conto cancellato con successo</t>
+  </si>
+  <si>
+    <t>la cuenta se ha eliminado con éxito</t>
+  </si>
+  <si>
+    <t>Your account was successfully deleted. We regret that you have left. However, you can register again at any time with this e-mail address by</t>
+  </si>
+  <si>
+    <t>Votre compte a été supprimé avec succès. Nous regrettons que vous soyez parti. Cependant, vous pouvez vous réenregistrer à tout moment avec cette adresse électronique en</t>
+  </si>
+  <si>
+    <t>Il tuo account è stato cancellato con successo. Ci dispiace che se ne sia andato. Tuttavia, è possibile registrarsi di nuovo in qualsiasi momento con questo indirizzo e-mail da</t>
   </si>
 </sst>
 </file>
@@ -6147,16 +6183,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B355"/>
+  <dimension ref="A1:B357"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A346" workbookViewId="0">
-      <selection activeCell="A356" sqref="A356:XFD356"/>
+    <sheetView topLeftCell="A328" workbookViewId="0">
+      <selection activeCell="B356" sqref="B356"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="35.1796875" style="6" customWidth="1"/>
-    <col min="2" max="2" width="57.6328125" style="4" customWidth="1"/>
+    <col min="2" max="2" width="57.7265625" style="4" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
@@ -8997,6 +9033,22 @@
       </c>
       <c r="B355" s="4" t="s">
         <v>1896</v>
+      </c>
+    </row>
+    <row r="356" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A356" s="6" t="s">
+        <v>1901</v>
+      </c>
+      <c r="B356" s="4" t="s">
+        <v>1910</v>
+      </c>
+    </row>
+    <row r="357" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A357" s="6" t="s">
+        <v>1904</v>
+      </c>
+      <c r="B357" s="4" t="s">
+        <v>1905</v>
       </c>
     </row>
   </sheetData>
@@ -9012,10 +9064,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:B355"/>
+  <dimension ref="A1:B357"/>
   <sheetViews>
-    <sheetView topLeftCell="A331" workbookViewId="0">
-      <selection activeCell="A356" sqref="A356:XFD356"/>
+    <sheetView topLeftCell="A32" workbookViewId="0">
+      <selection activeCell="A55" sqref="A55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -11862,6 +11914,22 @@
       </c>
       <c r="B355" s="9" t="s">
         <v>1900</v>
+      </c>
+    </row>
+    <row r="356" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A356" s="6" t="s">
+        <v>1901</v>
+      </c>
+      <c r="B356" s="4" t="s">
+        <v>1902</v>
+      </c>
+    </row>
+    <row r="357" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A357" s="6" t="s">
+        <v>1904</v>
+      </c>
+      <c r="B357" s="4" t="s">
+        <v>1906</v>
       </c>
     </row>
   </sheetData>
@@ -11877,10 +11945,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1802D85A-2FA6-4DB3-A31F-68A2D623BDD9}">
-  <dimension ref="A1:B355"/>
+  <dimension ref="A1:B357"/>
   <sheetViews>
     <sheetView topLeftCell="A346" workbookViewId="0">
-      <selection activeCell="A355" sqref="A355:B355"/>
+      <selection activeCell="B356" sqref="B356"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -14727,6 +14795,22 @@
       </c>
       <c r="B355" s="4" t="s">
         <v>1897</v>
+      </c>
+    </row>
+    <row r="356" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A356" s="6" t="s">
+        <v>1901</v>
+      </c>
+      <c r="B356" s="4" t="s">
+        <v>1911</v>
+      </c>
+    </row>
+    <row r="357" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A357" s="6" t="s">
+        <v>1904</v>
+      </c>
+      <c r="B357" s="4" t="s">
+        <v>1907</v>
       </c>
     </row>
   </sheetData>
@@ -14741,10 +14825,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{21647760-4677-48F5-BA10-2363314EC080}">
-  <dimension ref="A1:B355"/>
+  <dimension ref="A1:B357"/>
   <sheetViews>
-    <sheetView topLeftCell="A331" workbookViewId="0">
-      <selection activeCell="A355" sqref="A355:B355"/>
+    <sheetView topLeftCell="A332" workbookViewId="0">
+      <selection activeCell="D357" sqref="D356:D357"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -17591,6 +17675,22 @@
       </c>
       <c r="B355" s="4" t="s">
         <v>1898</v>
+      </c>
+    </row>
+    <row r="356" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A356" s="6" t="s">
+        <v>1901</v>
+      </c>
+      <c r="B356" s="4" t="s">
+        <v>1912</v>
+      </c>
+    </row>
+    <row r="357" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A357" s="6" t="s">
+        <v>1904</v>
+      </c>
+      <c r="B357" s="4" t="s">
+        <v>1908</v>
       </c>
     </row>
   </sheetData>
@@ -17606,10 +17706,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A8220B7-2614-4C14-91F7-8D47B2A1113F}">
-  <dimension ref="A1:B355"/>
+  <dimension ref="A1:B357"/>
   <sheetViews>
-    <sheetView topLeftCell="A322" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B352" sqref="B352"/>
+    <sheetView tabSelected="1" topLeftCell="A326" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B354" sqref="B354"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -20458,6 +20558,22 @@
         <v>1899</v>
       </c>
     </row>
+    <row r="356" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A356" s="6" t="s">
+        <v>1901</v>
+      </c>
+      <c r="B356" s="4" t="s">
+        <v>1903</v>
+      </c>
+    </row>
+    <row r="357" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A357" s="6" t="s">
+        <v>1904</v>
+      </c>
+      <c r="B357" s="4" t="s">
+        <v>1909</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:B315" xr:uid="{02DBC401-891D-402F-BB4B-45044BD9BA28}">
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B354">

</xml_diff>

<commit_message>
English CV language added
</commit_message>
<xml_diff>
--- a/Vitae/Library/Resources/SharedResource.xlsx
+++ b/Vitae/Library/Resources/SharedResource.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\Vitae\Library\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E099448E-3267-4341-ABD7-24CDBC7576F3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DCA4F49-DAF5-48CD-B580-823AF47637D1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="30220" windowHeight="19620" tabRatio="406" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3570" uniqueCount="1913">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3580" uniqueCount="1919">
   <si>
     <t>City</t>
   </si>
@@ -5775,6 +5775,24 @@
   </si>
   <si>
     <t>Il tuo account è stato cancellato con successo. Ci dispiace che se ne sia andato. Tuttavia, è possibile registrarsi di nuovo in qualsiasi momento con questo indirizzo e-mail da</t>
+  </si>
+  <si>
+    <t>CompanyDescription</t>
+  </si>
+  <si>
+    <t>Company description</t>
+  </si>
+  <si>
+    <t>Firmenbeschreibung</t>
+  </si>
+  <si>
+    <t>Description de l'entreprise</t>
+  </si>
+  <si>
+    <t>Descrizione dell'azienda</t>
+  </si>
+  <si>
+    <t>Descripción de la empresa</t>
   </si>
 </sst>
 </file>
@@ -6183,10 +6201,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B357"/>
+  <dimension ref="A1:B358"/>
   <sheetViews>
     <sheetView topLeftCell="A328" workbookViewId="0">
-      <selection activeCell="B356" sqref="B356"/>
+      <selection activeCell="A358" sqref="A358:B358"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -9049,6 +9067,14 @@
       </c>
       <c r="B357" s="4" t="s">
         <v>1905</v>
+      </c>
+    </row>
+    <row r="358" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A358" s="6" t="s">
+        <v>1913</v>
+      </c>
+      <c r="B358" s="4" t="s">
+        <v>1914</v>
       </c>
     </row>
   </sheetData>
@@ -9064,10 +9090,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:B357"/>
+  <dimension ref="A1:B358"/>
   <sheetViews>
-    <sheetView topLeftCell="A32" workbookViewId="0">
-      <selection activeCell="A55" sqref="A55"/>
+    <sheetView topLeftCell="A342" workbookViewId="0">
+      <selection activeCell="B358" sqref="B358"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -11930,6 +11956,14 @@
       </c>
       <c r="B357" s="4" t="s">
         <v>1906</v>
+      </c>
+    </row>
+    <row r="358" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A358" s="6" t="s">
+        <v>1913</v>
+      </c>
+      <c r="B358" s="4" t="s">
+        <v>1915</v>
       </c>
     </row>
   </sheetData>
@@ -11945,10 +11979,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1802D85A-2FA6-4DB3-A31F-68A2D623BDD9}">
-  <dimension ref="A1:B357"/>
+  <dimension ref="A1:B358"/>
   <sheetViews>
-    <sheetView topLeftCell="A346" workbookViewId="0">
-      <selection activeCell="B356" sqref="B356"/>
+    <sheetView topLeftCell="A64" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -14811,6 +14845,14 @@
       </c>
       <c r="B357" s="4" t="s">
         <v>1907</v>
+      </c>
+    </row>
+    <row r="358" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A358" s="6" t="s">
+        <v>1913</v>
+      </c>
+      <c r="B358" s="4" t="s">
+        <v>1916</v>
       </c>
     </row>
   </sheetData>
@@ -14825,10 +14867,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{21647760-4677-48F5-BA10-2363314EC080}">
-  <dimension ref="A1:B357"/>
+  <dimension ref="A1:B358"/>
   <sheetViews>
     <sheetView topLeftCell="A332" workbookViewId="0">
-      <selection activeCell="D357" sqref="D356:D357"/>
+      <selection activeCell="A358" sqref="A358:B358"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -17691,6 +17733,14 @@
       </c>
       <c r="B357" s="4" t="s">
         <v>1908</v>
+      </c>
+    </row>
+    <row r="358" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A358" s="6" t="s">
+        <v>1913</v>
+      </c>
+      <c r="B358" s="4" t="s">
+        <v>1917</v>
       </c>
     </row>
   </sheetData>
@@ -17706,10 +17756,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A8220B7-2614-4C14-91F7-8D47B2A1113F}">
-  <dimension ref="A1:B357"/>
+  <dimension ref="A1:B358"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A326" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B354" sqref="B354"/>
+      <selection activeCell="A358" sqref="A358:B358"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -20574,6 +20624,14 @@
         <v>1909</v>
       </c>
     </row>
+    <row r="358" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A358" s="6" t="s">
+        <v>1913</v>
+      </c>
+      <c r="B358" s="4" t="s">
+        <v>1918</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:B315" xr:uid="{02DBC401-891D-402F-BB4B-45044BD9BA28}">
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B354">

</xml_diff>

<commit_message>
Beta / preview ribbons added
</commit_message>
<xml_diff>
--- a/Vitae/Library/Resources/SharedResource.xlsx
+++ b/Vitae/Library/Resources/SharedResource.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\Vitae\Library\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACBB21EA-114F-4417-9283-4021377DA816}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA413022-7A05-44ED-8498-9E77C11BD688}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="30220" windowHeight="19620" tabRatio="406" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3590" uniqueCount="1923">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3600" uniqueCount="1929">
   <si>
     <t>City</t>
   </si>
@@ -5805,6 +5805,24 @@
   </si>
   <si>
     <t>Adiós</t>
+  </si>
+  <si>
+    <t>Preview</t>
+  </si>
+  <si>
+    <t>Preview only</t>
+  </si>
+  <si>
+    <t>Vorschau</t>
+  </si>
+  <si>
+    <t>Aperçu</t>
+  </si>
+  <si>
+    <t>Anteprima</t>
+  </si>
+  <si>
+    <t>Vista previa</t>
   </si>
 </sst>
 </file>
@@ -6213,9 +6231,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B359"/>
+  <dimension ref="A1:B360"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A334" workbookViewId="0">
       <selection activeCell="A360" sqref="A360"/>
     </sheetView>
   </sheetViews>
@@ -9095,6 +9113,14 @@
       </c>
       <c r="B359" s="3" t="s">
         <v>9</v>
+      </c>
+    </row>
+    <row r="360" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A360" s="6" t="s">
+        <v>1923</v>
+      </c>
+      <c r="B360" s="4" t="s">
+        <v>1924</v>
       </c>
     </row>
   </sheetData>
@@ -9110,10 +9136,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:B359"/>
+  <dimension ref="A1:B360"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A359" sqref="A359:B359"/>
+    <sheetView topLeftCell="A355" workbookViewId="0">
+      <selection activeCell="A360" sqref="A360"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -11992,6 +12018,14 @@
       </c>
       <c r="B359" s="8" t="s">
         <v>41</v>
+      </c>
+    </row>
+    <row r="360" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A360" s="6" t="s">
+        <v>1923</v>
+      </c>
+      <c r="B360" s="9" t="s">
+        <v>1925</v>
       </c>
     </row>
   </sheetData>
@@ -12007,10 +12041,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1802D85A-2FA6-4DB3-A31F-68A2D623BDD9}">
-  <dimension ref="A1:B359"/>
+  <dimension ref="A1:B360"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B142" sqref="B142"/>
+    <sheetView topLeftCell="A342" workbookViewId="0">
+      <selection activeCell="B360" sqref="B360"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -14889,6 +14923,14 @@
       </c>
       <c r="B359" s="3" t="s">
         <v>1042</v>
+      </c>
+    </row>
+    <row r="360" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A360" s="6" t="s">
+        <v>1923</v>
+      </c>
+      <c r="B360" s="4" t="s">
+        <v>1926</v>
       </c>
     </row>
   </sheetData>
@@ -14903,9 +14945,11 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{21647760-4677-48F5-BA10-2363314EC080}">
-  <dimension ref="A1:B359"/>
+  <dimension ref="A1:B360"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A340" workbookViewId="0">
+      <selection activeCell="A361" sqref="A361"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -17783,6 +17827,14 @@
       </c>
       <c r="B359" s="3" t="s">
         <v>1315</v>
+      </c>
+    </row>
+    <row r="360" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A360" s="6" t="s">
+        <v>1923</v>
+      </c>
+      <c r="B360" s="4" t="s">
+        <v>1927</v>
       </c>
     </row>
   </sheetData>
@@ -17798,10 +17850,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A8220B7-2614-4C14-91F7-8D47B2A1113F}">
-  <dimension ref="A1:B359"/>
+  <dimension ref="A1:B360"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A359" sqref="A359:B359"/>
+    <sheetView tabSelected="1" topLeftCell="A335" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A361" sqref="A361"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -20682,6 +20734,14 @@
         <v>1592</v>
       </c>
     </row>
+    <row r="360" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A360" s="6" t="s">
+        <v>1923</v>
+      </c>
+      <c r="B360" s="4" t="s">
+        <v>1928</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:B315" xr:uid="{02DBC401-891D-402F-BB4B-45044BD9BA28}">
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B359">

</xml_diff>

<commit_message>
Logo changed Bugfix on delete
</commit_message>
<xml_diff>
--- a/Vitae/Library/Resources/SharedResource.xlsx
+++ b/Vitae/Library/Resources/SharedResource.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\Vitae\Library\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{641D1F7F-450C-4395-BBEE-3E2101E24777}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68CB1340-329C-4176-AFA1-840FBE0846D8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="30220" windowHeight="19620" tabRatio="406" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="30220" windowHeight="19620" tabRatio="406" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="en" sheetId="3" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3600" uniqueCount="1928">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3610" uniqueCount="1932">
   <si>
     <t>City</t>
   </si>
@@ -5820,6 +5820,18 @@
   </si>
   <si>
     <t>Diese Sprache kann erst geändert werden, wenn sämtliche darauf referenzierende Veröffentlichungen gelöscht werden.</t>
+  </si>
+  <si>
+    <t>Error</t>
+  </si>
+  <si>
+    <t>Fehler</t>
+  </si>
+  <si>
+    <t>Erreur</t>
+  </si>
+  <si>
+    <t>Errore</t>
   </si>
 </sst>
 </file>
@@ -6228,10 +6240,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B360"/>
+  <dimension ref="A1:B361"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A326" workbookViewId="0">
-      <selection activeCell="B361" sqref="B361"/>
+    <sheetView topLeftCell="A341" workbookViewId="0">
+      <selection activeCell="B362" sqref="B362"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -9118,6 +9130,14 @@
       </c>
       <c r="B360" s="4" t="s">
         <v>1922</v>
+      </c>
+    </row>
+    <row r="361" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A361" s="6" t="s">
+        <v>1928</v>
+      </c>
+      <c r="B361" s="4" t="s">
+        <v>1928</v>
       </c>
     </row>
   </sheetData>
@@ -9133,10 +9153,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:B360"/>
+  <dimension ref="A1:B361"/>
   <sheetViews>
-    <sheetView topLeftCell="A279" workbookViewId="0">
-      <selection activeCell="E302" sqref="E302"/>
+    <sheetView topLeftCell="A357" workbookViewId="0">
+      <selection activeCell="A361" sqref="A361"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -12023,6 +12043,14 @@
       </c>
       <c r="B360" s="9" t="s">
         <v>1923</v>
+      </c>
+    </row>
+    <row r="361" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A361" s="6" t="s">
+        <v>1928</v>
+      </c>
+      <c r="B361" s="9" t="s">
+        <v>1929</v>
       </c>
     </row>
   </sheetData>
@@ -12038,10 +12066,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1802D85A-2FA6-4DB3-A31F-68A2D623BDD9}">
-  <dimension ref="A1:B360"/>
+  <dimension ref="A1:B361"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:B1048576"/>
+    <sheetView topLeftCell="A341" workbookViewId="0">
+      <selection activeCell="B362" sqref="B362"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -14928,6 +14956,14 @@
       </c>
       <c r="B360" s="4" t="s">
         <v>1924</v>
+      </c>
+    </row>
+    <row r="361" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A361" s="6" t="s">
+        <v>1928</v>
+      </c>
+      <c r="B361" s="4" t="s">
+        <v>1930</v>
       </c>
     </row>
   </sheetData>
@@ -14942,10 +14978,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{21647760-4677-48F5-BA10-2363314EC080}">
-  <dimension ref="A1:B360"/>
+  <dimension ref="A1:B361"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:B1048576"/>
+    <sheetView topLeftCell="A332" workbookViewId="0">
+      <selection activeCell="A361" sqref="A361"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -17832,6 +17868,14 @@
       </c>
       <c r="B360" s="4" t="s">
         <v>1925</v>
+      </c>
+    </row>
+    <row r="361" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A361" s="6" t="s">
+        <v>1928</v>
+      </c>
+      <c r="B361" s="4" t="s">
+        <v>1931</v>
       </c>
     </row>
   </sheetData>
@@ -17847,10 +17891,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A8220B7-2614-4C14-91F7-8D47B2A1113F}">
-  <dimension ref="A1:B360"/>
+  <dimension ref="A1:B361"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:B1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A339" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A362" sqref="A362"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -20739,6 +20783,14 @@
         <v>1926</v>
       </c>
     </row>
+    <row r="361" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A361" s="6" t="s">
+        <v>1928</v>
+      </c>
+      <c r="B361" s="4" t="s">
+        <v>1928</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:B315" xr:uid="{02DBC401-891D-402F-BB4B-45044BD9BA28}">
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B359">

</xml_diff>

<commit_message>
Save button to header added
</commit_message>
<xml_diff>
--- a/Vitae/Library/Resources/SharedResource.xlsx
+++ b/Vitae/Library/Resources/SharedResource.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\Vitae\Library\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A7AF585-28CB-4EB3-AF35-7EA7572D1EE7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA0D642A-EFEC-4F90-AA14-1C6F974FF62C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="30220" windowHeight="19620" tabRatio="406" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2130" yWindow="3580" windowWidth="22500" windowHeight="14280" tabRatio="406" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="en" sheetId="3" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3620" uniqueCount="1934">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3636" uniqueCount="1943">
   <si>
     <t>City</t>
   </si>
@@ -5838,6 +5838,33 @@
   </si>
   <si>
     <t>Listen Sie Weiterbildungskurse und kleinere Ausbildungen auf.</t>
+  </si>
+  <si>
+    <t>Up</t>
+  </si>
+  <si>
+    <t>Nach oben</t>
+  </si>
+  <si>
+    <t>Down</t>
+  </si>
+  <si>
+    <t>Vers le haut</t>
+  </si>
+  <si>
+    <t>En bas</t>
+  </si>
+  <si>
+    <t>Su</t>
+  </si>
+  <si>
+    <t>Giù</t>
+  </si>
+  <si>
+    <t>Arriba</t>
+  </si>
+  <si>
+    <t>Abajo</t>
   </si>
 </sst>
 </file>
@@ -6246,10 +6273,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B362"/>
+  <dimension ref="A1:B363"/>
   <sheetViews>
-    <sheetView topLeftCell="A49" workbookViewId="0">
-      <selection activeCell="B75" sqref="B75"/>
+    <sheetView topLeftCell="A347" workbookViewId="0">
+      <selection activeCell="B363" sqref="B363"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -9152,6 +9179,14 @@
       </c>
       <c r="B362" s="4" t="s">
         <v>1927</v>
+      </c>
+    </row>
+    <row r="363" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A363" s="6" t="s">
+        <v>1936</v>
+      </c>
+      <c r="B363" s="4" t="s">
+        <v>1936</v>
       </c>
     </row>
   </sheetData>
@@ -9167,10 +9202,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:B362"/>
+  <dimension ref="A1:B363"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A76" workbookViewId="0">
-      <selection activeCell="C95" sqref="C94:C95"/>
+    <sheetView topLeftCell="A352" workbookViewId="0">
+      <selection activeCell="B364" sqref="B364"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -12073,6 +12108,14 @@
       </c>
       <c r="B362" s="4" t="s">
         <v>1927</v>
+      </c>
+    </row>
+    <row r="363" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A363" s="6" t="s">
+        <v>1934</v>
+      </c>
+      <c r="B363" s="9" t="s">
+        <v>1935</v>
       </c>
     </row>
   </sheetData>
@@ -12088,10 +12131,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1802D85A-2FA6-4DB3-A31F-68A2D623BDD9}">
-  <dimension ref="A1:B362"/>
+  <dimension ref="A1:B364"/>
   <sheetViews>
-    <sheetView topLeftCell="A51" workbookViewId="0">
-      <selection activeCell="A74" sqref="A74"/>
+    <sheetView topLeftCell="A352" workbookViewId="0">
+      <selection activeCell="B364" sqref="A363:B364"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -14994,6 +15037,22 @@
       </c>
       <c r="B362" s="4" t="s">
         <v>1928</v>
+      </c>
+    </row>
+    <row r="363" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A363" s="6" t="s">
+        <v>1934</v>
+      </c>
+      <c r="B363" s="4" t="s">
+        <v>1937</v>
+      </c>
+    </row>
+    <row r="364" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A364" s="6" t="s">
+        <v>1936</v>
+      </c>
+      <c r="B364" s="4" t="s">
+        <v>1938</v>
       </c>
     </row>
   </sheetData>
@@ -15008,10 +15067,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{21647760-4677-48F5-BA10-2363314EC080}">
-  <dimension ref="A1:B362"/>
+  <dimension ref="A1:B364"/>
   <sheetViews>
-    <sheetView topLeftCell="A50" workbookViewId="0">
-      <selection activeCell="B75" sqref="B75"/>
+    <sheetView topLeftCell="A356" workbookViewId="0">
+      <selection activeCell="B364" sqref="A363:B364"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -17914,6 +17973,22 @@
       </c>
       <c r="B362" s="4" t="s">
         <v>1927</v>
+      </c>
+    </row>
+    <row r="363" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A363" s="6" t="s">
+        <v>1934</v>
+      </c>
+      <c r="B363" s="4" t="s">
+        <v>1939</v>
+      </c>
+    </row>
+    <row r="364" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A364" s="6" t="s">
+        <v>1936</v>
+      </c>
+      <c r="B364" s="4" t="s">
+        <v>1940</v>
       </c>
     </row>
   </sheetData>
@@ -17929,10 +18004,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A8220B7-2614-4C14-91F7-8D47B2A1113F}">
-  <dimension ref="A1:B362"/>
+  <dimension ref="A1:B364"/>
   <sheetViews>
-    <sheetView topLeftCell="A50" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A74" sqref="A74"/>
+    <sheetView tabSelected="1" topLeftCell="A352" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B363" sqref="B363:B364"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -20837,6 +20912,22 @@
         <v>1927</v>
       </c>
     </row>
+    <row r="363" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A363" s="6" t="s">
+        <v>1934</v>
+      </c>
+      <c r="B363" s="4" t="s">
+        <v>1941</v>
+      </c>
+    </row>
+    <row r="364" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A364" s="6" t="s">
+        <v>1936</v>
+      </c>
+      <c r="B364" s="4" t="s">
+        <v>1942</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:B315" xr:uid="{02DBC401-891D-402F-BB4B-45044BD9BA28}">
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B359">

</xml_diff>

<commit_message>
Error page layout included in main Layout
</commit_message>
<xml_diff>
--- a/Vitae/Library/Resources/SharedResource.xlsx
+++ b/Vitae/Library/Resources/SharedResource.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\Vitae\Library\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA0D642A-EFEC-4F90-AA14-1C6F974FF62C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{913AE930-E2CE-40A5-B814-BB5DA0FCF6AB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2130" yWindow="3580" windowWidth="22500" windowHeight="14280" tabRatio="406" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2130" yWindow="3580" windowWidth="22500" windowHeight="14280" tabRatio="406" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="en" sheetId="3" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3636" uniqueCount="1943">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3640" uniqueCount="1944">
   <si>
     <t>City</t>
   </si>
@@ -5865,6 +5865,9 @@
   </si>
   <si>
     <t>Abajo</t>
+  </si>
+  <si>
+    <t>Nach unten</t>
   </si>
 </sst>
 </file>
@@ -6273,10 +6276,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B363"/>
+  <dimension ref="A1:B364"/>
   <sheetViews>
-    <sheetView topLeftCell="A347" workbookViewId="0">
-      <selection activeCell="B363" sqref="B363"/>
+    <sheetView topLeftCell="A350" workbookViewId="0">
+      <selection activeCell="A363" sqref="A363:B364"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -9183,9 +9186,17 @@
     </row>
     <row r="363" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A363" s="6" t="s">
+        <v>1934</v>
+      </c>
+      <c r="B363" s="4" t="s">
+        <v>1934</v>
+      </c>
+    </row>
+    <row r="364" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A364" s="6" t="s">
         <v>1936</v>
       </c>
-      <c r="B363" s="4" t="s">
+      <c r="B364" s="4" t="s">
         <v>1936</v>
       </c>
     </row>
@@ -9202,9 +9213,9 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:B363"/>
+  <dimension ref="A1:B364"/>
   <sheetViews>
-    <sheetView topLeftCell="A352" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A354" workbookViewId="0">
       <selection activeCell="B364" sqref="B364"/>
     </sheetView>
   </sheetViews>
@@ -12114,8 +12125,16 @@
       <c r="A363" s="6" t="s">
         <v>1934</v>
       </c>
-      <c r="B363" s="9" t="s">
+      <c r="B363" s="4" t="s">
         <v>1935</v>
+      </c>
+    </row>
+    <row r="364" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A364" s="6" t="s">
+        <v>1936</v>
+      </c>
+      <c r="B364" s="4" t="s">
+        <v>1943</v>
       </c>
     </row>
   </sheetData>
@@ -12133,8 +12152,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1802D85A-2FA6-4DB3-A31F-68A2D623BDD9}">
   <dimension ref="A1:B364"/>
   <sheetViews>
-    <sheetView topLeftCell="A352" workbookViewId="0">
-      <selection activeCell="B364" sqref="A363:B364"/>
+    <sheetView topLeftCell="A350" workbookViewId="0">
+      <selection activeCell="A363" sqref="A363:A364"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -15069,8 +15088,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{21647760-4677-48F5-BA10-2363314EC080}">
   <dimension ref="A1:B364"/>
   <sheetViews>
-    <sheetView topLeftCell="A356" workbookViewId="0">
-      <selection activeCell="B364" sqref="A363:B364"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A34" sqref="A34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -18006,8 +18025,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A8220B7-2614-4C14-91F7-8D47B2A1113F}">
   <dimension ref="A1:B364"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A352" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B363" sqref="B363:B364"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:B1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
Reduced load time due to parallel tasks
</commit_message>
<xml_diff>
--- a/Vitae/Library/Resources/SharedResource.xlsx
+++ b/Vitae/Library/Resources/SharedResource.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\Vitae\Library\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4BB1406-701D-4CFA-A1BB-768CDAE96E9A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A7F004C-0FB7-4D13-B810-F81509E548A1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="30220" windowHeight="19620" tabRatio="406" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="30220" windowHeight="19620" tabRatio="406" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="en" sheetId="3" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -5752,9 +5752,6 @@
     <t>la cuenta se ha eliminado con éxito</t>
   </si>
   <si>
-    <t>Your account was successfully deleted. We regret that you have left. However, you can register again at any time with this e-mail address by</t>
-  </si>
-  <si>
     <t>Votre compte a été supprimé avec succès. Nous regrettons que vous soyez parti. Cependant, vous pouvez vous réenregistrer à tout moment avec cette adresse électronique en</t>
   </si>
   <si>
@@ -6107,6 +6104,9 @@
   </si>
   <si>
     <t>Imprimir</t>
+  </si>
+  <si>
+    <t>Your account has been successfully deleted. We regret that you have left. However, you can register again at any time with this e-mail address by</t>
   </si>
 </sst>
 </file>
@@ -6494,8 +6494,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B500"/>
   <sheetViews>
-    <sheetView topLeftCell="A367" workbookViewId="0">
-      <selection activeCell="A367" sqref="A1:B1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A353" workbookViewId="0">
+      <selection activeCell="A377" sqref="A377"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -6954,10 +6954,10 @@
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A57" s="5" t="s">
+        <v>1898</v>
+      </c>
+      <c r="B57" s="3" t="s">
         <v>1899</v>
-      </c>
-      <c r="B57" s="3" t="s">
-        <v>1900</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.35">
@@ -7085,7 +7085,7 @@
         <v>1838</v>
       </c>
       <c r="B73" s="8" t="s">
-        <v>1924</v>
+        <v>1923</v>
       </c>
     </row>
     <row r="74" spans="1:2" ht="116" x14ac:dyDescent="0.35">
@@ -7650,10 +7650,10 @@
     </row>
     <row r="144" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A144" s="5" t="s">
-        <v>1905</v>
+        <v>1904</v>
       </c>
       <c r="B144" s="3" t="s">
-        <v>1905</v>
+        <v>1904</v>
       </c>
     </row>
     <row r="145" spans="1:2" x14ac:dyDescent="0.35">
@@ -8125,7 +8125,7 @@
         <v>1887</v>
       </c>
       <c r="B203" s="3" t="s">
-        <v>1896</v>
+        <v>2014</v>
       </c>
     </row>
     <row r="204" spans="1:2" x14ac:dyDescent="0.35">
@@ -8845,7 +8845,7 @@
         <v>1757</v>
       </c>
       <c r="B293" s="8" t="s">
-        <v>1959</v>
+        <v>1958</v>
       </c>
     </row>
     <row r="294" spans="1:2" x14ac:dyDescent="0.35">
@@ -9061,7 +9061,7 @@
         <v>716</v>
       </c>
       <c r="B320" s="3" t="s">
-        <v>1955</v>
+        <v>1954</v>
       </c>
     </row>
     <row r="321" spans="1:2" x14ac:dyDescent="0.35">
@@ -9370,766 +9370,766 @@
     </row>
     <row r="359" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A359" s="5" t="s">
-        <v>1910</v>
+        <v>1909</v>
       </c>
       <c r="B359" s="3" t="s">
-        <v>1910</v>
+        <v>1909</v>
       </c>
     </row>
     <row r="360" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A360" s="5" t="s">
-        <v>1916</v>
+        <v>1915</v>
       </c>
       <c r="B360" s="3" t="s">
-        <v>1916</v>
+        <v>1915</v>
       </c>
     </row>
     <row r="361" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A361" s="5" t="s">
-        <v>1920</v>
+        <v>1919</v>
       </c>
       <c r="B361" s="3" t="s">
-        <v>1920</v>
+        <v>1919</v>
       </c>
     </row>
     <row r="362" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A362" s="5" t="s">
-        <v>1927</v>
+        <v>1926</v>
       </c>
       <c r="B362" s="3" t="s">
-        <v>1927</v>
+        <v>1926</v>
       </c>
     </row>
     <row r="363" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A363" s="5" t="s">
-        <v>1929</v>
+        <v>1928</v>
       </c>
       <c r="B363" s="3" t="s">
-        <v>1929</v>
+        <v>1928</v>
       </c>
     </row>
     <row r="364" spans="1:2" ht="29" x14ac:dyDescent="0.35">
       <c r="A364" s="5" t="s">
-        <v>1937</v>
+        <v>1936</v>
       </c>
       <c r="B364" s="8" t="s">
-        <v>1949</v>
+        <v>1948</v>
       </c>
     </row>
     <row r="365" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A365" s="5" t="s">
+        <v>1941</v>
+      </c>
+      <c r="B365" s="3" t="s">
         <v>1942</v>
-      </c>
-      <c r="B365" s="3" t="s">
-        <v>1943</v>
       </c>
     </row>
     <row r="366" spans="1:2" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A366" s="5" t="s">
-        <v>1951</v>
+        <v>1950</v>
       </c>
       <c r="B366" s="3" t="s">
-        <v>1954</v>
+        <v>1953</v>
       </c>
     </row>
     <row r="367" spans="1:2" ht="29" x14ac:dyDescent="0.35">
       <c r="A367" s="5" t="s">
+        <v>1951</v>
+      </c>
+      <c r="B367" s="3" t="s">
         <v>1952</v>
-      </c>
-      <c r="B367" s="3" t="s">
-        <v>1953</v>
       </c>
     </row>
     <row r="368" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A368" s="5" t="s">
-        <v>1956</v>
+        <v>1955</v>
       </c>
       <c r="B368" s="3" t="s">
-        <v>1956</v>
+        <v>1955</v>
       </c>
     </row>
     <row r="369" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A369" s="5" t="s">
-        <v>1957</v>
+        <v>1956</v>
       </c>
       <c r="B369" s="3" t="s">
-        <v>1960</v>
+        <v>1959</v>
       </c>
     </row>
     <row r="370" spans="1:2" ht="29" x14ac:dyDescent="0.35">
       <c r="A370" s="5" t="s">
-        <v>1948</v>
+        <v>1947</v>
       </c>
       <c r="B370" s="3" t="s">
-        <v>1958</v>
+        <v>1957</v>
       </c>
     </row>
     <row r="371" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A371" s="5" t="s">
-        <v>1965</v>
+        <v>1964</v>
       </c>
       <c r="B371" s="3" t="s">
-        <v>1965</v>
+        <v>1964</v>
       </c>
     </row>
     <row r="372" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A372" s="5" t="s">
+        <v>1965</v>
+      </c>
+      <c r="B372" s="3" t="s">
         <v>1966</v>
-      </c>
-      <c r="B372" s="3" t="s">
-        <v>1967</v>
       </c>
     </row>
     <row r="373" spans="1:2" ht="116" x14ac:dyDescent="0.35">
       <c r="A373" s="5" t="s">
+        <v>1967</v>
+      </c>
+      <c r="B373" s="3" t="s">
         <v>1968</v>
-      </c>
-      <c r="B373" s="3" t="s">
-        <v>1969</v>
       </c>
     </row>
     <row r="374" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A374" s="5" t="s">
+        <v>1969</v>
+      </c>
+      <c r="B374" s="3" t="s">
         <v>1970</v>
-      </c>
-      <c r="B374" s="3" t="s">
-        <v>1971</v>
       </c>
     </row>
     <row r="375" spans="1:2" ht="261" x14ac:dyDescent="0.35">
       <c r="A375" s="5" t="s">
+        <v>1971</v>
+      </c>
+      <c r="B375" s="3" t="s">
         <v>1972</v>
-      </c>
-      <c r="B375" s="3" t="s">
-        <v>1973</v>
       </c>
     </row>
     <row r="376" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A376" s="5" t="s">
-        <v>2010</v>
+        <v>2009</v>
       </c>
       <c r="B376" s="3" t="s">
-        <v>2010</v>
+        <v>2009</v>
       </c>
     </row>
     <row r="377" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A377" s="5" t="s">
-        <v>1941</v>
+        <v>1940</v>
       </c>
     </row>
     <row r="378" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A378" s="5" t="s">
-        <v>1941</v>
+        <v>1940</v>
       </c>
     </row>
     <row r="379" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A379" s="5" t="s">
-        <v>1941</v>
+        <v>1940</v>
       </c>
     </row>
     <row r="380" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A380" s="5" t="s">
-        <v>1941</v>
+        <v>1940</v>
       </c>
     </row>
     <row r="381" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A381" s="5" t="s">
-        <v>1941</v>
+        <v>1940</v>
       </c>
     </row>
     <row r="382" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A382" s="5" t="s">
-        <v>1941</v>
+        <v>1940</v>
       </c>
     </row>
     <row r="383" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A383" s="5" t="s">
-        <v>1941</v>
+        <v>1940</v>
       </c>
     </row>
     <row r="384" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A384" s="5" t="s">
-        <v>1941</v>
+        <v>1940</v>
       </c>
     </row>
     <row r="385" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A385" s="5" t="s">
-        <v>1941</v>
+        <v>1940</v>
       </c>
     </row>
     <row r="386" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A386" s="5" t="s">
-        <v>1941</v>
+        <v>1940</v>
       </c>
     </row>
     <row r="387" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A387" s="5" t="s">
-        <v>1941</v>
+        <v>1940</v>
       </c>
     </row>
     <row r="388" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A388" s="5" t="s">
-        <v>1941</v>
+        <v>1940</v>
       </c>
     </row>
     <row r="389" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A389" s="5" t="s">
-        <v>1941</v>
+        <v>1940</v>
       </c>
     </row>
     <row r="390" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A390" s="5" t="s">
-        <v>1941</v>
+        <v>1940</v>
       </c>
     </row>
     <row r="391" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A391" s="5" t="s">
-        <v>1941</v>
+        <v>1940</v>
       </c>
     </row>
     <row r="392" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A392" s="5" t="s">
-        <v>1941</v>
+        <v>1940</v>
       </c>
     </row>
     <row r="393" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A393" s="5" t="s">
-        <v>1941</v>
+        <v>1940</v>
       </c>
     </row>
     <row r="394" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A394" s="5" t="s">
-        <v>1941</v>
+        <v>1940</v>
       </c>
     </row>
     <row r="395" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A395" s="5" t="s">
-        <v>1941</v>
+        <v>1940</v>
       </c>
     </row>
     <row r="396" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A396" s="5" t="s">
-        <v>1941</v>
+        <v>1940</v>
       </c>
     </row>
     <row r="397" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A397" s="5" t="s">
-        <v>1941</v>
+        <v>1940</v>
       </c>
     </row>
     <row r="398" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A398" s="5" t="s">
-        <v>1941</v>
+        <v>1940</v>
       </c>
     </row>
     <row r="399" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A399" s="5" t="s">
-        <v>1941</v>
+        <v>1940</v>
       </c>
     </row>
     <row r="400" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A400" s="5" t="s">
-        <v>1941</v>
+        <v>1940</v>
       </c>
     </row>
     <row r="401" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A401" s="5" t="s">
-        <v>1941</v>
+        <v>1940</v>
       </c>
     </row>
     <row r="402" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A402" s="5" t="s">
-        <v>1941</v>
+        <v>1940</v>
       </c>
     </row>
     <row r="403" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A403" s="5" t="s">
-        <v>1941</v>
+        <v>1940</v>
       </c>
     </row>
     <row r="404" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A404" s="5" t="s">
-        <v>1941</v>
+        <v>1940</v>
       </c>
     </row>
     <row r="405" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A405" s="5" t="s">
-        <v>1941</v>
+        <v>1940</v>
       </c>
     </row>
     <row r="406" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A406" s="5" t="s">
-        <v>1941</v>
+        <v>1940</v>
       </c>
     </row>
     <row r="407" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A407" s="5" t="s">
-        <v>1941</v>
+        <v>1940</v>
       </c>
     </row>
     <row r="408" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A408" s="5" t="s">
-        <v>1941</v>
+        <v>1940</v>
       </c>
     </row>
     <row r="409" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A409" s="5" t="s">
-        <v>1941</v>
+        <v>1940</v>
       </c>
     </row>
     <row r="410" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A410" s="5" t="s">
-        <v>1941</v>
+        <v>1940</v>
       </c>
     </row>
     <row r="411" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A411" s="5" t="s">
-        <v>1941</v>
+        <v>1940</v>
       </c>
     </row>
     <row r="412" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A412" s="5" t="s">
-        <v>1941</v>
+        <v>1940</v>
       </c>
     </row>
     <row r="413" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A413" s="5" t="s">
-        <v>1941</v>
+        <v>1940</v>
       </c>
     </row>
     <row r="414" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A414" s="5" t="s">
-        <v>1941</v>
+        <v>1940</v>
       </c>
     </row>
     <row r="415" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A415" s="5" t="s">
-        <v>1941</v>
+        <v>1940</v>
       </c>
     </row>
     <row r="416" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A416" s="5" t="s">
-        <v>1941</v>
+        <v>1940</v>
       </c>
     </row>
     <row r="417" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A417" s="5" t="s">
-        <v>1941</v>
+        <v>1940</v>
       </c>
     </row>
     <row r="418" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A418" s="5" t="s">
-        <v>1941</v>
+        <v>1940</v>
       </c>
     </row>
     <row r="419" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A419" s="5" t="s">
-        <v>1941</v>
+        <v>1940</v>
       </c>
     </row>
     <row r="420" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A420" s="5" t="s">
-        <v>1941</v>
+        <v>1940</v>
       </c>
     </row>
     <row r="421" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A421" s="5" t="s">
-        <v>1941</v>
+        <v>1940</v>
       </c>
     </row>
     <row r="422" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A422" s="5" t="s">
-        <v>1941</v>
+        <v>1940</v>
       </c>
     </row>
     <row r="423" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A423" s="5" t="s">
-        <v>1941</v>
+        <v>1940</v>
       </c>
     </row>
     <row r="424" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A424" s="5" t="s">
-        <v>1941</v>
+        <v>1940</v>
       </c>
     </row>
     <row r="425" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A425" s="5" t="s">
-        <v>1941</v>
+        <v>1940</v>
       </c>
     </row>
     <row r="426" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A426" s="5" t="s">
-        <v>1941</v>
+        <v>1940</v>
       </c>
     </row>
     <row r="427" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A427" s="5" t="s">
-        <v>1941</v>
+        <v>1940</v>
       </c>
     </row>
     <row r="428" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A428" s="5" t="s">
-        <v>1941</v>
+        <v>1940</v>
       </c>
     </row>
     <row r="429" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A429" s="5" t="s">
-        <v>1941</v>
+        <v>1940</v>
       </c>
     </row>
     <row r="430" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A430" s="5" t="s">
-        <v>1941</v>
+        <v>1940</v>
       </c>
     </row>
     <row r="431" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A431" s="5" t="s">
-        <v>1941</v>
+        <v>1940</v>
       </c>
     </row>
     <row r="432" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A432" s="5" t="s">
-        <v>1941</v>
+        <v>1940</v>
       </c>
     </row>
     <row r="433" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A433" s="5" t="s">
-        <v>1941</v>
+        <v>1940</v>
       </c>
     </row>
     <row r="434" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A434" s="5" t="s">
-        <v>1941</v>
+        <v>1940</v>
       </c>
     </row>
     <row r="435" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A435" s="5" t="s">
-        <v>1941</v>
+        <v>1940</v>
       </c>
     </row>
     <row r="436" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A436" s="5" t="s">
-        <v>1941</v>
+        <v>1940</v>
       </c>
     </row>
     <row r="437" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A437" s="5" t="s">
-        <v>1941</v>
+        <v>1940</v>
       </c>
     </row>
     <row r="438" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A438" s="5" t="s">
-        <v>1941</v>
+        <v>1940</v>
       </c>
     </row>
     <row r="439" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A439" s="5" t="s">
-        <v>1941</v>
+        <v>1940</v>
       </c>
     </row>
     <row r="440" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A440" s="5" t="s">
-        <v>1941</v>
+        <v>1940</v>
       </c>
     </row>
     <row r="441" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A441" s="5" t="s">
-        <v>1941</v>
+        <v>1940</v>
       </c>
     </row>
     <row r="442" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A442" s="5" t="s">
-        <v>1941</v>
+        <v>1940</v>
       </c>
     </row>
     <row r="443" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A443" s="5" t="s">
-        <v>1941</v>
+        <v>1940</v>
       </c>
     </row>
     <row r="444" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A444" s="5" t="s">
-        <v>1941</v>
+        <v>1940</v>
       </c>
     </row>
     <row r="445" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A445" s="5" t="s">
-        <v>1941</v>
+        <v>1940</v>
       </c>
     </row>
     <row r="446" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A446" s="5" t="s">
-        <v>1941</v>
+        <v>1940</v>
       </c>
     </row>
     <row r="447" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A447" s="5" t="s">
-        <v>1941</v>
+        <v>1940</v>
       </c>
     </row>
     <row r="448" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A448" s="5" t="s">
-        <v>1941</v>
+        <v>1940</v>
       </c>
     </row>
     <row r="449" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A449" s="5" t="s">
-        <v>1941</v>
+        <v>1940</v>
       </c>
     </row>
     <row r="450" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A450" s="5" t="s">
-        <v>1941</v>
+        <v>1940</v>
       </c>
     </row>
     <row r="451" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A451" s="5" t="s">
-        <v>1941</v>
+        <v>1940</v>
       </c>
     </row>
     <row r="452" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A452" s="5" t="s">
-        <v>1941</v>
+        <v>1940</v>
       </c>
     </row>
     <row r="453" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A453" s="5" t="s">
-        <v>1941</v>
+        <v>1940</v>
       </c>
     </row>
     <row r="454" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A454" s="5" t="s">
-        <v>1941</v>
+        <v>1940</v>
       </c>
     </row>
     <row r="455" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A455" s="5" t="s">
-        <v>1941</v>
+        <v>1940</v>
       </c>
     </row>
     <row r="456" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A456" s="5" t="s">
-        <v>1941</v>
+        <v>1940</v>
       </c>
     </row>
     <row r="457" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A457" s="5" t="s">
-        <v>1941</v>
+        <v>1940</v>
       </c>
     </row>
     <row r="458" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A458" s="5" t="s">
-        <v>1941</v>
+        <v>1940</v>
       </c>
     </row>
     <row r="459" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A459" s="5" t="s">
-        <v>1941</v>
+        <v>1940</v>
       </c>
     </row>
     <row r="460" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A460" s="5" t="s">
-        <v>1941</v>
+        <v>1940</v>
       </c>
     </row>
     <row r="461" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A461" s="5" t="s">
-        <v>1941</v>
+        <v>1940</v>
       </c>
     </row>
     <row r="462" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A462" s="5" t="s">
-        <v>1941</v>
+        <v>1940</v>
       </c>
     </row>
     <row r="463" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A463" s="5" t="s">
-        <v>1941</v>
+        <v>1940</v>
       </c>
     </row>
     <row r="464" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A464" s="5" t="s">
-        <v>1941</v>
+        <v>1940</v>
       </c>
     </row>
     <row r="465" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A465" s="5" t="s">
-        <v>1941</v>
+        <v>1940</v>
       </c>
     </row>
     <row r="466" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A466" s="5" t="s">
-        <v>1941</v>
+        <v>1940</v>
       </c>
     </row>
     <row r="467" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A467" s="5" t="s">
-        <v>1941</v>
+        <v>1940</v>
       </c>
     </row>
     <row r="468" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A468" s="5" t="s">
-        <v>1941</v>
+        <v>1940</v>
       </c>
     </row>
     <row r="469" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A469" s="5" t="s">
-        <v>1941</v>
+        <v>1940</v>
       </c>
     </row>
     <row r="470" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A470" s="5" t="s">
-        <v>1941</v>
+        <v>1940</v>
       </c>
     </row>
     <row r="471" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A471" s="5" t="s">
-        <v>1941</v>
+        <v>1940</v>
       </c>
     </row>
     <row r="472" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A472" s="5" t="s">
-        <v>1941</v>
+        <v>1940</v>
       </c>
     </row>
     <row r="473" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A473" s="5" t="s">
-        <v>1941</v>
+        <v>1940</v>
       </c>
     </row>
     <row r="474" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A474" s="5" t="s">
-        <v>1941</v>
+        <v>1940</v>
       </c>
     </row>
     <row r="475" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A475" s="5" t="s">
-        <v>1941</v>
+        <v>1940</v>
       </c>
     </row>
     <row r="476" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A476" s="5" t="s">
-        <v>1941</v>
+        <v>1940</v>
       </c>
     </row>
     <row r="477" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A477" s="5" t="s">
-        <v>1941</v>
+        <v>1940</v>
       </c>
     </row>
     <row r="478" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A478" s="5" t="s">
-        <v>1941</v>
+        <v>1940</v>
       </c>
     </row>
     <row r="479" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A479" s="5" t="s">
-        <v>1941</v>
+        <v>1940</v>
       </c>
     </row>
     <row r="480" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A480" s="5" t="s">
-        <v>1941</v>
+        <v>1940</v>
       </c>
     </row>
     <row r="481" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A481" s="5" t="s">
-        <v>1941</v>
+        <v>1940</v>
       </c>
     </row>
     <row r="482" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A482" s="5" t="s">
-        <v>1941</v>
+        <v>1940</v>
       </c>
     </row>
     <row r="483" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A483" s="5" t="s">
-        <v>1941</v>
+        <v>1940</v>
       </c>
     </row>
     <row r="484" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A484" s="5" t="s">
-        <v>1941</v>
+        <v>1940</v>
       </c>
     </row>
     <row r="485" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A485" s="5" t="s">
-        <v>1941</v>
+        <v>1940</v>
       </c>
     </row>
     <row r="486" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A486" s="5" t="s">
-        <v>1941</v>
+        <v>1940</v>
       </c>
     </row>
     <row r="487" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A487" s="5" t="s">
-        <v>1941</v>
+        <v>1940</v>
       </c>
     </row>
     <row r="488" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A488" s="5" t="s">
-        <v>1941</v>
+        <v>1940</v>
       </c>
     </row>
     <row r="489" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A489" s="5" t="s">
-        <v>1941</v>
+        <v>1940</v>
       </c>
     </row>
     <row r="490" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A490" s="5" t="s">
-        <v>1941</v>
+        <v>1940</v>
       </c>
     </row>
     <row r="491" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A491" s="5" t="s">
-        <v>1941</v>
+        <v>1940</v>
       </c>
     </row>
     <row r="492" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A492" s="5" t="s">
-        <v>1941</v>
+        <v>1940</v>
       </c>
     </row>
     <row r="493" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A493" s="5" t="s">
-        <v>1941</v>
+        <v>1940</v>
       </c>
     </row>
     <row r="494" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A494" s="5" t="s">
-        <v>1941</v>
+        <v>1940</v>
       </c>
     </row>
     <row r="495" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A495" s="5" t="s">
-        <v>1941</v>
+        <v>1940</v>
       </c>
     </row>
     <row r="496" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A496" s="5" t="s">
-        <v>1941</v>
+        <v>1940</v>
       </c>
     </row>
     <row r="497" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A497" s="5" t="s">
-        <v>1941</v>
+        <v>1940</v>
       </c>
     </row>
     <row r="498" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A498" s="5" t="s">
-        <v>1941</v>
+        <v>1940</v>
       </c>
     </row>
     <row r="499" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A499" s="5" t="s">
-        <v>1941</v>
+        <v>1940</v>
       </c>
     </row>
     <row r="500" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A500" s="5" t="s">
-        <v>1941</v>
+        <v>1940</v>
       </c>
     </row>
   </sheetData>
@@ -10142,8 +10142,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B499"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A365" workbookViewId="0">
-      <selection activeCell="A374" sqref="A1:B1048576"/>
+    <sheetView topLeftCell="A365" workbookViewId="0">
+      <selection activeCell="B377" sqref="B377"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -10278,7 +10278,7 @@
         <v>AdTextA0</v>
       </c>
       <c r="B16" s="8" t="s">
-        <v>1922</v>
+        <v>1921</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.35">
@@ -10606,7 +10606,7 @@
         <v>CompanyDescription</v>
       </c>
       <c r="B57" s="3" t="s">
-        <v>1901</v>
+        <v>1900</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.35">
@@ -10734,7 +10734,7 @@
         <v>CookiesText1</v>
       </c>
       <c r="B73" s="8" t="s">
-        <v>1923</v>
+        <v>1922</v>
       </c>
     </row>
     <row r="74" spans="1:2" ht="159.5" x14ac:dyDescent="0.35">
@@ -10830,7 +10830,7 @@
         <v>CoursesDescription</v>
       </c>
       <c r="B85" s="7" t="s">
-        <v>1926</v>
+        <v>1925</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.35">
@@ -11302,7 +11302,7 @@
         <v>Goodbye</v>
       </c>
       <c r="B144" s="8" t="s">
-        <v>1906</v>
+        <v>1905</v>
       </c>
     </row>
     <row r="145" spans="1:2" x14ac:dyDescent="0.35">
@@ -12494,7 +12494,7 @@
         <v>SavePublicationsDescription</v>
       </c>
       <c r="B293" s="8" t="s">
-        <v>1961</v>
+        <v>1960</v>
       </c>
     </row>
     <row r="294" spans="1:2" x14ac:dyDescent="0.35">
@@ -12550,7 +12550,7 @@
         <v>SettingsLanguageHint</v>
       </c>
       <c r="B300" s="7" t="s">
-        <v>1915</v>
+        <v>1914</v>
       </c>
     </row>
     <row r="301" spans="1:2" ht="29" x14ac:dyDescent="0.35">
@@ -13022,7 +13022,7 @@
         <v>Preview</v>
       </c>
       <c r="B359" s="8" t="s">
-        <v>1911</v>
+        <v>1910</v>
       </c>
     </row>
     <row r="360" spans="1:2" x14ac:dyDescent="0.35">
@@ -13030,7 +13030,7 @@
         <v>Error</v>
       </c>
       <c r="B360" s="8" t="s">
-        <v>1917</v>
+        <v>1916</v>
       </c>
     </row>
     <row r="361" spans="1:2" x14ac:dyDescent="0.35">
@@ -13038,7 +13038,7 @@
         <v>Demo</v>
       </c>
       <c r="B361" s="3" t="s">
-        <v>1920</v>
+        <v>1919</v>
       </c>
     </row>
     <row r="362" spans="1:2" x14ac:dyDescent="0.35">
@@ -13046,7 +13046,7 @@
         <v>Up</v>
       </c>
       <c r="B362" s="3" t="s">
-        <v>1928</v>
+        <v>1927</v>
       </c>
     </row>
     <row r="363" spans="1:2" x14ac:dyDescent="0.35">
@@ -13054,7 +13054,7 @@
         <v>Down</v>
       </c>
       <c r="B363" s="3" t="s">
-        <v>1936</v>
+        <v>1935</v>
       </c>
     </row>
     <row r="364" spans="1:2" ht="28.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -13062,7 +13062,7 @@
         <v>PasswordProtectionDesc</v>
       </c>
       <c r="B364" s="8" t="s">
-        <v>1950</v>
+        <v>1949</v>
       </c>
     </row>
     <row r="365" spans="1:2" x14ac:dyDescent="0.35">
@@ -13070,7 +13070,7 @@
         <v>SecurityCheck</v>
       </c>
       <c r="B365" s="8" t="s">
-        <v>1944</v>
+        <v>1943</v>
       </c>
     </row>
     <row r="366" spans="1:2" x14ac:dyDescent="0.35">
@@ -13078,7 +13078,7 @@
         <v>Status403</v>
       </c>
       <c r="B366" s="8" t="s">
-        <v>1974</v>
+        <v>1973</v>
       </c>
     </row>
     <row r="367" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
@@ -13086,7 +13086,7 @@
         <v>Status500</v>
       </c>
       <c r="B367" s="8" t="s">
-        <v>1975</v>
+        <v>1974</v>
       </c>
     </row>
     <row r="368" spans="1:2" x14ac:dyDescent="0.35">
@@ -13094,7 +13094,7 @@
         <v>Secure</v>
       </c>
       <c r="B368" s="8" t="s">
-        <v>1981</v>
+        <v>1980</v>
       </c>
     </row>
     <row r="369" spans="1:2" ht="29" x14ac:dyDescent="0.35">
@@ -13102,7 +13102,7 @@
         <v>SecureDescription</v>
       </c>
       <c r="B369" s="8" t="s">
-        <v>2009</v>
+        <v>2008</v>
       </c>
     </row>
     <row r="370" spans="1:2" ht="29" x14ac:dyDescent="0.35">
@@ -13110,7 +13110,7 @@
         <v>SecurityCheckDesc</v>
       </c>
       <c r="B370" s="8" t="s">
-        <v>1976</v>
+        <v>1975</v>
       </c>
     </row>
     <row r="371" spans="1:2" x14ac:dyDescent="0.35">
@@ -13118,7 +13118,7 @@
         <v>Contact</v>
       </c>
       <c r="B371" s="8" t="s">
-        <v>1977</v>
+        <v>1976</v>
       </c>
     </row>
     <row r="372" spans="1:2" x14ac:dyDescent="0.35">
@@ -13126,7 +13126,7 @@
         <v>GoogleCaptcha</v>
       </c>
       <c r="B372" s="8" t="s">
-        <v>1967</v>
+        <v>1966</v>
       </c>
     </row>
     <row r="373" spans="1:2" ht="174" x14ac:dyDescent="0.35">
@@ -13134,7 +13134,7 @@
         <v>GoogleCaptchaDesc</v>
       </c>
       <c r="B373" s="8" t="s">
-        <v>1978</v>
+        <v>1977</v>
       </c>
     </row>
     <row r="374" spans="1:2" x14ac:dyDescent="0.35">
@@ -13142,7 +13142,7 @@
         <v>DataCollection</v>
       </c>
       <c r="B374" s="8" t="s">
-        <v>1979</v>
+        <v>1978</v>
       </c>
     </row>
     <row r="375" spans="1:2" ht="304.5" x14ac:dyDescent="0.35">
@@ -13150,7 +13150,7 @@
         <v>DataCollectionDesc</v>
       </c>
       <c r="B375" s="8" t="s">
-        <v>1980</v>
+        <v>1979</v>
       </c>
     </row>
     <row r="376" spans="1:2" x14ac:dyDescent="0.35">
@@ -13158,7 +13158,7 @@
         <v>Imprint</v>
       </c>
       <c r="B376" s="8" t="s">
-        <v>2011</v>
+        <v>2010</v>
       </c>
     </row>
     <row r="377" spans="1:2" x14ac:dyDescent="0.35">
@@ -13786,8 +13786,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1802D85A-2FA6-4DB3-A31F-68A2D623BDD9}">
   <dimension ref="A1:B499"/>
   <sheetViews>
-    <sheetView topLeftCell="A367" workbookViewId="0">
-      <selection activeCell="A367" sqref="A1:B1048576"/>
+    <sheetView topLeftCell="A374" workbookViewId="0">
+      <selection activeCell="B377" sqref="B377"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -14250,7 +14250,7 @@
         <v>CompanyDescription</v>
       </c>
       <c r="B57" s="3" t="s">
-        <v>1902</v>
+        <v>1901</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.35">
@@ -14946,7 +14946,7 @@
         <v>Goodbye</v>
       </c>
       <c r="B144" s="8" t="s">
-        <v>1907</v>
+        <v>1906</v>
       </c>
     </row>
     <row r="145" spans="1:2" x14ac:dyDescent="0.35">
@@ -15418,7 +15418,7 @@
         <v>MailBye3</v>
       </c>
       <c r="B203" s="3" t="s">
-        <v>1897</v>
+        <v>1896</v>
       </c>
     </row>
     <row r="204" spans="1:2" x14ac:dyDescent="0.35">
@@ -16138,7 +16138,7 @@
         <v>SavePublicationsDescription</v>
       </c>
       <c r="B293" s="3" t="s">
-        <v>1962</v>
+        <v>1961</v>
       </c>
     </row>
     <row r="294" spans="1:2" x14ac:dyDescent="0.35">
@@ -16666,7 +16666,7 @@
         <v>Preview</v>
       </c>
       <c r="B359" s="3" t="s">
-        <v>1912</v>
+        <v>1911</v>
       </c>
     </row>
     <row r="360" spans="1:2" x14ac:dyDescent="0.35">
@@ -16674,7 +16674,7 @@
         <v>Error</v>
       </c>
       <c r="B360" s="3" t="s">
-        <v>1918</v>
+        <v>1917</v>
       </c>
     </row>
     <row r="361" spans="1:2" x14ac:dyDescent="0.35">
@@ -16682,7 +16682,7 @@
         <v>Demo</v>
       </c>
       <c r="B361" s="3" t="s">
-        <v>1921</v>
+        <v>1920</v>
       </c>
     </row>
     <row r="362" spans="1:2" x14ac:dyDescent="0.35">
@@ -16690,7 +16690,7 @@
         <v>Up</v>
       </c>
       <c r="B362" s="3" t="s">
-        <v>1930</v>
+        <v>1929</v>
       </c>
     </row>
     <row r="363" spans="1:2" x14ac:dyDescent="0.35">
@@ -16698,7 +16698,7 @@
         <v>Down</v>
       </c>
       <c r="B363" s="3" t="s">
-        <v>1931</v>
+        <v>1930</v>
       </c>
     </row>
     <row r="364" spans="1:2" ht="29" x14ac:dyDescent="0.35">
@@ -16706,7 +16706,7 @@
         <v>PasswordProtectionDesc</v>
       </c>
       <c r="B364" s="8" t="s">
-        <v>1938</v>
+        <v>1937</v>
       </c>
     </row>
     <row r="365" spans="1:2" x14ac:dyDescent="0.35">
@@ -16714,7 +16714,7 @@
         <v>SecurityCheck</v>
       </c>
       <c r="B365" s="3" t="s">
-        <v>1945</v>
+        <v>1944</v>
       </c>
     </row>
     <row r="366" spans="1:2" x14ac:dyDescent="0.35">
@@ -16722,7 +16722,7 @@
         <v>Status403</v>
       </c>
       <c r="B366" s="3" t="s">
-        <v>1982</v>
+        <v>1981</v>
       </c>
     </row>
     <row r="367" spans="1:2" ht="29" x14ac:dyDescent="0.35">
@@ -16730,7 +16730,7 @@
         <v>Status500</v>
       </c>
       <c r="B367" s="3" t="s">
-        <v>1983</v>
+        <v>1982</v>
       </c>
     </row>
     <row r="368" spans="1:2" x14ac:dyDescent="0.35">
@@ -16738,7 +16738,7 @@
         <v>Secure</v>
       </c>
       <c r="B368" s="3" t="s">
-        <v>1984</v>
+        <v>1983</v>
       </c>
     </row>
     <row r="369" spans="1:2" ht="29" x14ac:dyDescent="0.35">
@@ -16746,7 +16746,7 @@
         <v>SecureDescription</v>
       </c>
       <c r="B369" s="3" t="s">
-        <v>1985</v>
+        <v>1984</v>
       </c>
     </row>
     <row r="370" spans="1:2" x14ac:dyDescent="0.35">
@@ -16754,7 +16754,7 @@
         <v>SecurityCheckDesc</v>
       </c>
       <c r="B370" s="3" t="s">
-        <v>1986</v>
+        <v>1985</v>
       </c>
     </row>
     <row r="371" spans="1:2" x14ac:dyDescent="0.35">
@@ -16762,7 +16762,7 @@
         <v>Contact</v>
       </c>
       <c r="B371" s="3" t="s">
-        <v>1987</v>
+        <v>1986</v>
       </c>
     </row>
     <row r="372" spans="1:2" x14ac:dyDescent="0.35">
@@ -16770,7 +16770,7 @@
         <v>GoogleCaptcha</v>
       </c>
       <c r="B372" s="3" t="s">
-        <v>1967</v>
+        <v>1966</v>
       </c>
     </row>
     <row r="373" spans="1:2" ht="130.5" x14ac:dyDescent="0.35">
@@ -16778,7 +16778,7 @@
         <v>GoogleCaptchaDesc</v>
       </c>
       <c r="B373" s="3" t="s">
-        <v>1988</v>
+        <v>1987</v>
       </c>
     </row>
     <row r="374" spans="1:2" x14ac:dyDescent="0.35">
@@ -16786,7 +16786,7 @@
         <v>DataCollection</v>
       </c>
       <c r="B374" s="3" t="s">
-        <v>1989</v>
+        <v>1988</v>
       </c>
     </row>
     <row r="375" spans="1:2" ht="307" customHeight="1" x14ac:dyDescent="0.35">
@@ -16794,7 +16794,7 @@
         <v>DataCollectionDesc</v>
       </c>
       <c r="B375" s="3" t="s">
-        <v>1990</v>
+        <v>1989</v>
       </c>
     </row>
     <row r="376" spans="1:2" x14ac:dyDescent="0.35">
@@ -16802,7 +16802,7 @@
         <v>Imprint</v>
       </c>
       <c r="B376" s="3" t="s">
-        <v>2012</v>
+        <v>2011</v>
       </c>
     </row>
     <row r="377" spans="1:2" x14ac:dyDescent="0.35">
@@ -17429,8 +17429,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{21647760-4677-48F5-BA10-2363314EC080}">
   <dimension ref="A1:B499"/>
   <sheetViews>
-    <sheetView topLeftCell="A357" workbookViewId="0">
-      <selection activeCell="A357" sqref="A1:B1048576"/>
+    <sheetView topLeftCell="A363" workbookViewId="0">
+      <selection activeCell="B377" sqref="B377"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -17893,7 +17893,7 @@
         <v>CompanyDescription</v>
       </c>
       <c r="B57" s="3" t="s">
-        <v>1903</v>
+        <v>1902</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.35">
@@ -18021,7 +18021,7 @@
         <v>CookiesText1</v>
       </c>
       <c r="B73" s="3" t="s">
-        <v>1925</v>
+        <v>1924</v>
       </c>
     </row>
     <row r="74" spans="1:2" ht="130.5" x14ac:dyDescent="0.35">
@@ -18589,7 +18589,7 @@
         <v>Goodbye</v>
       </c>
       <c r="B144" t="s">
-        <v>1908</v>
+        <v>1907</v>
       </c>
     </row>
     <row r="145" spans="1:2" x14ac:dyDescent="0.35">
@@ -19061,7 +19061,7 @@
         <v>MailBye3</v>
       </c>
       <c r="B203" s="3" t="s">
-        <v>1898</v>
+        <v>1897</v>
       </c>
     </row>
     <row r="204" spans="1:2" x14ac:dyDescent="0.35">
@@ -19781,7 +19781,7 @@
         <v>SavePublicationsDescription</v>
       </c>
       <c r="B293" s="3" t="s">
-        <v>1963</v>
+        <v>1962</v>
       </c>
     </row>
     <row r="294" spans="1:2" x14ac:dyDescent="0.35">
@@ -20309,7 +20309,7 @@
         <v>Preview</v>
       </c>
       <c r="B359" s="3" t="s">
-        <v>1913</v>
+        <v>1912</v>
       </c>
     </row>
     <row r="360" spans="1:2" x14ac:dyDescent="0.35">
@@ -20317,7 +20317,7 @@
         <v>Error</v>
       </c>
       <c r="B360" s="3" t="s">
-        <v>1919</v>
+        <v>1918</v>
       </c>
     </row>
     <row r="361" spans="1:2" x14ac:dyDescent="0.35">
@@ -20325,7 +20325,7 @@
         <v>Demo</v>
       </c>
       <c r="B361" s="3" t="s">
-        <v>1920</v>
+        <v>1919</v>
       </c>
     </row>
     <row r="362" spans="1:2" x14ac:dyDescent="0.35">
@@ -20333,7 +20333,7 @@
         <v>Up</v>
       </c>
       <c r="B362" s="3" t="s">
-        <v>1932</v>
+        <v>1931</v>
       </c>
     </row>
     <row r="363" spans="1:2" x14ac:dyDescent="0.35">
@@ -20341,7 +20341,7 @@
         <v>Down</v>
       </c>
       <c r="B363" s="3" t="s">
-        <v>1933</v>
+        <v>1932</v>
       </c>
     </row>
     <row r="364" spans="1:2" ht="29" x14ac:dyDescent="0.35">
@@ -20349,7 +20349,7 @@
         <v>PasswordProtectionDesc</v>
       </c>
       <c r="B364" s="3" t="s">
-        <v>1940</v>
+        <v>1939</v>
       </c>
     </row>
     <row r="365" spans="1:2" x14ac:dyDescent="0.35">
@@ -20357,7 +20357,7 @@
         <v>SecurityCheck</v>
       </c>
       <c r="B365" s="3" t="s">
-        <v>1946</v>
+        <v>1945</v>
       </c>
     </row>
     <row r="366" spans="1:2" x14ac:dyDescent="0.35">
@@ -20365,7 +20365,7 @@
         <v>Status403</v>
       </c>
       <c r="B366" s="3" t="s">
-        <v>1991</v>
+        <v>1990</v>
       </c>
     </row>
     <row r="367" spans="1:2" ht="29" x14ac:dyDescent="0.35">
@@ -20373,7 +20373,7 @@
         <v>Status500</v>
       </c>
       <c r="B367" s="3" t="s">
-        <v>1992</v>
+        <v>1991</v>
       </c>
     </row>
     <row r="368" spans="1:2" x14ac:dyDescent="0.35">
@@ -20381,7 +20381,7 @@
         <v>Secure</v>
       </c>
       <c r="B368" s="3" t="s">
-        <v>1993</v>
+        <v>1992</v>
       </c>
     </row>
     <row r="369" spans="1:2" x14ac:dyDescent="0.35">
@@ -20389,7 +20389,7 @@
         <v>SecureDescription</v>
       </c>
       <c r="B369" s="3" t="s">
-        <v>1994</v>
+        <v>1993</v>
       </c>
     </row>
     <row r="370" spans="1:2" x14ac:dyDescent="0.35">
@@ -20397,7 +20397,7 @@
         <v>SecurityCheckDesc</v>
       </c>
       <c r="B370" s="3" t="s">
-        <v>1995</v>
+        <v>1994</v>
       </c>
     </row>
     <row r="371" spans="1:2" x14ac:dyDescent="0.35">
@@ -20405,7 +20405,7 @@
         <v>Contact</v>
       </c>
       <c r="B371" s="3" t="s">
-        <v>1996</v>
+        <v>1995</v>
       </c>
     </row>
     <row r="372" spans="1:2" x14ac:dyDescent="0.35">
@@ -20413,7 +20413,7 @@
         <v>GoogleCaptcha</v>
       </c>
       <c r="B372" s="3" t="s">
-        <v>1967</v>
+        <v>1966</v>
       </c>
     </row>
     <row r="373" spans="1:2" ht="116" x14ac:dyDescent="0.35">
@@ -20421,7 +20421,7 @@
         <v>GoogleCaptchaDesc</v>
       </c>
       <c r="B373" s="3" t="s">
-        <v>1997</v>
+        <v>1996</v>
       </c>
     </row>
     <row r="374" spans="1:2" x14ac:dyDescent="0.35">
@@ -20429,7 +20429,7 @@
         <v>DataCollection</v>
       </c>
       <c r="B374" s="3" t="s">
-        <v>1998</v>
+        <v>1997</v>
       </c>
     </row>
     <row r="375" spans="1:2" ht="261" x14ac:dyDescent="0.35">
@@ -20437,7 +20437,7 @@
         <v>DataCollectionDesc</v>
       </c>
       <c r="B375" s="3" t="s">
-        <v>1999</v>
+        <v>1998</v>
       </c>
     </row>
     <row r="376" spans="1:2" x14ac:dyDescent="0.35">
@@ -20445,7 +20445,7 @@
         <v>Imprint</v>
       </c>
       <c r="B376" s="3" t="s">
-        <v>2013</v>
+        <v>2012</v>
       </c>
     </row>
     <row r="377" spans="1:2" x14ac:dyDescent="0.35">
@@ -21074,7 +21074,7 @@
   <dimension ref="A1:B499"/>
   <sheetViews>
     <sheetView topLeftCell="A365" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A365" sqref="A1:B1048576"/>
+      <selection activeCell="B377" sqref="B377"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -21537,7 +21537,7 @@
         <v>CompanyDescription</v>
       </c>
       <c r="B57" s="3" t="s">
-        <v>1904</v>
+        <v>1903</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.35">
@@ -22233,7 +22233,7 @@
         <v>Goodbye</v>
       </c>
       <c r="B144" s="3" t="s">
-        <v>1909</v>
+        <v>1908</v>
       </c>
     </row>
     <row r="145" spans="1:2" x14ac:dyDescent="0.35">
@@ -23425,7 +23425,7 @@
         <v>SavePublicationsDescription</v>
       </c>
       <c r="B293" s="3" t="s">
-        <v>1964</v>
+        <v>1963</v>
       </c>
     </row>
     <row r="294" spans="1:2" x14ac:dyDescent="0.35">
@@ -23953,7 +23953,7 @@
         <v>Preview</v>
       </c>
       <c r="B359" s="3" t="s">
-        <v>1914</v>
+        <v>1913</v>
       </c>
     </row>
     <row r="360" spans="1:2" x14ac:dyDescent="0.35">
@@ -23961,7 +23961,7 @@
         <v>Error</v>
       </c>
       <c r="B360" s="3" t="s">
-        <v>1916</v>
+        <v>1915</v>
       </c>
     </row>
     <row r="361" spans="1:2" x14ac:dyDescent="0.35">
@@ -23969,7 +23969,7 @@
         <v>Demo</v>
       </c>
       <c r="B361" s="3" t="s">
-        <v>1920</v>
+        <v>1919</v>
       </c>
     </row>
     <row r="362" spans="1:2" x14ac:dyDescent="0.35">
@@ -23977,7 +23977,7 @@
         <v>Up</v>
       </c>
       <c r="B362" s="3" t="s">
-        <v>1934</v>
+        <v>1933</v>
       </c>
     </row>
     <row r="363" spans="1:2" x14ac:dyDescent="0.35">
@@ -23985,7 +23985,7 @@
         <v>Down</v>
       </c>
       <c r="B363" s="3" t="s">
-        <v>1935</v>
+        <v>1934</v>
       </c>
     </row>
     <row r="364" spans="1:2" ht="29" x14ac:dyDescent="0.35">
@@ -23993,7 +23993,7 @@
         <v>PasswordProtectionDesc</v>
       </c>
       <c r="B364" s="3" t="s">
-        <v>1939</v>
+        <v>1938</v>
       </c>
     </row>
     <row r="365" spans="1:2" x14ac:dyDescent="0.35">
@@ -24001,7 +24001,7 @@
         <v>SecurityCheck</v>
       </c>
       <c r="B365" s="3" t="s">
-        <v>1947</v>
+        <v>1946</v>
       </c>
     </row>
     <row r="366" spans="1:2" x14ac:dyDescent="0.35">
@@ -24009,7 +24009,7 @@
         <v>Status403</v>
       </c>
       <c r="B366" s="3" t="s">
-        <v>2000</v>
+        <v>1999</v>
       </c>
     </row>
     <row r="367" spans="1:2" ht="29" x14ac:dyDescent="0.35">
@@ -24017,7 +24017,7 @@
         <v>Status500</v>
       </c>
       <c r="B367" s="3" t="s">
-        <v>2001</v>
+        <v>2000</v>
       </c>
     </row>
     <row r="368" spans="1:2" x14ac:dyDescent="0.35">
@@ -24025,7 +24025,7 @@
         <v>Secure</v>
       </c>
       <c r="B368" s="3" t="s">
-        <v>2002</v>
+        <v>2001</v>
       </c>
     </row>
     <row r="369" spans="1:2" x14ac:dyDescent="0.35">
@@ -24033,7 +24033,7 @@
         <v>SecureDescription</v>
       </c>
       <c r="B369" s="3" t="s">
-        <v>2003</v>
+        <v>2002</v>
       </c>
     </row>
     <row r="370" spans="1:2" ht="29" x14ac:dyDescent="0.35">
@@ -24041,7 +24041,7 @@
         <v>SecurityCheckDesc</v>
       </c>
       <c r="B370" s="3" t="s">
-        <v>2004</v>
+        <v>2003</v>
       </c>
     </row>
     <row r="371" spans="1:2" x14ac:dyDescent="0.35">
@@ -24049,7 +24049,7 @@
         <v>Contact</v>
       </c>
       <c r="B371" s="3" t="s">
-        <v>2005</v>
+        <v>2004</v>
       </c>
     </row>
     <row r="372" spans="1:2" x14ac:dyDescent="0.35">
@@ -24057,7 +24057,7 @@
         <v>GoogleCaptcha</v>
       </c>
       <c r="B372" s="3" t="s">
-        <v>1967</v>
+        <v>1966</v>
       </c>
     </row>
     <row r="373" spans="1:2" ht="116" x14ac:dyDescent="0.35">
@@ -24065,7 +24065,7 @@
         <v>GoogleCaptchaDesc</v>
       </c>
       <c r="B373" s="3" t="s">
-        <v>2006</v>
+        <v>2005</v>
       </c>
     </row>
     <row r="374" spans="1:2" x14ac:dyDescent="0.35">
@@ -24073,7 +24073,7 @@
         <v>DataCollection</v>
       </c>
       <c r="B374" s="3" t="s">
-        <v>2007</v>
+        <v>2006</v>
       </c>
     </row>
     <row r="375" spans="1:2" ht="290" x14ac:dyDescent="0.35">
@@ -24081,7 +24081,7 @@
         <v>DataCollectionDesc</v>
       </c>
       <c r="B375" s="3" t="s">
-        <v>2008</v>
+        <v>2007</v>
       </c>
     </row>
     <row r="376" spans="1:2" x14ac:dyDescent="0.35">
@@ -24089,7 +24089,7 @@
         <v>Imprint</v>
       </c>
       <c r="B376" s="3" t="s">
-        <v>2014</v>
+        <v>2013</v>
       </c>
     </row>
     <row r="377" spans="1:2" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Bugfixes Captcha added to registration form
</commit_message>
<xml_diff>
--- a/Vitae/Library/Resources/SharedResource.xlsx
+++ b/Vitae/Library/Resources/SharedResource.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\Vitae\Library\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FFC0233-337C-4F27-9EBC-4D1795FEC831}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38079A23-B47C-4AAD-8170-3065373AEF17}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="30220" windowHeight="19620" tabRatio="406" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="30220" windowHeight="19620" tabRatio="406" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="en" sheetId="3" r:id="rId1"/>
@@ -62,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2404" uniqueCount="2040">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2409" uniqueCount="2045">
   <si>
     <t>City</t>
   </si>
@@ -6182,6 +6182,21 @@
   </si>
   <si>
     <t>Cambie el color de su myVitae</t>
+  </si>
+  <si>
+    <t>Prefix</t>
+  </si>
+  <si>
+    <t>Präfix</t>
+  </si>
+  <si>
+    <t>Préfixe</t>
+  </si>
+  <si>
+    <t>Prefisso</t>
+  </si>
+  <si>
+    <t>Prefijo</t>
   </si>
 </sst>
 </file>
@@ -6570,7 +6585,7 @@
   <dimension ref="A1:B500"/>
   <sheetViews>
     <sheetView topLeftCell="A374" workbookViewId="0">
-      <selection activeCell="B383" sqref="B383"/>
+      <selection activeCell="C382" sqref="C382"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -9626,7 +9641,10 @@
     </row>
     <row r="382" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A382" s="5" t="s">
-        <v>1940</v>
+        <v>2040</v>
+      </c>
+      <c r="B382" s="3" t="s">
+        <v>2040</v>
       </c>
     </row>
     <row r="383" spans="1:2" x14ac:dyDescent="0.35">
@@ -10229,8 +10247,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B499"/>
   <sheetViews>
-    <sheetView topLeftCell="A376" workbookViewId="0">
-      <selection activeCell="B392" sqref="B392"/>
+    <sheetView topLeftCell="A373" workbookViewId="0">
+      <selection activeCell="B383" sqref="B383"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -13290,7 +13308,10 @@
     </row>
     <row r="382" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A382" s="5" t="str">
-        <v xml:space="preserve"> </v>
+        <v>Prefix</v>
+      </c>
+      <c r="B382" s="8" t="s">
+        <v>2041</v>
       </c>
     </row>
     <row r="383" spans="1:2" x14ac:dyDescent="0.35">
@@ -13889,7 +13910,7 @@
   <dimension ref="A1:B499"/>
   <sheetViews>
     <sheetView topLeftCell="A374" workbookViewId="0">
-      <selection activeCell="B382" sqref="B382"/>
+      <selection activeCell="A382" sqref="A382:B382"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -16949,7 +16970,10 @@
     </row>
     <row r="382" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A382" s="5" t="str">
-        <v xml:space="preserve"> </v>
+        <v>Prefix</v>
+      </c>
+      <c r="B382" s="3" t="s">
+        <v>2042</v>
       </c>
     </row>
     <row r="383" spans="1:2" x14ac:dyDescent="0.35">
@@ -17546,8 +17570,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{21647760-4677-48F5-BA10-2363314EC080}">
   <dimension ref="A1:B499"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A374" workbookViewId="0">
-      <selection activeCell="B381" sqref="B381"/>
+    <sheetView topLeftCell="A374" workbookViewId="0">
+      <selection activeCell="A382" sqref="A382:B382"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -20607,7 +20631,10 @@
     </row>
     <row r="382" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A382" s="5" t="str">
-        <v xml:space="preserve"> </v>
+        <v>Prefix</v>
+      </c>
+      <c r="B382" s="3" t="s">
+        <v>2043</v>
       </c>
     </row>
     <row r="383" spans="1:2" x14ac:dyDescent="0.35">
@@ -21205,8 +21232,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A8220B7-2614-4C14-91F7-8D47B2A1113F}">
   <dimension ref="A1:B499"/>
   <sheetViews>
-    <sheetView topLeftCell="A371" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B382" sqref="B382"/>
+    <sheetView tabSelected="1" topLeftCell="A371" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A382" sqref="A382:B382"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -24266,7 +24293,10 @@
     </row>
     <row r="382" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A382" s="5" t="str">
-        <v xml:space="preserve"> </v>
+        <v>Prefix</v>
+      </c>
+      <c r="B382" s="3" t="s">
+        <v>2044</v>
       </c>
     </row>
     <row r="383" spans="1:2" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
New texts added, layout bugfixes
</commit_message>
<xml_diff>
--- a/Vitae/Library/Resources/SharedResource.xlsx
+++ b/Vitae/Library/Resources/SharedResource.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\Vitae\Library\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90BDF201-E559-4828-896F-0464EB877487}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A6CB632-5AEA-4A84-B92C-46226B69A8AF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="30220" windowHeight="19620" tabRatio="406" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="30220" windowHeight="19620" tabRatio="406" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="en" sheetId="3" r:id="rId1"/>
@@ -62,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2449" uniqueCount="2094">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2464" uniqueCount="2112">
   <si>
     <t>City</t>
   </si>
@@ -5209,9 +5209,6 @@
     <t>Suma de las últimas llamadas de myVitae (las últimas 50)</t>
   </si>
   <si>
-    <t>Want to improve your curriculum vitae? No problem - with myVitae you present yourself in the best possible light. Create a free account now!</t>
-  </si>
-  <si>
     <t>Welcome to myVitae</t>
   </si>
   <si>
@@ -5236,9 +5233,6 @@
     <t>Diese E-Mail wurde von myVitae gesendet an</t>
   </si>
   <si>
-    <t>Möchten Sie Ihren Lebenslauf verbessern? Kein Problem - mit myVitae präsentieren Sie sich im bestmöglichen Licht. Erstellen Sie jetzt ein kostenloses Konto!</t>
-  </si>
-  <si>
     <t>Bienvenue à myVitae</t>
   </si>
   <si>
@@ -5251,9 +5245,6 @@
     <t>Cet e-mail a été envoyé de myVitae à</t>
   </si>
   <si>
-    <t>Vous souhaitez améliorer votre curriculum vitae ? Pas de problème - avec myVitae, vous vous présentez sous le meilleur jour possible. Créez un compte gratuit dès maintenant !</t>
-  </si>
-  <si>
     <t>Benvenuti a myVitae</t>
   </si>
   <si>
@@ -5266,9 +5257,6 @@
     <t>Questa e-mail è stata inviata da myVitae a</t>
   </si>
   <si>
-    <t>Vuoi migliorare il tuo curriculum vitae? Nessun problema - con myVitae vi presentate nella migliore luce possibile. Crea subito un account gratuito!</t>
-  </si>
-  <si>
     <t>Te deseamos mucho éxito en tu búsqueda de trabajo con myVitae... ¡mantente en el baile!</t>
   </si>
   <si>
@@ -5278,9 +5266,6 @@
     <t>Este correo electrónico fue enviado desde myVitae a</t>
   </si>
   <si>
-    <t>¿Quieres mejorar tu curriculum vitae? No hay problema, con myVitae te presentas de la mejor manera posible. Crea una cuenta gratis ahora!</t>
-  </si>
-  <si>
     <t>WhyMyVitae</t>
   </si>
   <si>
@@ -5347,99 +5332,54 @@
     <t>Always keep full control</t>
   </si>
   <si>
-    <t>The dashboard gives you a good overview of your published CVs. You can enter your resume in up to four languages.</t>
-  </si>
-  <si>
     <t>Protect your publications</t>
   </si>
   <si>
     <t>Show your strengths</t>
   </si>
   <si>
-    <t>With your myVitae website you can focus on the essentials and present yourself in the best possible light.</t>
-  </si>
-  <si>
-    <t>Creating a good CV and keeping it up to date is a very time-consuming process. Furthermore, with the design you can quickly reach your limits. However, design is not always so central for many employers. It's the content that counts and that needs to be presented clearly and concisely. This is where myVitae comes into play and focuses on clear content. With ease you can create your personal CV website.</t>
-  </si>
-  <si>
     <t>Immer die volle Kontrolle behalten</t>
   </si>
   <si>
-    <t>Das Dashboard gibt Ihnen einen guten Überblick über Ihre veröffentlichten Lebensläufe. Sie können Ihren Lebenslauf in bis zu vier Sprachen eingeben.</t>
-  </si>
-  <si>
     <t>Schützen Sie Ihre Veröffentlichungen</t>
   </si>
   <si>
-    <t>Mit Ihrer myVitae Website können Sie sich auf das Wesentliche konzentrieren und sich im bestmöglichen Licht präsentieren.</t>
-  </si>
-  <si>
     <t>Pourquoi myVitae ?</t>
   </si>
   <si>
-    <t>Créer un bon CV et le tenir à jour est un processus qui prend beaucoup de temps. De plus, avec la conception, vous pouvez rapidement atteindre vos limites. Cependant, le design n'est pas toujours aussi central pour de nombreux employeurs. C'est le contenu qui compte et qui doit être présenté de manière claire et concise. C'est là que myVitae entre en jeu et se concentre sur un contenu clair. Vous pouvez facilement créer votre site web de CV personnel.</t>
-  </si>
-  <si>
     <t>Gardez toujours le contrôle</t>
   </si>
   <si>
-    <t>Le tableau de bord vous donne un bon aperçu des CV publiés. Vous pouvez saisir votre CV dans quatre langues au maximum.</t>
-  </si>
-  <si>
     <t>Protégez vos publications</t>
   </si>
   <si>
     <t>Montrez vos points forts</t>
   </si>
   <si>
-    <t>Avec votre site web myVitae, vous pouvez vous concentrer sur l'essentiel et vous présenter sous le meilleur jour possible.</t>
-  </si>
-  <si>
     <t>Perché myVitae?</t>
   </si>
   <si>
-    <t>Creare un buon CV e mantenerlo aggiornato è un processo che richiede molto tempo. Inoltre, con il design si possono raggiungere rapidamente i propri limiti. Tuttavia, il design non è sempre così centrale per molti datori di lavoro. È il contenuto che conta e che deve essere presentato in modo chiaro e conciso. È qui che entra in gioco myVitae e si concentra su contenuti chiari. Con facilità puoi creare il tuo sito web personale per il CV.</t>
-  </si>
-  <si>
     <t>Mantenere sempre il pieno controllo</t>
   </si>
   <si>
-    <t>Il cruscotto vi offre una buona panoramica dei vostri CV pubblicati. Puoi inserire il tuo curriculum vitae in un massimo di quattro lingue.</t>
-  </si>
-  <si>
     <t>Proteggi le tue pubblicazioni</t>
   </si>
   <si>
     <t>Mostra i tuoi punti di forza</t>
   </si>
   <si>
-    <t>Con il vostro sito myVitae potete concentrarvi sull'essenziale e presentarvi nella migliore luce possibile.</t>
-  </si>
-  <si>
     <t>¿Por qué miVitae?</t>
   </si>
   <si>
-    <t>Crear un buen currículum y mantenerlo actualizado es un proceso que lleva mucho tiempo. Además, con el diseño puedes alcanzar rápidamente tus límites. Sin embargo, el diseño no siempre es tan central para muchos empleadores. Es el contenido lo que cuenta y que debe ser presentado de forma clara y concisa. Aquí es donde entra en juego myVitae y se centra en un contenido claro. Con facilidad puedes crear tu página web de currículums personales.</t>
-  </si>
-  <si>
     <t>Mantenga siempre el control total</t>
   </si>
   <si>
-    <t>El tablero de mandos te da una buena visión general de tus currículums publicados. Puedes introducir tu currículum en hasta cuatro idiomas.</t>
-  </si>
-  <si>
     <t>Proteja sus publicaciones</t>
   </si>
   <si>
     <t>Muestra tus puntos fuertes</t>
   </si>
   <si>
-    <t>Con tu página web myVitae puedes concentrarte en lo esencial y presentarte de la mejor manera posible.</t>
-  </si>
-  <si>
-    <t>Einen guten Lebenslauf zu erstellen und stets auf dem neuesten Stand zu halten, ist ein sehr zeitaufwändiger Prozess. Zudem kann man bei der Gestaltung schnell an seine Grenzen stossen. Für viele Arbeitgeber ist die Gestaltung jedoch nicht immer so zentral. Es ist der Inhalt der zählt und welcher klar und prägnant präsentiert werden muss. An dieser Stelle sprint myVitae ein und setzt auf klare Inhalte. Mit Leichtigkeit können Sie Ihre persönliche Lebenslauf-Website erstellen.</t>
-  </si>
-  <si>
     <t>Check it out - you will be thrilled!</t>
   </si>
   <si>
@@ -5932,24 +5872,9 @@
     <t>Before you proceed to the resume, please complete the captcha below.</t>
   </si>
   <si>
-    <t>Your myVitae-CV is protected by a unique link and a captcha. Additionally, assign a password and anonymise sensitive information if necessary.</t>
-  </si>
-  <si>
     <t>Additionally secure your myVitae with a captcha (blocking bots)</t>
   </si>
   <si>
-    <t>Ihr myVitae-CV ist durch einen einzigartigen Link und ein captcha geschützt. Vergeben Sie zusätzlich ein Passwort und anonymisieren Sie sensible Informationen, falls erforderlich.</t>
-  </si>
-  <si>
-    <t>Votre myVitae-CV est protégé par un lien unique et un captcha. En outre, vous devez attribuer un mot de passe et anonymiser les informations sensibles si nécessaire.</t>
-  </si>
-  <si>
-    <t>La vostra myVitae-CV è protetta da un link unico e da un captcha. Inoltre, assegnare una password e rendere anonime le informazioni sensibili, se necessario.</t>
-  </si>
-  <si>
-    <t>Su myVitae-CV está protegido por un enlace único y un captcha. Además, asigna una contraseña y anonimiza la información sensible si es necesario.</t>
-  </si>
-  <si>
     <t>Contact</t>
   </si>
   <si>
@@ -6344,6 +6269,135 @@
   </si>
   <si>
     <t>Un ordre chronologique ascendant est recommandé.</t>
+  </si>
+  <si>
+    <t>OptionalInformation</t>
+  </si>
+  <si>
+    <t>Optional information</t>
+  </si>
+  <si>
+    <t>Optionale Angaben</t>
+  </si>
+  <si>
+    <t>Informations facultatives</t>
+  </si>
+  <si>
+    <t>Informazioni facoltative</t>
+  </si>
+  <si>
+    <t>Información opcional</t>
+  </si>
+  <si>
+    <t>MyVitaeSlogan</t>
+  </si>
+  <si>
+    <t>MyVitae - Votre CV en ligne</t>
+  </si>
+  <si>
+    <t>MyVitae - Ihr online Lebenslauf</t>
+  </si>
+  <si>
+    <t>MyVitae - Your online CV</t>
+  </si>
+  <si>
+    <t>MyVitae - Il tuo CV online</t>
+  </si>
+  <si>
+    <t>MyVitae - Su CV en línea</t>
+  </si>
+  <si>
+    <t>Download QR code</t>
+  </si>
+  <si>
+    <t>DownloadQR</t>
+  </si>
+  <si>
+    <t>QR-Code herunterladen</t>
+  </si>
+  <si>
+    <t>Télécharger le code QR</t>
+  </si>
+  <si>
+    <t>Scarica il codice QR</t>
+  </si>
+  <si>
+    <t>Descargar el código QR</t>
+  </si>
+  <si>
+    <t>Would you like to improve your chances on the job market? No problem, because with myVitae you can create your personal resume website in no time at all. Create a free account now and get started!</t>
+  </si>
+  <si>
+    <t>Vous souhaitez améliorer vos chances sur le marché du travail ? Pas de problème, car avec myVitae, vous pouvez créer votre site web de CV personnel en un rien de temps. Créez un compte gratuit maintenant et commencez !</t>
+  </si>
+  <si>
+    <t>Volete migliorare le vostre possibilità sul mercato del lavoro? Nessun problema, perché con myVitae potete creare in poco tempo il vostro sito web personale per il curriculum vitae. Crea subito un account gratuito e inizia a lavorare!</t>
+  </si>
+  <si>
+    <t>¿Te gustaría mejorar tus posibilidades en el mercado laboral? No hay problema, porque con myVitae puede crear su sitio web de currículum personal en poco tiempo. Cree una cuenta gratuita ahora y empiece a trabajar!</t>
+  </si>
+  <si>
+    <t>Möchten Sie Ihre Chancen auf dem Arbeitsmarkt verbessern? Kein Problem, denn mit myVitae können Sie im Handumdrehen Ihre persönliche Lebenslauf-Website erstellen. Eröffnen Sie jetzt ein kostenloses Konto und starten Sie durch!</t>
+  </si>
+  <si>
+    <t>Creating a good CV and keeping it up to date is a very time-consuming process. In addition, you can quickly reach your limits when designing. However, an applicant has to put everything on the scales, because "there is no second chance for a first impression" (Mark Twain). This is where myVitae steps in and focuses on a clear and concise design. With ease you can create your secure personal resume website - and best of all, it's free! So nothing stands in the way of your successful application.</t>
+  </si>
+  <si>
+    <t>Einen guten Lebenslauf zu erstellen und diesen stets auf dem neuesten Stand zu halten, ist ein sehr zeitaufwändiger Prozess. Zudem kann man bei der Gestaltung schnell an seine Grenzen stossen. Ein Bewerber muss jedoch alles in eine Waagschale werfen, denn "es gibt keine zweite Chance für den ersten Eindruck" (Mark Twain). An dieser Stelle springt myVitae ein und setzt auf ein klares und übersichtliches Design. Mit Leichtigkeit können Sie Ihre persönliche passwortgeschützte Lebenslauf-Website erstellen – und dies erst noch kostenlos! Ihrer erfolgreichen Bewerbung steht also nichts mehr im Wege.</t>
+  </si>
+  <si>
+    <t>Créer un bon CV et le tenir à jour est un processus qui prend beaucoup de temps. En outre, vous pouvez rapidement atteindre vos limites lors de la conception. Cependant, un candidat doit tout mettre sur la balance, car "il n'y a pas de seconde chance pour une première impression" (Mark Twain). C'est là que myVitae intervient et se concentre sur un design clair et concis. Vous pouvez facilement créer votre site web de CV personnel - et surtout, c'est gratuit ! Ainsi, rien ne s'oppose à ce que votre candidature soit retenue.</t>
+  </si>
+  <si>
+    <t>Creare un buon CV e mantenerlo aggiornato è un processo che richiede molto tempo. Inoltre, è possibile raggiungere rapidamente i propri limiti durante la progettazione. Tuttavia, un candidato deve mettere tutto sulla bilancia, perché "non c'è una seconda possibilità per una prima impressione" (Mark Twain). È qui che myVitae interviene e si concentra su un design chiaro e conciso. Con facilità si può creare il proprio sito web di curriculum personale - e soprattutto è gratuito! Così nulla ostacola il successo della vostra applicazione.</t>
+  </si>
+  <si>
+    <t>Crear un buen currículum y mantenerlo actualizado es un proceso que lleva mucho tiempo. Además, puede llegar rápidamente a sus límites durante el proceso de diseño. Sin embargo, un candidato debe poner todo en la balanza, porque "no hay una segunda oportunidad para una primera impresión" (Mark Twain). Aquí es donde entra myVitae y se centra en un diseño claro y conciso. Puedes crear fácilmente tu propio sitio web de currículums personales, y sobre todo, ¡es gratis! Así que nada se interpone en el camino del éxito de su solicitud.</t>
+  </si>
+  <si>
+    <t>Damit Ihr Lebenslauf veröffentlicht werden kann, wird von der myVitae Webapplikation ein zufälliger Publikationslink erstellt. Diesen können Sie dann für eine oder mehrere Vakanzen verwenden und, nach erfolgreicher Bewerbung, wieder komplett löschen. Das Dashboard zeigt Ihnen dabei den Erfolgsverlauf Ihrer veröffentlichten Lebensläufe auf, in dem die Anzahl Klicks auf den versendeten Publikationslink aufgezeigt werden. Sie können Ihren Lebenslauf zudem in bis zu fünf Sprachen erfassen.</t>
+  </si>
+  <si>
+    <t>In order for your CV to be published, a random publication link is created by the myVitae web application. You can then use this link for one or more vacancies and delete it completely after you have successfully applied. The dashboard shows you the success of your published CVs by displaying the number of clicks on the sent publication link. You can also enter your resume in up to five languages.</t>
+  </si>
+  <si>
+    <t>Pour que votre CV soit publié, un lien de publication aléatoire est créé par l'application web myVitae. Vous pouvez ensuite utiliser ce lien pour un ou plusieurs postes vacants et le supprimer complètement après avoir postulé avec succès. Le tableau de bord vous indique le succès de vos CV publiés en affichant le nombre de clics sur le lien de publication envoyé. Vous pouvez également saisir votre CV dans cinq langues au maximum.</t>
+  </si>
+  <si>
+    <t>Affinché il vostro CV venga pubblicato, l'applicazione web myVitae crea un link di pubblicazione casuale. Potete quindi utilizzare questo link per uno o più posti vacanti e cancellarlo completamente dopo aver presentato la vostra candidatura con successo. Il cruscotto mostra il successo dei vostri CV pubblicati visualizzando il numero di clic sul link di pubblicazione inviato. Potete anche inserire il vostro curriculum vitae in un massimo di cinque lingue.</t>
+  </si>
+  <si>
+    <t>Para que su CV sea publicado, la aplicación web myVitae crea un enlace de publicación aleatorio. A continuación, puedes utilizar este enlace para una o más vacantes y eliminarlo completamente después de haber presentado tu solicitud con éxito. El panel de control le muestra el éxito de sus CVs publicados mostrando el número de clics en el enlace de publicación enviado. También puedes introducir tu currículum en un máximo de cinco idiomas.</t>
+  </si>
+  <si>
+    <t>Der Publikationslink ist anfänglich nur Ihnen bekannt und kann zusätzlich mit einem Passwort geschützt werden. Ausserdem kann mit einem Google Catcha ein weiterer Zusatzschutz gegen Bots eingesetzt werden. Für Blindbewerbungen eignet sich ausserdem die Anonymisierungsfunktion, welche einige sensible Informationen ausblendet.</t>
+  </si>
+  <si>
+    <t>The publication link is initially known only to you and can also be protected with a password. Furthermore, a Google Catcha can be used to provide additional protection against bots. For blind applications, the anonymization function, which hides some sensitive information, is also suitable.</t>
+  </si>
+  <si>
+    <t>Le lien de publication est initialement connu de vous seul et peut également être protégé par un mot de passe. En outre, un Google Catcha peut être utilisé pour fournir une protection supplémentaire contre les robots. Pour les applications en aveugle, la fonction d'anonymisation, qui permet de cacher certaines informations sensibles, est également adaptée.</t>
+  </si>
+  <si>
+    <t>Il link della pubblicazione è inizialmente noto solo a voi e può essere protetto anche con una password. Inoltre, un Google Catcha può essere utilizzato per fornire una protezione aggiuntiva contro i bot. Per le applicazioni cieche è adatta anche la funzione di anonimizzazione, che nasconde alcune informazioni sensibili.</t>
+  </si>
+  <si>
+    <t>El enlace de publicación es conocido inicialmente sólo por usted y también puede ser protegido con una contraseña. Además, un Google Catcha puede ser usado para proveer protección adicional contra los bots. Para aplicaciones ciegas, la función de anonimización, que oculta alguna información sensible, también es adecuada.</t>
+  </si>
+  <si>
+    <t>Mit Ihrer persönlichen Lebenslauf-Webseite halten Sie Ihre Daten stets aktuell und können sich mit ein paar wenigen Klicks auf die nächste Stelle bewerben. Dabei können Sie sich von Anfang an auf Wesentliche konzentrieren und sich im bestmöglichen Licht präsentieren. Der neuen Traumstelle steht also nichts mehr im Weg. Wir wünschen viel Erfolg!</t>
+  </si>
+  <si>
+    <t>With your personal CV website you can keep your data up to date and apply for the next job with just a few clicks. You can focus on the essentials from the very beginning and present yourself in the best possible light. So nothing stands in the way of your new dream job. We wish you much success!</t>
+  </si>
+  <si>
+    <t>Grâce à votre site web de CV personnel, vous pouvez tenir vos données à jour et postuler pour le prochain emploi en quelques clics. Vous pouvez vous concentrer sur l'essentiel dès le début et vous présenter sous le meilleur jour possible. Ainsi, rien ne s'oppose à votre nouvel emploi de rêve. Nous vous souhaitons beaucoup de succès !</t>
+  </si>
+  <si>
+    <t>Con il tuo sito web personale di CV puoi tenere aggiornati i tuoi dati e candidarti per il prossimo lavoro con pochi click. Puoi concentrarti sull'essenziale fin dall'inizio e presentarti nella migliore luce possibile. Così nulla ostacola il vostro nuovo lavoro dei sogni. Vi auguriamo un grande successo!</t>
+  </si>
+  <si>
+    <t>Con tu página web de currículums personales puedes mantener tus datos actualizados y solicitar el siguiente trabajo con sólo unos pocos clics. Puedes concentrarte en lo esencial desde el principio y presentarte de la mejor manera posible. Así que nada se interpone en el camino de tu nuevo trabajo soñado. Le deseamos mucho éxito!</t>
   </si>
 </sst>
 </file>
@@ -6731,8 +6785,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B499"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A377" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A391" sqref="A391:XFD391"/>
+    <sheetView topLeftCell="A287" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A287" sqref="A1:B1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -6823,10 +6877,10 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" s="5" t="s">
-        <v>1888</v>
+        <v>1868</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>1889</v>
+        <v>1869</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.35">
@@ -6885,12 +6939,12 @@
         <v>583</v>
       </c>
     </row>
-    <row r="19" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:2" ht="58" x14ac:dyDescent="0.35">
       <c r="A19" s="6" t="s">
         <v>581</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>1715</v>
+        <v>2087</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.35">
@@ -7079,10 +7133,10 @@
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A43" s="5" t="s">
-        <v>1749</v>
+        <v>1744</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>1751</v>
+        <v>1746</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.35">
@@ -7191,10 +7245,10 @@
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A57" s="5" t="s">
-        <v>1896</v>
+        <v>1876</v>
       </c>
       <c r="B57" s="3" t="s">
-        <v>1897</v>
+        <v>1877</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.35">
@@ -7290,12 +7344,12 @@
         <v>692</v>
       </c>
       <c r="B69" s="3" t="s">
-        <v>1805</v>
+        <v>1785</v>
       </c>
     </row>
     <row r="70" spans="1:2" ht="29" x14ac:dyDescent="0.35">
       <c r="A70" s="5" t="s">
-        <v>1804</v>
+        <v>1784</v>
       </c>
       <c r="B70" s="9" t="s">
         <v>696</v>
@@ -7311,26 +7365,26 @@
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A72" s="5" t="s">
-        <v>1835</v>
+        <v>1815</v>
       </c>
       <c r="B72" s="3" t="s">
-        <v>1835</v>
+        <v>1815</v>
       </c>
     </row>
     <row r="73" spans="1:2" ht="87" x14ac:dyDescent="0.35">
       <c r="A73" s="5" t="s">
-        <v>1836</v>
+        <v>1816</v>
       </c>
       <c r="B73" s="8" t="s">
-        <v>1921</v>
+        <v>1901</v>
       </c>
     </row>
     <row r="74" spans="1:2" ht="116" x14ac:dyDescent="0.35">
       <c r="A74" s="5" t="s">
-        <v>1838</v>
+        <v>1818</v>
       </c>
       <c r="B74" s="8" t="s">
-        <v>1847</v>
+        <v>1827</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.35">
@@ -7343,26 +7397,26 @@
     </row>
     <row r="76" spans="1:2" ht="29" x14ac:dyDescent="0.35">
       <c r="A76" s="5" t="s">
-        <v>1833</v>
+        <v>1813</v>
       </c>
       <c r="B76" s="3" t="s">
-        <v>1834</v>
+        <v>1814</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A77" s="5" t="s">
-        <v>1850</v>
+        <v>1830</v>
       </c>
       <c r="B77" s="3" t="s">
-        <v>1833</v>
+        <v>1813</v>
       </c>
     </row>
     <row r="78" spans="1:2" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A78" s="5" t="s">
-        <v>1853</v>
+        <v>1833</v>
       </c>
       <c r="B78" s="3" t="s">
-        <v>1855</v>
+        <v>1835</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.35">
@@ -7458,7 +7512,7 @@
         <v>95</v>
       </c>
       <c r="B90" s="2" t="s">
-        <v>1747</v>
+        <v>1742</v>
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.35">
@@ -7493,28 +7547,28 @@
         <v>1673</v>
       </c>
     </row>
-    <row r="95" spans="1:2" ht="29" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:2" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A95" s="5" t="s">
-        <v>1744</v>
+        <v>1739</v>
       </c>
       <c r="B95" s="8" t="s">
-        <v>1761</v>
+        <v>2098</v>
       </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A96" s="5" t="s">
-        <v>1820</v>
+        <v>1800</v>
       </c>
       <c r="B96" s="3" t="s">
-        <v>1821</v>
+        <v>1801</v>
       </c>
     </row>
     <row r="97" spans="1:2" ht="130.5" x14ac:dyDescent="0.35">
       <c r="A97" s="5" t="s">
-        <v>1829</v>
+        <v>1809</v>
       </c>
       <c r="B97" s="3" t="s">
-        <v>1827</v>
+        <v>1807</v>
       </c>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.35">
@@ -7527,10 +7581,10 @@
     </row>
     <row r="99" spans="1:2" ht="130.5" x14ac:dyDescent="0.35">
       <c r="A99" s="5" t="s">
-        <v>1825</v>
+        <v>1805</v>
       </c>
       <c r="B99" s="3" t="s">
-        <v>1827</v>
+        <v>1807</v>
       </c>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.35">
@@ -7591,18 +7645,18 @@
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A107" s="5" t="s">
-        <v>1797</v>
+        <v>1777</v>
       </c>
       <c r="B107" s="5" t="s">
-        <v>1797</v>
+        <v>1777</v>
       </c>
     </row>
     <row r="108" spans="1:2" ht="246.5" x14ac:dyDescent="0.35">
       <c r="A108" s="5" t="s">
-        <v>1814</v>
+        <v>1794</v>
       </c>
       <c r="B108" s="3" t="s">
-        <v>1815</v>
+        <v>1795</v>
       </c>
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.35">
@@ -7887,34 +7941,34 @@
     </row>
     <row r="144" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A144" s="5" t="s">
-        <v>1902</v>
+        <v>1882</v>
       </c>
       <c r="B144" s="3" t="s">
-        <v>1902</v>
+        <v>1882</v>
       </c>
     </row>
     <row r="145" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A145" s="5" t="s">
-        <v>1840</v>
+        <v>1820</v>
       </c>
       <c r="B145" s="5" t="s">
-        <v>1839</v>
+        <v>1819</v>
       </c>
     </row>
     <row r="146" spans="1:2" ht="232" x14ac:dyDescent="0.35">
       <c r="A146" s="5" t="s">
-        <v>1842</v>
+        <v>1822</v>
       </c>
       <c r="B146" s="3" t="s">
-        <v>1845</v>
+        <v>1825</v>
       </c>
     </row>
     <row r="147" spans="1:2" ht="116" x14ac:dyDescent="0.35">
       <c r="A147" s="5" t="s">
-        <v>1843</v>
+        <v>1823</v>
       </c>
       <c r="B147" s="3" t="s">
-        <v>1846</v>
+        <v>1826</v>
       </c>
     </row>
     <row r="148" spans="1:2" x14ac:dyDescent="0.35">
@@ -8103,10 +8157,10 @@
     </row>
     <row r="171" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A171" s="5" t="s">
-        <v>1743</v>
+        <v>1738</v>
       </c>
       <c r="B171" s="8" t="s">
-        <v>1760</v>
+        <v>1755</v>
       </c>
     </row>
     <row r="172" spans="1:2" x14ac:dyDescent="0.35">
@@ -8191,18 +8245,18 @@
     </row>
     <row r="182" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A182" s="5" t="s">
-        <v>1802</v>
+        <v>1782</v>
       </c>
       <c r="B182" s="3" t="s">
-        <v>1803</v>
+        <v>1783</v>
       </c>
     </row>
     <row r="183" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A183" s="5" t="s">
-        <v>1848</v>
+        <v>1828</v>
       </c>
       <c r="B183" s="3" t="s">
-        <v>1854</v>
+        <v>1834</v>
       </c>
     </row>
     <row r="184" spans="1:2" x14ac:dyDescent="0.35">
@@ -8338,7 +8392,7 @@
         <v>1612</v>
       </c>
       <c r="B200" s="3" t="s">
-        <v>1717</v>
+        <v>1716</v>
       </c>
     </row>
     <row r="201" spans="1:2" x14ac:dyDescent="0.35">
@@ -8346,7 +8400,7 @@
         <v>1618</v>
       </c>
       <c r="B201" s="3" t="s">
-        <v>1718</v>
+        <v>1717</v>
       </c>
     </row>
     <row r="202" spans="1:2" x14ac:dyDescent="0.35">
@@ -8359,10 +8413,10 @@
     </row>
     <row r="203" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A203" s="5" t="s">
-        <v>1885</v>
+        <v>1865</v>
       </c>
       <c r="B203" s="3" t="s">
-        <v>2011</v>
+        <v>1986</v>
       </c>
     </row>
     <row r="204" spans="1:2" x14ac:dyDescent="0.35">
@@ -8370,7 +8424,7 @@
         <v>1620</v>
       </c>
       <c r="B204" s="3" t="s">
-        <v>1719</v>
+        <v>1718</v>
       </c>
     </row>
     <row r="205" spans="1:2" ht="29" x14ac:dyDescent="0.35">
@@ -9071,18 +9125,18 @@
     </row>
     <row r="292" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A292" s="5" t="s">
-        <v>1745</v>
+        <v>1740</v>
       </c>
       <c r="B292" s="8" t="s">
-        <v>1762</v>
-      </c>
-    </row>
-    <row r="293" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
+        <v>1756</v>
+      </c>
+    </row>
+    <row r="293" spans="1:2" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A293" s="5" t="s">
-        <v>1755</v>
+        <v>1750</v>
       </c>
       <c r="B293" s="8" t="s">
-        <v>1956</v>
+        <v>2103</v>
       </c>
     </row>
     <row r="294" spans="1:2" x14ac:dyDescent="0.35">
@@ -9159,18 +9213,18 @@
     </row>
     <row r="303" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A303" s="5" t="s">
-        <v>1756</v>
+        <v>1751</v>
       </c>
       <c r="B303" s="8" t="s">
-        <v>1763</v>
-      </c>
-    </row>
-    <row r="304" spans="1:2" ht="29" x14ac:dyDescent="0.35">
+        <v>1757</v>
+      </c>
+    </row>
+    <row r="304" spans="1:2" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A304" s="5" t="s">
-        <v>1758</v>
+        <v>1753</v>
       </c>
       <c r="B304" s="8" t="s">
-        <v>1764</v>
+        <v>2108</v>
       </c>
     </row>
     <row r="305" spans="1:2" x14ac:dyDescent="0.35">
@@ -9298,7 +9352,7 @@
         <v>716</v>
       </c>
       <c r="B320" s="3" t="s">
-        <v>1952</v>
+        <v>1932</v>
       </c>
     </row>
     <row r="321" spans="1:2" x14ac:dyDescent="0.35">
@@ -9351,10 +9405,10 @@
     </row>
     <row r="327" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A327" s="5" t="s">
-        <v>1880</v>
+        <v>1860</v>
       </c>
       <c r="B327" s="3" t="s">
-        <v>1880</v>
+        <v>1860</v>
       </c>
     </row>
     <row r="328" spans="1:2" x14ac:dyDescent="0.35">
@@ -9522,31 +9576,31 @@
         <v>380</v>
       </c>
       <c r="B348" s="2" t="s">
-        <v>1716</v>
+        <v>1715</v>
       </c>
     </row>
     <row r="349" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A349" s="5" t="s">
-        <v>1739</v>
+        <v>1734</v>
       </c>
       <c r="B349" s="8" t="s">
-        <v>1759</v>
-      </c>
-    </row>
-    <row r="350" spans="1:2" ht="101.5" x14ac:dyDescent="0.35">
+        <v>1754</v>
+      </c>
+    </row>
+    <row r="350" spans="1:2" ht="116" x14ac:dyDescent="0.35">
       <c r="A350" s="5" t="s">
-        <v>1741</v>
+        <v>1736</v>
       </c>
       <c r="B350" s="8" t="s">
-        <v>1765</v>
+        <v>2092</v>
       </c>
     </row>
     <row r="351" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A351" s="5" t="s">
-        <v>1742</v>
+        <v>1737</v>
       </c>
       <c r="B351" s="8" t="s">
-        <v>1792</v>
+        <v>1772</v>
       </c>
     </row>
     <row r="352" spans="1:2" x14ac:dyDescent="0.35">
@@ -9607,803 +9661,812 @@
     </row>
     <row r="359" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A359" s="5" t="s">
-        <v>1907</v>
+        <v>1887</v>
       </c>
       <c r="B359" s="3" t="s">
-        <v>1907</v>
+        <v>1887</v>
       </c>
     </row>
     <row r="360" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A360" s="5" t="s">
-        <v>1913</v>
+        <v>1893</v>
       </c>
       <c r="B360" s="3" t="s">
-        <v>1913</v>
+        <v>1893</v>
       </c>
     </row>
     <row r="361" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A361" s="5" t="s">
-        <v>1917</v>
+        <v>1897</v>
       </c>
       <c r="B361" s="3" t="s">
-        <v>1917</v>
+        <v>1897</v>
       </c>
     </row>
     <row r="362" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A362" s="5" t="s">
-        <v>1924</v>
+        <v>1904</v>
       </c>
       <c r="B362" s="3" t="s">
-        <v>1924</v>
+        <v>1904</v>
       </c>
     </row>
     <row r="363" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A363" s="5" t="s">
-        <v>1926</v>
+        <v>1906</v>
       </c>
       <c r="B363" s="3" t="s">
-        <v>1926</v>
+        <v>1906</v>
       </c>
     </row>
     <row r="364" spans="1:2" ht="29" x14ac:dyDescent="0.35">
       <c r="A364" s="5" t="s">
-        <v>1934</v>
+        <v>1914</v>
       </c>
       <c r="B364" s="8" t="s">
-        <v>1946</v>
+        <v>1926</v>
       </c>
     </row>
     <row r="365" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A365" s="5" t="s">
-        <v>1939</v>
+        <v>1919</v>
       </c>
       <c r="B365" s="3" t="s">
-        <v>1940</v>
+        <v>1920</v>
       </c>
     </row>
     <row r="366" spans="1:2" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A366" s="5" t="s">
-        <v>1948</v>
+        <v>1928</v>
       </c>
       <c r="B366" s="3" t="s">
-        <v>1951</v>
+        <v>1931</v>
       </c>
     </row>
     <row r="367" spans="1:2" ht="29" x14ac:dyDescent="0.35">
       <c r="A367" s="5" t="s">
-        <v>1949</v>
+        <v>1929</v>
       </c>
       <c r="B367" s="3" t="s">
-        <v>1950</v>
+        <v>1930</v>
       </c>
     </row>
     <row r="368" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A368" s="5" t="s">
-        <v>1953</v>
+        <v>1933</v>
       </c>
       <c r="B368" s="3" t="s">
-        <v>1953</v>
+        <v>1933</v>
       </c>
     </row>
     <row r="369" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A369" s="5" t="s">
-        <v>1954</v>
+        <v>1934</v>
       </c>
       <c r="B369" s="3" t="s">
-        <v>1957</v>
+        <v>1936</v>
       </c>
     </row>
     <row r="370" spans="1:2" ht="29" x14ac:dyDescent="0.35">
       <c r="A370" s="5" t="s">
-        <v>1945</v>
+        <v>1925</v>
       </c>
       <c r="B370" s="3" t="s">
-        <v>1955</v>
+        <v>1935</v>
       </c>
     </row>
     <row r="371" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A371" s="5" t="s">
-        <v>1962</v>
+        <v>1937</v>
       </c>
       <c r="B371" s="3" t="s">
-        <v>1962</v>
+        <v>1937</v>
       </c>
     </row>
     <row r="372" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A372" s="5" t="s">
-        <v>1963</v>
+        <v>1938</v>
       </c>
       <c r="B372" s="3" t="s">
-        <v>1964</v>
+        <v>1939</v>
       </c>
     </row>
     <row r="373" spans="1:2" ht="116" x14ac:dyDescent="0.35">
       <c r="A373" s="5" t="s">
-        <v>1965</v>
+        <v>1940</v>
       </c>
       <c r="B373" s="3" t="s">
-        <v>1966</v>
+        <v>1941</v>
       </c>
     </row>
     <row r="374" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A374" s="5" t="s">
-        <v>2081</v>
+        <v>2056</v>
       </c>
       <c r="B374" s="3" t="s">
-        <v>1967</v>
+        <v>1942</v>
       </c>
     </row>
     <row r="375" spans="1:2" ht="261" x14ac:dyDescent="0.35">
       <c r="A375" s="5" t="s">
-        <v>1968</v>
+        <v>1943</v>
       </c>
       <c r="B375" s="3" t="s">
-        <v>1969</v>
+        <v>1944</v>
       </c>
     </row>
     <row r="376" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A376" s="5" t="s">
-        <v>2006</v>
+        <v>1981</v>
       </c>
       <c r="B376" s="3" t="s">
-        <v>2006</v>
+        <v>1981</v>
       </c>
     </row>
     <row r="377" spans="1:2" ht="29" x14ac:dyDescent="0.35">
       <c r="A377" s="5" t="s">
-        <v>2017</v>
+        <v>1992</v>
       </c>
       <c r="B377" s="3" t="s">
-        <v>2012</v>
+        <v>1987</v>
       </c>
     </row>
     <row r="378" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A378" s="5" t="s">
-        <v>2018</v>
+        <v>1993</v>
       </c>
       <c r="B378" s="3" t="s">
-        <v>2018</v>
+        <v>1993</v>
       </c>
     </row>
     <row r="379" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A379" s="5" t="s">
-        <v>2023</v>
+        <v>1998</v>
       </c>
       <c r="B379" s="3" t="s">
-        <v>2023</v>
+        <v>1998</v>
       </c>
     </row>
     <row r="380" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A380" s="5" t="s">
-        <v>2028</v>
+        <v>2003</v>
       </c>
       <c r="B380" s="3" t="s">
-        <v>2028</v>
+        <v>2003</v>
       </c>
     </row>
     <row r="381" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A381" s="5" t="s">
-        <v>2032</v>
+        <v>2007</v>
       </c>
       <c r="B381" s="3" t="s">
-        <v>2033</v>
+        <v>2008</v>
       </c>
     </row>
     <row r="382" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A382" s="5" t="s">
-        <v>2038</v>
+        <v>2013</v>
       </c>
       <c r="B382" s="3" t="s">
-        <v>2038</v>
+        <v>2013</v>
       </c>
     </row>
     <row r="383" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A383" s="5" t="s">
-        <v>2045</v>
+        <v>2020</v>
       </c>
       <c r="B383" s="3" t="s">
-        <v>2046</v>
+        <v>2021</v>
       </c>
     </row>
     <row r="384" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A384" s="5" t="s">
-        <v>2047</v>
+        <v>2022</v>
       </c>
       <c r="B384" s="3" t="s">
-        <v>2048</v>
+        <v>2023</v>
       </c>
     </row>
     <row r="385" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A385" s="5" t="s">
-        <v>2049</v>
+        <v>2024</v>
       </c>
       <c r="B385" s="3" t="s">
-        <v>2056</v>
+        <v>2031</v>
       </c>
     </row>
     <row r="386" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A386" s="5" t="s">
-        <v>2050</v>
+        <v>2025</v>
       </c>
       <c r="B386" s="3" t="s">
-        <v>2051</v>
+        <v>2026</v>
       </c>
     </row>
     <row r="387" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A387" s="5" t="s">
-        <v>2052</v>
+        <v>2027</v>
       </c>
       <c r="B387" s="3" t="s">
-        <v>2053</v>
+        <v>2028</v>
       </c>
     </row>
     <row r="388" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A388" s="5" t="s">
-        <v>2054</v>
+        <v>2029</v>
       </c>
       <c r="B388" s="3" t="s">
-        <v>2055</v>
+        <v>2030</v>
       </c>
     </row>
     <row r="389" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A389" s="5" t="s">
-        <v>2082</v>
+        <v>2057</v>
       </c>
       <c r="B389" s="3" t="s">
-        <v>2084</v>
+        <v>2059</v>
       </c>
     </row>
     <row r="390" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A390" s="5" t="s">
-        <v>2083</v>
+        <v>2058</v>
       </c>
       <c r="B390" s="3" t="s">
-        <v>2085</v>
+        <v>2060</v>
       </c>
     </row>
     <row r="391" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A391" s="5" t="s">
-        <v>1938</v>
-      </c>
-    </row>
-    <row r="392" spans="1:2" x14ac:dyDescent="0.35">
+        <v>2069</v>
+      </c>
+      <c r="B391" s="3" t="s">
+        <v>2070</v>
+      </c>
+    </row>
+    <row r="392" spans="1:2" ht="14" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A392" s="5" t="s">
-        <v>1938</v>
+        <v>2075</v>
+      </c>
+      <c r="B392" s="3" t="s">
+        <v>2078</v>
       </c>
     </row>
     <row r="393" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A393" s="5" t="s">
-        <v>1938</v>
+        <v>2082</v>
+      </c>
+      <c r="B393" s="3" t="s">
+        <v>2081</v>
       </c>
     </row>
     <row r="394" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A394" s="5" t="s">
-        <v>1938</v>
+        <v>1918</v>
       </c>
     </row>
     <row r="395" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A395" s="5" t="s">
-        <v>1938</v>
+        <v>1918</v>
       </c>
     </row>
     <row r="396" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A396" s="5" t="s">
-        <v>1938</v>
+        <v>1918</v>
       </c>
     </row>
     <row r="397" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A397" s="5" t="s">
-        <v>1938</v>
+        <v>1918</v>
       </c>
     </row>
     <row r="398" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A398" s="5" t="s">
-        <v>1938</v>
+        <v>1918</v>
       </c>
     </row>
     <row r="399" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A399" s="5" t="s">
-        <v>1938</v>
+        <v>1918</v>
       </c>
     </row>
     <row r="400" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A400" s="5" t="s">
-        <v>1938</v>
+        <v>1918</v>
       </c>
     </row>
     <row r="401" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A401" s="5" t="s">
-        <v>1938</v>
+        <v>1918</v>
       </c>
     </row>
     <row r="402" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A402" s="5" t="s">
-        <v>1938</v>
+        <v>1918</v>
       </c>
     </row>
     <row r="403" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A403" s="5" t="s">
-        <v>1938</v>
+        <v>1918</v>
       </c>
     </row>
     <row r="404" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A404" s="5" t="s">
-        <v>1938</v>
+        <v>1918</v>
       </c>
     </row>
     <row r="405" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A405" s="5" t="s">
-        <v>1938</v>
+        <v>1918</v>
       </c>
     </row>
     <row r="406" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A406" s="5" t="s">
-        <v>1938</v>
+        <v>1918</v>
       </c>
     </row>
     <row r="407" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A407" s="5" t="s">
-        <v>1938</v>
+        <v>1918</v>
       </c>
     </row>
     <row r="408" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A408" s="5" t="s">
-        <v>1938</v>
+        <v>1918</v>
       </c>
     </row>
     <row r="409" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A409" s="5" t="s">
-        <v>1938</v>
+        <v>1918</v>
       </c>
     </row>
     <row r="410" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A410" s="5" t="s">
-        <v>1938</v>
+        <v>1918</v>
       </c>
     </row>
     <row r="411" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A411" s="5" t="s">
-        <v>1938</v>
+        <v>1918</v>
       </c>
     </row>
     <row r="412" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A412" s="5" t="s">
-        <v>1938</v>
+        <v>1918</v>
       </c>
     </row>
     <row r="413" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A413" s="5" t="s">
-        <v>1938</v>
+        <v>1918</v>
       </c>
     </row>
     <row r="414" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A414" s="5" t="s">
-        <v>1938</v>
+        <v>1918</v>
       </c>
     </row>
     <row r="415" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A415" s="5" t="s">
-        <v>1938</v>
+        <v>1918</v>
       </c>
     </row>
     <row r="416" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A416" s="5" t="s">
-        <v>1938</v>
+        <v>1918</v>
       </c>
     </row>
     <row r="417" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A417" s="5" t="s">
-        <v>1938</v>
+        <v>1918</v>
       </c>
     </row>
     <row r="418" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A418" s="5" t="s">
-        <v>1938</v>
+        <v>1918</v>
       </c>
     </row>
     <row r="419" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A419" s="5" t="s">
-        <v>1938</v>
+        <v>1918</v>
       </c>
     </row>
     <row r="420" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A420" s="5" t="s">
-        <v>1938</v>
+        <v>1918</v>
       </c>
     </row>
     <row r="421" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A421" s="5" t="s">
-        <v>1938</v>
+        <v>1918</v>
       </c>
     </row>
     <row r="422" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A422" s="5" t="s">
-        <v>1938</v>
+        <v>1918</v>
       </c>
     </row>
     <row r="423" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A423" s="5" t="s">
-        <v>1938</v>
+        <v>1918</v>
       </c>
     </row>
     <row r="424" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A424" s="5" t="s">
-        <v>1938</v>
+        <v>1918</v>
       </c>
     </row>
     <row r="425" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A425" s="5" t="s">
-        <v>1938</v>
+        <v>1918</v>
       </c>
     </row>
     <row r="426" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A426" s="5" t="s">
-        <v>1938</v>
+        <v>1918</v>
       </c>
     </row>
     <row r="427" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A427" s="5" t="s">
-        <v>1938</v>
+        <v>1918</v>
       </c>
     </row>
     <row r="428" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A428" s="5" t="s">
-        <v>1938</v>
+        <v>1918</v>
       </c>
     </row>
     <row r="429" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A429" s="5" t="s">
-        <v>1938</v>
+        <v>1918</v>
       </c>
     </row>
     <row r="430" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A430" s="5" t="s">
-        <v>1938</v>
+        <v>1918</v>
       </c>
     </row>
     <row r="431" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A431" s="5" t="s">
-        <v>1938</v>
+        <v>1918</v>
       </c>
     </row>
     <row r="432" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A432" s="5" t="s">
-        <v>1938</v>
+        <v>1918</v>
       </c>
     </row>
     <row r="433" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A433" s="5" t="s">
-        <v>1938</v>
+        <v>1918</v>
       </c>
     </row>
     <row r="434" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A434" s="5" t="s">
-        <v>1938</v>
+        <v>1918</v>
       </c>
     </row>
     <row r="435" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A435" s="5" t="s">
-        <v>1938</v>
+        <v>1918</v>
       </c>
     </row>
     <row r="436" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A436" s="5" t="s">
-        <v>1938</v>
+        <v>1918</v>
       </c>
     </row>
     <row r="437" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A437" s="5" t="s">
-        <v>1938</v>
+        <v>1918</v>
       </c>
     </row>
     <row r="438" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A438" s="5" t="s">
-        <v>1938</v>
+        <v>1918</v>
       </c>
     </row>
     <row r="439" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A439" s="5" t="s">
-        <v>1938</v>
+        <v>1918</v>
       </c>
     </row>
     <row r="440" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A440" s="5" t="s">
-        <v>1938</v>
+        <v>1918</v>
       </c>
     </row>
     <row r="441" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A441" s="5" t="s">
-        <v>1938</v>
+        <v>1918</v>
       </c>
     </row>
     <row r="442" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A442" s="5" t="s">
-        <v>1938</v>
+        <v>1918</v>
       </c>
     </row>
     <row r="443" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A443" s="5" t="s">
-        <v>1938</v>
+        <v>1918</v>
       </c>
     </row>
     <row r="444" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A444" s="5" t="s">
-        <v>1938</v>
+        <v>1918</v>
       </c>
     </row>
     <row r="445" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A445" s="5" t="s">
-        <v>1938</v>
+        <v>1918</v>
       </c>
     </row>
     <row r="446" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A446" s="5" t="s">
-        <v>1938</v>
+        <v>1918</v>
       </c>
     </row>
     <row r="447" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A447" s="5" t="s">
-        <v>1938</v>
+        <v>1918</v>
       </c>
     </row>
     <row r="448" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A448" s="5" t="s">
-        <v>1938</v>
+        <v>1918</v>
       </c>
     </row>
     <row r="449" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A449" s="5" t="s">
-        <v>1938</v>
+        <v>1918</v>
       </c>
     </row>
     <row r="450" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A450" s="5" t="s">
-        <v>1938</v>
+        <v>1918</v>
       </c>
     </row>
     <row r="451" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A451" s="5" t="s">
-        <v>1938</v>
+        <v>1918</v>
       </c>
     </row>
     <row r="452" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A452" s="5" t="s">
-        <v>1938</v>
+        <v>1918</v>
       </c>
     </row>
     <row r="453" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A453" s="5" t="s">
-        <v>1938</v>
+        <v>1918</v>
       </c>
     </row>
     <row r="454" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A454" s="5" t="s">
-        <v>1938</v>
+        <v>1918</v>
       </c>
     </row>
     <row r="455" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A455" s="5" t="s">
-        <v>1938</v>
+        <v>1918</v>
       </c>
     </row>
     <row r="456" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A456" s="5" t="s">
-        <v>1938</v>
+        <v>1918</v>
       </c>
     </row>
     <row r="457" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A457" s="5" t="s">
-        <v>1938</v>
+        <v>1918</v>
       </c>
     </row>
     <row r="458" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A458" s="5" t="s">
-        <v>1938</v>
+        <v>1918</v>
       </c>
     </row>
     <row r="459" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A459" s="5" t="s">
-        <v>1938</v>
+        <v>1918</v>
       </c>
     </row>
     <row r="460" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A460" s="5" t="s">
-        <v>1938</v>
+        <v>1918</v>
       </c>
     </row>
     <row r="461" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A461" s="5" t="s">
-        <v>1938</v>
+        <v>1918</v>
       </c>
     </row>
     <row r="462" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A462" s="5" t="s">
-        <v>1938</v>
+        <v>1918</v>
       </c>
     </row>
     <row r="463" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A463" s="5" t="s">
-        <v>1938</v>
+        <v>1918</v>
       </c>
     </row>
     <row r="464" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A464" s="5" t="s">
-        <v>1938</v>
+        <v>1918</v>
       </c>
     </row>
     <row r="465" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A465" s="5" t="s">
-        <v>1938</v>
+        <v>1918</v>
       </c>
     </row>
     <row r="466" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A466" s="5" t="s">
-        <v>1938</v>
+        <v>1918</v>
       </c>
     </row>
     <row r="467" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A467" s="5" t="s">
-        <v>1938</v>
+        <v>1918</v>
       </c>
     </row>
     <row r="468" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A468" s="5" t="s">
-        <v>1938</v>
+        <v>1918</v>
       </c>
     </row>
     <row r="469" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A469" s="5" t="s">
-        <v>1938</v>
+        <v>1918</v>
       </c>
     </row>
     <row r="470" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A470" s="5" t="s">
-        <v>1938</v>
+        <v>1918</v>
       </c>
     </row>
     <row r="471" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A471" s="5" t="s">
-        <v>1938</v>
+        <v>1918</v>
       </c>
     </row>
     <row r="472" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A472" s="5" t="s">
-        <v>1938</v>
+        <v>1918</v>
       </c>
     </row>
     <row r="473" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A473" s="5" t="s">
-        <v>1938</v>
+        <v>1918</v>
       </c>
     </row>
     <row r="474" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A474" s="5" t="s">
-        <v>1938</v>
+        <v>1918</v>
       </c>
     </row>
     <row r="475" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A475" s="5" t="s">
-        <v>1938</v>
+        <v>1918</v>
       </c>
     </row>
     <row r="476" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A476" s="5" t="s">
-        <v>1938</v>
+        <v>1918</v>
       </c>
     </row>
     <row r="477" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A477" s="5" t="s">
-        <v>1938</v>
+        <v>1918</v>
       </c>
     </row>
     <row r="478" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A478" s="5" t="s">
-        <v>1938</v>
+        <v>1918</v>
       </c>
     </row>
     <row r="479" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A479" s="5" t="s">
-        <v>1938</v>
+        <v>1918</v>
       </c>
     </row>
     <row r="480" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A480" s="5" t="s">
-        <v>1938</v>
+        <v>1918</v>
       </c>
     </row>
     <row r="481" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A481" s="5" t="s">
-        <v>1938</v>
+        <v>1918</v>
       </c>
     </row>
     <row r="482" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A482" s="5" t="s">
-        <v>1938</v>
+        <v>1918</v>
       </c>
     </row>
     <row r="483" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A483" s="5" t="s">
-        <v>1938</v>
+        <v>1918</v>
       </c>
     </row>
     <row r="484" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A484" s="5" t="s">
-        <v>1938</v>
+        <v>1918</v>
       </c>
     </row>
     <row r="485" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A485" s="5" t="s">
-        <v>1938</v>
+        <v>1918</v>
       </c>
     </row>
     <row r="486" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A486" s="5" t="s">
-        <v>1938</v>
+        <v>1918</v>
       </c>
     </row>
     <row r="487" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A487" s="5" t="s">
-        <v>1938</v>
+        <v>1918</v>
       </c>
     </row>
     <row r="488" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A488" s="5" t="s">
-        <v>1938</v>
+        <v>1918</v>
       </c>
     </row>
     <row r="489" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A489" s="5" t="s">
-        <v>1938</v>
+        <v>1918</v>
       </c>
     </row>
     <row r="490" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A490" s="5" t="s">
-        <v>1938</v>
+        <v>1918</v>
       </c>
     </row>
     <row r="491" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A491" s="5" t="s">
-        <v>1938</v>
+        <v>1918</v>
       </c>
     </row>
     <row r="492" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A492" s="5" t="s">
-        <v>1938</v>
+        <v>1918</v>
       </c>
     </row>
     <row r="493" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A493" s="5" t="s">
-        <v>1938</v>
+        <v>1918</v>
       </c>
     </row>
     <row r="494" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A494" s="5" t="s">
-        <v>1938</v>
+        <v>1918</v>
       </c>
     </row>
     <row r="495" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A495" s="5" t="s">
-        <v>1938</v>
+        <v>1918</v>
       </c>
     </row>
     <row r="496" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A496" s="5" t="s">
-        <v>1938</v>
+        <v>1918</v>
       </c>
     </row>
     <row r="497" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A497" s="5" t="s">
-        <v>1938</v>
+        <v>1918</v>
       </c>
     </row>
     <row r="498" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A498" s="5" t="s">
-        <v>1938</v>
+        <v>1918</v>
       </c>
     </row>
     <row r="499" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A499" s="5" t="s">
-        <v>1938</v>
+        <v>1918</v>
       </c>
     </row>
   </sheetData>
@@ -10416,8 +10479,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B498"/>
   <sheetViews>
-    <sheetView topLeftCell="A385" workbookViewId="0">
-      <selection activeCell="B395" sqref="B394:B395"/>
+    <sheetView tabSelected="1" topLeftCell="A275" workbookViewId="0">
+      <selection activeCell="A275" sqref="A1:B1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -10440,7 +10503,7 @@
         <v>AboutDetailsDescription</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>2043</v>
+        <v>2018</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
@@ -10512,7 +10575,7 @@
         <v>AccountDeleted</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>1890</v>
+        <v>1870</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.35">
@@ -10552,7 +10615,7 @@
         <v>AdTextA0</v>
       </c>
       <c r="B16" s="8" t="s">
-        <v>1919</v>
+        <v>1899</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.35">
@@ -10571,12 +10634,12 @@
         <v>582</v>
       </c>
     </row>
-    <row r="19" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:2" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A19" s="6" t="str">
         <v>AdTextB0</v>
       </c>
       <c r="B19" s="7" t="s">
-        <v>1724</v>
+        <v>2091</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.35">
@@ -10768,7 +10831,7 @@
         <v>ChangeLanguageDescriptionSmall</v>
       </c>
       <c r="B43" s="8" t="s">
-        <v>1750</v>
+        <v>1745</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.35">
@@ -10824,7 +10887,7 @@
         <v>ChooseFile</v>
       </c>
       <c r="B50" s="7" t="s">
-        <v>2044</v>
+        <v>2019</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.35">
@@ -10880,7 +10943,7 @@
         <v>CompanyDescription</v>
       </c>
       <c r="B57" s="3" t="s">
-        <v>1898</v>
+        <v>1878</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.35">
@@ -10976,7 +11039,7 @@
         <v>CookiePolicy</v>
       </c>
       <c r="B69" s="8" t="s">
-        <v>1807</v>
+        <v>1787</v>
       </c>
     </row>
     <row r="70" spans="1:2" ht="29" x14ac:dyDescent="0.35">
@@ -11000,7 +11063,7 @@
         <v>Cookies</v>
       </c>
       <c r="B72" s="3" t="s">
-        <v>1835</v>
+        <v>1815</v>
       </c>
     </row>
     <row r="73" spans="1:2" ht="116" x14ac:dyDescent="0.35">
@@ -11008,7 +11071,7 @@
         <v>CookiesText1</v>
       </c>
       <c r="B73" s="8" t="s">
-        <v>1920</v>
+        <v>1900</v>
       </c>
     </row>
     <row r="74" spans="1:2" ht="159.5" x14ac:dyDescent="0.35">
@@ -11016,7 +11079,7 @@
         <v>CookiesText2</v>
       </c>
       <c r="B74" s="8" t="s">
-        <v>1837</v>
+        <v>1817</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.35">
@@ -11032,7 +11095,7 @@
         <v>Copyright</v>
       </c>
       <c r="B76" s="8" t="s">
-        <v>1832</v>
+        <v>1812</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.35">
@@ -11040,7 +11103,7 @@
         <v>CopyrightLaw</v>
       </c>
       <c r="B77" s="8" t="s">
-        <v>1851</v>
+        <v>1831</v>
       </c>
     </row>
     <row r="78" spans="1:2" ht="101.5" x14ac:dyDescent="0.35">
@@ -11048,7 +11111,7 @@
         <v>CopyrightLawText</v>
       </c>
       <c r="B78" s="8" t="s">
-        <v>1852</v>
+        <v>1832</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.35">
@@ -11104,7 +11167,7 @@
         <v>CoursesDescription</v>
       </c>
       <c r="B85" s="7" t="s">
-        <v>1923</v>
+        <v>1903</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.35">
@@ -11179,12 +11242,12 @@
         <v>1680</v>
       </c>
     </row>
-    <row r="95" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:2" ht="130.5" x14ac:dyDescent="0.35">
       <c r="A95" s="5" t="str">
         <v>DashboardOverview</v>
       </c>
       <c r="B95" s="8" t="s">
-        <v>1767</v>
+        <v>2097</v>
       </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.35">
@@ -11192,7 +11255,7 @@
         <v>DataProtection</v>
       </c>
       <c r="B96" s="8" t="s">
-        <v>1822</v>
+        <v>1802</v>
       </c>
     </row>
     <row r="97" spans="1:2" ht="174" x14ac:dyDescent="0.35">
@@ -11200,7 +11263,7 @@
         <v>DataProtectionText</v>
       </c>
       <c r="B97" s="8" t="s">
-        <v>1826</v>
+        <v>1806</v>
       </c>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.35">
@@ -11216,7 +11279,7 @@
         <v>DateProtectionText</v>
       </c>
       <c r="B99" s="8" t="s">
-        <v>1826</v>
+        <v>1806</v>
       </c>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.35">
@@ -11280,7 +11343,7 @@
         <v>Disclaimer</v>
       </c>
       <c r="B107" s="8" t="s">
-        <v>1798</v>
+        <v>1778</v>
       </c>
     </row>
     <row r="108" spans="1:2" ht="319" x14ac:dyDescent="0.35">
@@ -11288,7 +11351,7 @@
         <v>DisclaimerText</v>
       </c>
       <c r="B108" s="8" t="s">
-        <v>1816</v>
+        <v>1796</v>
       </c>
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.35">
@@ -11576,7 +11639,7 @@
         <v>Goodbye</v>
       </c>
       <c r="B144" s="8" t="s">
-        <v>1903</v>
+        <v>1883</v>
       </c>
     </row>
     <row r="145" spans="1:2" x14ac:dyDescent="0.35">
@@ -11584,7 +11647,7 @@
         <v>GoogleAnalytics</v>
       </c>
       <c r="B145" s="5" t="s">
-        <v>1839</v>
+        <v>1819</v>
       </c>
     </row>
     <row r="146" spans="1:2" ht="290" x14ac:dyDescent="0.35">
@@ -11592,7 +11655,7 @@
         <v>GoogleAnalyticsText1</v>
       </c>
       <c r="B146" s="3" t="s">
-        <v>1841</v>
+        <v>1821</v>
       </c>
     </row>
     <row r="147" spans="1:2" ht="159.5" x14ac:dyDescent="0.35">
@@ -11600,7 +11663,7 @@
         <v>GoogleAnalyticsText2</v>
       </c>
       <c r="B147" s="3" t="s">
-        <v>1844</v>
+        <v>1824</v>
       </c>
     </row>
     <row r="148" spans="1:2" x14ac:dyDescent="0.35">
@@ -11792,7 +11855,7 @@
         <v>KeepControl</v>
       </c>
       <c r="B171" s="8" t="s">
-        <v>1766</v>
+        <v>1758</v>
       </c>
     </row>
     <row r="172" spans="1:2" x14ac:dyDescent="0.35">
@@ -11880,7 +11943,7 @@
         <v>LegalNotice</v>
       </c>
       <c r="B182" s="8" t="s">
-        <v>1806</v>
+        <v>1786</v>
       </c>
     </row>
     <row r="183" spans="1:2" x14ac:dyDescent="0.35">
@@ -11888,7 +11951,7 @@
         <v>LegalNoticeResponsible</v>
       </c>
       <c r="B183" s="8" t="s">
-        <v>1849</v>
+        <v>1829</v>
       </c>
     </row>
     <row r="184" spans="1:2" x14ac:dyDescent="0.35">
@@ -12024,7 +12087,7 @@
         <v>MailAdvert4</v>
       </c>
       <c r="B200" s="8" t="s">
-        <v>1721</v>
+        <v>1720</v>
       </c>
     </row>
     <row r="201" spans="1:2" x14ac:dyDescent="0.35">
@@ -12032,7 +12095,7 @@
         <v>MailAdvert5</v>
       </c>
       <c r="B201" s="8" t="s">
-        <v>1722</v>
+        <v>1721</v>
       </c>
     </row>
     <row r="202" spans="1:2" x14ac:dyDescent="0.35">
@@ -12048,7 +12111,7 @@
         <v>MailBye3</v>
       </c>
       <c r="B203" s="3" t="s">
-        <v>1886</v>
+        <v>1866</v>
       </c>
     </row>
     <row r="204" spans="1:2" x14ac:dyDescent="0.35">
@@ -12056,7 +12119,7 @@
         <v>MailFooter1</v>
       </c>
       <c r="B204" s="8" t="s">
-        <v>1723</v>
+        <v>1722</v>
       </c>
     </row>
     <row r="205" spans="1:2" ht="29" x14ac:dyDescent="0.35">
@@ -12760,15 +12823,15 @@
         <v>SavePublications</v>
       </c>
       <c r="B292" s="8" t="s">
-        <v>1768</v>
-      </c>
-    </row>
-    <row r="293" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
+        <v>1759</v>
+      </c>
+    </row>
+    <row r="293" spans="1:2" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A293" s="5" t="str">
         <v>SavePublicationsDescription</v>
       </c>
       <c r="B293" s="8" t="s">
-        <v>1958</v>
+        <v>2102</v>
       </c>
     </row>
     <row r="294" spans="1:2" x14ac:dyDescent="0.35">
@@ -12824,7 +12887,7 @@
         <v>SettingsLanguageHint</v>
       </c>
       <c r="B300" s="7" t="s">
-        <v>1912</v>
+        <v>1892</v>
       </c>
     </row>
     <row r="301" spans="1:2" ht="29" x14ac:dyDescent="0.35">
@@ -12848,15 +12911,15 @@
         <v>ShowYourStrengths</v>
       </c>
       <c r="B303" s="8" t="s">
-        <v>1757</v>
-      </c>
-    </row>
-    <row r="304" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
+        <v>1752</v>
+      </c>
+    </row>
+    <row r="304" spans="1:2" ht="87" x14ac:dyDescent="0.35">
       <c r="A304" s="5" t="str">
         <v>ShowYourStrengthsDescription</v>
       </c>
       <c r="B304" s="8" t="s">
-        <v>1769</v>
+        <v>2107</v>
       </c>
     </row>
     <row r="305" spans="1:2" x14ac:dyDescent="0.35">
@@ -13040,7 +13103,7 @@
         <v>Switzerland</v>
       </c>
       <c r="B327" s="8" t="s">
-        <v>1884</v>
+        <v>1864</v>
       </c>
     </row>
     <row r="328" spans="1:2" x14ac:dyDescent="0.35">
@@ -13208,7 +13271,7 @@
         <v>WelcomeToVitae</v>
       </c>
       <c r="B348" s="7" t="s">
-        <v>1720</v>
+        <v>1719</v>
       </c>
     </row>
     <row r="349" spans="1:2" x14ac:dyDescent="0.35">
@@ -13216,15 +13279,15 @@
         <v>WhyMyVitae</v>
       </c>
       <c r="B349" s="8" t="s">
-        <v>1740</v>
-      </c>
-    </row>
-    <row r="350" spans="1:2" ht="130.5" x14ac:dyDescent="0.35">
+        <v>1735</v>
+      </c>
+    </row>
+    <row r="350" spans="1:2" ht="159.5" x14ac:dyDescent="0.35">
       <c r="A350" s="5" t="str">
         <v>WhyMyVitaeReason</v>
       </c>
       <c r="B350" s="8" t="s">
-        <v>1791</v>
+        <v>2093</v>
       </c>
     </row>
     <row r="351" spans="1:2" x14ac:dyDescent="0.35">
@@ -13232,7 +13295,7 @@
         <v>WhyMyVitaeTest</v>
       </c>
       <c r="B351" s="8" t="s">
-        <v>1794</v>
+        <v>1774</v>
       </c>
     </row>
     <row r="352" spans="1:2" x14ac:dyDescent="0.35">
@@ -13296,7 +13359,7 @@
         <v>Preview</v>
       </c>
       <c r="B359" s="8" t="s">
-        <v>1908</v>
+        <v>1888</v>
       </c>
     </row>
     <row r="360" spans="1:2" x14ac:dyDescent="0.35">
@@ -13304,7 +13367,7 @@
         <v>Error</v>
       </c>
       <c r="B360" s="8" t="s">
-        <v>1914</v>
+        <v>1894</v>
       </c>
     </row>
     <row r="361" spans="1:2" x14ac:dyDescent="0.35">
@@ -13312,7 +13375,7 @@
         <v>Demo</v>
       </c>
       <c r="B361" s="3" t="s">
-        <v>1917</v>
+        <v>1897</v>
       </c>
     </row>
     <row r="362" spans="1:2" x14ac:dyDescent="0.35">
@@ -13320,7 +13383,7 @@
         <v>Up</v>
       </c>
       <c r="B362" s="3" t="s">
-        <v>1925</v>
+        <v>1905</v>
       </c>
     </row>
     <row r="363" spans="1:2" x14ac:dyDescent="0.35">
@@ -13328,7 +13391,7 @@
         <v>Down</v>
       </c>
       <c r="B363" s="3" t="s">
-        <v>1933</v>
+        <v>1913</v>
       </c>
     </row>
     <row r="364" spans="1:2" ht="28.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -13336,7 +13399,7 @@
         <v>PasswordProtectionDesc</v>
       </c>
       <c r="B364" s="8" t="s">
-        <v>1947</v>
+        <v>1927</v>
       </c>
     </row>
     <row r="365" spans="1:2" x14ac:dyDescent="0.35">
@@ -13344,7 +13407,7 @@
         <v>SecurityCheck</v>
       </c>
       <c r="B365" s="8" t="s">
-        <v>1941</v>
+        <v>1921</v>
       </c>
     </row>
     <row r="366" spans="1:2" x14ac:dyDescent="0.35">
@@ -13352,7 +13415,7 @@
         <v>Status403</v>
       </c>
       <c r="B366" s="8" t="s">
-        <v>1970</v>
+        <v>1945</v>
       </c>
     </row>
     <row r="367" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
@@ -13360,7 +13423,7 @@
         <v>Status500</v>
       </c>
       <c r="B367" s="8" t="s">
-        <v>1971</v>
+        <v>1946</v>
       </c>
     </row>
     <row r="368" spans="1:2" x14ac:dyDescent="0.35">
@@ -13368,7 +13431,7 @@
         <v>Secure</v>
       </c>
       <c r="B368" s="8" t="s">
-        <v>1977</v>
+        <v>1952</v>
       </c>
     </row>
     <row r="369" spans="1:2" ht="29" x14ac:dyDescent="0.35">
@@ -13376,7 +13439,7 @@
         <v>SecureDescription</v>
       </c>
       <c r="B369" s="8" t="s">
-        <v>2005</v>
+        <v>1980</v>
       </c>
     </row>
     <row r="370" spans="1:2" ht="29" x14ac:dyDescent="0.35">
@@ -13384,7 +13447,7 @@
         <v>SecurityCheckDesc</v>
       </c>
       <c r="B370" s="8" t="s">
-        <v>1972</v>
+        <v>1947</v>
       </c>
     </row>
     <row r="371" spans="1:2" x14ac:dyDescent="0.35">
@@ -13392,7 +13455,7 @@
         <v>Contact</v>
       </c>
       <c r="B371" s="8" t="s">
-        <v>1973</v>
+        <v>1948</v>
       </c>
     </row>
     <row r="372" spans="1:2" x14ac:dyDescent="0.35">
@@ -13400,7 +13463,7 @@
         <v>GoogleCaptcha</v>
       </c>
       <c r="B372" s="8" t="s">
-        <v>1964</v>
+        <v>1939</v>
       </c>
     </row>
     <row r="373" spans="1:2" ht="174" x14ac:dyDescent="0.35">
@@ -13408,7 +13471,7 @@
         <v>GoogleCaptchaDesc</v>
       </c>
       <c r="B373" s="8" t="s">
-        <v>1974</v>
+        <v>1949</v>
       </c>
     </row>
     <row r="374" spans="1:2" x14ac:dyDescent="0.35">
@@ -13416,7 +13479,7 @@
         <v>DataCollection</v>
       </c>
       <c r="B374" s="8" t="s">
-        <v>1975</v>
+        <v>1950</v>
       </c>
     </row>
     <row r="375" spans="1:2" ht="304.5" x14ac:dyDescent="0.35">
@@ -13424,7 +13487,7 @@
         <v>DataCollectionDesc</v>
       </c>
       <c r="B375" s="8" t="s">
-        <v>1976</v>
+        <v>1951</v>
       </c>
     </row>
     <row r="376" spans="1:2" x14ac:dyDescent="0.35">
@@ -13432,7 +13495,7 @@
         <v>Imprint</v>
       </c>
       <c r="B376" s="8" t="s">
-        <v>2007</v>
+        <v>1982</v>
       </c>
     </row>
     <row r="377" spans="1:2" ht="29" x14ac:dyDescent="0.35">
@@ -13440,7 +13503,7 @@
         <v>ErrorInfoMail</v>
       </c>
       <c r="B377" s="3" t="s">
-        <v>2013</v>
+        <v>1988</v>
       </c>
     </row>
     <row r="378" spans="1:2" x14ac:dyDescent="0.35">
@@ -13448,7 +13511,7 @@
         <v>Management</v>
       </c>
       <c r="B378" s="8" t="s">
-        <v>2019</v>
+        <v>1994</v>
       </c>
     </row>
     <row r="379" spans="1:2" x14ac:dyDescent="0.35">
@@ -13456,7 +13519,7 @@
         <v>Data</v>
       </c>
       <c r="B379" s="8" t="s">
-        <v>2024</v>
+        <v>1999</v>
       </c>
     </row>
     <row r="380" spans="1:2" x14ac:dyDescent="0.35">
@@ -13464,7 +13527,7 @@
         <v>Color</v>
       </c>
       <c r="B380" s="8" t="s">
-        <v>2029</v>
+        <v>2004</v>
       </c>
     </row>
     <row r="381" spans="1:2" x14ac:dyDescent="0.35">
@@ -13472,7 +13535,7 @@
         <v>ColorDescription</v>
       </c>
       <c r="B381" s="3" t="s">
-        <v>2034</v>
+        <v>2009</v>
       </c>
     </row>
     <row r="382" spans="1:2" x14ac:dyDescent="0.35">
@@ -13480,7 +13543,7 @@
         <v>Prefix</v>
       </c>
       <c r="B382" s="8" t="s">
-        <v>2039</v>
+        <v>2014</v>
       </c>
     </row>
     <row r="383" spans="1:2" x14ac:dyDescent="0.35">
@@ -13488,7 +13551,7 @@
         <v>LinkExperience</v>
       </c>
       <c r="B383" s="8" t="s">
-        <v>2057</v>
+        <v>2032</v>
       </c>
     </row>
     <row r="384" spans="1:2" x14ac:dyDescent="0.35">
@@ -13496,7 +13559,7 @@
         <v>LinkEducation</v>
       </c>
       <c r="B384" s="8" t="s">
-        <v>2058</v>
+        <v>2033</v>
       </c>
     </row>
     <row r="385" spans="1:2" x14ac:dyDescent="0.35">
@@ -13504,7 +13567,7 @@
         <v>LinkInterest</v>
       </c>
       <c r="B385" s="8" t="s">
-        <v>2059</v>
+        <v>2034</v>
       </c>
     </row>
     <row r="386" spans="1:2" x14ac:dyDescent="0.35">
@@ -13512,7 +13575,7 @@
         <v>LinkAwards</v>
       </c>
       <c r="B386" s="8" t="s">
-        <v>2060</v>
+        <v>2035</v>
       </c>
     </row>
     <row r="387" spans="1:2" x14ac:dyDescent="0.35">
@@ -13520,7 +13583,7 @@
         <v>LinkCertificate</v>
       </c>
       <c r="B387" s="8" t="s">
-        <v>2061</v>
+        <v>2036</v>
       </c>
     </row>
     <row r="388" spans="1:2" x14ac:dyDescent="0.35">
@@ -13528,7 +13591,7 @@
         <v>LinkReference</v>
       </c>
       <c r="B388" s="8" t="s">
-        <v>2062</v>
+        <v>2037</v>
       </c>
     </row>
     <row r="389" spans="1:2" ht="29" x14ac:dyDescent="0.35">
@@ -13536,7 +13599,7 @@
         <v>ChronologicalAsc</v>
       </c>
       <c r="B389" s="3" t="s">
-        <v>2086</v>
+        <v>2061</v>
       </c>
     </row>
     <row r="390" spans="1:2" ht="29" x14ac:dyDescent="0.35">
@@ -13544,22 +13607,31 @@
         <v>ChronologicalDesc</v>
       </c>
       <c r="B390" s="3" t="s">
-        <v>2087</v>
+        <v>2062</v>
       </c>
     </row>
     <row r="391" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A391" s="5" t="str">
-        <v xml:space="preserve"> </v>
+        <v>OptionalInformation</v>
+      </c>
+      <c r="B391" s="8" t="s">
+        <v>2071</v>
       </c>
     </row>
     <row r="392" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A392" s="5" t="str">
-        <v xml:space="preserve"> </v>
+        <v>MyVitaeSlogan</v>
+      </c>
+      <c r="B392" s="8" t="s">
+        <v>2077</v>
       </c>
     </row>
     <row r="393" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A393" s="5" t="str">
-        <v xml:space="preserve"> </v>
+        <v>DownloadQR</v>
+      </c>
+      <c r="B393" s="8" t="s">
+        <v>2083</v>
       </c>
     </row>
     <row r="394" spans="1:2" x14ac:dyDescent="0.35">
@@ -14097,8 +14169,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1802D85A-2FA6-4DB3-A31F-68A2D623BDD9}">
   <dimension ref="A1:B498"/>
   <sheetViews>
-    <sheetView topLeftCell="A383" workbookViewId="0">
-      <selection activeCell="B392" sqref="B392"/>
+    <sheetView topLeftCell="A275" workbookViewId="0">
+      <selection activeCell="A275" sqref="A1:B1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -14193,7 +14265,7 @@
         <v>AccountDeleted</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>1891</v>
+        <v>1871</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.35">
@@ -14252,12 +14324,12 @@
         <v>804</v>
       </c>
     </row>
-    <row r="19" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:2" ht="58" x14ac:dyDescent="0.35">
       <c r="A19" s="6" t="str">
         <v>AdTextB0</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>1729</v>
+        <v>2088</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.35">
@@ -14449,7 +14521,7 @@
         <v>ChangeLanguageDescriptionSmall</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>1752</v>
+        <v>1747</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.35">
@@ -14561,7 +14633,7 @@
         <v>CompanyDescription</v>
       </c>
       <c r="B57" s="3" t="s">
-        <v>1899</v>
+        <v>1879</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.35">
@@ -14657,7 +14729,7 @@
         <v>CookiePolicy</v>
       </c>
       <c r="B69" s="3" t="s">
-        <v>1809</v>
+        <v>1789</v>
       </c>
     </row>
     <row r="70" spans="1:2" ht="29" x14ac:dyDescent="0.35">
@@ -14681,7 +14753,7 @@
         <v>Cookies</v>
       </c>
       <c r="B72" s="3" t="s">
-        <v>1835</v>
+        <v>1815</v>
       </c>
     </row>
     <row r="73" spans="1:2" ht="101.5" x14ac:dyDescent="0.35">
@@ -14689,7 +14761,7 @@
         <v>CookiesText1</v>
       </c>
       <c r="B73" s="3" t="s">
-        <v>1856</v>
+        <v>1836</v>
       </c>
     </row>
     <row r="74" spans="1:2" ht="130.5" x14ac:dyDescent="0.35">
@@ -14697,7 +14769,7 @@
         <v>CookiesText2</v>
       </c>
       <c r="B74" s="3" t="s">
-        <v>1857</v>
+        <v>1837</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.35">
@@ -14713,7 +14785,7 @@
         <v>Copyright</v>
       </c>
       <c r="B76" s="3" t="s">
-        <v>1876</v>
+        <v>1856</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.35">
@@ -14721,7 +14793,7 @@
         <v>CopyrightLaw</v>
       </c>
       <c r="B77" s="3" t="s">
-        <v>1833</v>
+        <v>1813</v>
       </c>
     </row>
     <row r="78" spans="1:2" ht="72.5" x14ac:dyDescent="0.35">
@@ -14729,7 +14801,7 @@
         <v>CopyrightLawText</v>
       </c>
       <c r="B78" s="3" t="s">
-        <v>1862</v>
+        <v>1842</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.35">
@@ -14817,7 +14889,7 @@
         <v>CurriculumVitae</v>
       </c>
       <c r="B89" s="3" t="s">
-        <v>1748</v>
+        <v>1743</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.35">
@@ -14825,7 +14897,7 @@
         <v>CV</v>
       </c>
       <c r="B90" s="2" t="s">
-        <v>1748</v>
+        <v>1743</v>
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.35">
@@ -14860,12 +14932,12 @@
         <v>1691</v>
       </c>
     </row>
-    <row r="95" spans="1:2" ht="29" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:2" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A95" s="5" t="str">
         <v>DashboardOverview</v>
       </c>
       <c r="B95" s="3" t="s">
-        <v>1773</v>
+        <v>2099</v>
       </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.35">
@@ -14873,7 +14945,7 @@
         <v>DataProtection</v>
       </c>
       <c r="B96" s="5" t="s">
-        <v>1879</v>
+        <v>1859</v>
       </c>
     </row>
     <row r="97" spans="1:2" ht="159.5" x14ac:dyDescent="0.35">
@@ -14881,7 +14953,7 @@
         <v>DataProtectionText</v>
       </c>
       <c r="B97" s="3" t="s">
-        <v>1828</v>
+        <v>1808</v>
       </c>
     </row>
     <row r="98" spans="1:2" ht="159.5" x14ac:dyDescent="0.35">
@@ -14889,7 +14961,7 @@
         <v>DateCompareError</v>
       </c>
       <c r="B98" s="3" t="s">
-        <v>1828</v>
+        <v>1808</v>
       </c>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.35">
@@ -14961,7 +15033,7 @@
         <v>Disclaimer</v>
       </c>
       <c r="B107" s="3" t="s">
-        <v>1799</v>
+        <v>1779</v>
       </c>
     </row>
     <row r="108" spans="1:2" ht="275.5" x14ac:dyDescent="0.35">
@@ -14969,7 +15041,7 @@
         <v>DisclaimerText</v>
       </c>
       <c r="B108" s="3" t="s">
-        <v>1817</v>
+        <v>1797</v>
       </c>
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.35">
@@ -15257,7 +15329,7 @@
         <v>Goodbye</v>
       </c>
       <c r="B144" s="8" t="s">
-        <v>1904</v>
+        <v>1884</v>
       </c>
     </row>
     <row r="145" spans="1:2" x14ac:dyDescent="0.35">
@@ -15265,7 +15337,7 @@
         <v>GoogleAnalytics</v>
       </c>
       <c r="B145" s="3" t="s">
-        <v>1858</v>
+        <v>1838</v>
       </c>
     </row>
     <row r="146" spans="1:2" ht="261" x14ac:dyDescent="0.35">
@@ -15273,7 +15345,7 @@
         <v>GoogleAnalyticsText1</v>
       </c>
       <c r="B146" s="3" t="s">
-        <v>1859</v>
+        <v>1839</v>
       </c>
     </row>
     <row r="147" spans="1:2" ht="130.5" x14ac:dyDescent="0.35">
@@ -15281,7 +15353,7 @@
         <v>GoogleAnalyticsText2</v>
       </c>
       <c r="B147" s="3" t="s">
-        <v>1860</v>
+        <v>1840</v>
       </c>
     </row>
     <row r="148" spans="1:2" x14ac:dyDescent="0.35">
@@ -15473,7 +15545,7 @@
         <v>KeepControl</v>
       </c>
       <c r="B171" s="3" t="s">
-        <v>1772</v>
+        <v>1761</v>
       </c>
     </row>
     <row r="172" spans="1:2" x14ac:dyDescent="0.35">
@@ -15561,7 +15633,7 @@
         <v>LegalNotice</v>
       </c>
       <c r="B182" s="3" t="s">
-        <v>1808</v>
+        <v>1788</v>
       </c>
     </row>
     <row r="183" spans="1:2" x14ac:dyDescent="0.35">
@@ -15569,7 +15641,7 @@
         <v>LegalNoticeResponsible</v>
       </c>
       <c r="B183" s="3" t="s">
-        <v>1861</v>
+        <v>1841</v>
       </c>
     </row>
     <row r="184" spans="1:2" x14ac:dyDescent="0.35">
@@ -15705,7 +15777,7 @@
         <v>MailAdvert4</v>
       </c>
       <c r="B200" s="3" t="s">
-        <v>1726</v>
+        <v>1724</v>
       </c>
     </row>
     <row r="201" spans="1:2" x14ac:dyDescent="0.35">
@@ -15713,7 +15785,7 @@
         <v>MailAdvert5</v>
       </c>
       <c r="B201" s="3" t="s">
-        <v>1727</v>
+        <v>1725</v>
       </c>
     </row>
     <row r="202" spans="1:2" x14ac:dyDescent="0.35">
@@ -15729,7 +15801,7 @@
         <v>MailBye3</v>
       </c>
       <c r="B203" s="3" t="s">
-        <v>1894</v>
+        <v>1874</v>
       </c>
     </row>
     <row r="204" spans="1:2" x14ac:dyDescent="0.35">
@@ -15737,7 +15809,7 @@
         <v>MailFooter1</v>
       </c>
       <c r="B204" s="3" t="s">
-        <v>1728</v>
+        <v>1726</v>
       </c>
     </row>
     <row r="205" spans="1:2" ht="29" x14ac:dyDescent="0.35">
@@ -16441,15 +16513,15 @@
         <v>SavePublications</v>
       </c>
       <c r="B292" s="3" t="s">
-        <v>1774</v>
-      </c>
-    </row>
-    <row r="293" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
+        <v>1762</v>
+      </c>
+    </row>
+    <row r="293" spans="1:2" ht="87" x14ac:dyDescent="0.35">
       <c r="A293" s="5" t="str">
         <v>SavePublicationsDescription</v>
       </c>
       <c r="B293" s="3" t="s">
-        <v>1959</v>
+        <v>2104</v>
       </c>
     </row>
     <row r="294" spans="1:2" x14ac:dyDescent="0.35">
@@ -16529,15 +16601,15 @@
         <v>ShowYourStrengths</v>
       </c>
       <c r="B303" s="3" t="s">
-        <v>1775</v>
-      </c>
-    </row>
-    <row r="304" spans="1:2" ht="29" x14ac:dyDescent="0.35">
+        <v>1763</v>
+      </c>
+    </row>
+    <row r="304" spans="1:2" ht="87" x14ac:dyDescent="0.35">
       <c r="A304" s="5" t="str">
         <v>ShowYourStrengthsDescription</v>
       </c>
       <c r="B304" s="3" t="s">
-        <v>1776</v>
+        <v>2109</v>
       </c>
     </row>
     <row r="305" spans="1:2" x14ac:dyDescent="0.35">
@@ -16721,7 +16793,7 @@
         <v>Switzerland</v>
       </c>
       <c r="B327" s="3" t="s">
-        <v>1881</v>
+        <v>1861</v>
       </c>
     </row>
     <row r="328" spans="1:2" x14ac:dyDescent="0.35">
@@ -16889,7 +16961,7 @@
         <v>WelcomeToVitae</v>
       </c>
       <c r="B348" s="2" t="s">
-        <v>1725</v>
+        <v>1723</v>
       </c>
     </row>
     <row r="349" spans="1:2" x14ac:dyDescent="0.35">
@@ -16897,7 +16969,7 @@
         <v>WhyMyVitae</v>
       </c>
       <c r="B349" s="3" t="s">
-        <v>1770</v>
+        <v>1760</v>
       </c>
     </row>
     <row r="350" spans="1:2" ht="116" x14ac:dyDescent="0.35">
@@ -16905,7 +16977,7 @@
         <v>WhyMyVitaeReason</v>
       </c>
       <c r="B350" s="3" t="s">
-        <v>1771</v>
+        <v>2094</v>
       </c>
     </row>
     <row r="351" spans="1:2" x14ac:dyDescent="0.35">
@@ -16913,7 +16985,7 @@
         <v>WhyMyVitaeTest</v>
       </c>
       <c r="B351" s="3" t="s">
-        <v>1795</v>
+        <v>1775</v>
       </c>
     </row>
     <row r="352" spans="1:2" x14ac:dyDescent="0.35">
@@ -16977,7 +17049,7 @@
         <v>Preview</v>
       </c>
       <c r="B359" s="3" t="s">
-        <v>1909</v>
+        <v>1889</v>
       </c>
     </row>
     <row r="360" spans="1:2" x14ac:dyDescent="0.35">
@@ -16985,7 +17057,7 @@
         <v>Error</v>
       </c>
       <c r="B360" s="3" t="s">
-        <v>1915</v>
+        <v>1895</v>
       </c>
     </row>
     <row r="361" spans="1:2" x14ac:dyDescent="0.35">
@@ -16993,7 +17065,7 @@
         <v>Demo</v>
       </c>
       <c r="B361" s="3" t="s">
-        <v>1918</v>
+        <v>1898</v>
       </c>
     </row>
     <row r="362" spans="1:2" x14ac:dyDescent="0.35">
@@ -17001,7 +17073,7 @@
         <v>Up</v>
       </c>
       <c r="B362" s="3" t="s">
-        <v>1927</v>
+        <v>1907</v>
       </c>
     </row>
     <row r="363" spans="1:2" x14ac:dyDescent="0.35">
@@ -17009,7 +17081,7 @@
         <v>Down</v>
       </c>
       <c r="B363" s="3" t="s">
-        <v>1928</v>
+        <v>1908</v>
       </c>
     </row>
     <row r="364" spans="1:2" ht="29" x14ac:dyDescent="0.35">
@@ -17017,7 +17089,7 @@
         <v>PasswordProtectionDesc</v>
       </c>
       <c r="B364" s="8" t="s">
-        <v>1935</v>
+        <v>1915</v>
       </c>
     </row>
     <row r="365" spans="1:2" x14ac:dyDescent="0.35">
@@ -17025,7 +17097,7 @@
         <v>SecurityCheck</v>
       </c>
       <c r="B365" s="3" t="s">
-        <v>1942</v>
+        <v>1922</v>
       </c>
     </row>
     <row r="366" spans="1:2" x14ac:dyDescent="0.35">
@@ -17033,7 +17105,7 @@
         <v>Status403</v>
       </c>
       <c r="B366" s="3" t="s">
-        <v>1978</v>
+        <v>1953</v>
       </c>
     </row>
     <row r="367" spans="1:2" ht="29" x14ac:dyDescent="0.35">
@@ -17041,7 +17113,7 @@
         <v>Status500</v>
       </c>
       <c r="B367" s="3" t="s">
-        <v>1979</v>
+        <v>1954</v>
       </c>
     </row>
     <row r="368" spans="1:2" x14ac:dyDescent="0.35">
@@ -17049,7 +17121,7 @@
         <v>Secure</v>
       </c>
       <c r="B368" s="3" t="s">
-        <v>1980</v>
+        <v>1955</v>
       </c>
     </row>
     <row r="369" spans="1:2" ht="29" x14ac:dyDescent="0.35">
@@ -17057,7 +17129,7 @@
         <v>SecureDescription</v>
       </c>
       <c r="B369" s="3" t="s">
-        <v>1981</v>
+        <v>1956</v>
       </c>
     </row>
     <row r="370" spans="1:2" x14ac:dyDescent="0.35">
@@ -17065,7 +17137,7 @@
         <v>SecurityCheckDesc</v>
       </c>
       <c r="B370" s="3" t="s">
-        <v>1982</v>
+        <v>1957</v>
       </c>
     </row>
     <row r="371" spans="1:2" x14ac:dyDescent="0.35">
@@ -17073,7 +17145,7 @@
         <v>Contact</v>
       </c>
       <c r="B371" s="3" t="s">
-        <v>1983</v>
+        <v>1958</v>
       </c>
     </row>
     <row r="372" spans="1:2" x14ac:dyDescent="0.35">
@@ -17081,7 +17153,7 @@
         <v>GoogleCaptcha</v>
       </c>
       <c r="B372" s="3" t="s">
-        <v>1964</v>
+        <v>1939</v>
       </c>
     </row>
     <row r="373" spans="1:2" ht="130.5" x14ac:dyDescent="0.35">
@@ -17089,7 +17161,7 @@
         <v>GoogleCaptchaDesc</v>
       </c>
       <c r="B373" s="3" t="s">
-        <v>1984</v>
+        <v>1959</v>
       </c>
     </row>
     <row r="374" spans="1:2" x14ac:dyDescent="0.35">
@@ -17097,7 +17169,7 @@
         <v>DataCollection</v>
       </c>
       <c r="B374" s="3" t="s">
-        <v>1985</v>
+        <v>1960</v>
       </c>
     </row>
     <row r="375" spans="1:2" ht="307" customHeight="1" x14ac:dyDescent="0.35">
@@ -17105,7 +17177,7 @@
         <v>DataCollectionDesc</v>
       </c>
       <c r="B375" s="3" t="s">
-        <v>1986</v>
+        <v>1961</v>
       </c>
     </row>
     <row r="376" spans="1:2" x14ac:dyDescent="0.35">
@@ -17113,7 +17185,7 @@
         <v>Imprint</v>
       </c>
       <c r="B376" s="3" t="s">
-        <v>2008</v>
+        <v>1983</v>
       </c>
     </row>
     <row r="377" spans="1:2" ht="29" x14ac:dyDescent="0.35">
@@ -17121,7 +17193,7 @@
         <v>ErrorInfoMail</v>
       </c>
       <c r="B377" s="3" t="s">
-        <v>2014</v>
+        <v>1989</v>
       </c>
     </row>
     <row r="378" spans="1:2" x14ac:dyDescent="0.35">
@@ -17129,7 +17201,7 @@
         <v>Management</v>
       </c>
       <c r="B378" s="3" t="s">
-        <v>2020</v>
+        <v>1995</v>
       </c>
     </row>
     <row r="379" spans="1:2" x14ac:dyDescent="0.35">
@@ -17137,7 +17209,7 @@
         <v>Data</v>
       </c>
       <c r="B379" s="3" t="s">
-        <v>2025</v>
+        <v>2000</v>
       </c>
     </row>
     <row r="380" spans="1:2" x14ac:dyDescent="0.35">
@@ -17145,7 +17217,7 @@
         <v>Color</v>
       </c>
       <c r="B380" s="3" t="s">
-        <v>2030</v>
+        <v>2005</v>
       </c>
     </row>
     <row r="381" spans="1:2" x14ac:dyDescent="0.35">
@@ -17153,7 +17225,7 @@
         <v>ColorDescription</v>
       </c>
       <c r="B381" s="3" t="s">
-        <v>2035</v>
+        <v>2010</v>
       </c>
     </row>
     <row r="382" spans="1:2" x14ac:dyDescent="0.35">
@@ -17161,7 +17233,7 @@
         <v>Prefix</v>
       </c>
       <c r="B382" s="3" t="s">
-        <v>2040</v>
+        <v>2015</v>
       </c>
     </row>
     <row r="383" spans="1:2" x14ac:dyDescent="0.35">
@@ -17169,7 +17241,7 @@
         <v>LinkExperience</v>
       </c>
       <c r="B383" s="3" t="s">
-        <v>2063</v>
+        <v>2038</v>
       </c>
     </row>
     <row r="384" spans="1:2" x14ac:dyDescent="0.35">
@@ -17177,7 +17249,7 @@
         <v>LinkEducation</v>
       </c>
       <c r="B384" s="3" t="s">
-        <v>2064</v>
+        <v>2039</v>
       </c>
     </row>
     <row r="385" spans="1:2" x14ac:dyDescent="0.35">
@@ -17185,7 +17257,7 @@
         <v>LinkInterest</v>
       </c>
       <c r="B385" s="3" t="s">
-        <v>2065</v>
+        <v>2040</v>
       </c>
     </row>
     <row r="386" spans="1:2" x14ac:dyDescent="0.35">
@@ -17193,7 +17265,7 @@
         <v>LinkAwards</v>
       </c>
       <c r="B386" s="3" t="s">
-        <v>2066</v>
+        <v>2041</v>
       </c>
     </row>
     <row r="387" spans="1:2" x14ac:dyDescent="0.35">
@@ -17201,7 +17273,7 @@
         <v>LinkCertificate</v>
       </c>
       <c r="B387" s="3" t="s">
-        <v>2067</v>
+        <v>2042</v>
       </c>
     </row>
     <row r="388" spans="1:2" x14ac:dyDescent="0.35">
@@ -17209,7 +17281,7 @@
         <v>LinkReference</v>
       </c>
       <c r="B388" s="3" t="s">
-        <v>2068</v>
+        <v>2043</v>
       </c>
     </row>
     <row r="389" spans="1:2" x14ac:dyDescent="0.35">
@@ -17217,7 +17289,7 @@
         <v>ChronologicalAsc</v>
       </c>
       <c r="B389" s="3" t="s">
-        <v>2093</v>
+        <v>2068</v>
       </c>
     </row>
     <row r="390" spans="1:2" x14ac:dyDescent="0.35">
@@ -17225,22 +17297,31 @@
         <v>ChronologicalDesc</v>
       </c>
       <c r="B390" s="3" t="s">
-        <v>2088</v>
+        <v>2063</v>
       </c>
     </row>
     <row r="391" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A391" s="5" t="str">
-        <v xml:space="preserve"> </v>
+        <v>OptionalInformation</v>
+      </c>
+      <c r="B391" s="3" t="s">
+        <v>2072</v>
       </c>
     </row>
     <row r="392" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A392" s="5" t="str">
-        <v xml:space="preserve"> </v>
+        <v>MyVitaeSlogan</v>
+      </c>
+      <c r="B392" s="3" t="s">
+        <v>2076</v>
       </c>
     </row>
     <row r="393" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A393" s="5" t="str">
-        <v xml:space="preserve"> </v>
+        <v>DownloadQR</v>
+      </c>
+      <c r="B393" s="3" t="s">
+        <v>2084</v>
       </c>
     </row>
     <row r="394" spans="1:2" x14ac:dyDescent="0.35">
@@ -17777,8 +17858,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{21647760-4677-48F5-BA10-2363314EC080}">
   <dimension ref="A1:B498"/>
   <sheetViews>
-    <sheetView topLeftCell="A380" workbookViewId="0">
-      <selection activeCell="B391" sqref="B391"/>
+    <sheetView topLeftCell="A270" workbookViewId="0">
+      <selection activeCell="A270" sqref="A1:B1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -17873,7 +17954,7 @@
         <v>AccountDeleted</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>1892</v>
+        <v>1872</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.35">
@@ -17932,12 +18013,12 @@
         <v>1070</v>
       </c>
     </row>
-    <row r="19" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:2" ht="58" x14ac:dyDescent="0.35">
       <c r="A19" s="6" t="str">
         <v>AdTextB0</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>1734</v>
+        <v>2089</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.35">
@@ -18129,7 +18210,7 @@
         <v>ChangeLanguageDescriptionSmall</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>1753</v>
+        <v>1748</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.35">
@@ -18241,7 +18322,7 @@
         <v>CompanyDescription</v>
       </c>
       <c r="B57" s="3" t="s">
-        <v>1900</v>
+        <v>1880</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.35">
@@ -18337,7 +18418,7 @@
         <v>CookiePolicy</v>
       </c>
       <c r="B69" s="3" t="s">
-        <v>1811</v>
+        <v>1791</v>
       </c>
     </row>
     <row r="70" spans="1:2" ht="29" x14ac:dyDescent="0.35">
@@ -18361,7 +18442,7 @@
         <v>Cookies</v>
       </c>
       <c r="B72" s="3" t="s">
-        <v>1863</v>
+        <v>1843</v>
       </c>
     </row>
     <row r="73" spans="1:2" ht="101.5" x14ac:dyDescent="0.35">
@@ -18369,7 +18450,7 @@
         <v>CookiesText1</v>
       </c>
       <c r="B73" s="3" t="s">
-        <v>1922</v>
+        <v>1902</v>
       </c>
     </row>
     <row r="74" spans="1:2" ht="130.5" x14ac:dyDescent="0.35">
@@ -18377,7 +18458,7 @@
         <v>CookiesText2</v>
       </c>
       <c r="B74" s="3" t="s">
-        <v>1864</v>
+        <v>1844</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.35">
@@ -18393,7 +18474,7 @@
         <v>Copyright</v>
       </c>
       <c r="B76" s="3" t="s">
-        <v>1877</v>
+        <v>1857</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.35">
@@ -18401,7 +18482,7 @@
         <v>CopyrightLaw</v>
       </c>
       <c r="B77" s="3" t="s">
-        <v>1833</v>
+        <v>1813</v>
       </c>
     </row>
     <row r="78" spans="1:2" ht="72.5" x14ac:dyDescent="0.35">
@@ -18409,7 +18490,7 @@
         <v>CopyrightLawText</v>
       </c>
       <c r="B78" s="3" t="s">
-        <v>1868</v>
+        <v>1848</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.35">
@@ -18505,7 +18586,7 @@
         <v>CV</v>
       </c>
       <c r="B90" s="2" t="s">
-        <v>1748</v>
+        <v>1743</v>
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.35">
@@ -18540,12 +18621,12 @@
         <v>1701</v>
       </c>
     </row>
-    <row r="95" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:2" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A95" s="5" t="str">
         <v>DashboardOverview</v>
       </c>
       <c r="B95" s="3" t="s">
-        <v>1780</v>
+        <v>2100</v>
       </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.35">
@@ -18553,7 +18634,7 @@
         <v>DataProtection</v>
       </c>
       <c r="B96" s="3" t="s">
-        <v>1823</v>
+        <v>1803</v>
       </c>
     </row>
     <row r="97" spans="1:2" ht="145" x14ac:dyDescent="0.35">
@@ -18561,7 +18642,7 @@
         <v>DataProtectionText</v>
       </c>
       <c r="B97" s="3" t="s">
-        <v>1830</v>
+        <v>1810</v>
       </c>
     </row>
     <row r="98" spans="1:2" ht="145" x14ac:dyDescent="0.35">
@@ -18569,7 +18650,7 @@
         <v>DateCompareError</v>
       </c>
       <c r="B98" s="3" t="s">
-        <v>1830</v>
+        <v>1810</v>
       </c>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.35">
@@ -18641,7 +18722,7 @@
         <v>Disclaimer</v>
       </c>
       <c r="B107" t="s">
-        <v>1801</v>
+        <v>1781</v>
       </c>
     </row>
     <row r="108" spans="1:2" ht="275.5" x14ac:dyDescent="0.35">
@@ -18649,7 +18730,7 @@
         <v>DisclaimerText</v>
       </c>
       <c r="B108" s="3" t="s">
-        <v>1818</v>
+        <v>1798</v>
       </c>
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.35">
@@ -18937,7 +19018,7 @@
         <v>Goodbye</v>
       </c>
       <c r="B144" t="s">
-        <v>1905</v>
+        <v>1885</v>
       </c>
     </row>
     <row r="145" spans="1:2" x14ac:dyDescent="0.35">
@@ -18945,7 +19026,7 @@
         <v>GoogleAnalytics</v>
       </c>
       <c r="B145" s="3" t="s">
-        <v>1858</v>
+        <v>1838</v>
       </c>
     </row>
     <row r="146" spans="1:2" ht="232" x14ac:dyDescent="0.35">
@@ -18953,7 +19034,7 @@
         <v>GoogleAnalyticsText1</v>
       </c>
       <c r="B146" s="3" t="s">
-        <v>1865</v>
+        <v>1845</v>
       </c>
     </row>
     <row r="147" spans="1:2" ht="130.5" x14ac:dyDescent="0.35">
@@ -18961,7 +19042,7 @@
         <v>GoogleAnalyticsText2</v>
       </c>
       <c r="B147" s="3" t="s">
-        <v>1866</v>
+        <v>1846</v>
       </c>
     </row>
     <row r="148" spans="1:2" x14ac:dyDescent="0.35">
@@ -19153,7 +19234,7 @@
         <v>KeepControl</v>
       </c>
       <c r="B171" s="3" t="s">
-        <v>1779</v>
+        <v>1765</v>
       </c>
     </row>
     <row r="172" spans="1:2" x14ac:dyDescent="0.35">
@@ -19241,7 +19322,7 @@
         <v>LegalNotice</v>
       </c>
       <c r="B182" s="3" t="s">
-        <v>1810</v>
+        <v>1790</v>
       </c>
     </row>
     <row r="183" spans="1:2" x14ac:dyDescent="0.35">
@@ -19249,7 +19330,7 @@
         <v>LegalNoticeResponsible</v>
       </c>
       <c r="B183" s="3" t="s">
-        <v>1867</v>
+        <v>1847</v>
       </c>
     </row>
     <row r="184" spans="1:2" x14ac:dyDescent="0.35">
@@ -19385,7 +19466,7 @@
         <v>MailAdvert4</v>
       </c>
       <c r="B200" s="3" t="s">
-        <v>1731</v>
+        <v>1728</v>
       </c>
     </row>
     <row r="201" spans="1:2" x14ac:dyDescent="0.35">
@@ -19393,7 +19474,7 @@
         <v>MailAdvert5</v>
       </c>
       <c r="B201" s="3" t="s">
-        <v>1732</v>
+        <v>1729</v>
       </c>
     </row>
     <row r="202" spans="1:2" x14ac:dyDescent="0.35">
@@ -19409,7 +19490,7 @@
         <v>MailBye3</v>
       </c>
       <c r="B203" s="3" t="s">
-        <v>1895</v>
+        <v>1875</v>
       </c>
     </row>
     <row r="204" spans="1:2" x14ac:dyDescent="0.35">
@@ -19417,7 +19498,7 @@
         <v>MailFooter1</v>
       </c>
       <c r="B204" s="3" t="s">
-        <v>1733</v>
+        <v>1730</v>
       </c>
     </row>
     <row r="205" spans="1:2" x14ac:dyDescent="0.35">
@@ -20121,15 +20202,15 @@
         <v>SavePublications</v>
       </c>
       <c r="B292" s="3" t="s">
-        <v>1781</v>
-      </c>
-    </row>
-    <row r="293" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
+        <v>1766</v>
+      </c>
+    </row>
+    <row r="293" spans="1:2" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A293" s="5" t="str">
         <v>SavePublicationsDescription</v>
       </c>
       <c r="B293" s="3" t="s">
-        <v>1960</v>
+        <v>2105</v>
       </c>
     </row>
     <row r="294" spans="1:2" x14ac:dyDescent="0.35">
@@ -20209,15 +20290,15 @@
         <v>ShowYourStrengths</v>
       </c>
       <c r="B303" s="3" t="s">
-        <v>1782</v>
-      </c>
-    </row>
-    <row r="304" spans="1:2" ht="29" x14ac:dyDescent="0.35">
+        <v>1767</v>
+      </c>
+    </row>
+    <row r="304" spans="1:2" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A304" s="5" t="str">
         <v>ShowYourStrengthsDescription</v>
       </c>
       <c r="B304" s="3" t="s">
-        <v>1783</v>
+        <v>2110</v>
       </c>
     </row>
     <row r="305" spans="1:2" x14ac:dyDescent="0.35">
@@ -20401,7 +20482,7 @@
         <v>Switzerland</v>
       </c>
       <c r="B327" s="3" t="s">
-        <v>1882</v>
+        <v>1862</v>
       </c>
     </row>
     <row r="328" spans="1:2" x14ac:dyDescent="0.35">
@@ -20569,7 +20650,7 @@
         <v>WelcomeToVitae</v>
       </c>
       <c r="B348" s="2" t="s">
-        <v>1730</v>
+        <v>1727</v>
       </c>
     </row>
     <row r="349" spans="1:2" x14ac:dyDescent="0.35">
@@ -20577,15 +20658,15 @@
         <v>WhyMyVitae</v>
       </c>
       <c r="B349" s="3" t="s">
-        <v>1777</v>
-      </c>
-    </row>
-    <row r="350" spans="1:2" ht="101.5" x14ac:dyDescent="0.35">
+        <v>1764</v>
+      </c>
+    </row>
+    <row r="350" spans="1:2" ht="130.5" x14ac:dyDescent="0.35">
       <c r="A350" s="5" t="str">
         <v>WhyMyVitaeReason</v>
       </c>
       <c r="B350" s="3" t="s">
-        <v>1778</v>
+        <v>2095</v>
       </c>
     </row>
     <row r="351" spans="1:2" x14ac:dyDescent="0.35">
@@ -20593,7 +20674,7 @@
         <v>WhyMyVitaeTest</v>
       </c>
       <c r="B351" s="3" t="s">
-        <v>1796</v>
+        <v>1776</v>
       </c>
     </row>
     <row r="352" spans="1:2" x14ac:dyDescent="0.35">
@@ -20657,7 +20738,7 @@
         <v>Preview</v>
       </c>
       <c r="B359" s="3" t="s">
-        <v>1910</v>
+        <v>1890</v>
       </c>
     </row>
     <row r="360" spans="1:2" x14ac:dyDescent="0.35">
@@ -20665,7 +20746,7 @@
         <v>Error</v>
       </c>
       <c r="B360" s="3" t="s">
-        <v>1916</v>
+        <v>1896</v>
       </c>
     </row>
     <row r="361" spans="1:2" x14ac:dyDescent="0.35">
@@ -20673,7 +20754,7 @@
         <v>Demo</v>
       </c>
       <c r="B361" s="3" t="s">
-        <v>1917</v>
+        <v>1897</v>
       </c>
     </row>
     <row r="362" spans="1:2" x14ac:dyDescent="0.35">
@@ -20681,7 +20762,7 @@
         <v>Up</v>
       </c>
       <c r="B362" s="3" t="s">
-        <v>1929</v>
+        <v>1909</v>
       </c>
     </row>
     <row r="363" spans="1:2" x14ac:dyDescent="0.35">
@@ -20689,7 +20770,7 @@
         <v>Down</v>
       </c>
       <c r="B363" s="3" t="s">
-        <v>1930</v>
+        <v>1910</v>
       </c>
     </row>
     <row r="364" spans="1:2" ht="29" x14ac:dyDescent="0.35">
@@ -20697,7 +20778,7 @@
         <v>PasswordProtectionDesc</v>
       </c>
       <c r="B364" s="3" t="s">
-        <v>1937</v>
+        <v>1917</v>
       </c>
     </row>
     <row r="365" spans="1:2" x14ac:dyDescent="0.35">
@@ -20705,7 +20786,7 @@
         <v>SecurityCheck</v>
       </c>
       <c r="B365" s="3" t="s">
-        <v>1943</v>
+        <v>1923</v>
       </c>
     </row>
     <row r="366" spans="1:2" x14ac:dyDescent="0.35">
@@ -20713,7 +20794,7 @@
         <v>Status403</v>
       </c>
       <c r="B366" s="3" t="s">
-        <v>1987</v>
+        <v>1962</v>
       </c>
     </row>
     <row r="367" spans="1:2" ht="29" x14ac:dyDescent="0.35">
@@ -20721,7 +20802,7 @@
         <v>Status500</v>
       </c>
       <c r="B367" s="3" t="s">
-        <v>1988</v>
+        <v>1963</v>
       </c>
     </row>
     <row r="368" spans="1:2" x14ac:dyDescent="0.35">
@@ -20729,7 +20810,7 @@
         <v>Secure</v>
       </c>
       <c r="B368" s="3" t="s">
-        <v>1989</v>
+        <v>1964</v>
       </c>
     </row>
     <row r="369" spans="1:2" x14ac:dyDescent="0.35">
@@ -20737,7 +20818,7 @@
         <v>SecureDescription</v>
       </c>
       <c r="B369" s="3" t="s">
-        <v>1990</v>
+        <v>1965</v>
       </c>
     </row>
     <row r="370" spans="1:2" x14ac:dyDescent="0.35">
@@ -20745,7 +20826,7 @@
         <v>SecurityCheckDesc</v>
       </c>
       <c r="B370" s="3" t="s">
-        <v>1991</v>
+        <v>1966</v>
       </c>
     </row>
     <row r="371" spans="1:2" x14ac:dyDescent="0.35">
@@ -20753,7 +20834,7 @@
         <v>Contact</v>
       </c>
       <c r="B371" s="3" t="s">
-        <v>1992</v>
+        <v>1967</v>
       </c>
     </row>
     <row r="372" spans="1:2" x14ac:dyDescent="0.35">
@@ -20761,7 +20842,7 @@
         <v>GoogleCaptcha</v>
       </c>
       <c r="B372" s="3" t="s">
-        <v>1964</v>
+        <v>1939</v>
       </c>
     </row>
     <row r="373" spans="1:2" ht="116" x14ac:dyDescent="0.35">
@@ -20769,7 +20850,7 @@
         <v>GoogleCaptchaDesc</v>
       </c>
       <c r="B373" s="3" t="s">
-        <v>1993</v>
+        <v>1968</v>
       </c>
     </row>
     <row r="374" spans="1:2" x14ac:dyDescent="0.35">
@@ -20777,7 +20858,7 @@
         <v>DataCollection</v>
       </c>
       <c r="B374" s="3" t="s">
-        <v>1994</v>
+        <v>1969</v>
       </c>
     </row>
     <row r="375" spans="1:2" ht="261" x14ac:dyDescent="0.35">
@@ -20785,7 +20866,7 @@
         <v>DataCollectionDesc</v>
       </c>
       <c r="B375" s="3" t="s">
-        <v>1995</v>
+        <v>1970</v>
       </c>
     </row>
     <row r="376" spans="1:2" x14ac:dyDescent="0.35">
@@ -20793,7 +20874,7 @@
         <v>Imprint</v>
       </c>
       <c r="B376" s="3" t="s">
-        <v>2009</v>
+        <v>1984</v>
       </c>
     </row>
     <row r="377" spans="1:2" ht="29" x14ac:dyDescent="0.35">
@@ -20801,7 +20882,7 @@
         <v>ErrorInfoMail</v>
       </c>
       <c r="B377" s="3" t="s">
-        <v>2015</v>
+        <v>1990</v>
       </c>
     </row>
     <row r="378" spans="1:2" x14ac:dyDescent="0.35">
@@ -20809,7 +20890,7 @@
         <v>Management</v>
       </c>
       <c r="B378" s="3" t="s">
-        <v>2021</v>
+        <v>1996</v>
       </c>
     </row>
     <row r="379" spans="1:2" x14ac:dyDescent="0.35">
@@ -20817,7 +20898,7 @@
         <v>Data</v>
       </c>
       <c r="B379" s="3" t="s">
-        <v>2026</v>
+        <v>2001</v>
       </c>
     </row>
     <row r="380" spans="1:2" x14ac:dyDescent="0.35">
@@ -20825,7 +20906,7 @@
         <v>Color</v>
       </c>
       <c r="B380" s="3" t="s">
-        <v>2031</v>
+        <v>2006</v>
       </c>
     </row>
     <row r="381" spans="1:2" x14ac:dyDescent="0.35">
@@ -20833,7 +20914,7 @@
         <v>ColorDescription</v>
       </c>
       <c r="B381" s="3" t="s">
-        <v>2036</v>
+        <v>2011</v>
       </c>
     </row>
     <row r="382" spans="1:2" x14ac:dyDescent="0.35">
@@ -20841,7 +20922,7 @@
         <v>Prefix</v>
       </c>
       <c r="B382" s="3" t="s">
-        <v>2041</v>
+        <v>2016</v>
       </c>
     </row>
     <row r="383" spans="1:2" x14ac:dyDescent="0.35">
@@ -20849,7 +20930,7 @@
         <v>LinkExperience</v>
       </c>
       <c r="B383" s="3" t="s">
-        <v>2069</v>
+        <v>2044</v>
       </c>
     </row>
     <row r="384" spans="1:2" x14ac:dyDescent="0.35">
@@ -20857,7 +20938,7 @@
         <v>LinkEducation</v>
       </c>
       <c r="B384" s="3" t="s">
-        <v>2070</v>
+        <v>2045</v>
       </c>
     </row>
     <row r="385" spans="1:2" x14ac:dyDescent="0.35">
@@ -20865,7 +20946,7 @@
         <v>LinkInterest</v>
       </c>
       <c r="B385" s="3" t="s">
-        <v>2071</v>
+        <v>2046</v>
       </c>
     </row>
     <row r="386" spans="1:2" x14ac:dyDescent="0.35">
@@ -20873,7 +20954,7 @@
         <v>LinkAwards</v>
       </c>
       <c r="B386" s="3" t="s">
-        <v>2072</v>
+        <v>2047</v>
       </c>
     </row>
     <row r="387" spans="1:2" x14ac:dyDescent="0.35">
@@ -20881,7 +20962,7 @@
         <v>LinkCertificate</v>
       </c>
       <c r="B387" s="3" t="s">
-        <v>2073</v>
+        <v>2048</v>
       </c>
     </row>
     <row r="388" spans="1:2" x14ac:dyDescent="0.35">
@@ -20889,7 +20970,7 @@
         <v>LinkReference</v>
       </c>
       <c r="B388" s="3" t="s">
-        <v>2074</v>
+        <v>2049</v>
       </c>
     </row>
     <row r="389" spans="1:2" x14ac:dyDescent="0.35">
@@ -20897,7 +20978,7 @@
         <v>ChronologicalAsc</v>
       </c>
       <c r="B389" s="3" t="s">
-        <v>2092</v>
+        <v>2067</v>
       </c>
     </row>
     <row r="390" spans="1:2" x14ac:dyDescent="0.35">
@@ -20905,22 +20986,31 @@
         <v>ChronologicalDesc</v>
       </c>
       <c r="B390" s="3" t="s">
-        <v>2089</v>
+        <v>2064</v>
       </c>
     </row>
     <row r="391" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A391" s="5" t="str">
-        <v xml:space="preserve"> </v>
+        <v>OptionalInformation</v>
+      </c>
+      <c r="B391" s="3" t="s">
+        <v>2073</v>
       </c>
     </row>
     <row r="392" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A392" s="5" t="str">
-        <v xml:space="preserve"> </v>
+        <v>MyVitaeSlogan</v>
+      </c>
+      <c r="B392" s="3" t="s">
+        <v>2079</v>
       </c>
     </row>
     <row r="393" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A393" s="5" t="str">
-        <v xml:space="preserve"> </v>
+        <v>DownloadQR</v>
+      </c>
+      <c r="B393" s="3" t="s">
+        <v>2085</v>
       </c>
     </row>
     <row r="394" spans="1:2" x14ac:dyDescent="0.35">
@@ -21458,8 +21548,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A8220B7-2614-4C14-91F7-8D47B2A1113F}">
   <dimension ref="A1:B498"/>
   <sheetViews>
-    <sheetView topLeftCell="A377" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B393" sqref="B393"/>
+    <sheetView topLeftCell="A275" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A275" sqref="A1:B1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -21554,7 +21644,7 @@
         <v>AccountDeleted</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>1893</v>
+        <v>1873</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.35">
@@ -21613,12 +21703,12 @@
         <v>1340</v>
       </c>
     </row>
-    <row r="19" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:2" ht="58" x14ac:dyDescent="0.35">
       <c r="A19" s="6" t="str">
         <v>AdTextB0</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>1738</v>
+        <v>2090</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.35">
@@ -21810,7 +21900,7 @@
         <v>ChangeLanguageDescriptionSmall</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>1754</v>
+        <v>1749</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.35">
@@ -21922,7 +22012,7 @@
         <v>CompanyDescription</v>
       </c>
       <c r="B57" s="3" t="s">
-        <v>1901</v>
+        <v>1881</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.35">
@@ -22018,7 +22108,7 @@
         <v>CookiePolicy</v>
       </c>
       <c r="B69" s="3" t="s">
-        <v>1813</v>
+        <v>1793</v>
       </c>
     </row>
     <row r="70" spans="1:2" ht="29" x14ac:dyDescent="0.35">
@@ -22042,7 +22132,7 @@
         <v>Cookies</v>
       </c>
       <c r="B72" s="3" t="s">
-        <v>1835</v>
+        <v>1815</v>
       </c>
     </row>
     <row r="73" spans="1:2" ht="116" x14ac:dyDescent="0.35">
@@ -22050,7 +22140,7 @@
         <v>CookiesText1</v>
       </c>
       <c r="B73" s="3" t="s">
-        <v>1869</v>
+        <v>1849</v>
       </c>
     </row>
     <row r="74" spans="1:2" ht="130.5" x14ac:dyDescent="0.35">
@@ -22058,7 +22148,7 @@
         <v>CookiesText2</v>
       </c>
       <c r="B74" s="3" t="s">
-        <v>1870</v>
+        <v>1850</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.35">
@@ -22074,7 +22164,7 @@
         <v>Copyright</v>
       </c>
       <c r="B76" s="3" t="s">
-        <v>1878</v>
+        <v>1858</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.35">
@@ -22082,7 +22172,7 @@
         <v>CopyrightLaw</v>
       </c>
       <c r="B77" s="3" t="s">
-        <v>1874</v>
+        <v>1854</v>
       </c>
     </row>
     <row r="78" spans="1:2" ht="87" x14ac:dyDescent="0.35">
@@ -22090,7 +22180,7 @@
         <v>CopyrightLawText</v>
       </c>
       <c r="B78" s="3" t="s">
-        <v>1875</v>
+        <v>1855</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.35">
@@ -22178,7 +22268,7 @@
         <v>CurriculumVitae</v>
       </c>
       <c r="B89" s="3" t="s">
-        <v>1746</v>
+        <v>1741</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.35">
@@ -22221,12 +22311,12 @@
         <v>1586</v>
       </c>
     </row>
-    <row r="95" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:2" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A95" s="5" t="str">
         <v>DashboardOverview</v>
       </c>
       <c r="B95" s="3" t="s">
-        <v>1787</v>
+        <v>2101</v>
       </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.35">
@@ -22234,7 +22324,7 @@
         <v>DataProtection</v>
       </c>
       <c r="B96" s="3" t="s">
-        <v>1824</v>
+        <v>1804</v>
       </c>
     </row>
     <row r="97" spans="1:2" ht="159.5" x14ac:dyDescent="0.35">
@@ -22242,7 +22332,7 @@
         <v>DataProtectionText</v>
       </c>
       <c r="B97" s="3" t="s">
-        <v>1831</v>
+        <v>1811</v>
       </c>
     </row>
     <row r="98" spans="1:2" ht="159.5" x14ac:dyDescent="0.35">
@@ -22250,7 +22340,7 @@
         <v>DateCompareError</v>
       </c>
       <c r="B98" s="3" t="s">
-        <v>1831</v>
+        <v>1811</v>
       </c>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.35">
@@ -22322,7 +22412,7 @@
         <v>Disclaimer</v>
       </c>
       <c r="B107" s="3" t="s">
-        <v>1800</v>
+        <v>1780</v>
       </c>
     </row>
     <row r="108" spans="1:2" ht="304.5" x14ac:dyDescent="0.35">
@@ -22330,7 +22420,7 @@
         <v>DisclaimerText</v>
       </c>
       <c r="B108" s="3" t="s">
-        <v>1819</v>
+        <v>1799</v>
       </c>
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.35">
@@ -22618,7 +22708,7 @@
         <v>Goodbye</v>
       </c>
       <c r="B144" s="3" t="s">
-        <v>1906</v>
+        <v>1886</v>
       </c>
     </row>
     <row r="145" spans="1:2" x14ac:dyDescent="0.35">
@@ -22626,7 +22716,7 @@
         <v>GoogleAnalytics</v>
       </c>
       <c r="B145" s="3" t="s">
-        <v>1858</v>
+        <v>1838</v>
       </c>
     </row>
     <row r="146" spans="1:2" ht="246.5" x14ac:dyDescent="0.35">
@@ -22634,7 +22724,7 @@
         <v>GoogleAnalyticsText1</v>
       </c>
       <c r="B146" s="3" t="s">
-        <v>1871</v>
+        <v>1851</v>
       </c>
     </row>
     <row r="147" spans="1:2" ht="130.5" x14ac:dyDescent="0.35">
@@ -22642,7 +22732,7 @@
         <v>GoogleAnalyticsText2</v>
       </c>
       <c r="B147" s="3" t="s">
-        <v>1872</v>
+        <v>1852</v>
       </c>
     </row>
     <row r="148" spans="1:2" x14ac:dyDescent="0.35">
@@ -22834,7 +22924,7 @@
         <v>KeepControl</v>
       </c>
       <c r="B171" s="3" t="s">
-        <v>1786</v>
+        <v>1769</v>
       </c>
     </row>
     <row r="172" spans="1:2" x14ac:dyDescent="0.35">
@@ -22922,7 +23012,7 @@
         <v>LegalNotice</v>
       </c>
       <c r="B182" s="3" t="s">
-        <v>1812</v>
+        <v>1792</v>
       </c>
     </row>
     <row r="183" spans="1:2" x14ac:dyDescent="0.35">
@@ -22930,7 +23020,7 @@
         <v>LegalNoticeResponsible</v>
       </c>
       <c r="B183" s="3" t="s">
-        <v>1873</v>
+        <v>1853</v>
       </c>
     </row>
     <row r="184" spans="1:2" x14ac:dyDescent="0.35">
@@ -23066,7 +23156,7 @@
         <v>MailAdvert4</v>
       </c>
       <c r="B200" s="3" t="s">
-        <v>1735</v>
+        <v>1731</v>
       </c>
     </row>
     <row r="201" spans="1:2" x14ac:dyDescent="0.35">
@@ -23074,7 +23164,7 @@
         <v>MailAdvert5</v>
       </c>
       <c r="B201" s="3" t="s">
-        <v>1736</v>
+        <v>1732</v>
       </c>
     </row>
     <row r="202" spans="1:2" x14ac:dyDescent="0.35">
@@ -23090,7 +23180,7 @@
         <v>MailBye3</v>
       </c>
       <c r="B203" s="3" t="s">
-        <v>1887</v>
+        <v>1867</v>
       </c>
     </row>
     <row r="204" spans="1:2" x14ac:dyDescent="0.35">
@@ -23098,7 +23188,7 @@
         <v>MailFooter1</v>
       </c>
       <c r="B204" s="3" t="s">
-        <v>1737</v>
+        <v>1733</v>
       </c>
     </row>
     <row r="205" spans="1:2" ht="29" x14ac:dyDescent="0.35">
@@ -23802,15 +23892,15 @@
         <v>SavePublications</v>
       </c>
       <c r="B292" s="3" t="s">
-        <v>1788</v>
-      </c>
-    </row>
-    <row r="293" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
+        <v>1770</v>
+      </c>
+    </row>
+    <row r="293" spans="1:2" ht="87" x14ac:dyDescent="0.35">
       <c r="A293" s="5" t="str">
         <v>SavePublicationsDescription</v>
       </c>
       <c r="B293" s="3" t="s">
-        <v>1961</v>
+        <v>2106</v>
       </c>
     </row>
     <row r="294" spans="1:2" x14ac:dyDescent="0.35">
@@ -23890,15 +23980,15 @@
         <v>ShowYourStrengths</v>
       </c>
       <c r="B303" s="3" t="s">
-        <v>1789</v>
-      </c>
-    </row>
-    <row r="304" spans="1:2" ht="29" x14ac:dyDescent="0.35">
+        <v>1771</v>
+      </c>
+    </row>
+    <row r="304" spans="1:2" ht="87" x14ac:dyDescent="0.35">
       <c r="A304" s="5" t="str">
         <v>ShowYourStrengthsDescription</v>
       </c>
       <c r="B304" s="3" t="s">
-        <v>1790</v>
+        <v>2111</v>
       </c>
     </row>
     <row r="305" spans="1:2" x14ac:dyDescent="0.35">
@@ -24082,7 +24172,7 @@
         <v>Switzerland</v>
       </c>
       <c r="B327" s="3" t="s">
-        <v>1883</v>
+        <v>1863</v>
       </c>
     </row>
     <row r="328" spans="1:2" x14ac:dyDescent="0.35">
@@ -24258,15 +24348,15 @@
         <v>WhyMyVitae</v>
       </c>
       <c r="B349" s="3" t="s">
-        <v>1784</v>
-      </c>
-    </row>
-    <row r="350" spans="1:2" ht="101.5" x14ac:dyDescent="0.35">
+        <v>1768</v>
+      </c>
+    </row>
+    <row r="350" spans="1:2" ht="130.5" x14ac:dyDescent="0.35">
       <c r="A350" s="5" t="str">
         <v>WhyMyVitaeReason</v>
       </c>
       <c r="B350" s="3" t="s">
-        <v>1785</v>
+        <v>2096</v>
       </c>
     </row>
     <row r="351" spans="1:2" x14ac:dyDescent="0.35">
@@ -24274,7 +24364,7 @@
         <v>WhyMyVitaeTest</v>
       </c>
       <c r="B351" s="3" t="s">
-        <v>1793</v>
+        <v>1773</v>
       </c>
     </row>
     <row r="352" spans="1:2" x14ac:dyDescent="0.35">
@@ -24338,7 +24428,7 @@
         <v>Preview</v>
       </c>
       <c r="B359" s="3" t="s">
-        <v>1911</v>
+        <v>1891</v>
       </c>
     </row>
     <row r="360" spans="1:2" x14ac:dyDescent="0.35">
@@ -24346,7 +24436,7 @@
         <v>Error</v>
       </c>
       <c r="B360" s="3" t="s">
-        <v>1913</v>
+        <v>1893</v>
       </c>
     </row>
     <row r="361" spans="1:2" x14ac:dyDescent="0.35">
@@ -24354,7 +24444,7 @@
         <v>Demo</v>
       </c>
       <c r="B361" s="3" t="s">
-        <v>1917</v>
+        <v>1897</v>
       </c>
     </row>
     <row r="362" spans="1:2" x14ac:dyDescent="0.35">
@@ -24362,7 +24452,7 @@
         <v>Up</v>
       </c>
       <c r="B362" s="3" t="s">
-        <v>1931</v>
+        <v>1911</v>
       </c>
     </row>
     <row r="363" spans="1:2" x14ac:dyDescent="0.35">
@@ -24370,7 +24460,7 @@
         <v>Down</v>
       </c>
       <c r="B363" s="3" t="s">
-        <v>1932</v>
+        <v>1912</v>
       </c>
     </row>
     <row r="364" spans="1:2" ht="29" x14ac:dyDescent="0.35">
@@ -24378,7 +24468,7 @@
         <v>PasswordProtectionDesc</v>
       </c>
       <c r="B364" s="3" t="s">
-        <v>1936</v>
+        <v>1916</v>
       </c>
     </row>
     <row r="365" spans="1:2" x14ac:dyDescent="0.35">
@@ -24386,7 +24476,7 @@
         <v>SecurityCheck</v>
       </c>
       <c r="B365" s="3" t="s">
-        <v>1944</v>
+        <v>1924</v>
       </c>
     </row>
     <row r="366" spans="1:2" x14ac:dyDescent="0.35">
@@ -24394,7 +24484,7 @@
         <v>Status403</v>
       </c>
       <c r="B366" s="3" t="s">
-        <v>1996</v>
+        <v>1971</v>
       </c>
     </row>
     <row r="367" spans="1:2" ht="29" x14ac:dyDescent="0.35">
@@ -24402,7 +24492,7 @@
         <v>Status500</v>
       </c>
       <c r="B367" s="3" t="s">
-        <v>1997</v>
+        <v>1972</v>
       </c>
     </row>
     <row r="368" spans="1:2" x14ac:dyDescent="0.35">
@@ -24410,7 +24500,7 @@
         <v>Secure</v>
       </c>
       <c r="B368" s="3" t="s">
-        <v>1998</v>
+        <v>1973</v>
       </c>
     </row>
     <row r="369" spans="1:2" x14ac:dyDescent="0.35">
@@ -24418,7 +24508,7 @@
         <v>SecureDescription</v>
       </c>
       <c r="B369" s="3" t="s">
-        <v>1999</v>
+        <v>1974</v>
       </c>
     </row>
     <row r="370" spans="1:2" ht="29" x14ac:dyDescent="0.35">
@@ -24426,7 +24516,7 @@
         <v>SecurityCheckDesc</v>
       </c>
       <c r="B370" s="3" t="s">
-        <v>2000</v>
+        <v>1975</v>
       </c>
     </row>
     <row r="371" spans="1:2" x14ac:dyDescent="0.35">
@@ -24434,7 +24524,7 @@
         <v>Contact</v>
       </c>
       <c r="B371" s="3" t="s">
-        <v>2001</v>
+        <v>1976</v>
       </c>
     </row>
     <row r="372" spans="1:2" x14ac:dyDescent="0.35">
@@ -24442,7 +24532,7 @@
         <v>GoogleCaptcha</v>
       </c>
       <c r="B372" s="3" t="s">
-        <v>1964</v>
+        <v>1939</v>
       </c>
     </row>
     <row r="373" spans="1:2" ht="116" x14ac:dyDescent="0.35">
@@ -24450,7 +24540,7 @@
         <v>GoogleCaptchaDesc</v>
       </c>
       <c r="B373" s="3" t="s">
-        <v>2002</v>
+        <v>1977</v>
       </c>
     </row>
     <row r="374" spans="1:2" x14ac:dyDescent="0.35">
@@ -24458,7 +24548,7 @@
         <v>DataCollection</v>
       </c>
       <c r="B374" s="3" t="s">
-        <v>2003</v>
+        <v>1978</v>
       </c>
     </row>
     <row r="375" spans="1:2" ht="290" x14ac:dyDescent="0.35">
@@ -24466,7 +24556,7 @@
         <v>DataCollectionDesc</v>
       </c>
       <c r="B375" s="3" t="s">
-        <v>2004</v>
+        <v>1979</v>
       </c>
     </row>
     <row r="376" spans="1:2" x14ac:dyDescent="0.35">
@@ -24474,7 +24564,7 @@
         <v>Imprint</v>
       </c>
       <c r="B376" s="3" t="s">
-        <v>2010</v>
+        <v>1985</v>
       </c>
     </row>
     <row r="377" spans="1:2" ht="29" x14ac:dyDescent="0.35">
@@ -24482,7 +24572,7 @@
         <v>ErrorInfoMail</v>
       </c>
       <c r="B377" s="3" t="s">
-        <v>2016</v>
+        <v>1991</v>
       </c>
     </row>
     <row r="378" spans="1:2" x14ac:dyDescent="0.35">
@@ -24490,7 +24580,7 @@
         <v>Management</v>
       </c>
       <c r="B378" s="3" t="s">
-        <v>2022</v>
+        <v>1997</v>
       </c>
     </row>
     <row r="379" spans="1:2" x14ac:dyDescent="0.35">
@@ -24498,7 +24588,7 @@
         <v>Data</v>
       </c>
       <c r="B379" s="3" t="s">
-        <v>2027</v>
+        <v>2002</v>
       </c>
     </row>
     <row r="380" spans="1:2" x14ac:dyDescent="0.35">
@@ -24506,7 +24596,7 @@
         <v>Color</v>
       </c>
       <c r="B380" s="3" t="s">
-        <v>2028</v>
+        <v>2003</v>
       </c>
     </row>
     <row r="381" spans="1:2" x14ac:dyDescent="0.35">
@@ -24514,7 +24604,7 @@
         <v>ColorDescription</v>
       </c>
       <c r="B381" s="3" t="s">
-        <v>2037</v>
+        <v>2012</v>
       </c>
     </row>
     <row r="382" spans="1:2" x14ac:dyDescent="0.35">
@@ -24522,7 +24612,7 @@
         <v>Prefix</v>
       </c>
       <c r="B382" s="3" t="s">
-        <v>2042</v>
+        <v>2017</v>
       </c>
     </row>
     <row r="383" spans="1:2" x14ac:dyDescent="0.35">
@@ -24530,7 +24620,7 @@
         <v>LinkExperience</v>
       </c>
       <c r="B383" s="3" t="s">
-        <v>2075</v>
+        <v>2050</v>
       </c>
     </row>
     <row r="384" spans="1:2" x14ac:dyDescent="0.35">
@@ -24538,7 +24628,7 @@
         <v>LinkEducation</v>
       </c>
       <c r="B384" s="3" t="s">
-        <v>2076</v>
+        <v>2051</v>
       </c>
     </row>
     <row r="385" spans="1:2" x14ac:dyDescent="0.35">
@@ -24546,7 +24636,7 @@
         <v>LinkInterest</v>
       </c>
       <c r="B385" s="3" t="s">
-        <v>2077</v>
+        <v>2052</v>
       </c>
     </row>
     <row r="386" spans="1:2" x14ac:dyDescent="0.35">
@@ -24554,7 +24644,7 @@
         <v>LinkAwards</v>
       </c>
       <c r="B386" s="3" t="s">
-        <v>2078</v>
+        <v>2053</v>
       </c>
     </row>
     <row r="387" spans="1:2" x14ac:dyDescent="0.35">
@@ -24562,7 +24652,7 @@
         <v>LinkCertificate</v>
       </c>
       <c r="B387" s="3" t="s">
-        <v>2079</v>
+        <v>2054</v>
       </c>
     </row>
     <row r="388" spans="1:2" x14ac:dyDescent="0.35">
@@ -24570,7 +24660,7 @@
         <v>LinkReference</v>
       </c>
       <c r="B388" s="3" t="s">
-        <v>2080</v>
+        <v>2055</v>
       </c>
     </row>
     <row r="389" spans="1:2" x14ac:dyDescent="0.35">
@@ -24578,7 +24668,7 @@
         <v>ChronologicalAsc</v>
       </c>
       <c r="B389" s="3" t="s">
-        <v>2091</v>
+        <v>2066</v>
       </c>
     </row>
     <row r="390" spans="1:2" x14ac:dyDescent="0.35">
@@ -24586,22 +24676,31 @@
         <v>ChronologicalDesc</v>
       </c>
       <c r="B390" s="3" t="s">
-        <v>2090</v>
+        <v>2065</v>
       </c>
     </row>
     <row r="391" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A391" s="5" t="str">
-        <v xml:space="preserve"> </v>
+        <v>OptionalInformation</v>
+      </c>
+      <c r="B391" s="3" t="s">
+        <v>2074</v>
       </c>
     </row>
     <row r="392" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A392" s="5" t="str">
-        <v xml:space="preserve"> </v>
+        <v>MyVitaeSlogan</v>
+      </c>
+      <c r="B392" s="3" t="s">
+        <v>2080</v>
       </c>
     </row>
     <row r="393" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A393" s="5" t="str">
-        <v xml:space="preserve"> </v>
+        <v>DownloadQR</v>
+      </c>
+      <c r="B393" s="3" t="s">
+        <v>2086</v>
       </c>
     </row>
     <row r="394" spans="1:2" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Layout fixes with ViewBag
</commit_message>
<xml_diff>
--- a/Vitae/Library/Resources/SharedResource.xlsx
+++ b/Vitae/Library/Resources/SharedResource.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\Vitae\Library\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A6CB632-5AEA-4A84-B92C-46226B69A8AF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F95D589-D88F-4BFD-9EC5-A6C0C384029B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="30220" windowHeight="19620" tabRatio="406" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -5917,9 +5917,6 @@
     <t>Datenerfassung</t>
   </si>
   <si>
-    <t>Wenn Sie sich für myVitae anmelden, geben Sie uns freiwillig sensible Informationen. Dazu gehören Ihr Name, Ihr Geschlecht, Ihre E-Mail-Adresse, Ihre Telefonnummer, Ihr Profilfoto, Ihre Adresse, Ihr Familienstand und andere sensible Lebenslaufdaten. Diese Daten werden nicht an Dritte weitergegeben und ausschliesslich für die myVitae-Bewerbung verwendet. Zusätzlich werden die folgenden Daten ohne Ihr Zutun erhoben und bis zur automatisierten Löschung gespeichert: IP-Adresse des anfragenden Rechners sowie Geräte-ID bzw. individuelle Gerätekennung und Gerätetyp, Beschreibung des Typs des verwendeten Internet-Browsers und ggf. des Betriebssystems Ihres Endgerätes sowie der Name Ihres Zugangsproviders. Unser berechtigtes Interesse im Sinne des DSGVO an der Datenerhebung beruht auf den folgenden Zwecken: Die Sicherstellung einer komfortablen Nutzung der Website, die Bewertung der Systemsicherheit und -stabilität sowie die Nutzung für weitere administrative Zwecke. n Keinesfalls verwenden wir die erhobenen Daten, um Rückschlüsse auf Sie zu ziehen. Auf Anfrage teilen wir Ihnen gerne mit, ob und welche eindeutig personenbezogenen Daten über Sie gespeichert sind (GDPR).</t>
-  </si>
-  <si>
     <t>Sichern</t>
   </si>
   <si>
@@ -6370,9 +6367,6 @@
     <t>Para que su CV sea publicado, la aplicación web myVitae crea un enlace de publicación aleatorio. A continuación, puedes utilizar este enlace para una o más vacantes y eliminarlo completamente después de haber presentado tu solicitud con éxito. El panel de control le muestra el éxito de sus CVs publicados mostrando el número de clics en el enlace de publicación enviado. También puedes introducir tu currículum en un máximo de cinco idiomas.</t>
   </si>
   <si>
-    <t>Der Publikationslink ist anfänglich nur Ihnen bekannt und kann zusätzlich mit einem Passwort geschützt werden. Ausserdem kann mit einem Google Catcha ein weiterer Zusatzschutz gegen Bots eingesetzt werden. Für Blindbewerbungen eignet sich ausserdem die Anonymisierungsfunktion, welche einige sensible Informationen ausblendet.</t>
-  </si>
-  <si>
     <t>The publication link is initially known only to you and can also be protected with a password. Furthermore, a Google Catcha can be used to provide additional protection against bots. For blind applications, the anonymization function, which hides some sensitive information, is also suitable.</t>
   </si>
   <si>
@@ -6398,6 +6392,12 @@
   </si>
   <si>
     <t>Con tu página web de currículums personales puedes mantener tus datos actualizados y solicitar el siguiente trabajo con sólo unos pocos clics. Puedes concentrarte en lo esencial desde el principio y presentarte de la mejor manera posible. Así que nada se interpone en el camino de tu nuevo trabajo soñado. Le deseamos mucho éxito!</t>
+  </si>
+  <si>
+    <t>Der Publikationslink ist anfänglich nur Ihnen bekannt und kann zusätzlich mit einem Passwort geschützt werden. Ausserdem kann mit einem Google Catcha ein weiterer Zusatzschutz gegen Bots eingesetzt werden. Für Blindbewerbungen eignet sich zudem die Anonymisierungsfunktion, welche einige sensible Informationen ausblendet.</t>
+  </si>
+  <si>
+    <t>Wenn Sie sich für myVitae anmelden, geben Sie uns freiwillig sensible Informationen. Dazu gehören Ihr Name, Ihr Geschlecht, Ihre E-Mail-Adresse, Ihre Telefonnummer, Ihr Profilfoto, Ihre Adresse, Ihr Familienstand und andere sensible Lebenslaufdaten. Diese Daten werden nicht an Dritte weitergegeben und ausschliesslich für die myVitae-Bewerbung verwendet. Zusätzlich werden die folgenden Daten ohne Ihr Zutun erhoben und bis zur automatisierten Löschung gespeichert: IP-Adresse des anfragenden Rechners sowie Geräte-ID bzw. individuelle Gerätekennung und Gerätetyp, Beschreibung des Typs des verwendeten Internet-Browsers und ggf. des Betriebssystems Ihres Endgerätes sowie der Name Ihres Zugangsproviders. Unser berechtigtes Interesse im Sinne des DSGVO an der Datenerhebung beruht auf den folgenden Zwecken: Die Sicherstellung einer komfortablen Nutzung der Website, die Bewertung der Systemsicherheit und -stabilität sowie die Nutzung für weitere administrative Zwecke. Keinesfalls verwenden wir die erhobenen Daten, um Rückschlüsse auf Sie zu ziehen. Auf Anfrage teilen wir Ihnen gerne mit, ob und welche eindeutig personenbezogenen Daten über Sie gespeichert sind (GDPR).</t>
   </si>
 </sst>
 </file>
@@ -6944,7 +6944,7 @@
         <v>581</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>2087</v>
+        <v>2086</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.35">
@@ -7552,7 +7552,7 @@
         <v>1739</v>
       </c>
       <c r="B95" s="8" t="s">
-        <v>2098</v>
+        <v>2097</v>
       </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.35">
@@ -8416,7 +8416,7 @@
         <v>1865</v>
       </c>
       <c r="B203" s="3" t="s">
-        <v>1986</v>
+        <v>1985</v>
       </c>
     </row>
     <row r="204" spans="1:2" x14ac:dyDescent="0.35">
@@ -9136,7 +9136,7 @@
         <v>1750</v>
       </c>
       <c r="B293" s="8" t="s">
-        <v>2103</v>
+        <v>2101</v>
       </c>
     </row>
     <row r="294" spans="1:2" x14ac:dyDescent="0.35">
@@ -9224,7 +9224,7 @@
         <v>1753</v>
       </c>
       <c r="B304" s="8" t="s">
-        <v>2108</v>
+        <v>2106</v>
       </c>
     </row>
     <row r="305" spans="1:2" x14ac:dyDescent="0.35">
@@ -9592,7 +9592,7 @@
         <v>1736</v>
       </c>
       <c r="B350" s="8" t="s">
-        <v>2092</v>
+        <v>2091</v>
       </c>
     </row>
     <row r="351" spans="1:2" x14ac:dyDescent="0.35">
@@ -9781,7 +9781,7 @@
     </row>
     <row r="374" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A374" s="5" t="s">
-        <v>2056</v>
+        <v>2055</v>
       </c>
       <c r="B374" s="3" t="s">
         <v>1942</v>
@@ -9797,146 +9797,146 @@
     </row>
     <row r="376" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A376" s="5" t="s">
-        <v>1981</v>
+        <v>1980</v>
       </c>
       <c r="B376" s="3" t="s">
-        <v>1981</v>
+        <v>1980</v>
       </c>
     </row>
     <row r="377" spans="1:2" ht="29" x14ac:dyDescent="0.35">
       <c r="A377" s="5" t="s">
-        <v>1992</v>
+        <v>1991</v>
       </c>
       <c r="B377" s="3" t="s">
-        <v>1987</v>
+        <v>1986</v>
       </c>
     </row>
     <row r="378" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A378" s="5" t="s">
-        <v>1993</v>
+        <v>1992</v>
       </c>
       <c r="B378" s="3" t="s">
-        <v>1993</v>
+        <v>1992</v>
       </c>
     </row>
     <row r="379" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A379" s="5" t="s">
-        <v>1998</v>
+        <v>1997</v>
       </c>
       <c r="B379" s="3" t="s">
-        <v>1998</v>
+        <v>1997</v>
       </c>
     </row>
     <row r="380" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A380" s="5" t="s">
-        <v>2003</v>
+        <v>2002</v>
       </c>
       <c r="B380" s="3" t="s">
-        <v>2003</v>
+        <v>2002</v>
       </c>
     </row>
     <row r="381" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A381" s="5" t="s">
+        <v>2006</v>
+      </c>
+      <c r="B381" s="3" t="s">
         <v>2007</v>
-      </c>
-      <c r="B381" s="3" t="s">
-        <v>2008</v>
       </c>
     </row>
     <row r="382" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A382" s="5" t="s">
-        <v>2013</v>
+        <v>2012</v>
       </c>
       <c r="B382" s="3" t="s">
-        <v>2013</v>
+        <v>2012</v>
       </c>
     </row>
     <row r="383" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A383" s="5" t="s">
+        <v>2019</v>
+      </c>
+      <c r="B383" s="3" t="s">
         <v>2020</v>
-      </c>
-      <c r="B383" s="3" t="s">
-        <v>2021</v>
       </c>
     </row>
     <row r="384" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A384" s="5" t="s">
+        <v>2021</v>
+      </c>
+      <c r="B384" s="3" t="s">
         <v>2022</v>
-      </c>
-      <c r="B384" s="3" t="s">
-        <v>2023</v>
       </c>
     </row>
     <row r="385" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A385" s="5" t="s">
-        <v>2024</v>
+        <v>2023</v>
       </c>
       <c r="B385" s="3" t="s">
-        <v>2031</v>
+        <v>2030</v>
       </c>
     </row>
     <row r="386" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A386" s="5" t="s">
+        <v>2024</v>
+      </c>
+      <c r="B386" s="3" t="s">
         <v>2025</v>
-      </c>
-      <c r="B386" s="3" t="s">
-        <v>2026</v>
       </c>
     </row>
     <row r="387" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A387" s="5" t="s">
+        <v>2026</v>
+      </c>
+      <c r="B387" s="3" t="s">
         <v>2027</v>
-      </c>
-      <c r="B387" s="3" t="s">
-        <v>2028</v>
       </c>
     </row>
     <row r="388" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A388" s="5" t="s">
+        <v>2028</v>
+      </c>
+      <c r="B388" s="3" t="s">
         <v>2029</v>
-      </c>
-      <c r="B388" s="3" t="s">
-        <v>2030</v>
       </c>
     </row>
     <row r="389" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A389" s="5" t="s">
-        <v>2057</v>
+        <v>2056</v>
       </c>
       <c r="B389" s="3" t="s">
-        <v>2059</v>
+        <v>2058</v>
       </c>
     </row>
     <row r="390" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A390" s="5" t="s">
-        <v>2058</v>
+        <v>2057</v>
       </c>
       <c r="B390" s="3" t="s">
-        <v>2060</v>
+        <v>2059</v>
       </c>
     </row>
     <row r="391" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A391" s="5" t="s">
+        <v>2068</v>
+      </c>
+      <c r="B391" s="3" t="s">
         <v>2069</v>
-      </c>
-      <c r="B391" s="3" t="s">
-        <v>2070</v>
       </c>
     </row>
     <row r="392" spans="1:2" ht="14" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A392" s="5" t="s">
-        <v>2075</v>
+        <v>2074</v>
       </c>
       <c r="B392" s="3" t="s">
-        <v>2078</v>
+        <v>2077</v>
       </c>
     </row>
     <row r="393" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A393" s="5" t="s">
-        <v>2082</v>
+        <v>2081</v>
       </c>
       <c r="B393" s="3" t="s">
-        <v>2081</v>
+        <v>2080</v>
       </c>
     </row>
     <row r="394" spans="1:2" x14ac:dyDescent="0.35">
@@ -10479,8 +10479,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B498"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A275" workbookViewId="0">
-      <selection activeCell="A275" sqref="A1:B1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A365" workbookViewId="0">
+      <selection activeCell="J374" sqref="J374"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -10503,7 +10503,7 @@
         <v>AboutDetailsDescription</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>2018</v>
+        <v>2017</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
@@ -10639,7 +10639,7 @@
         <v>AdTextB0</v>
       </c>
       <c r="B19" s="7" t="s">
-        <v>2091</v>
+        <v>2090</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.35">
@@ -10887,7 +10887,7 @@
         <v>ChooseFile</v>
       </c>
       <c r="B50" s="7" t="s">
-        <v>2019</v>
+        <v>2018</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.35">
@@ -11247,7 +11247,7 @@
         <v>DashboardOverview</v>
       </c>
       <c r="B95" s="8" t="s">
-        <v>2097</v>
+        <v>2096</v>
       </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.35">
@@ -12831,7 +12831,7 @@
         <v>SavePublicationsDescription</v>
       </c>
       <c r="B293" s="8" t="s">
-        <v>2102</v>
+        <v>2110</v>
       </c>
     </row>
     <row r="294" spans="1:2" x14ac:dyDescent="0.35">
@@ -12919,7 +12919,7 @@
         <v>ShowYourStrengthsDescription</v>
       </c>
       <c r="B304" s="8" t="s">
-        <v>2107</v>
+        <v>2105</v>
       </c>
     </row>
     <row r="305" spans="1:2" x14ac:dyDescent="0.35">
@@ -13287,7 +13287,7 @@
         <v>WhyMyVitaeReason</v>
       </c>
       <c r="B350" s="8" t="s">
-        <v>2093</v>
+        <v>2092</v>
       </c>
     </row>
     <row r="351" spans="1:2" x14ac:dyDescent="0.35">
@@ -13431,7 +13431,7 @@
         <v>Secure</v>
       </c>
       <c r="B368" s="8" t="s">
-        <v>1952</v>
+        <v>1951</v>
       </c>
     </row>
     <row r="369" spans="1:2" ht="29" x14ac:dyDescent="0.35">
@@ -13439,7 +13439,7 @@
         <v>SecureDescription</v>
       </c>
       <c r="B369" s="8" t="s">
-        <v>1980</v>
+        <v>1979</v>
       </c>
     </row>
     <row r="370" spans="1:2" ht="29" x14ac:dyDescent="0.35">
@@ -13487,7 +13487,7 @@
         <v>DataCollectionDesc</v>
       </c>
       <c r="B375" s="8" t="s">
-        <v>1951</v>
+        <v>2111</v>
       </c>
     </row>
     <row r="376" spans="1:2" x14ac:dyDescent="0.35">
@@ -13495,7 +13495,7 @@
         <v>Imprint</v>
       </c>
       <c r="B376" s="8" t="s">
-        <v>1982</v>
+        <v>1981</v>
       </c>
     </row>
     <row r="377" spans="1:2" ht="29" x14ac:dyDescent="0.35">
@@ -13503,7 +13503,7 @@
         <v>ErrorInfoMail</v>
       </c>
       <c r="B377" s="3" t="s">
-        <v>1988</v>
+        <v>1987</v>
       </c>
     </row>
     <row r="378" spans="1:2" x14ac:dyDescent="0.35">
@@ -13511,7 +13511,7 @@
         <v>Management</v>
       </c>
       <c r="B378" s="8" t="s">
-        <v>1994</v>
+        <v>1993</v>
       </c>
     </row>
     <row r="379" spans="1:2" x14ac:dyDescent="0.35">
@@ -13519,7 +13519,7 @@
         <v>Data</v>
       </c>
       <c r="B379" s="8" t="s">
-        <v>1999</v>
+        <v>1998</v>
       </c>
     </row>
     <row r="380" spans="1:2" x14ac:dyDescent="0.35">
@@ -13527,7 +13527,7 @@
         <v>Color</v>
       </c>
       <c r="B380" s="8" t="s">
-        <v>2004</v>
+        <v>2003</v>
       </c>
     </row>
     <row r="381" spans="1:2" x14ac:dyDescent="0.35">
@@ -13535,7 +13535,7 @@
         <v>ColorDescription</v>
       </c>
       <c r="B381" s="3" t="s">
-        <v>2009</v>
+        <v>2008</v>
       </c>
     </row>
     <row r="382" spans="1:2" x14ac:dyDescent="0.35">
@@ -13543,7 +13543,7 @@
         <v>Prefix</v>
       </c>
       <c r="B382" s="8" t="s">
-        <v>2014</v>
+        <v>2013</v>
       </c>
     </row>
     <row r="383" spans="1:2" x14ac:dyDescent="0.35">
@@ -13551,7 +13551,7 @@
         <v>LinkExperience</v>
       </c>
       <c r="B383" s="8" t="s">
-        <v>2032</v>
+        <v>2031</v>
       </c>
     </row>
     <row r="384" spans="1:2" x14ac:dyDescent="0.35">
@@ -13559,7 +13559,7 @@
         <v>LinkEducation</v>
       </c>
       <c r="B384" s="8" t="s">
-        <v>2033</v>
+        <v>2032</v>
       </c>
     </row>
     <row r="385" spans="1:2" x14ac:dyDescent="0.35">
@@ -13567,7 +13567,7 @@
         <v>LinkInterest</v>
       </c>
       <c r="B385" s="8" t="s">
-        <v>2034</v>
+        <v>2033</v>
       </c>
     </row>
     <row r="386" spans="1:2" x14ac:dyDescent="0.35">
@@ -13575,7 +13575,7 @@
         <v>LinkAwards</v>
       </c>
       <c r="B386" s="8" t="s">
-        <v>2035</v>
+        <v>2034</v>
       </c>
     </row>
     <row r="387" spans="1:2" x14ac:dyDescent="0.35">
@@ -13583,7 +13583,7 @@
         <v>LinkCertificate</v>
       </c>
       <c r="B387" s="8" t="s">
-        <v>2036</v>
+        <v>2035</v>
       </c>
     </row>
     <row r="388" spans="1:2" x14ac:dyDescent="0.35">
@@ -13591,7 +13591,7 @@
         <v>LinkReference</v>
       </c>
       <c r="B388" s="8" t="s">
-        <v>2037</v>
+        <v>2036</v>
       </c>
     </row>
     <row r="389" spans="1:2" ht="29" x14ac:dyDescent="0.35">
@@ -13599,7 +13599,7 @@
         <v>ChronologicalAsc</v>
       </c>
       <c r="B389" s="3" t="s">
-        <v>2061</v>
+        <v>2060</v>
       </c>
     </row>
     <row r="390" spans="1:2" ht="29" x14ac:dyDescent="0.35">
@@ -13607,7 +13607,7 @@
         <v>ChronologicalDesc</v>
       </c>
       <c r="B390" s="3" t="s">
-        <v>2062</v>
+        <v>2061</v>
       </c>
     </row>
     <row r="391" spans="1:2" x14ac:dyDescent="0.35">
@@ -13615,7 +13615,7 @@
         <v>OptionalInformation</v>
       </c>
       <c r="B391" s="8" t="s">
-        <v>2071</v>
+        <v>2070</v>
       </c>
     </row>
     <row r="392" spans="1:2" x14ac:dyDescent="0.35">
@@ -13623,7 +13623,7 @@
         <v>MyVitaeSlogan</v>
       </c>
       <c r="B392" s="8" t="s">
-        <v>2077</v>
+        <v>2076</v>
       </c>
     </row>
     <row r="393" spans="1:2" x14ac:dyDescent="0.35">
@@ -13631,7 +13631,7 @@
         <v>DownloadQR</v>
       </c>
       <c r="B393" s="8" t="s">
-        <v>2083</v>
+        <v>2082</v>
       </c>
     </row>
     <row r="394" spans="1:2" x14ac:dyDescent="0.35">
@@ -14329,7 +14329,7 @@
         <v>AdTextB0</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>2088</v>
+        <v>2087</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.35">
@@ -14937,7 +14937,7 @@
         <v>DashboardOverview</v>
       </c>
       <c r="B95" s="3" t="s">
-        <v>2099</v>
+        <v>2098</v>
       </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.35">
@@ -16521,7 +16521,7 @@
         <v>SavePublicationsDescription</v>
       </c>
       <c r="B293" s="3" t="s">
-        <v>2104</v>
+        <v>2102</v>
       </c>
     </row>
     <row r="294" spans="1:2" x14ac:dyDescent="0.35">
@@ -16609,7 +16609,7 @@
         <v>ShowYourStrengthsDescription</v>
       </c>
       <c r="B304" s="3" t="s">
-        <v>2109</v>
+        <v>2107</v>
       </c>
     </row>
     <row r="305" spans="1:2" x14ac:dyDescent="0.35">
@@ -16977,7 +16977,7 @@
         <v>WhyMyVitaeReason</v>
       </c>
       <c r="B350" s="3" t="s">
-        <v>2094</v>
+        <v>2093</v>
       </c>
     </row>
     <row r="351" spans="1:2" x14ac:dyDescent="0.35">
@@ -17105,7 +17105,7 @@
         <v>Status403</v>
       </c>
       <c r="B366" s="3" t="s">
-        <v>1953</v>
+        <v>1952</v>
       </c>
     </row>
     <row r="367" spans="1:2" ht="29" x14ac:dyDescent="0.35">
@@ -17113,7 +17113,7 @@
         <v>Status500</v>
       </c>
       <c r="B367" s="3" t="s">
-        <v>1954</v>
+        <v>1953</v>
       </c>
     </row>
     <row r="368" spans="1:2" x14ac:dyDescent="0.35">
@@ -17121,7 +17121,7 @@
         <v>Secure</v>
       </c>
       <c r="B368" s="3" t="s">
-        <v>1955</v>
+        <v>1954</v>
       </c>
     </row>
     <row r="369" spans="1:2" ht="29" x14ac:dyDescent="0.35">
@@ -17129,7 +17129,7 @@
         <v>SecureDescription</v>
       </c>
       <c r="B369" s="3" t="s">
-        <v>1956</v>
+        <v>1955</v>
       </c>
     </row>
     <row r="370" spans="1:2" x14ac:dyDescent="0.35">
@@ -17137,7 +17137,7 @@
         <v>SecurityCheckDesc</v>
       </c>
       <c r="B370" s="3" t="s">
-        <v>1957</v>
+        <v>1956</v>
       </c>
     </row>
     <row r="371" spans="1:2" x14ac:dyDescent="0.35">
@@ -17145,7 +17145,7 @@
         <v>Contact</v>
       </c>
       <c r="B371" s="3" t="s">
-        <v>1958</v>
+        <v>1957</v>
       </c>
     </row>
     <row r="372" spans="1:2" x14ac:dyDescent="0.35">
@@ -17161,7 +17161,7 @@
         <v>GoogleCaptchaDesc</v>
       </c>
       <c r="B373" s="3" t="s">
-        <v>1959</v>
+        <v>1958</v>
       </c>
     </row>
     <row r="374" spans="1:2" x14ac:dyDescent="0.35">
@@ -17169,7 +17169,7 @@
         <v>DataCollection</v>
       </c>
       <c r="B374" s="3" t="s">
-        <v>1960</v>
+        <v>1959</v>
       </c>
     </row>
     <row r="375" spans="1:2" ht="307" customHeight="1" x14ac:dyDescent="0.35">
@@ -17177,7 +17177,7 @@
         <v>DataCollectionDesc</v>
       </c>
       <c r="B375" s="3" t="s">
-        <v>1961</v>
+        <v>1960</v>
       </c>
     </row>
     <row r="376" spans="1:2" x14ac:dyDescent="0.35">
@@ -17185,7 +17185,7 @@
         <v>Imprint</v>
       </c>
       <c r="B376" s="3" t="s">
-        <v>1983</v>
+        <v>1982</v>
       </c>
     </row>
     <row r="377" spans="1:2" ht="29" x14ac:dyDescent="0.35">
@@ -17193,7 +17193,7 @@
         <v>ErrorInfoMail</v>
       </c>
       <c r="B377" s="3" t="s">
-        <v>1989</v>
+        <v>1988</v>
       </c>
     </row>
     <row r="378" spans="1:2" x14ac:dyDescent="0.35">
@@ -17201,7 +17201,7 @@
         <v>Management</v>
       </c>
       <c r="B378" s="3" t="s">
-        <v>1995</v>
+        <v>1994</v>
       </c>
     </row>
     <row r="379" spans="1:2" x14ac:dyDescent="0.35">
@@ -17209,7 +17209,7 @@
         <v>Data</v>
       </c>
       <c r="B379" s="3" t="s">
-        <v>2000</v>
+        <v>1999</v>
       </c>
     </row>
     <row r="380" spans="1:2" x14ac:dyDescent="0.35">
@@ -17217,7 +17217,7 @@
         <v>Color</v>
       </c>
       <c r="B380" s="3" t="s">
-        <v>2005</v>
+        <v>2004</v>
       </c>
     </row>
     <row r="381" spans="1:2" x14ac:dyDescent="0.35">
@@ -17225,7 +17225,7 @@
         <v>ColorDescription</v>
       </c>
       <c r="B381" s="3" t="s">
-        <v>2010</v>
+        <v>2009</v>
       </c>
     </row>
     <row r="382" spans="1:2" x14ac:dyDescent="0.35">
@@ -17233,7 +17233,7 @@
         <v>Prefix</v>
       </c>
       <c r="B382" s="3" t="s">
-        <v>2015</v>
+        <v>2014</v>
       </c>
     </row>
     <row r="383" spans="1:2" x14ac:dyDescent="0.35">
@@ -17241,7 +17241,7 @@
         <v>LinkExperience</v>
       </c>
       <c r="B383" s="3" t="s">
-        <v>2038</v>
+        <v>2037</v>
       </c>
     </row>
     <row r="384" spans="1:2" x14ac:dyDescent="0.35">
@@ -17249,7 +17249,7 @@
         <v>LinkEducation</v>
       </c>
       <c r="B384" s="3" t="s">
-        <v>2039</v>
+        <v>2038</v>
       </c>
     </row>
     <row r="385" spans="1:2" x14ac:dyDescent="0.35">
@@ -17257,7 +17257,7 @@
         <v>LinkInterest</v>
       </c>
       <c r="B385" s="3" t="s">
-        <v>2040</v>
+        <v>2039</v>
       </c>
     </row>
     <row r="386" spans="1:2" x14ac:dyDescent="0.35">
@@ -17265,7 +17265,7 @@
         <v>LinkAwards</v>
       </c>
       <c r="B386" s="3" t="s">
-        <v>2041</v>
+        <v>2040</v>
       </c>
     </row>
     <row r="387" spans="1:2" x14ac:dyDescent="0.35">
@@ -17273,7 +17273,7 @@
         <v>LinkCertificate</v>
       </c>
       <c r="B387" s="3" t="s">
-        <v>2042</v>
+        <v>2041</v>
       </c>
     </row>
     <row r="388" spans="1:2" x14ac:dyDescent="0.35">
@@ -17281,7 +17281,7 @@
         <v>LinkReference</v>
       </c>
       <c r="B388" s="3" t="s">
-        <v>2043</v>
+        <v>2042</v>
       </c>
     </row>
     <row r="389" spans="1:2" x14ac:dyDescent="0.35">
@@ -17289,7 +17289,7 @@
         <v>ChronologicalAsc</v>
       </c>
       <c r="B389" s="3" t="s">
-        <v>2068</v>
+        <v>2067</v>
       </c>
     </row>
     <row r="390" spans="1:2" x14ac:dyDescent="0.35">
@@ -17297,7 +17297,7 @@
         <v>ChronologicalDesc</v>
       </c>
       <c r="B390" s="3" t="s">
-        <v>2063</v>
+        <v>2062</v>
       </c>
     </row>
     <row r="391" spans="1:2" x14ac:dyDescent="0.35">
@@ -17305,7 +17305,7 @@
         <v>OptionalInformation</v>
       </c>
       <c r="B391" s="3" t="s">
-        <v>2072</v>
+        <v>2071</v>
       </c>
     </row>
     <row r="392" spans="1:2" x14ac:dyDescent="0.35">
@@ -17313,7 +17313,7 @@
         <v>MyVitaeSlogan</v>
       </c>
       <c r="B392" s="3" t="s">
-        <v>2076</v>
+        <v>2075</v>
       </c>
     </row>
     <row r="393" spans="1:2" x14ac:dyDescent="0.35">
@@ -17321,7 +17321,7 @@
         <v>DownloadQR</v>
       </c>
       <c r="B393" s="3" t="s">
-        <v>2084</v>
+        <v>2083</v>
       </c>
     </row>
     <row r="394" spans="1:2" x14ac:dyDescent="0.35">
@@ -18018,7 +18018,7 @@
         <v>AdTextB0</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>2089</v>
+        <v>2088</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.35">
@@ -18626,7 +18626,7 @@
         <v>DashboardOverview</v>
       </c>
       <c r="B95" s="3" t="s">
-        <v>2100</v>
+        <v>2099</v>
       </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.35">
@@ -20210,7 +20210,7 @@
         <v>SavePublicationsDescription</v>
       </c>
       <c r="B293" s="3" t="s">
-        <v>2105</v>
+        <v>2103</v>
       </c>
     </row>
     <row r="294" spans="1:2" x14ac:dyDescent="0.35">
@@ -20298,7 +20298,7 @@
         <v>ShowYourStrengthsDescription</v>
       </c>
       <c r="B304" s="3" t="s">
-        <v>2110</v>
+        <v>2108</v>
       </c>
     </row>
     <row r="305" spans="1:2" x14ac:dyDescent="0.35">
@@ -20666,7 +20666,7 @@
         <v>WhyMyVitaeReason</v>
       </c>
       <c r="B350" s="3" t="s">
-        <v>2095</v>
+        <v>2094</v>
       </c>
     </row>
     <row r="351" spans="1:2" x14ac:dyDescent="0.35">
@@ -20794,7 +20794,7 @@
         <v>Status403</v>
       </c>
       <c r="B366" s="3" t="s">
-        <v>1962</v>
+        <v>1961</v>
       </c>
     </row>
     <row r="367" spans="1:2" ht="29" x14ac:dyDescent="0.35">
@@ -20802,7 +20802,7 @@
         <v>Status500</v>
       </c>
       <c r="B367" s="3" t="s">
-        <v>1963</v>
+        <v>1962</v>
       </c>
     </row>
     <row r="368" spans="1:2" x14ac:dyDescent="0.35">
@@ -20810,7 +20810,7 @@
         <v>Secure</v>
       </c>
       <c r="B368" s="3" t="s">
-        <v>1964</v>
+        <v>1963</v>
       </c>
     </row>
     <row r="369" spans="1:2" x14ac:dyDescent="0.35">
@@ -20818,15 +20818,15 @@
         <v>SecureDescription</v>
       </c>
       <c r="B369" s="3" t="s">
-        <v>1965</v>
-      </c>
-    </row>
-    <row r="370" spans="1:2" x14ac:dyDescent="0.35">
+        <v>1964</v>
+      </c>
+    </row>
+    <row r="370" spans="1:2" ht="29" x14ac:dyDescent="0.35">
       <c r="A370" s="5" t="str">
         <v>SecurityCheckDesc</v>
       </c>
       <c r="B370" s="3" t="s">
-        <v>1966</v>
+        <v>1965</v>
       </c>
     </row>
     <row r="371" spans="1:2" x14ac:dyDescent="0.35">
@@ -20834,7 +20834,7 @@
         <v>Contact</v>
       </c>
       <c r="B371" s="3" t="s">
-        <v>1967</v>
+        <v>1966</v>
       </c>
     </row>
     <row r="372" spans="1:2" x14ac:dyDescent="0.35">
@@ -20850,7 +20850,7 @@
         <v>GoogleCaptchaDesc</v>
       </c>
       <c r="B373" s="3" t="s">
-        <v>1968</v>
+        <v>1967</v>
       </c>
     </row>
     <row r="374" spans="1:2" x14ac:dyDescent="0.35">
@@ -20858,7 +20858,7 @@
         <v>DataCollection</v>
       </c>
       <c r="B374" s="3" t="s">
-        <v>1969</v>
+        <v>1968</v>
       </c>
     </row>
     <row r="375" spans="1:2" ht="261" x14ac:dyDescent="0.35">
@@ -20866,7 +20866,7 @@
         <v>DataCollectionDesc</v>
       </c>
       <c r="B375" s="3" t="s">
-        <v>1970</v>
+        <v>1969</v>
       </c>
     </row>
     <row r="376" spans="1:2" x14ac:dyDescent="0.35">
@@ -20874,7 +20874,7 @@
         <v>Imprint</v>
       </c>
       <c r="B376" s="3" t="s">
-        <v>1984</v>
+        <v>1983</v>
       </c>
     </row>
     <row r="377" spans="1:2" ht="29" x14ac:dyDescent="0.35">
@@ -20882,7 +20882,7 @@
         <v>ErrorInfoMail</v>
       </c>
       <c r="B377" s="3" t="s">
-        <v>1990</v>
+        <v>1989</v>
       </c>
     </row>
     <row r="378" spans="1:2" x14ac:dyDescent="0.35">
@@ -20890,7 +20890,7 @@
         <v>Management</v>
       </c>
       <c r="B378" s="3" t="s">
-        <v>1996</v>
+        <v>1995</v>
       </c>
     </row>
     <row r="379" spans="1:2" x14ac:dyDescent="0.35">
@@ -20898,7 +20898,7 @@
         <v>Data</v>
       </c>
       <c r="B379" s="3" t="s">
-        <v>2001</v>
+        <v>2000</v>
       </c>
     </row>
     <row r="380" spans="1:2" x14ac:dyDescent="0.35">
@@ -20906,7 +20906,7 @@
         <v>Color</v>
       </c>
       <c r="B380" s="3" t="s">
-        <v>2006</v>
+        <v>2005</v>
       </c>
     </row>
     <row r="381" spans="1:2" x14ac:dyDescent="0.35">
@@ -20914,7 +20914,7 @@
         <v>ColorDescription</v>
       </c>
       <c r="B381" s="3" t="s">
-        <v>2011</v>
+        <v>2010</v>
       </c>
     </row>
     <row r="382" spans="1:2" x14ac:dyDescent="0.35">
@@ -20922,7 +20922,7 @@
         <v>Prefix</v>
       </c>
       <c r="B382" s="3" t="s">
-        <v>2016</v>
+        <v>2015</v>
       </c>
     </row>
     <row r="383" spans="1:2" x14ac:dyDescent="0.35">
@@ -20930,7 +20930,7 @@
         <v>LinkExperience</v>
       </c>
       <c r="B383" s="3" t="s">
-        <v>2044</v>
+        <v>2043</v>
       </c>
     </row>
     <row r="384" spans="1:2" x14ac:dyDescent="0.35">
@@ -20938,7 +20938,7 @@
         <v>LinkEducation</v>
       </c>
       <c r="B384" s="3" t="s">
-        <v>2045</v>
+        <v>2044</v>
       </c>
     </row>
     <row r="385" spans="1:2" x14ac:dyDescent="0.35">
@@ -20946,7 +20946,7 @@
         <v>LinkInterest</v>
       </c>
       <c r="B385" s="3" t="s">
-        <v>2046</v>
+        <v>2045</v>
       </c>
     </row>
     <row r="386" spans="1:2" x14ac:dyDescent="0.35">
@@ -20954,7 +20954,7 @@
         <v>LinkAwards</v>
       </c>
       <c r="B386" s="3" t="s">
-        <v>2047</v>
+        <v>2046</v>
       </c>
     </row>
     <row r="387" spans="1:2" x14ac:dyDescent="0.35">
@@ -20962,7 +20962,7 @@
         <v>LinkCertificate</v>
       </c>
       <c r="B387" s="3" t="s">
-        <v>2048</v>
+        <v>2047</v>
       </c>
     </row>
     <row r="388" spans="1:2" x14ac:dyDescent="0.35">
@@ -20970,7 +20970,7 @@
         <v>LinkReference</v>
       </c>
       <c r="B388" s="3" t="s">
-        <v>2049</v>
+        <v>2048</v>
       </c>
     </row>
     <row r="389" spans="1:2" x14ac:dyDescent="0.35">
@@ -20978,7 +20978,7 @@
         <v>ChronologicalAsc</v>
       </c>
       <c r="B389" s="3" t="s">
-        <v>2067</v>
+        <v>2066</v>
       </c>
     </row>
     <row r="390" spans="1:2" x14ac:dyDescent="0.35">
@@ -20986,7 +20986,7 @@
         <v>ChronologicalDesc</v>
       </c>
       <c r="B390" s="3" t="s">
-        <v>2064</v>
+        <v>2063</v>
       </c>
     </row>
     <row r="391" spans="1:2" x14ac:dyDescent="0.35">
@@ -20994,7 +20994,7 @@
         <v>OptionalInformation</v>
       </c>
       <c r="B391" s="3" t="s">
-        <v>2073</v>
+        <v>2072</v>
       </c>
     </row>
     <row r="392" spans="1:2" x14ac:dyDescent="0.35">
@@ -21002,7 +21002,7 @@
         <v>MyVitaeSlogan</v>
       </c>
       <c r="B392" s="3" t="s">
-        <v>2079</v>
+        <v>2078</v>
       </c>
     </row>
     <row r="393" spans="1:2" x14ac:dyDescent="0.35">
@@ -21010,7 +21010,7 @@
         <v>DownloadQR</v>
       </c>
       <c r="B393" s="3" t="s">
-        <v>2085</v>
+        <v>2084</v>
       </c>
     </row>
     <row r="394" spans="1:2" x14ac:dyDescent="0.35">
@@ -21708,7 +21708,7 @@
         <v>AdTextB0</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>2090</v>
+        <v>2089</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.35">
@@ -22316,7 +22316,7 @@
         <v>DashboardOverview</v>
       </c>
       <c r="B95" s="3" t="s">
-        <v>2101</v>
+        <v>2100</v>
       </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.35">
@@ -23900,7 +23900,7 @@
         <v>SavePublicationsDescription</v>
       </c>
       <c r="B293" s="3" t="s">
-        <v>2106</v>
+        <v>2104</v>
       </c>
     </row>
     <row r="294" spans="1:2" x14ac:dyDescent="0.35">
@@ -23988,7 +23988,7 @@
         <v>ShowYourStrengthsDescription</v>
       </c>
       <c r="B304" s="3" t="s">
-        <v>2111</v>
+        <v>2109</v>
       </c>
     </row>
     <row r="305" spans="1:2" x14ac:dyDescent="0.35">
@@ -24356,7 +24356,7 @@
         <v>WhyMyVitaeReason</v>
       </c>
       <c r="B350" s="3" t="s">
-        <v>2096</v>
+        <v>2095</v>
       </c>
     </row>
     <row r="351" spans="1:2" x14ac:dyDescent="0.35">
@@ -24484,7 +24484,7 @@
         <v>Status403</v>
       </c>
       <c r="B366" s="3" t="s">
-        <v>1971</v>
+        <v>1970</v>
       </c>
     </row>
     <row r="367" spans="1:2" ht="29" x14ac:dyDescent="0.35">
@@ -24492,7 +24492,7 @@
         <v>Status500</v>
       </c>
       <c r="B367" s="3" t="s">
-        <v>1972</v>
+        <v>1971</v>
       </c>
     </row>
     <row r="368" spans="1:2" x14ac:dyDescent="0.35">
@@ -24500,7 +24500,7 @@
         <v>Secure</v>
       </c>
       <c r="B368" s="3" t="s">
-        <v>1973</v>
+        <v>1972</v>
       </c>
     </row>
     <row r="369" spans="1:2" x14ac:dyDescent="0.35">
@@ -24508,7 +24508,7 @@
         <v>SecureDescription</v>
       </c>
       <c r="B369" s="3" t="s">
-        <v>1974</v>
+        <v>1973</v>
       </c>
     </row>
     <row r="370" spans="1:2" ht="29" x14ac:dyDescent="0.35">
@@ -24516,7 +24516,7 @@
         <v>SecurityCheckDesc</v>
       </c>
       <c r="B370" s="3" t="s">
-        <v>1975</v>
+        <v>1974</v>
       </c>
     </row>
     <row r="371" spans="1:2" x14ac:dyDescent="0.35">
@@ -24524,7 +24524,7 @@
         <v>Contact</v>
       </c>
       <c r="B371" s="3" t="s">
-        <v>1976</v>
+        <v>1975</v>
       </c>
     </row>
     <row r="372" spans="1:2" x14ac:dyDescent="0.35">
@@ -24540,7 +24540,7 @@
         <v>GoogleCaptchaDesc</v>
       </c>
       <c r="B373" s="3" t="s">
-        <v>1977</v>
+        <v>1976</v>
       </c>
     </row>
     <row r="374" spans="1:2" x14ac:dyDescent="0.35">
@@ -24548,7 +24548,7 @@
         <v>DataCollection</v>
       </c>
       <c r="B374" s="3" t="s">
-        <v>1978</v>
+        <v>1977</v>
       </c>
     </row>
     <row r="375" spans="1:2" ht="290" x14ac:dyDescent="0.35">
@@ -24556,7 +24556,7 @@
         <v>DataCollectionDesc</v>
       </c>
       <c r="B375" s="3" t="s">
-        <v>1979</v>
+        <v>1978</v>
       </c>
     </row>
     <row r="376" spans="1:2" x14ac:dyDescent="0.35">
@@ -24564,7 +24564,7 @@
         <v>Imprint</v>
       </c>
       <c r="B376" s="3" t="s">
-        <v>1985</v>
+        <v>1984</v>
       </c>
     </row>
     <row r="377" spans="1:2" ht="29" x14ac:dyDescent="0.35">
@@ -24572,7 +24572,7 @@
         <v>ErrorInfoMail</v>
       </c>
       <c r="B377" s="3" t="s">
-        <v>1991</v>
+        <v>1990</v>
       </c>
     </row>
     <row r="378" spans="1:2" x14ac:dyDescent="0.35">
@@ -24580,7 +24580,7 @@
         <v>Management</v>
       </c>
       <c r="B378" s="3" t="s">
-        <v>1997</v>
+        <v>1996</v>
       </c>
     </row>
     <row r="379" spans="1:2" x14ac:dyDescent="0.35">
@@ -24588,7 +24588,7 @@
         <v>Data</v>
       </c>
       <c r="B379" s="3" t="s">
-        <v>2002</v>
+        <v>2001</v>
       </c>
     </row>
     <row r="380" spans="1:2" x14ac:dyDescent="0.35">
@@ -24596,7 +24596,7 @@
         <v>Color</v>
       </c>
       <c r="B380" s="3" t="s">
-        <v>2003</v>
+        <v>2002</v>
       </c>
     </row>
     <row r="381" spans="1:2" x14ac:dyDescent="0.35">
@@ -24604,7 +24604,7 @@
         <v>ColorDescription</v>
       </c>
       <c r="B381" s="3" t="s">
-        <v>2012</v>
+        <v>2011</v>
       </c>
     </row>
     <row r="382" spans="1:2" x14ac:dyDescent="0.35">
@@ -24612,7 +24612,7 @@
         <v>Prefix</v>
       </c>
       <c r="B382" s="3" t="s">
-        <v>2017</v>
+        <v>2016</v>
       </c>
     </row>
     <row r="383" spans="1:2" x14ac:dyDescent="0.35">
@@ -24620,7 +24620,7 @@
         <v>LinkExperience</v>
       </c>
       <c r="B383" s="3" t="s">
-        <v>2050</v>
+        <v>2049</v>
       </c>
     </row>
     <row r="384" spans="1:2" x14ac:dyDescent="0.35">
@@ -24628,7 +24628,7 @@
         <v>LinkEducation</v>
       </c>
       <c r="B384" s="3" t="s">
-        <v>2051</v>
+        <v>2050</v>
       </c>
     </row>
     <row r="385" spans="1:2" x14ac:dyDescent="0.35">
@@ -24636,7 +24636,7 @@
         <v>LinkInterest</v>
       </c>
       <c r="B385" s="3" t="s">
-        <v>2052</v>
+        <v>2051</v>
       </c>
     </row>
     <row r="386" spans="1:2" x14ac:dyDescent="0.35">
@@ -24644,7 +24644,7 @@
         <v>LinkAwards</v>
       </c>
       <c r="B386" s="3" t="s">
-        <v>2053</v>
+        <v>2052</v>
       </c>
     </row>
     <row r="387" spans="1:2" x14ac:dyDescent="0.35">
@@ -24652,7 +24652,7 @@
         <v>LinkCertificate</v>
       </c>
       <c r="B387" s="3" t="s">
-        <v>2054</v>
+        <v>2053</v>
       </c>
     </row>
     <row r="388" spans="1:2" x14ac:dyDescent="0.35">
@@ -24660,7 +24660,7 @@
         <v>LinkReference</v>
       </c>
       <c r="B388" s="3" t="s">
-        <v>2055</v>
+        <v>2054</v>
       </c>
     </row>
     <row r="389" spans="1:2" x14ac:dyDescent="0.35">
@@ -24668,7 +24668,7 @@
         <v>ChronologicalAsc</v>
       </c>
       <c r="B389" s="3" t="s">
-        <v>2066</v>
+        <v>2065</v>
       </c>
     </row>
     <row r="390" spans="1:2" x14ac:dyDescent="0.35">
@@ -24676,7 +24676,7 @@
         <v>ChronologicalDesc</v>
       </c>
       <c r="B390" s="3" t="s">
-        <v>2065</v>
+        <v>2064</v>
       </c>
     </row>
     <row r="391" spans="1:2" x14ac:dyDescent="0.35">
@@ -24684,7 +24684,7 @@
         <v>OptionalInformation</v>
       </c>
       <c r="B391" s="3" t="s">
-        <v>2074</v>
+        <v>2073</v>
       </c>
     </row>
     <row r="392" spans="1:2" x14ac:dyDescent="0.35">
@@ -24692,7 +24692,7 @@
         <v>MyVitaeSlogan</v>
       </c>
       <c r="B392" s="3" t="s">
-        <v>2080</v>
+        <v>2079</v>
       </c>
     </row>
     <row r="393" spans="1:2" x14ac:dyDescent="0.35">
@@ -24700,7 +24700,7 @@
         <v>DownloadQR</v>
       </c>
       <c r="B393" s="3" t="s">
-        <v>2086</v>
+        <v>2085</v>
       </c>
     </row>
     <row r="394" spans="1:2" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Several testing bugfixes, added Demo password
</commit_message>
<xml_diff>
--- a/Vitae/Library/Resources/SharedResource.xlsx
+++ b/Vitae/Library/Resources/SharedResource.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\Vitae\Library\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A86F28C7-6CA5-4C6E-AA41-7B254A7AD771}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2448BB7-D714-4C57-8908-04B8E56C3E12}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="30220" windowHeight="19620" tabRatio="406" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="30220" windowHeight="19620" tabRatio="406" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="en" sheetId="3" r:id="rId1"/>
@@ -5836,9 +5836,6 @@
     <t>Status500</t>
   </si>
   <si>
-    <t>An internal error has occured. Please send an e-mail to "admin@vitae.ch" if this error persists.</t>
-  </si>
-  <si>
     <t>Your access to this page has been denied.</t>
   </si>
   <si>
@@ -5881,9 +5878,6 @@
     <t>Ihr Zugang zu dieser Seite wurde Ihnen verweigert.</t>
   </si>
   <si>
-    <t>Es ist ein interner Fehler aufgetreten. Bitte senden Sie eine E-Mail an "admin@vitae.ch", wenn dieser Fehler weiterhin besteht.</t>
-  </si>
-  <si>
     <t>Bevor Sie mit dem Lebenslauf fortfahren, füllen Sie bitte das unten stehende Captcha aus.</t>
   </si>
   <si>
@@ -5902,9 +5896,6 @@
     <t>Votre accès à cette page vous a été refusé.</t>
   </si>
   <si>
-    <t>Une erreur interne s'est produite. Veuillez envoyer un e-mail à "admin@vitae.ch" si cette erreur persiste.</t>
-  </si>
-  <si>
     <t>Sécurisé</t>
   </si>
   <si>
@@ -5926,9 +5917,6 @@
     <t>L'accesso a questa pagina è stato negato.</t>
   </si>
   <si>
-    <t>Si è verificato un errore interno. Se l'errore persiste, si prega di inviare un'e-mail a "admin@vitae.ch".</t>
-  </si>
-  <si>
     <t>Sicuro</t>
   </si>
   <si>
@@ -5950,9 +5938,6 @@
     <t>Su acceso a esta página ha sido denegado.</t>
   </si>
   <si>
-    <t>Ha ocurrido un error interno. Por favor, envíe un e-mail a "admin@vitae.ch" si este error persiste.</t>
-  </si>
-  <si>
     <t>Asegure</t>
   </si>
   <si>
@@ -6398,6 +6383,21 @@
   </si>
   <si>
     <t>La aplicación web myVitae es propiedad exclusiva de Alexandros Theodoracatos y está protegida por la ley suiza de derechos de autor. Por lo tanto, el sitio web no puede ser reproducido o puesto a disposición en su totalidad o en parte de ninguna manera, ni puede ser utilizado de ninguna otra manera que la autorizada, sin el consentimiento previo de Alexandros Theodoracatos.</t>
+  </si>
+  <si>
+    <t>An internal error has occured.</t>
+  </si>
+  <si>
+    <t>Es ist ein interner Fehler aufgetreten.</t>
+  </si>
+  <si>
+    <t>Une erreur interne s'est produite.</t>
+  </si>
+  <si>
+    <t>Si è verificato un errore interno.</t>
+  </si>
+  <si>
+    <t>Ha ocurrido un error interno.</t>
   </si>
 </sst>
 </file>
@@ -6785,8 +6785,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B499"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A77" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B78" sqref="B78"/>
+    <sheetView topLeftCell="A348" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B368" sqref="B368"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -6944,7 +6944,7 @@
         <v>581</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>2076</v>
+        <v>2071</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.35">
@@ -7416,7 +7416,7 @@
         <v>1831</v>
       </c>
       <c r="B78" s="3" t="s">
-        <v>2108</v>
+        <v>2103</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.35">
@@ -7552,7 +7552,7 @@
         <v>1739</v>
       </c>
       <c r="B95" s="8" t="s">
-        <v>2082</v>
+        <v>2077</v>
       </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.35">
@@ -8416,7 +8416,7 @@
         <v>1859</v>
       </c>
       <c r="B203" s="3" t="s">
-        <v>1975</v>
+        <v>1970</v>
       </c>
     </row>
     <row r="204" spans="1:2" x14ac:dyDescent="0.35">
@@ -9136,7 +9136,7 @@
         <v>1750</v>
       </c>
       <c r="B293" s="8" t="s">
-        <v>2086</v>
+        <v>2081</v>
       </c>
     </row>
     <row r="294" spans="1:2" x14ac:dyDescent="0.35">
@@ -9224,7 +9224,7 @@
         <v>1753</v>
       </c>
       <c r="B304" s="8" t="s">
-        <v>2091</v>
+        <v>2086</v>
       </c>
     </row>
     <row r="305" spans="1:2" x14ac:dyDescent="0.35">
@@ -9352,7 +9352,7 @@
         <v>716</v>
       </c>
       <c r="B320" s="3" t="s">
-        <v>1926</v>
+        <v>1925</v>
       </c>
     </row>
     <row r="321" spans="1:2" x14ac:dyDescent="0.35">
@@ -9592,7 +9592,7 @@
         <v>1736</v>
       </c>
       <c r="B350" s="8" t="s">
-        <v>2098</v>
+        <v>2093</v>
       </c>
     </row>
     <row r="351" spans="1:2" x14ac:dyDescent="0.35">
@@ -9720,31 +9720,31 @@
         <v>1922</v>
       </c>
       <c r="B366" s="3" t="s">
-        <v>1925</v>
-      </c>
-    </row>
-    <row r="367" spans="1:2" ht="29" x14ac:dyDescent="0.35">
+        <v>1924</v>
+      </c>
+    </row>
+    <row r="367" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A367" s="5" t="s">
         <v>1923</v>
       </c>
       <c r="B367" s="3" t="s">
-        <v>1924</v>
+        <v>2107</v>
       </c>
     </row>
     <row r="368" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A368" s="5" t="s">
-        <v>1927</v>
+        <v>1926</v>
       </c>
       <c r="B368" s="3" t="s">
-        <v>1927</v>
+        <v>1926</v>
       </c>
     </row>
     <row r="369" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A369" s="5" t="s">
-        <v>1928</v>
+        <v>1927</v>
       </c>
       <c r="B369" s="3" t="s">
-        <v>1930</v>
+        <v>1929</v>
       </c>
     </row>
     <row r="370" spans="1:2" ht="29" x14ac:dyDescent="0.35">
@@ -9752,191 +9752,191 @@
         <v>1919</v>
       </c>
       <c r="B370" s="3" t="s">
-        <v>1929</v>
+        <v>1928</v>
       </c>
     </row>
     <row r="371" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A371" s="5" t="s">
-        <v>1931</v>
+        <v>1930</v>
       </c>
       <c r="B371" s="3" t="s">
-        <v>1931</v>
+        <v>1930</v>
       </c>
     </row>
     <row r="372" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A372" s="5" t="s">
+        <v>1931</v>
+      </c>
+      <c r="B372" s="3" t="s">
         <v>1932</v>
-      </c>
-      <c r="B372" s="3" t="s">
-        <v>1933</v>
       </c>
     </row>
     <row r="373" spans="1:2" ht="116" x14ac:dyDescent="0.35">
       <c r="A373" s="5" t="s">
+        <v>1933</v>
+      </c>
+      <c r="B373" s="3" t="s">
         <v>1934</v>
-      </c>
-      <c r="B373" s="3" t="s">
-        <v>1935</v>
       </c>
     </row>
     <row r="374" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A374" s="5" t="s">
-        <v>2045</v>
+        <v>2040</v>
       </c>
       <c r="B374" s="3" t="s">
-        <v>1936</v>
+        <v>1935</v>
       </c>
     </row>
     <row r="375" spans="1:2" ht="246.5" x14ac:dyDescent="0.35">
       <c r="A375" s="5" t="s">
-        <v>1937</v>
+        <v>1936</v>
       </c>
       <c r="B375" s="3" t="s">
-        <v>2103</v>
+        <v>2098</v>
       </c>
     </row>
     <row r="376" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A376" s="5" t="s">
-        <v>1970</v>
+        <v>1965</v>
       </c>
       <c r="B376" s="3" t="s">
-        <v>1970</v>
+        <v>1965</v>
       </c>
     </row>
     <row r="377" spans="1:2" ht="29" x14ac:dyDescent="0.35">
       <c r="A377" s="5" t="s">
-        <v>1981</v>
+        <v>1976</v>
       </c>
       <c r="B377" s="3" t="s">
-        <v>1976</v>
+        <v>1971</v>
       </c>
     </row>
     <row r="378" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A378" s="5" t="s">
-        <v>1982</v>
+        <v>1977</v>
       </c>
       <c r="B378" s="3" t="s">
-        <v>1982</v>
+        <v>1977</v>
       </c>
     </row>
     <row r="379" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A379" s="5" t="s">
-        <v>1987</v>
+        <v>1982</v>
       </c>
       <c r="B379" s="3" t="s">
-        <v>1987</v>
+        <v>1982</v>
       </c>
     </row>
     <row r="380" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A380" s="5" t="s">
-        <v>1992</v>
+        <v>1987</v>
       </c>
       <c r="B380" s="3" t="s">
-        <v>1992</v>
+        <v>1987</v>
       </c>
     </row>
     <row r="381" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A381" s="5" t="s">
-        <v>1996</v>
+        <v>1991</v>
       </c>
       <c r="B381" s="3" t="s">
-        <v>1997</v>
+        <v>1992</v>
       </c>
     </row>
     <row r="382" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A382" s="5" t="s">
-        <v>2002</v>
+        <v>1997</v>
       </c>
       <c r="B382" s="3" t="s">
-        <v>2002</v>
+        <v>1997</v>
       </c>
     </row>
     <row r="383" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A383" s="5" t="s">
-        <v>2009</v>
+        <v>2004</v>
       </c>
       <c r="B383" s="3" t="s">
-        <v>2010</v>
+        <v>2005</v>
       </c>
     </row>
     <row r="384" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A384" s="5" t="s">
-        <v>2011</v>
+        <v>2006</v>
       </c>
       <c r="B384" s="3" t="s">
-        <v>2012</v>
+        <v>2007</v>
       </c>
     </row>
     <row r="385" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A385" s="5" t="s">
-        <v>2013</v>
+        <v>2008</v>
       </c>
       <c r="B385" s="3" t="s">
-        <v>2020</v>
+        <v>2015</v>
       </c>
     </row>
     <row r="386" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A386" s="5" t="s">
-        <v>2014</v>
+        <v>2009</v>
       </c>
       <c r="B386" s="3" t="s">
-        <v>2015</v>
+        <v>2010</v>
       </c>
     </row>
     <row r="387" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A387" s="5" t="s">
-        <v>2016</v>
+        <v>2011</v>
       </c>
       <c r="B387" s="3" t="s">
-        <v>2017</v>
+        <v>2012</v>
       </c>
     </row>
     <row r="388" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A388" s="5" t="s">
-        <v>2018</v>
+        <v>2013</v>
       </c>
       <c r="B388" s="3" t="s">
-        <v>2019</v>
+        <v>2014</v>
       </c>
     </row>
     <row r="389" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A389" s="5" t="s">
-        <v>2046</v>
+        <v>2041</v>
       </c>
       <c r="B389" s="3" t="s">
-        <v>2048</v>
+        <v>2043</v>
       </c>
     </row>
     <row r="390" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A390" s="5" t="s">
-        <v>2047</v>
+        <v>2042</v>
       </c>
       <c r="B390" s="3" t="s">
-        <v>2049</v>
+        <v>2044</v>
       </c>
     </row>
     <row r="391" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A391" s="5" t="s">
-        <v>2058</v>
+        <v>2053</v>
       </c>
       <c r="B391" s="3" t="s">
-        <v>2059</v>
+        <v>2054</v>
       </c>
     </row>
     <row r="392" spans="1:2" ht="14" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A392" s="5" t="s">
-        <v>2064</v>
+        <v>2059</v>
       </c>
       <c r="B392" s="3" t="s">
-        <v>2067</v>
+        <v>2062</v>
       </c>
     </row>
     <row r="393" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A393" s="5" t="s">
-        <v>2071</v>
+        <v>2066</v>
       </c>
       <c r="B393" s="3" t="s">
-        <v>2070</v>
+        <v>2065</v>
       </c>
     </row>
     <row r="394" spans="1:2" x14ac:dyDescent="0.35">
@@ -10479,8 +10479,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B498"/>
   <sheetViews>
-    <sheetView topLeftCell="A72" workbookViewId="0">
-      <selection activeCell="B78" sqref="B78"/>
+    <sheetView topLeftCell="A351" workbookViewId="0">
+      <selection activeCell="B368" sqref="B368"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -10503,7 +10503,7 @@
         <v>AboutDetailsDescription</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>2007</v>
+        <v>2002</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
@@ -10639,7 +10639,7 @@
         <v>AdTextB0</v>
       </c>
       <c r="B19" s="7" t="s">
-        <v>2080</v>
+        <v>2075</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.35">
@@ -10887,7 +10887,7 @@
         <v>ChooseFile</v>
       </c>
       <c r="B50" s="7" t="s">
-        <v>2008</v>
+        <v>2003</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.35">
@@ -11111,7 +11111,7 @@
         <v>CopyrightLawText</v>
       </c>
       <c r="B78" s="8" t="s">
-        <v>2107</v>
+        <v>2102</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.35">
@@ -11247,7 +11247,7 @@
         <v>DashboardOverview</v>
       </c>
       <c r="B95" s="8" t="s">
-        <v>2081</v>
+        <v>2076</v>
       </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.35">
@@ -11655,7 +11655,7 @@
         <v>GoogleAnalyticsText1</v>
       </c>
       <c r="B146" s="3" t="s">
-        <v>2096</v>
+        <v>2091</v>
       </c>
     </row>
     <row r="147" spans="1:2" ht="159.5" x14ac:dyDescent="0.35">
@@ -12831,7 +12831,7 @@
         <v>SavePublicationsDescription</v>
       </c>
       <c r="B293" s="8" t="s">
-        <v>2095</v>
+        <v>2090</v>
       </c>
     </row>
     <row r="294" spans="1:2" x14ac:dyDescent="0.35">
@@ -12919,7 +12919,7 @@
         <v>ShowYourStrengthsDescription</v>
       </c>
       <c r="B304" s="8" t="s">
-        <v>2090</v>
+        <v>2085</v>
       </c>
     </row>
     <row r="305" spans="1:2" x14ac:dyDescent="0.35">
@@ -13287,7 +13287,7 @@
         <v>WhyMyVitaeReason</v>
       </c>
       <c r="B350" s="8" t="s">
-        <v>2097</v>
+        <v>2092</v>
       </c>
     </row>
     <row r="351" spans="1:2" x14ac:dyDescent="0.35">
@@ -13415,15 +13415,15 @@
         <v>Status403</v>
       </c>
       <c r="B366" s="8" t="s">
-        <v>1938</v>
-      </c>
-    </row>
-    <row r="367" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
+        <v>1937</v>
+      </c>
+    </row>
+    <row r="367" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A367" s="5" t="str">
         <v>Status500</v>
       </c>
       <c r="B367" s="8" t="s">
-        <v>1939</v>
+        <v>2108</v>
       </c>
     </row>
     <row r="368" spans="1:2" x14ac:dyDescent="0.35">
@@ -13431,7 +13431,7 @@
         <v>Secure</v>
       </c>
       <c r="B368" s="8" t="s">
-        <v>1944</v>
+        <v>1942</v>
       </c>
     </row>
     <row r="369" spans="1:2" ht="29" x14ac:dyDescent="0.35">
@@ -13439,7 +13439,7 @@
         <v>SecureDescription</v>
       </c>
       <c r="B369" s="8" t="s">
-        <v>1969</v>
+        <v>1964</v>
       </c>
     </row>
     <row r="370" spans="1:2" ht="29" x14ac:dyDescent="0.35">
@@ -13447,7 +13447,7 @@
         <v>SecurityCheckDesc</v>
       </c>
       <c r="B370" s="8" t="s">
-        <v>1940</v>
+        <v>1938</v>
       </c>
     </row>
     <row r="371" spans="1:2" x14ac:dyDescent="0.35">
@@ -13455,7 +13455,7 @@
         <v>Contact</v>
       </c>
       <c r="B371" s="8" t="s">
-        <v>1941</v>
+        <v>1939</v>
       </c>
     </row>
     <row r="372" spans="1:2" x14ac:dyDescent="0.35">
@@ -13463,7 +13463,7 @@
         <v>GoogleCaptcha</v>
       </c>
       <c r="B372" s="8" t="s">
-        <v>1933</v>
+        <v>1932</v>
       </c>
     </row>
     <row r="373" spans="1:2" ht="174" x14ac:dyDescent="0.35">
@@ -13471,7 +13471,7 @@
         <v>GoogleCaptchaDesc</v>
       </c>
       <c r="B373" s="8" t="s">
-        <v>1942</v>
+        <v>1940</v>
       </c>
     </row>
     <row r="374" spans="1:2" x14ac:dyDescent="0.35">
@@ -13479,7 +13479,7 @@
         <v>DataCollection</v>
       </c>
       <c r="B374" s="8" t="s">
-        <v>1943</v>
+        <v>1941</v>
       </c>
     </row>
     <row r="375" spans="1:2" ht="290" x14ac:dyDescent="0.35">
@@ -13487,7 +13487,7 @@
         <v>DataCollectionDesc</v>
       </c>
       <c r="B375" s="8" t="s">
-        <v>2102</v>
+        <v>2097</v>
       </c>
     </row>
     <row r="376" spans="1:2" x14ac:dyDescent="0.35">
@@ -13495,7 +13495,7 @@
         <v>Imprint</v>
       </c>
       <c r="B376" s="8" t="s">
-        <v>1971</v>
+        <v>1966</v>
       </c>
     </row>
     <row r="377" spans="1:2" ht="29" x14ac:dyDescent="0.35">
@@ -13503,7 +13503,7 @@
         <v>ErrorInfoMail</v>
       </c>
       <c r="B377" s="3" t="s">
-        <v>1977</v>
+        <v>1972</v>
       </c>
     </row>
     <row r="378" spans="1:2" x14ac:dyDescent="0.35">
@@ -13511,7 +13511,7 @@
         <v>Management</v>
       </c>
       <c r="B378" s="8" t="s">
-        <v>1983</v>
+        <v>1978</v>
       </c>
     </row>
     <row r="379" spans="1:2" x14ac:dyDescent="0.35">
@@ -13519,7 +13519,7 @@
         <v>Data</v>
       </c>
       <c r="B379" s="8" t="s">
-        <v>1988</v>
+        <v>1983</v>
       </c>
     </row>
     <row r="380" spans="1:2" x14ac:dyDescent="0.35">
@@ -13527,7 +13527,7 @@
         <v>Color</v>
       </c>
       <c r="B380" s="8" t="s">
-        <v>1993</v>
+        <v>1988</v>
       </c>
     </row>
     <row r="381" spans="1:2" x14ac:dyDescent="0.35">
@@ -13535,7 +13535,7 @@
         <v>ColorDescription</v>
       </c>
       <c r="B381" s="3" t="s">
-        <v>1998</v>
+        <v>1993</v>
       </c>
     </row>
     <row r="382" spans="1:2" x14ac:dyDescent="0.35">
@@ -13543,7 +13543,7 @@
         <v>Prefix</v>
       </c>
       <c r="B382" s="8" t="s">
-        <v>2003</v>
+        <v>1998</v>
       </c>
     </row>
     <row r="383" spans="1:2" x14ac:dyDescent="0.35">
@@ -13551,7 +13551,7 @@
         <v>LinkExperience</v>
       </c>
       <c r="B383" s="8" t="s">
-        <v>2021</v>
+        <v>2016</v>
       </c>
     </row>
     <row r="384" spans="1:2" x14ac:dyDescent="0.35">
@@ -13559,7 +13559,7 @@
         <v>LinkEducation</v>
       </c>
       <c r="B384" s="8" t="s">
-        <v>2022</v>
+        <v>2017</v>
       </c>
     </row>
     <row r="385" spans="1:2" x14ac:dyDescent="0.35">
@@ -13567,7 +13567,7 @@
         <v>LinkInterest</v>
       </c>
       <c r="B385" s="8" t="s">
-        <v>2023</v>
+        <v>2018</v>
       </c>
     </row>
     <row r="386" spans="1:2" x14ac:dyDescent="0.35">
@@ -13575,7 +13575,7 @@
         <v>LinkAwards</v>
       </c>
       <c r="B386" s="8" t="s">
-        <v>2024</v>
+        <v>2019</v>
       </c>
     </row>
     <row r="387" spans="1:2" x14ac:dyDescent="0.35">
@@ -13583,7 +13583,7 @@
         <v>LinkCertificate</v>
       </c>
       <c r="B387" s="8" t="s">
-        <v>2025</v>
+        <v>2020</v>
       </c>
     </row>
     <row r="388" spans="1:2" x14ac:dyDescent="0.35">
@@ -13591,7 +13591,7 @@
         <v>LinkReference</v>
       </c>
       <c r="B388" s="8" t="s">
-        <v>2026</v>
+        <v>2021</v>
       </c>
     </row>
     <row r="389" spans="1:2" ht="29" x14ac:dyDescent="0.35">
@@ -13599,7 +13599,7 @@
         <v>ChronologicalAsc</v>
       </c>
       <c r="B389" s="3" t="s">
-        <v>2050</v>
+        <v>2045</v>
       </c>
     </row>
     <row r="390" spans="1:2" ht="29" x14ac:dyDescent="0.35">
@@ -13607,7 +13607,7 @@
         <v>ChronologicalDesc</v>
       </c>
       <c r="B390" s="3" t="s">
-        <v>2051</v>
+        <v>2046</v>
       </c>
     </row>
     <row r="391" spans="1:2" x14ac:dyDescent="0.35">
@@ -13615,7 +13615,7 @@
         <v>OptionalInformation</v>
       </c>
       <c r="B391" s="8" t="s">
-        <v>2060</v>
+        <v>2055</v>
       </c>
     </row>
     <row r="392" spans="1:2" x14ac:dyDescent="0.35">
@@ -13623,7 +13623,7 @@
         <v>MyVitaeSlogan</v>
       </c>
       <c r="B392" s="8" t="s">
-        <v>2066</v>
+        <v>2061</v>
       </c>
     </row>
     <row r="393" spans="1:2" x14ac:dyDescent="0.35">
@@ -13631,7 +13631,7 @@
         <v>DownloadQR</v>
       </c>
       <c r="B393" s="8" t="s">
-        <v>2072</v>
+        <v>2067</v>
       </c>
     </row>
     <row r="394" spans="1:2" x14ac:dyDescent="0.35">
@@ -14169,8 +14169,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1802D85A-2FA6-4DB3-A31F-68A2D623BDD9}">
   <dimension ref="A1:B498"/>
   <sheetViews>
-    <sheetView topLeftCell="A74" workbookViewId="0">
-      <selection activeCell="B85" sqref="B85"/>
+    <sheetView topLeftCell="A348" workbookViewId="0">
+      <selection activeCell="B368" sqref="B368"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -14329,7 +14329,7 @@
         <v>AdTextB0</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>2077</v>
+        <v>2072</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.35">
@@ -14801,7 +14801,7 @@
         <v>CopyrightLawText</v>
       </c>
       <c r="B78" s="3" t="s">
-        <v>2109</v>
+        <v>2104</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.35">
@@ -14937,7 +14937,7 @@
         <v>DashboardOverview</v>
       </c>
       <c r="B95" s="3" t="s">
-        <v>2083</v>
+        <v>2078</v>
       </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.35">
@@ -16521,7 +16521,7 @@
         <v>SavePublicationsDescription</v>
       </c>
       <c r="B293" s="3" t="s">
-        <v>2087</v>
+        <v>2082</v>
       </c>
     </row>
     <row r="294" spans="1:2" x14ac:dyDescent="0.35">
@@ -16609,7 +16609,7 @@
         <v>ShowYourStrengthsDescription</v>
       </c>
       <c r="B304" s="3" t="s">
-        <v>2092</v>
+        <v>2087</v>
       </c>
     </row>
     <row r="305" spans="1:2" x14ac:dyDescent="0.35">
@@ -16977,7 +16977,7 @@
         <v>WhyMyVitaeReason</v>
       </c>
       <c r="B350" s="3" t="s">
-        <v>2099</v>
+        <v>2094</v>
       </c>
     </row>
     <row r="351" spans="1:2" x14ac:dyDescent="0.35">
@@ -17105,15 +17105,15 @@
         <v>Status403</v>
       </c>
       <c r="B366" s="3" t="s">
-        <v>1945</v>
-      </c>
-    </row>
-    <row r="367" spans="1:2" ht="29" x14ac:dyDescent="0.35">
+        <v>1943</v>
+      </c>
+    </row>
+    <row r="367" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A367" s="5" t="str">
         <v>Status500</v>
       </c>
       <c r="B367" s="3" t="s">
-        <v>1946</v>
+        <v>2109</v>
       </c>
     </row>
     <row r="368" spans="1:2" x14ac:dyDescent="0.35">
@@ -17121,7 +17121,7 @@
         <v>Secure</v>
       </c>
       <c r="B368" s="3" t="s">
-        <v>1947</v>
+        <v>1944</v>
       </c>
     </row>
     <row r="369" spans="1:2" ht="29" x14ac:dyDescent="0.35">
@@ -17129,7 +17129,7 @@
         <v>SecureDescription</v>
       </c>
       <c r="B369" s="3" t="s">
-        <v>1948</v>
+        <v>1945</v>
       </c>
     </row>
     <row r="370" spans="1:2" x14ac:dyDescent="0.35">
@@ -17137,7 +17137,7 @@
         <v>SecurityCheckDesc</v>
       </c>
       <c r="B370" s="3" t="s">
-        <v>1949</v>
+        <v>1946</v>
       </c>
     </row>
     <row r="371" spans="1:2" x14ac:dyDescent="0.35">
@@ -17145,7 +17145,7 @@
         <v>Contact</v>
       </c>
       <c r="B371" s="3" t="s">
-        <v>1950</v>
+        <v>1947</v>
       </c>
     </row>
     <row r="372" spans="1:2" x14ac:dyDescent="0.35">
@@ -17153,7 +17153,7 @@
         <v>GoogleCaptcha</v>
       </c>
       <c r="B372" s="3" t="s">
-        <v>1933</v>
+        <v>1932</v>
       </c>
     </row>
     <row r="373" spans="1:2" ht="130.5" x14ac:dyDescent="0.35">
@@ -17161,7 +17161,7 @@
         <v>GoogleCaptchaDesc</v>
       </c>
       <c r="B373" s="3" t="s">
-        <v>1951</v>
+        <v>1948</v>
       </c>
     </row>
     <row r="374" spans="1:2" x14ac:dyDescent="0.35">
@@ -17169,7 +17169,7 @@
         <v>DataCollection</v>
       </c>
       <c r="B374" s="3" t="s">
-        <v>1952</v>
+        <v>1949</v>
       </c>
     </row>
     <row r="375" spans="1:2" ht="267" customHeight="1" x14ac:dyDescent="0.35">
@@ -17177,7 +17177,7 @@
         <v>DataCollectionDesc</v>
       </c>
       <c r="B375" s="3" t="s">
-        <v>2104</v>
+        <v>2099</v>
       </c>
     </row>
     <row r="376" spans="1:2" x14ac:dyDescent="0.35">
@@ -17185,7 +17185,7 @@
         <v>Imprint</v>
       </c>
       <c r="B376" s="3" t="s">
-        <v>1972</v>
+        <v>1967</v>
       </c>
     </row>
     <row r="377" spans="1:2" ht="29" x14ac:dyDescent="0.35">
@@ -17193,7 +17193,7 @@
         <v>ErrorInfoMail</v>
       </c>
       <c r="B377" s="3" t="s">
-        <v>1978</v>
+        <v>1973</v>
       </c>
     </row>
     <row r="378" spans="1:2" x14ac:dyDescent="0.35">
@@ -17201,7 +17201,7 @@
         <v>Management</v>
       </c>
       <c r="B378" s="3" t="s">
-        <v>1984</v>
+        <v>1979</v>
       </c>
     </row>
     <row r="379" spans="1:2" x14ac:dyDescent="0.35">
@@ -17209,7 +17209,7 @@
         <v>Data</v>
       </c>
       <c r="B379" s="3" t="s">
-        <v>1989</v>
+        <v>1984</v>
       </c>
     </row>
     <row r="380" spans="1:2" x14ac:dyDescent="0.35">
@@ -17217,7 +17217,7 @@
         <v>Color</v>
       </c>
       <c r="B380" s="3" t="s">
-        <v>1994</v>
+        <v>1989</v>
       </c>
     </row>
     <row r="381" spans="1:2" x14ac:dyDescent="0.35">
@@ -17225,7 +17225,7 @@
         <v>ColorDescription</v>
       </c>
       <c r="B381" s="3" t="s">
-        <v>1999</v>
+        <v>1994</v>
       </c>
     </row>
     <row r="382" spans="1:2" x14ac:dyDescent="0.35">
@@ -17233,7 +17233,7 @@
         <v>Prefix</v>
       </c>
       <c r="B382" s="3" t="s">
-        <v>2004</v>
+        <v>1999</v>
       </c>
     </row>
     <row r="383" spans="1:2" x14ac:dyDescent="0.35">
@@ -17241,7 +17241,7 @@
         <v>LinkExperience</v>
       </c>
       <c r="B383" s="3" t="s">
-        <v>2027</v>
+        <v>2022</v>
       </c>
     </row>
     <row r="384" spans="1:2" x14ac:dyDescent="0.35">
@@ -17249,7 +17249,7 @@
         <v>LinkEducation</v>
       </c>
       <c r="B384" s="3" t="s">
-        <v>2028</v>
+        <v>2023</v>
       </c>
     </row>
     <row r="385" spans="1:2" x14ac:dyDescent="0.35">
@@ -17257,7 +17257,7 @@
         <v>LinkInterest</v>
       </c>
       <c r="B385" s="3" t="s">
-        <v>2029</v>
+        <v>2024</v>
       </c>
     </row>
     <row r="386" spans="1:2" x14ac:dyDescent="0.35">
@@ -17265,7 +17265,7 @@
         <v>LinkAwards</v>
       </c>
       <c r="B386" s="3" t="s">
-        <v>2030</v>
+        <v>2025</v>
       </c>
     </row>
     <row r="387" spans="1:2" x14ac:dyDescent="0.35">
@@ -17273,7 +17273,7 @@
         <v>LinkCertificate</v>
       </c>
       <c r="B387" s="3" t="s">
-        <v>2031</v>
+        <v>2026</v>
       </c>
     </row>
     <row r="388" spans="1:2" x14ac:dyDescent="0.35">
@@ -17281,7 +17281,7 @@
         <v>LinkReference</v>
       </c>
       <c r="B388" s="3" t="s">
-        <v>2032</v>
+        <v>2027</v>
       </c>
     </row>
     <row r="389" spans="1:2" x14ac:dyDescent="0.35">
@@ -17289,7 +17289,7 @@
         <v>ChronologicalAsc</v>
       </c>
       <c r="B389" s="3" t="s">
-        <v>2057</v>
+        <v>2052</v>
       </c>
     </row>
     <row r="390" spans="1:2" x14ac:dyDescent="0.35">
@@ -17297,7 +17297,7 @@
         <v>ChronologicalDesc</v>
       </c>
       <c r="B390" s="3" t="s">
-        <v>2052</v>
+        <v>2047</v>
       </c>
     </row>
     <row r="391" spans="1:2" x14ac:dyDescent="0.35">
@@ -17305,7 +17305,7 @@
         <v>OptionalInformation</v>
       </c>
       <c r="B391" s="3" t="s">
-        <v>2061</v>
+        <v>2056</v>
       </c>
     </row>
     <row r="392" spans="1:2" x14ac:dyDescent="0.35">
@@ -17313,7 +17313,7 @@
         <v>MyVitaeSlogan</v>
       </c>
       <c r="B392" s="3" t="s">
-        <v>2065</v>
+        <v>2060</v>
       </c>
     </row>
     <row r="393" spans="1:2" x14ac:dyDescent="0.35">
@@ -17321,7 +17321,7 @@
         <v>DownloadQR</v>
       </c>
       <c r="B393" s="3" t="s">
-        <v>2073</v>
+        <v>2068</v>
       </c>
     </row>
     <row r="394" spans="1:2" x14ac:dyDescent="0.35">
@@ -17858,8 +17858,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{21647760-4677-48F5-BA10-2363314EC080}">
   <dimension ref="A1:B498"/>
   <sheetViews>
-    <sheetView topLeftCell="A73" workbookViewId="0">
-      <selection activeCell="B78" sqref="B78"/>
+    <sheetView topLeftCell="A349" workbookViewId="0">
+      <selection activeCell="B368" sqref="B368"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -18018,7 +18018,7 @@
         <v>AdTextB0</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>2078</v>
+        <v>2073</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.35">
@@ -18490,7 +18490,7 @@
         <v>CopyrightLawText</v>
       </c>
       <c r="B78" s="3" t="s">
-        <v>2110</v>
+        <v>2105</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.35">
@@ -18626,7 +18626,7 @@
         <v>DashboardOverview</v>
       </c>
       <c r="B95" s="3" t="s">
-        <v>2084</v>
+        <v>2079</v>
       </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.35">
@@ -20210,7 +20210,7 @@
         <v>SavePublicationsDescription</v>
       </c>
       <c r="B293" s="3" t="s">
-        <v>2088</v>
+        <v>2083</v>
       </c>
     </row>
     <row r="294" spans="1:2" x14ac:dyDescent="0.35">
@@ -20298,7 +20298,7 @@
         <v>ShowYourStrengthsDescription</v>
       </c>
       <c r="B304" s="3" t="s">
-        <v>2093</v>
+        <v>2088</v>
       </c>
     </row>
     <row r="305" spans="1:2" x14ac:dyDescent="0.35">
@@ -20666,7 +20666,7 @@
         <v>WhyMyVitaeReason</v>
       </c>
       <c r="B350" s="3" t="s">
-        <v>2100</v>
+        <v>2095</v>
       </c>
     </row>
     <row r="351" spans="1:2" x14ac:dyDescent="0.35">
@@ -20794,15 +20794,15 @@
         <v>Status403</v>
       </c>
       <c r="B366" s="3" t="s">
-        <v>1953</v>
-      </c>
-    </row>
-    <row r="367" spans="1:2" ht="29" x14ac:dyDescent="0.35">
+        <v>1950</v>
+      </c>
+    </row>
+    <row r="367" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A367" s="5" t="str">
         <v>Status500</v>
       </c>
       <c r="B367" s="3" t="s">
-        <v>1954</v>
+        <v>2110</v>
       </c>
     </row>
     <row r="368" spans="1:2" x14ac:dyDescent="0.35">
@@ -20810,7 +20810,7 @@
         <v>Secure</v>
       </c>
       <c r="B368" s="3" t="s">
-        <v>1955</v>
+        <v>1951</v>
       </c>
     </row>
     <row r="369" spans="1:2" x14ac:dyDescent="0.35">
@@ -20818,7 +20818,7 @@
         <v>SecureDescription</v>
       </c>
       <c r="B369" s="3" t="s">
-        <v>1956</v>
+        <v>1952</v>
       </c>
     </row>
     <row r="370" spans="1:2" ht="29" x14ac:dyDescent="0.35">
@@ -20826,7 +20826,7 @@
         <v>SecurityCheckDesc</v>
       </c>
       <c r="B370" s="3" t="s">
-        <v>1957</v>
+        <v>1953</v>
       </c>
     </row>
     <row r="371" spans="1:2" x14ac:dyDescent="0.35">
@@ -20834,7 +20834,7 @@
         <v>Contact</v>
       </c>
       <c r="B371" s="3" t="s">
-        <v>1958</v>
+        <v>1954</v>
       </c>
     </row>
     <row r="372" spans="1:2" x14ac:dyDescent="0.35">
@@ -20842,7 +20842,7 @@
         <v>GoogleCaptcha</v>
       </c>
       <c r="B372" s="3" t="s">
-        <v>1933</v>
+        <v>1932</v>
       </c>
     </row>
     <row r="373" spans="1:2" ht="116" x14ac:dyDescent="0.35">
@@ -20850,7 +20850,7 @@
         <v>GoogleCaptchaDesc</v>
       </c>
       <c r="B373" s="3" t="s">
-        <v>1959</v>
+        <v>1955</v>
       </c>
     </row>
     <row r="374" spans="1:2" x14ac:dyDescent="0.35">
@@ -20858,7 +20858,7 @@
         <v>DataCollection</v>
       </c>
       <c r="B374" s="3" t="s">
-        <v>1960</v>
+        <v>1956</v>
       </c>
     </row>
     <row r="375" spans="1:2" ht="246.5" x14ac:dyDescent="0.35">
@@ -20866,7 +20866,7 @@
         <v>DataCollectionDesc</v>
       </c>
       <c r="B375" s="3" t="s">
-        <v>2105</v>
+        <v>2100</v>
       </c>
     </row>
     <row r="376" spans="1:2" x14ac:dyDescent="0.35">
@@ -20874,7 +20874,7 @@
         <v>Imprint</v>
       </c>
       <c r="B376" s="3" t="s">
-        <v>1973</v>
+        <v>1968</v>
       </c>
     </row>
     <row r="377" spans="1:2" ht="29" x14ac:dyDescent="0.35">
@@ -20882,7 +20882,7 @@
         <v>ErrorInfoMail</v>
       </c>
       <c r="B377" s="3" t="s">
-        <v>1979</v>
+        <v>1974</v>
       </c>
     </row>
     <row r="378" spans="1:2" x14ac:dyDescent="0.35">
@@ -20890,7 +20890,7 @@
         <v>Management</v>
       </c>
       <c r="B378" s="3" t="s">
-        <v>1985</v>
+        <v>1980</v>
       </c>
     </row>
     <row r="379" spans="1:2" x14ac:dyDescent="0.35">
@@ -20898,7 +20898,7 @@
         <v>Data</v>
       </c>
       <c r="B379" s="3" t="s">
-        <v>1990</v>
+        <v>1985</v>
       </c>
     </row>
     <row r="380" spans="1:2" x14ac:dyDescent="0.35">
@@ -20906,7 +20906,7 @@
         <v>Color</v>
       </c>
       <c r="B380" s="3" t="s">
-        <v>1995</v>
+        <v>1990</v>
       </c>
     </row>
     <row r="381" spans="1:2" x14ac:dyDescent="0.35">
@@ -20914,7 +20914,7 @@
         <v>ColorDescription</v>
       </c>
       <c r="B381" s="3" t="s">
-        <v>2000</v>
+        <v>1995</v>
       </c>
     </row>
     <row r="382" spans="1:2" x14ac:dyDescent="0.35">
@@ -20922,7 +20922,7 @@
         <v>Prefix</v>
       </c>
       <c r="B382" s="3" t="s">
-        <v>2005</v>
+        <v>2000</v>
       </c>
     </row>
     <row r="383" spans="1:2" x14ac:dyDescent="0.35">
@@ -20930,7 +20930,7 @@
         <v>LinkExperience</v>
       </c>
       <c r="B383" s="3" t="s">
-        <v>2033</v>
+        <v>2028</v>
       </c>
     </row>
     <row r="384" spans="1:2" x14ac:dyDescent="0.35">
@@ -20938,7 +20938,7 @@
         <v>LinkEducation</v>
       </c>
       <c r="B384" s="3" t="s">
-        <v>2034</v>
+        <v>2029</v>
       </c>
     </row>
     <row r="385" spans="1:2" x14ac:dyDescent="0.35">
@@ -20946,7 +20946,7 @@
         <v>LinkInterest</v>
       </c>
       <c r="B385" s="3" t="s">
-        <v>2035</v>
+        <v>2030</v>
       </c>
     </row>
     <row r="386" spans="1:2" x14ac:dyDescent="0.35">
@@ -20954,7 +20954,7 @@
         <v>LinkAwards</v>
       </c>
       <c r="B386" s="3" t="s">
-        <v>2036</v>
+        <v>2031</v>
       </c>
     </row>
     <row r="387" spans="1:2" x14ac:dyDescent="0.35">
@@ -20962,7 +20962,7 @@
         <v>LinkCertificate</v>
       </c>
       <c r="B387" s="3" t="s">
-        <v>2037</v>
+        <v>2032</v>
       </c>
     </row>
     <row r="388" spans="1:2" x14ac:dyDescent="0.35">
@@ -20970,7 +20970,7 @@
         <v>LinkReference</v>
       </c>
       <c r="B388" s="3" t="s">
-        <v>2038</v>
+        <v>2033</v>
       </c>
     </row>
     <row r="389" spans="1:2" x14ac:dyDescent="0.35">
@@ -20978,7 +20978,7 @@
         <v>ChronologicalAsc</v>
       </c>
       <c r="B389" s="3" t="s">
-        <v>2056</v>
+        <v>2051</v>
       </c>
     </row>
     <row r="390" spans="1:2" x14ac:dyDescent="0.35">
@@ -20986,7 +20986,7 @@
         <v>ChronologicalDesc</v>
       </c>
       <c r="B390" s="3" t="s">
-        <v>2053</v>
+        <v>2048</v>
       </c>
     </row>
     <row r="391" spans="1:2" x14ac:dyDescent="0.35">
@@ -20994,7 +20994,7 @@
         <v>OptionalInformation</v>
       </c>
       <c r="B391" s="3" t="s">
-        <v>2062</v>
+        <v>2057</v>
       </c>
     </row>
     <row r="392" spans="1:2" x14ac:dyDescent="0.35">
@@ -21002,7 +21002,7 @@
         <v>MyVitaeSlogan</v>
       </c>
       <c r="B392" s="3" t="s">
-        <v>2068</v>
+        <v>2063</v>
       </c>
     </row>
     <row r="393" spans="1:2" x14ac:dyDescent="0.35">
@@ -21010,7 +21010,7 @@
         <v>DownloadQR</v>
       </c>
       <c r="B393" s="3" t="s">
-        <v>2074</v>
+        <v>2069</v>
       </c>
     </row>
     <row r="394" spans="1:2" x14ac:dyDescent="0.35">
@@ -21548,8 +21548,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A8220B7-2614-4C14-91F7-8D47B2A1113F}">
   <dimension ref="A1:B498"/>
   <sheetViews>
-    <sheetView topLeftCell="A77" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F93" sqref="F93"/>
+    <sheetView tabSelected="1" topLeftCell="A349" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B368" sqref="B368"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -21708,7 +21708,7 @@
         <v>AdTextB0</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>2079</v>
+        <v>2074</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.35">
@@ -22180,7 +22180,7 @@
         <v>CopyrightLawText</v>
       </c>
       <c r="B78" s="3" t="s">
-        <v>2111</v>
+        <v>2106</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.35">
@@ -22316,7 +22316,7 @@
         <v>DashboardOverview</v>
       </c>
       <c r="B95" s="3" t="s">
-        <v>2085</v>
+        <v>2080</v>
       </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.35">
@@ -23900,7 +23900,7 @@
         <v>SavePublicationsDescription</v>
       </c>
       <c r="B293" s="3" t="s">
-        <v>2089</v>
+        <v>2084</v>
       </c>
     </row>
     <row r="294" spans="1:2" x14ac:dyDescent="0.35">
@@ -23988,7 +23988,7 @@
         <v>ShowYourStrengthsDescription</v>
       </c>
       <c r="B304" s="3" t="s">
-        <v>2094</v>
+        <v>2089</v>
       </c>
     </row>
     <row r="305" spans="1:2" x14ac:dyDescent="0.35">
@@ -24356,7 +24356,7 @@
         <v>WhyMyVitaeReason</v>
       </c>
       <c r="B350" s="3" t="s">
-        <v>2101</v>
+        <v>2096</v>
       </c>
     </row>
     <row r="351" spans="1:2" x14ac:dyDescent="0.35">
@@ -24484,15 +24484,15 @@
         <v>Status403</v>
       </c>
       <c r="B366" s="3" t="s">
-        <v>1961</v>
-      </c>
-    </row>
-    <row r="367" spans="1:2" ht="29" x14ac:dyDescent="0.35">
+        <v>1957</v>
+      </c>
+    </row>
+    <row r="367" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A367" s="5" t="str">
         <v>Status500</v>
       </c>
       <c r="B367" s="3" t="s">
-        <v>1962</v>
+        <v>2111</v>
       </c>
     </row>
     <row r="368" spans="1:2" x14ac:dyDescent="0.35">
@@ -24500,7 +24500,7 @@
         <v>Secure</v>
       </c>
       <c r="B368" s="3" t="s">
-        <v>1963</v>
+        <v>1958</v>
       </c>
     </row>
     <row r="369" spans="1:2" x14ac:dyDescent="0.35">
@@ -24508,7 +24508,7 @@
         <v>SecureDescription</v>
       </c>
       <c r="B369" s="3" t="s">
-        <v>1964</v>
+        <v>1959</v>
       </c>
     </row>
     <row r="370" spans="1:2" ht="29" x14ac:dyDescent="0.35">
@@ -24516,7 +24516,7 @@
         <v>SecurityCheckDesc</v>
       </c>
       <c r="B370" s="3" t="s">
-        <v>1965</v>
+        <v>1960</v>
       </c>
     </row>
     <row r="371" spans="1:2" x14ac:dyDescent="0.35">
@@ -24524,7 +24524,7 @@
         <v>Contact</v>
       </c>
       <c r="B371" s="3" t="s">
-        <v>1966</v>
+        <v>1961</v>
       </c>
     </row>
     <row r="372" spans="1:2" x14ac:dyDescent="0.35">
@@ -24532,7 +24532,7 @@
         <v>GoogleCaptcha</v>
       </c>
       <c r="B372" s="3" t="s">
-        <v>1933</v>
+        <v>1932</v>
       </c>
     </row>
     <row r="373" spans="1:2" ht="116" x14ac:dyDescent="0.35">
@@ -24540,7 +24540,7 @@
         <v>GoogleCaptchaDesc</v>
       </c>
       <c r="B373" s="3" t="s">
-        <v>1967</v>
+        <v>1962</v>
       </c>
     </row>
     <row r="374" spans="1:2" x14ac:dyDescent="0.35">
@@ -24548,7 +24548,7 @@
         <v>DataCollection</v>
       </c>
       <c r="B374" s="3" t="s">
-        <v>1968</v>
+        <v>1963</v>
       </c>
     </row>
     <row r="375" spans="1:2" ht="261" x14ac:dyDescent="0.35">
@@ -24556,7 +24556,7 @@
         <v>DataCollectionDesc</v>
       </c>
       <c r="B375" s="3" t="s">
-        <v>2106</v>
+        <v>2101</v>
       </c>
     </row>
     <row r="376" spans="1:2" x14ac:dyDescent="0.35">
@@ -24564,7 +24564,7 @@
         <v>Imprint</v>
       </c>
       <c r="B376" s="3" t="s">
-        <v>1974</v>
+        <v>1969</v>
       </c>
     </row>
     <row r="377" spans="1:2" ht="29" x14ac:dyDescent="0.35">
@@ -24572,7 +24572,7 @@
         <v>ErrorInfoMail</v>
       </c>
       <c r="B377" s="3" t="s">
-        <v>1980</v>
+        <v>1975</v>
       </c>
     </row>
     <row r="378" spans="1:2" x14ac:dyDescent="0.35">
@@ -24580,7 +24580,7 @@
         <v>Management</v>
       </c>
       <c r="B378" s="3" t="s">
-        <v>1986</v>
+        <v>1981</v>
       </c>
     </row>
     <row r="379" spans="1:2" x14ac:dyDescent="0.35">
@@ -24588,7 +24588,7 @@
         <v>Data</v>
       </c>
       <c r="B379" s="3" t="s">
-        <v>1991</v>
+        <v>1986</v>
       </c>
     </row>
     <row r="380" spans="1:2" x14ac:dyDescent="0.35">
@@ -24596,7 +24596,7 @@
         <v>Color</v>
       </c>
       <c r="B380" s="3" t="s">
-        <v>1992</v>
+        <v>1987</v>
       </c>
     </row>
     <row r="381" spans="1:2" x14ac:dyDescent="0.35">
@@ -24604,7 +24604,7 @@
         <v>ColorDescription</v>
       </c>
       <c r="B381" s="3" t="s">
-        <v>2001</v>
+        <v>1996</v>
       </c>
     </row>
     <row r="382" spans="1:2" x14ac:dyDescent="0.35">
@@ -24612,7 +24612,7 @@
         <v>Prefix</v>
       </c>
       <c r="B382" s="3" t="s">
-        <v>2006</v>
+        <v>2001</v>
       </c>
     </row>
     <row r="383" spans="1:2" x14ac:dyDescent="0.35">
@@ -24620,7 +24620,7 @@
         <v>LinkExperience</v>
       </c>
       <c r="B383" s="3" t="s">
-        <v>2039</v>
+        <v>2034</v>
       </c>
     </row>
     <row r="384" spans="1:2" x14ac:dyDescent="0.35">
@@ -24628,7 +24628,7 @@
         <v>LinkEducation</v>
       </c>
       <c r="B384" s="3" t="s">
-        <v>2040</v>
+        <v>2035</v>
       </c>
     </row>
     <row r="385" spans="1:2" x14ac:dyDescent="0.35">
@@ -24636,7 +24636,7 @@
         <v>LinkInterest</v>
       </c>
       <c r="B385" s="3" t="s">
-        <v>2041</v>
+        <v>2036</v>
       </c>
     </row>
     <row r="386" spans="1:2" x14ac:dyDescent="0.35">
@@ -24644,7 +24644,7 @@
         <v>LinkAwards</v>
       </c>
       <c r="B386" s="3" t="s">
-        <v>2042</v>
+        <v>2037</v>
       </c>
     </row>
     <row r="387" spans="1:2" x14ac:dyDescent="0.35">
@@ -24652,7 +24652,7 @@
         <v>LinkCertificate</v>
       </c>
       <c r="B387" s="3" t="s">
-        <v>2043</v>
+        <v>2038</v>
       </c>
     </row>
     <row r="388" spans="1:2" x14ac:dyDescent="0.35">
@@ -24660,7 +24660,7 @@
         <v>LinkReference</v>
       </c>
       <c r="B388" s="3" t="s">
-        <v>2044</v>
+        <v>2039</v>
       </c>
     </row>
     <row r="389" spans="1:2" x14ac:dyDescent="0.35">
@@ -24668,7 +24668,7 @@
         <v>ChronologicalAsc</v>
       </c>
       <c r="B389" s="3" t="s">
-        <v>2055</v>
+        <v>2050</v>
       </c>
     </row>
     <row r="390" spans="1:2" x14ac:dyDescent="0.35">
@@ -24676,7 +24676,7 @@
         <v>ChronologicalDesc</v>
       </c>
       <c r="B390" s="3" t="s">
-        <v>2054</v>
+        <v>2049</v>
       </c>
     </row>
     <row r="391" spans="1:2" x14ac:dyDescent="0.35">
@@ -24684,7 +24684,7 @@
         <v>OptionalInformation</v>
       </c>
       <c r="B391" s="3" t="s">
-        <v>2063</v>
+        <v>2058</v>
       </c>
     </row>
     <row r="392" spans="1:2" x14ac:dyDescent="0.35">
@@ -24692,7 +24692,7 @@
         <v>MyVitaeSlogan</v>
       </c>
       <c r="B392" s="3" t="s">
-        <v>2069</v>
+        <v>2064</v>
       </c>
     </row>
     <row r="393" spans="1:2" x14ac:dyDescent="0.35">
@@ -24700,7 +24700,7 @@
         <v>DownloadQR</v>
       </c>
       <c r="B393" s="3" t="s">
-        <v>2075</v>
+        <v>2070</v>
       </c>
     </row>
     <row r="394" spans="1:2" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Collapsing added to Razor
</commit_message>
<xml_diff>
--- a/Vitae/Library/Resources/SharedResource.xlsx
+++ b/Vitae/Library/Resources/SharedResource.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\Vitae\Library\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2448BB7-D714-4C57-8908-04B8E56C3E12}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3BF9060-BB34-4B32-982F-9BCD9A31CFD9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="30220" windowHeight="19620" tabRatio="406" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="30220" windowHeight="19620" tabRatio="406" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="en" sheetId="3" r:id="rId1"/>
@@ -6115,9 +6115,6 @@
     <t>Website des Arbeitgebers</t>
   </si>
   <si>
-    <t>Website des Ausbildungszentrums</t>
-  </si>
-  <si>
     <t>Website der Vereinigung</t>
   </si>
   <si>
@@ -6398,6 +6395,9 @@
   </si>
   <si>
     <t>Ha ocurrido un error interno.</t>
+  </si>
+  <si>
+    <t>Website der Ausbildungsstätte</t>
   </si>
 </sst>
 </file>
@@ -6944,7 +6944,7 @@
         <v>581</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>2071</v>
+        <v>2070</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.35">
@@ -7416,7 +7416,7 @@
         <v>1831</v>
       </c>
       <c r="B78" s="3" t="s">
-        <v>2103</v>
+        <v>2102</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.35">
@@ -7552,7 +7552,7 @@
         <v>1739</v>
       </c>
       <c r="B95" s="8" t="s">
-        <v>2077</v>
+        <v>2076</v>
       </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.35">
@@ -9136,7 +9136,7 @@
         <v>1750</v>
       </c>
       <c r="B293" s="8" t="s">
-        <v>2081</v>
+        <v>2080</v>
       </c>
     </row>
     <row r="294" spans="1:2" x14ac:dyDescent="0.35">
@@ -9224,7 +9224,7 @@
         <v>1753</v>
       </c>
       <c r="B304" s="8" t="s">
-        <v>2086</v>
+        <v>2085</v>
       </c>
     </row>
     <row r="305" spans="1:2" x14ac:dyDescent="0.35">
@@ -9592,7 +9592,7 @@
         <v>1736</v>
       </c>
       <c r="B350" s="8" t="s">
-        <v>2093</v>
+        <v>2092</v>
       </c>
     </row>
     <row r="351" spans="1:2" x14ac:dyDescent="0.35">
@@ -9728,7 +9728,7 @@
         <v>1923</v>
       </c>
       <c r="B367" s="3" t="s">
-        <v>2107</v>
+        <v>2106</v>
       </c>
     </row>
     <row r="368" spans="1:2" x14ac:dyDescent="0.35">
@@ -9781,7 +9781,7 @@
     </row>
     <row r="374" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A374" s="5" t="s">
-        <v>2040</v>
+        <v>2039</v>
       </c>
       <c r="B374" s="3" t="s">
         <v>1935</v>
@@ -9792,7 +9792,7 @@
         <v>1936</v>
       </c>
       <c r="B375" s="3" t="s">
-        <v>2098</v>
+        <v>2097</v>
       </c>
     </row>
     <row r="376" spans="1:2" x14ac:dyDescent="0.35">
@@ -9901,42 +9901,42 @@
     </row>
     <row r="389" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A389" s="5" t="s">
-        <v>2041</v>
+        <v>2040</v>
       </c>
       <c r="B389" s="3" t="s">
-        <v>2043</v>
+        <v>2042</v>
       </c>
     </row>
     <row r="390" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A390" s="5" t="s">
-        <v>2042</v>
+        <v>2041</v>
       </c>
       <c r="B390" s="3" t="s">
-        <v>2044</v>
+        <v>2043</v>
       </c>
     </row>
     <row r="391" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A391" s="5" t="s">
+        <v>2052</v>
+      </c>
+      <c r="B391" s="3" t="s">
         <v>2053</v>
-      </c>
-      <c r="B391" s="3" t="s">
-        <v>2054</v>
       </c>
     </row>
     <row r="392" spans="1:2" ht="14" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A392" s="5" t="s">
-        <v>2059</v>
+        <v>2058</v>
       </c>
       <c r="B392" s="3" t="s">
-        <v>2062</v>
+        <v>2061</v>
       </c>
     </row>
     <row r="393" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A393" s="5" t="s">
-        <v>2066</v>
+        <v>2065</v>
       </c>
       <c r="B393" s="3" t="s">
-        <v>2065</v>
+        <v>2064</v>
       </c>
     </row>
     <row r="394" spans="1:2" x14ac:dyDescent="0.35">
@@ -10479,8 +10479,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B498"/>
   <sheetViews>
-    <sheetView topLeftCell="A351" workbookViewId="0">
-      <selection activeCell="B368" sqref="B368"/>
+    <sheetView tabSelected="1" topLeftCell="A381" workbookViewId="0">
+      <selection activeCell="B385" sqref="B385"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -10639,7 +10639,7 @@
         <v>AdTextB0</v>
       </c>
       <c r="B19" s="7" t="s">
-        <v>2075</v>
+        <v>2074</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.35">
@@ -11111,7 +11111,7 @@
         <v>CopyrightLawText</v>
       </c>
       <c r="B78" s="8" t="s">
-        <v>2102</v>
+        <v>2101</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.35">
@@ -11247,7 +11247,7 @@
         <v>DashboardOverview</v>
       </c>
       <c r="B95" s="8" t="s">
-        <v>2076</v>
+        <v>2075</v>
       </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.35">
@@ -11655,7 +11655,7 @@
         <v>GoogleAnalyticsText1</v>
       </c>
       <c r="B146" s="3" t="s">
-        <v>2091</v>
+        <v>2090</v>
       </c>
     </row>
     <row r="147" spans="1:2" ht="159.5" x14ac:dyDescent="0.35">
@@ -12831,7 +12831,7 @@
         <v>SavePublicationsDescription</v>
       </c>
       <c r="B293" s="8" t="s">
-        <v>2090</v>
+        <v>2089</v>
       </c>
     </row>
     <row r="294" spans="1:2" x14ac:dyDescent="0.35">
@@ -12919,7 +12919,7 @@
         <v>ShowYourStrengthsDescription</v>
       </c>
       <c r="B304" s="8" t="s">
-        <v>2085</v>
+        <v>2084</v>
       </c>
     </row>
     <row r="305" spans="1:2" x14ac:dyDescent="0.35">
@@ -13287,7 +13287,7 @@
         <v>WhyMyVitaeReason</v>
       </c>
       <c r="B350" s="8" t="s">
-        <v>2092</v>
+        <v>2091</v>
       </c>
     </row>
     <row r="351" spans="1:2" x14ac:dyDescent="0.35">
@@ -13423,7 +13423,7 @@
         <v>Status500</v>
       </c>
       <c r="B367" s="8" t="s">
-        <v>2108</v>
+        <v>2107</v>
       </c>
     </row>
     <row r="368" spans="1:2" x14ac:dyDescent="0.35">
@@ -13487,7 +13487,7 @@
         <v>DataCollectionDesc</v>
       </c>
       <c r="B375" s="8" t="s">
-        <v>2097</v>
+        <v>2096</v>
       </c>
     </row>
     <row r="376" spans="1:2" x14ac:dyDescent="0.35">
@@ -13559,7 +13559,7 @@
         <v>LinkEducation</v>
       </c>
       <c r="B384" s="8" t="s">
-        <v>2017</v>
+        <v>2111</v>
       </c>
     </row>
     <row r="385" spans="1:2" x14ac:dyDescent="0.35">
@@ -13567,7 +13567,7 @@
         <v>LinkInterest</v>
       </c>
       <c r="B385" s="8" t="s">
-        <v>2018</v>
+        <v>2017</v>
       </c>
     </row>
     <row r="386" spans="1:2" x14ac:dyDescent="0.35">
@@ -13575,7 +13575,7 @@
         <v>LinkAwards</v>
       </c>
       <c r="B386" s="8" t="s">
-        <v>2019</v>
+        <v>2018</v>
       </c>
     </row>
     <row r="387" spans="1:2" x14ac:dyDescent="0.35">
@@ -13583,7 +13583,7 @@
         <v>LinkCertificate</v>
       </c>
       <c r="B387" s="8" t="s">
-        <v>2020</v>
+        <v>2019</v>
       </c>
     </row>
     <row r="388" spans="1:2" x14ac:dyDescent="0.35">
@@ -13591,7 +13591,7 @@
         <v>LinkReference</v>
       </c>
       <c r="B388" s="8" t="s">
-        <v>2021</v>
+        <v>2020</v>
       </c>
     </row>
     <row r="389" spans="1:2" ht="29" x14ac:dyDescent="0.35">
@@ -13599,7 +13599,7 @@
         <v>ChronologicalAsc</v>
       </c>
       <c r="B389" s="3" t="s">
-        <v>2045</v>
+        <v>2044</v>
       </c>
     </row>
     <row r="390" spans="1:2" ht="29" x14ac:dyDescent="0.35">
@@ -13607,7 +13607,7 @@
         <v>ChronologicalDesc</v>
       </c>
       <c r="B390" s="3" t="s">
-        <v>2046</v>
+        <v>2045</v>
       </c>
     </row>
     <row r="391" spans="1:2" x14ac:dyDescent="0.35">
@@ -13615,7 +13615,7 @@
         <v>OptionalInformation</v>
       </c>
       <c r="B391" s="8" t="s">
-        <v>2055</v>
+        <v>2054</v>
       </c>
     </row>
     <row r="392" spans="1:2" x14ac:dyDescent="0.35">
@@ -13623,7 +13623,7 @@
         <v>MyVitaeSlogan</v>
       </c>
       <c r="B392" s="8" t="s">
-        <v>2061</v>
+        <v>2060</v>
       </c>
     </row>
     <row r="393" spans="1:2" x14ac:dyDescent="0.35">
@@ -13631,7 +13631,7 @@
         <v>DownloadQR</v>
       </c>
       <c r="B393" s="8" t="s">
-        <v>2067</v>
+        <v>2066</v>
       </c>
     </row>
     <row r="394" spans="1:2" x14ac:dyDescent="0.35">
@@ -14329,7 +14329,7 @@
         <v>AdTextB0</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>2072</v>
+        <v>2071</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.35">
@@ -14801,7 +14801,7 @@
         <v>CopyrightLawText</v>
       </c>
       <c r="B78" s="3" t="s">
-        <v>2104</v>
+        <v>2103</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.35">
@@ -14937,7 +14937,7 @@
         <v>DashboardOverview</v>
       </c>
       <c r="B95" s="3" t="s">
-        <v>2078</v>
+        <v>2077</v>
       </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.35">
@@ -16521,7 +16521,7 @@
         <v>SavePublicationsDescription</v>
       </c>
       <c r="B293" s="3" t="s">
-        <v>2082</v>
+        <v>2081</v>
       </c>
     </row>
     <row r="294" spans="1:2" x14ac:dyDescent="0.35">
@@ -16609,7 +16609,7 @@
         <v>ShowYourStrengthsDescription</v>
       </c>
       <c r="B304" s="3" t="s">
-        <v>2087</v>
+        <v>2086</v>
       </c>
     </row>
     <row r="305" spans="1:2" x14ac:dyDescent="0.35">
@@ -16977,7 +16977,7 @@
         <v>WhyMyVitaeReason</v>
       </c>
       <c r="B350" s="3" t="s">
-        <v>2094</v>
+        <v>2093</v>
       </c>
     </row>
     <row r="351" spans="1:2" x14ac:dyDescent="0.35">
@@ -17113,7 +17113,7 @@
         <v>Status500</v>
       </c>
       <c r="B367" s="3" t="s">
-        <v>2109</v>
+        <v>2108</v>
       </c>
     </row>
     <row r="368" spans="1:2" x14ac:dyDescent="0.35">
@@ -17177,7 +17177,7 @@
         <v>DataCollectionDesc</v>
       </c>
       <c r="B375" s="3" t="s">
-        <v>2099</v>
+        <v>2098</v>
       </c>
     </row>
     <row r="376" spans="1:2" x14ac:dyDescent="0.35">
@@ -17241,7 +17241,7 @@
         <v>LinkExperience</v>
       </c>
       <c r="B383" s="3" t="s">
-        <v>2022</v>
+        <v>2021</v>
       </c>
     </row>
     <row r="384" spans="1:2" x14ac:dyDescent="0.35">
@@ -17249,7 +17249,7 @@
         <v>LinkEducation</v>
       </c>
       <c r="B384" s="3" t="s">
-        <v>2023</v>
+        <v>2022</v>
       </c>
     </row>
     <row r="385" spans="1:2" x14ac:dyDescent="0.35">
@@ -17257,7 +17257,7 @@
         <v>LinkInterest</v>
       </c>
       <c r="B385" s="3" t="s">
-        <v>2024</v>
+        <v>2023</v>
       </c>
     </row>
     <row r="386" spans="1:2" x14ac:dyDescent="0.35">
@@ -17265,7 +17265,7 @@
         <v>LinkAwards</v>
       </c>
       <c r="B386" s="3" t="s">
-        <v>2025</v>
+        <v>2024</v>
       </c>
     </row>
     <row r="387" spans="1:2" x14ac:dyDescent="0.35">
@@ -17273,7 +17273,7 @@
         <v>LinkCertificate</v>
       </c>
       <c r="B387" s="3" t="s">
-        <v>2026</v>
+        <v>2025</v>
       </c>
     </row>
     <row r="388" spans="1:2" x14ac:dyDescent="0.35">
@@ -17281,7 +17281,7 @@
         <v>LinkReference</v>
       </c>
       <c r="B388" s="3" t="s">
-        <v>2027</v>
+        <v>2026</v>
       </c>
     </row>
     <row r="389" spans="1:2" x14ac:dyDescent="0.35">
@@ -17289,7 +17289,7 @@
         <v>ChronologicalAsc</v>
       </c>
       <c r="B389" s="3" t="s">
-        <v>2052</v>
+        <v>2051</v>
       </c>
     </row>
     <row r="390" spans="1:2" x14ac:dyDescent="0.35">
@@ -17297,7 +17297,7 @@
         <v>ChronologicalDesc</v>
       </c>
       <c r="B390" s="3" t="s">
-        <v>2047</v>
+        <v>2046</v>
       </c>
     </row>
     <row r="391" spans="1:2" x14ac:dyDescent="0.35">
@@ -17305,7 +17305,7 @@
         <v>OptionalInformation</v>
       </c>
       <c r="B391" s="3" t="s">
-        <v>2056</v>
+        <v>2055</v>
       </c>
     </row>
     <row r="392" spans="1:2" x14ac:dyDescent="0.35">
@@ -17313,7 +17313,7 @@
         <v>MyVitaeSlogan</v>
       </c>
       <c r="B392" s="3" t="s">
-        <v>2060</v>
+        <v>2059</v>
       </c>
     </row>
     <row r="393" spans="1:2" x14ac:dyDescent="0.35">
@@ -17321,7 +17321,7 @@
         <v>DownloadQR</v>
       </c>
       <c r="B393" s="3" t="s">
-        <v>2068</v>
+        <v>2067</v>
       </c>
     </row>
     <row r="394" spans="1:2" x14ac:dyDescent="0.35">
@@ -18018,7 +18018,7 @@
         <v>AdTextB0</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>2073</v>
+        <v>2072</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.35">
@@ -18490,7 +18490,7 @@
         <v>CopyrightLawText</v>
       </c>
       <c r="B78" s="3" t="s">
-        <v>2105</v>
+        <v>2104</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.35">
@@ -18626,7 +18626,7 @@
         <v>DashboardOverview</v>
       </c>
       <c r="B95" s="3" t="s">
-        <v>2079</v>
+        <v>2078</v>
       </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.35">
@@ -20210,7 +20210,7 @@
         <v>SavePublicationsDescription</v>
       </c>
       <c r="B293" s="3" t="s">
-        <v>2083</v>
+        <v>2082</v>
       </c>
     </row>
     <row r="294" spans="1:2" x14ac:dyDescent="0.35">
@@ -20298,7 +20298,7 @@
         <v>ShowYourStrengthsDescription</v>
       </c>
       <c r="B304" s="3" t="s">
-        <v>2088</v>
+        <v>2087</v>
       </c>
     </row>
     <row r="305" spans="1:2" x14ac:dyDescent="0.35">
@@ -20666,7 +20666,7 @@
         <v>WhyMyVitaeReason</v>
       </c>
       <c r="B350" s="3" t="s">
-        <v>2095</v>
+        <v>2094</v>
       </c>
     </row>
     <row r="351" spans="1:2" x14ac:dyDescent="0.35">
@@ -20802,7 +20802,7 @@
         <v>Status500</v>
       </c>
       <c r="B367" s="3" t="s">
-        <v>2110</v>
+        <v>2109</v>
       </c>
     </row>
     <row r="368" spans="1:2" x14ac:dyDescent="0.35">
@@ -20866,7 +20866,7 @@
         <v>DataCollectionDesc</v>
       </c>
       <c r="B375" s="3" t="s">
-        <v>2100</v>
+        <v>2099</v>
       </c>
     </row>
     <row r="376" spans="1:2" x14ac:dyDescent="0.35">
@@ -20930,7 +20930,7 @@
         <v>LinkExperience</v>
       </c>
       <c r="B383" s="3" t="s">
-        <v>2028</v>
+        <v>2027</v>
       </c>
     </row>
     <row r="384" spans="1:2" x14ac:dyDescent="0.35">
@@ -20938,7 +20938,7 @@
         <v>LinkEducation</v>
       </c>
       <c r="B384" s="3" t="s">
-        <v>2029</v>
+        <v>2028</v>
       </c>
     </row>
     <row r="385" spans="1:2" x14ac:dyDescent="0.35">
@@ -20946,7 +20946,7 @@
         <v>LinkInterest</v>
       </c>
       <c r="B385" s="3" t="s">
-        <v>2030</v>
+        <v>2029</v>
       </c>
     </row>
     <row r="386" spans="1:2" x14ac:dyDescent="0.35">
@@ -20954,7 +20954,7 @@
         <v>LinkAwards</v>
       </c>
       <c r="B386" s="3" t="s">
-        <v>2031</v>
+        <v>2030</v>
       </c>
     </row>
     <row r="387" spans="1:2" x14ac:dyDescent="0.35">
@@ -20962,7 +20962,7 @@
         <v>LinkCertificate</v>
       </c>
       <c r="B387" s="3" t="s">
-        <v>2032</v>
+        <v>2031</v>
       </c>
     </row>
     <row r="388" spans="1:2" x14ac:dyDescent="0.35">
@@ -20970,7 +20970,7 @@
         <v>LinkReference</v>
       </c>
       <c r="B388" s="3" t="s">
-        <v>2033</v>
+        <v>2032</v>
       </c>
     </row>
     <row r="389" spans="1:2" x14ac:dyDescent="0.35">
@@ -20978,7 +20978,7 @@
         <v>ChronologicalAsc</v>
       </c>
       <c r="B389" s="3" t="s">
-        <v>2051</v>
+        <v>2050</v>
       </c>
     </row>
     <row r="390" spans="1:2" x14ac:dyDescent="0.35">
@@ -20986,7 +20986,7 @@
         <v>ChronologicalDesc</v>
       </c>
       <c r="B390" s="3" t="s">
-        <v>2048</v>
+        <v>2047</v>
       </c>
     </row>
     <row r="391" spans="1:2" x14ac:dyDescent="0.35">
@@ -20994,7 +20994,7 @@
         <v>OptionalInformation</v>
       </c>
       <c r="B391" s="3" t="s">
-        <v>2057</v>
+        <v>2056</v>
       </c>
     </row>
     <row r="392" spans="1:2" x14ac:dyDescent="0.35">
@@ -21002,7 +21002,7 @@
         <v>MyVitaeSlogan</v>
       </c>
       <c r="B392" s="3" t="s">
-        <v>2063</v>
+        <v>2062</v>
       </c>
     </row>
     <row r="393" spans="1:2" x14ac:dyDescent="0.35">
@@ -21010,7 +21010,7 @@
         <v>DownloadQR</v>
       </c>
       <c r="B393" s="3" t="s">
-        <v>2069</v>
+        <v>2068</v>
       </c>
     </row>
     <row r="394" spans="1:2" x14ac:dyDescent="0.35">
@@ -21548,7 +21548,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A8220B7-2614-4C14-91F7-8D47B2A1113F}">
   <dimension ref="A1:B498"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A349" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A379" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B368" sqref="B368"/>
     </sheetView>
   </sheetViews>
@@ -21708,7 +21708,7 @@
         <v>AdTextB0</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>2074</v>
+        <v>2073</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.35">
@@ -22180,7 +22180,7 @@
         <v>CopyrightLawText</v>
       </c>
       <c r="B78" s="3" t="s">
-        <v>2106</v>
+        <v>2105</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.35">
@@ -22316,7 +22316,7 @@
         <v>DashboardOverview</v>
       </c>
       <c r="B95" s="3" t="s">
-        <v>2080</v>
+        <v>2079</v>
       </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.35">
@@ -23900,7 +23900,7 @@
         <v>SavePublicationsDescription</v>
       </c>
       <c r="B293" s="3" t="s">
-        <v>2084</v>
+        <v>2083</v>
       </c>
     </row>
     <row r="294" spans="1:2" x14ac:dyDescent="0.35">
@@ -23988,7 +23988,7 @@
         <v>ShowYourStrengthsDescription</v>
       </c>
       <c r="B304" s="3" t="s">
-        <v>2089</v>
+        <v>2088</v>
       </c>
     </row>
     <row r="305" spans="1:2" x14ac:dyDescent="0.35">
@@ -24356,7 +24356,7 @@
         <v>WhyMyVitaeReason</v>
       </c>
       <c r="B350" s="3" t="s">
-        <v>2096</v>
+        <v>2095</v>
       </c>
     </row>
     <row r="351" spans="1:2" x14ac:dyDescent="0.35">
@@ -24492,7 +24492,7 @@
         <v>Status500</v>
       </c>
       <c r="B367" s="3" t="s">
-        <v>2111</v>
+        <v>2110</v>
       </c>
     </row>
     <row r="368" spans="1:2" x14ac:dyDescent="0.35">
@@ -24556,7 +24556,7 @@
         <v>DataCollectionDesc</v>
       </c>
       <c r="B375" s="3" t="s">
-        <v>2101</v>
+        <v>2100</v>
       </c>
     </row>
     <row r="376" spans="1:2" x14ac:dyDescent="0.35">
@@ -24620,7 +24620,7 @@
         <v>LinkExperience</v>
       </c>
       <c r="B383" s="3" t="s">
-        <v>2034</v>
+        <v>2033</v>
       </c>
     </row>
     <row r="384" spans="1:2" x14ac:dyDescent="0.35">
@@ -24628,7 +24628,7 @@
         <v>LinkEducation</v>
       </c>
       <c r="B384" s="3" t="s">
-        <v>2035</v>
+        <v>2034</v>
       </c>
     </row>
     <row r="385" spans="1:2" x14ac:dyDescent="0.35">
@@ -24636,7 +24636,7 @@
         <v>LinkInterest</v>
       </c>
       <c r="B385" s="3" t="s">
-        <v>2036</v>
+        <v>2035</v>
       </c>
     </row>
     <row r="386" spans="1:2" x14ac:dyDescent="0.35">
@@ -24644,7 +24644,7 @@
         <v>LinkAwards</v>
       </c>
       <c r="B386" s="3" t="s">
-        <v>2037</v>
+        <v>2036</v>
       </c>
     </row>
     <row r="387" spans="1:2" x14ac:dyDescent="0.35">
@@ -24652,7 +24652,7 @@
         <v>LinkCertificate</v>
       </c>
       <c r="B387" s="3" t="s">
-        <v>2038</v>
+        <v>2037</v>
       </c>
     </row>
     <row r="388" spans="1:2" x14ac:dyDescent="0.35">
@@ -24660,7 +24660,7 @@
         <v>LinkReference</v>
       </c>
       <c r="B388" s="3" t="s">
-        <v>2039</v>
+        <v>2038</v>
       </c>
     </row>
     <row r="389" spans="1:2" x14ac:dyDescent="0.35">
@@ -24668,7 +24668,7 @@
         <v>ChronologicalAsc</v>
       </c>
       <c r="B389" s="3" t="s">
-        <v>2050</v>
+        <v>2049</v>
       </c>
     </row>
     <row r="390" spans="1:2" x14ac:dyDescent="0.35">
@@ -24676,7 +24676,7 @@
         <v>ChronologicalDesc</v>
       </c>
       <c r="B390" s="3" t="s">
-        <v>2049</v>
+        <v>2048</v>
       </c>
     </row>
     <row r="391" spans="1:2" x14ac:dyDescent="0.35">
@@ -24684,7 +24684,7 @@
         <v>OptionalInformation</v>
       </c>
       <c r="B391" s="3" t="s">
-        <v>2058</v>
+        <v>2057</v>
       </c>
     </row>
     <row r="392" spans="1:2" x14ac:dyDescent="0.35">
@@ -24692,7 +24692,7 @@
         <v>MyVitaeSlogan</v>
       </c>
       <c r="B392" s="3" t="s">
-        <v>2064</v>
+        <v>2063</v>
       </c>
     </row>
     <row r="393" spans="1:2" x14ac:dyDescent="0.35">
@@ -24700,7 +24700,7 @@
         <v>DownloadQR</v>
       </c>
       <c r="B393" s="3" t="s">
-        <v>2070</v>
+        <v>2069</v>
       </c>
     </row>
     <row r="394" spans="1:2" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Checkbox - click on label added
</commit_message>
<xml_diff>
--- a/Vitae/Library/Resources/SharedResource.xlsx
+++ b/Vitae/Library/Resources/SharedResource.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\Vitae\Library\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{302F4142-2895-475C-94C5-9B4291B5ED91}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98C6F8FC-FF90-49C6-8ED9-BC6089CEDCBE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="30220" windowHeight="19620" tabRatio="406" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -62,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2479" uniqueCount="2129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2484" uniqueCount="2135">
   <si>
     <t>City</t>
   </si>
@@ -6449,6 +6449,24 @@
   </si>
   <si>
     <t>Devi accettare i termini e le condizioni</t>
+  </si>
+  <si>
+    <t>PasswordCheckError</t>
+  </si>
+  <si>
+    <t>Please choose a password that complies with the password guidelines</t>
+  </si>
+  <si>
+    <t>Bitte wählen Sie ein Passwort, das den Passwort-Richtlinien entspricht</t>
+  </si>
+  <si>
+    <t>Veuillez choisir un mot de passe qui respecte les directives relatives aux mots de passe</t>
+  </si>
+  <si>
+    <t>Scegliere una password conforme alle linee guida sulle password</t>
+  </si>
+  <si>
+    <t>Por favor, elija una contraseña que cumpla con las directrices de la contraseña</t>
   </si>
 </sst>
 </file>
@@ -6836,8 +6854,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B499"/>
   <sheetViews>
-    <sheetView topLeftCell="A376" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B399" sqref="B399"/>
+    <sheetView topLeftCell="A383" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A434" sqref="A434:A435"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -10014,9 +10032,12 @@
         <v>2125</v>
       </c>
     </row>
-    <row r="397" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="397" spans="1:2" ht="29" x14ac:dyDescent="0.35">
       <c r="A397" s="5" t="s">
-        <v>1897</v>
+        <v>2129</v>
+      </c>
+      <c r="B397" s="3" t="s">
+        <v>2130</v>
       </c>
     </row>
     <row r="398" spans="1:2" x14ac:dyDescent="0.35">
@@ -13718,9 +13739,12 @@
         <v>2126</v>
       </c>
     </row>
-    <row r="397" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="397" spans="1:2" ht="29" x14ac:dyDescent="0.35">
       <c r="A397" s="5" t="str">
-        <v xml:space="preserve"> </v>
+        <v>PasswordCheckError</v>
+      </c>
+      <c r="B397" s="8" t="s">
+        <v>2131</v>
       </c>
     </row>
     <row r="398" spans="1:2" x14ac:dyDescent="0.35">
@@ -14239,7 +14263,7 @@
   <dimension ref="A1:B498"/>
   <sheetViews>
     <sheetView topLeftCell="A378" workbookViewId="0">
-      <selection activeCell="B396" sqref="B396"/>
+      <selection activeCell="B397" sqref="B397"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -17417,9 +17441,12 @@
         <v>2127</v>
       </c>
     </row>
-    <row r="397" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="397" spans="1:2" ht="29" x14ac:dyDescent="0.35">
       <c r="A397" s="5" t="str">
-        <v xml:space="preserve"> </v>
+        <v>PasswordCheckError</v>
+      </c>
+      <c r="B397" s="3" t="s">
+        <v>2132</v>
       </c>
     </row>
     <row r="398" spans="1:2" x14ac:dyDescent="0.35">
@@ -17936,8 +17963,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{21647760-4677-48F5-BA10-2363314EC080}">
   <dimension ref="A1:B498"/>
   <sheetViews>
-    <sheetView topLeftCell="A380" workbookViewId="0">
-      <selection activeCell="B405" sqref="B404:B405"/>
+    <sheetView topLeftCell="A384" workbookViewId="0">
+      <selection activeCell="B397" sqref="B397"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -21117,7 +21144,10 @@
     </row>
     <row r="397" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A397" s="5" t="str">
-        <v xml:space="preserve"> </v>
+        <v>PasswordCheckError</v>
+      </c>
+      <c r="B397" s="3" t="s">
+        <v>2133</v>
       </c>
     </row>
     <row r="398" spans="1:2" x14ac:dyDescent="0.35">
@@ -21636,7 +21666,7 @@
   <dimension ref="A1:B498"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A384" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B399" sqref="B399"/>
+      <selection activeCell="B406" sqref="B406"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -24814,9 +24844,12 @@
         <v>2127</v>
       </c>
     </row>
-    <row r="397" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="397" spans="1:2" ht="29" x14ac:dyDescent="0.35">
       <c r="A397" s="5" t="str">
-        <v xml:space="preserve"> </v>
+        <v>PasswordCheckError</v>
+      </c>
+      <c r="B397" s="3" t="s">
+        <v>2134</v>
       </c>
     </row>
     <row r="398" spans="1:2" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Small layout for mobile devices
</commit_message>
<xml_diff>
--- a/Vitae/Library/Resources/SharedResource.xlsx
+++ b/Vitae/Library/Resources/SharedResource.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\Vitae\Library\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CED3C068-B564-4E04-94BF-CEC3DCCB6CF0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DD0CD72-CAC3-4576-943E-ADE37D570169}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="30220" windowHeight="19620" tabRatio="406" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2810" yWindow="4260" windowWidth="22500" windowHeight="14280" tabRatio="406" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="en" sheetId="3" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -6265,9 +6265,6 @@
     <t>Der myVitae Lebenslauf wird zusätzlich mit einem Passwort geschützt</t>
   </si>
   <si>
-    <t>Die Sprache in der die myVitae Webseite geladen wird</t>
-  </si>
-  <si>
     <t>myVitae - Ihr online Lebenslauf</t>
   </si>
   <si>
@@ -6298,18 +6295,6 @@
     <t>Asegura tu currículum myVitae con una contraseña adicional</t>
   </si>
   <si>
-    <t>The language in which the myVitae website is loaded</t>
-  </si>
-  <si>
-    <t>La langue dans laquelle le site web myVitae est chargé</t>
-  </si>
-  <si>
-    <t>La lingua in cui è caricato il sito myVitae</t>
-  </si>
-  <si>
-    <t>El idioma en el que se carga el sitio web de myVitae</t>
-  </si>
-  <si>
     <t>myVitae - Your online CV</t>
   </si>
   <si>
@@ -6719,6 +6704,21 @@
   </si>
   <si>
     <t>El currículum creado puede ser enviado a través de un enlace o un código QR generado.</t>
+  </si>
+  <si>
+    <t>Wählen Sie die Sprache Ihres Lebenslaufes aus</t>
+  </si>
+  <si>
+    <t>Select the language of your resume</t>
+  </si>
+  <si>
+    <t>Sélectionnez la langue de votre CV</t>
+  </si>
+  <si>
+    <t>Seleziona la lingua del tuo curriculum vitae</t>
+  </si>
+  <si>
+    <t>Seleccione el idioma de su currículum vitae</t>
   </si>
 </sst>
 </file>
@@ -7106,8 +7106,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B497"/>
   <sheetViews>
-    <sheetView topLeftCell="A382" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B404" sqref="B404"/>
+    <sheetView topLeftCell="A169" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B177" sqref="B177"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -7865,7 +7865,7 @@
         <v>719</v>
       </c>
       <c r="B94" s="1" t="s">
-        <v>2070</v>
+        <v>2069</v>
       </c>
     </row>
     <row r="95" spans="1:2" ht="101.5" x14ac:dyDescent="0.35">
@@ -8089,7 +8089,7 @@
         <v>664</v>
       </c>
       <c r="B122" s="1" t="s">
-        <v>2074</v>
+        <v>2073</v>
       </c>
     </row>
     <row r="123" spans="1:2" x14ac:dyDescent="0.35">
@@ -8529,7 +8529,7 @@
         <v>665</v>
       </c>
       <c r="B177" s="1" t="s">
-        <v>2078</v>
+        <v>2215</v>
       </c>
     </row>
     <row r="178" spans="1:2" x14ac:dyDescent="0.35">
@@ -9081,7 +9081,7 @@
         <v>298</v>
       </c>
       <c r="B246" s="8" t="s">
-        <v>2113</v>
+        <v>2108</v>
       </c>
     </row>
     <row r="247" spans="1:2" x14ac:dyDescent="0.35">
@@ -9089,7 +9089,7 @@
         <v>299</v>
       </c>
       <c r="B247" s="8" t="s">
-        <v>2114</v>
+        <v>2109</v>
       </c>
     </row>
     <row r="248" spans="1:2" x14ac:dyDescent="0.35">
@@ -9097,7 +9097,7 @@
         <v>297</v>
       </c>
       <c r="B248" s="8" t="s">
-        <v>2115</v>
+        <v>2110</v>
       </c>
     </row>
     <row r="249" spans="1:2" x14ac:dyDescent="0.35">
@@ -9105,7 +9105,7 @@
         <v>300</v>
       </c>
       <c r="B249" s="8" t="s">
-        <v>2116</v>
+        <v>2111</v>
       </c>
     </row>
     <row r="250" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
@@ -9113,7 +9113,7 @@
         <v>442</v>
       </c>
       <c r="B250" s="7" t="s">
-        <v>2117</v>
+        <v>2112</v>
       </c>
     </row>
     <row r="251" spans="1:2" x14ac:dyDescent="0.35">
@@ -10249,7 +10249,7 @@
         <v>2017</v>
       </c>
       <c r="B392" s="3" t="s">
-        <v>2082</v>
+        <v>2077</v>
       </c>
     </row>
     <row r="393" spans="1:2" x14ac:dyDescent="0.35">
@@ -10262,146 +10262,146 @@
     </row>
     <row r="394" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A394" s="5" t="s">
-        <v>2086</v>
+        <v>2081</v>
       </c>
       <c r="B394" s="3" t="s">
-        <v>2089</v>
+        <v>2084</v>
       </c>
     </row>
     <row r="395" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A395" s="5" t="s">
-        <v>2088</v>
+        <v>2083</v>
       </c>
       <c r="B395" s="3" t="s">
-        <v>2090</v>
+        <v>2085</v>
       </c>
     </row>
     <row r="396" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A396" s="5" t="s">
-        <v>2098</v>
+        <v>2093</v>
       </c>
       <c r="B396" s="3" t="s">
-        <v>2099</v>
+        <v>2094</v>
       </c>
     </row>
     <row r="397" spans="1:2" ht="29" x14ac:dyDescent="0.35">
       <c r="A397" s="5" t="s">
-        <v>2103</v>
+        <v>2098</v>
       </c>
       <c r="B397" s="3" t="s">
-        <v>2104</v>
+        <v>2099</v>
       </c>
     </row>
     <row r="398" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A398" s="5" t="s">
-        <v>2144</v>
+        <v>2139</v>
       </c>
       <c r="B398" s="3" t="s">
-        <v>2145</v>
+        <v>2140</v>
       </c>
     </row>
     <row r="399" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A399" s="5" t="s">
-        <v>2134</v>
+        <v>2129</v>
       </c>
       <c r="B399" s="3" t="s">
-        <v>2154</v>
+        <v>2149</v>
       </c>
     </row>
     <row r="400" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A400" s="5" t="s">
-        <v>2202</v>
+        <v>2197</v>
       </c>
       <c r="B400" s="3" t="s">
-        <v>2155</v>
+        <v>2150</v>
       </c>
     </row>
     <row r="401" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A401" s="5" t="s">
-        <v>2203</v>
+        <v>2198</v>
       </c>
       <c r="B401" s="3" t="s">
-        <v>2156</v>
+        <v>2151</v>
       </c>
     </row>
     <row r="402" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A402" s="5" t="s">
-        <v>2204</v>
+        <v>2199</v>
       </c>
       <c r="B402" s="3" t="s">
-        <v>2157</v>
+        <v>2152</v>
       </c>
     </row>
     <row r="403" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A403" s="5" t="s">
-        <v>2205</v>
+        <v>2200</v>
       </c>
       <c r="B403" s="3" t="s">
-        <v>2215</v>
+        <v>2210</v>
       </c>
     </row>
     <row r="404" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A404" s="5" t="s">
-        <v>2206</v>
+        <v>2201</v>
       </c>
       <c r="B404" s="3" t="s">
-        <v>2158</v>
+        <v>2153</v>
       </c>
     </row>
     <row r="405" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A405" s="5" t="s">
-        <v>2207</v>
+        <v>2202</v>
       </c>
       <c r="B405" s="3" t="s">
-        <v>2159</v>
+        <v>2154</v>
       </c>
     </row>
     <row r="406" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A406" s="5" t="s">
-        <v>2208</v>
+        <v>2203</v>
       </c>
       <c r="B406" s="3" t="s">
-        <v>2160</v>
+        <v>2155</v>
       </c>
     </row>
     <row r="407" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A407" s="5" t="s">
-        <v>2209</v>
+        <v>2204</v>
       </c>
       <c r="B407" s="3" t="s">
-        <v>2161</v>
+        <v>2156</v>
       </c>
     </row>
     <row r="408" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A408" s="5" t="s">
-        <v>2210</v>
+        <v>2205</v>
       </c>
       <c r="B408" s="3" t="s">
-        <v>2162</v>
+        <v>2157</v>
       </c>
     </row>
     <row r="409" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A409" s="5" t="s">
-        <v>2211</v>
+        <v>2206</v>
       </c>
       <c r="B409" s="3" t="s">
-        <v>2163</v>
+        <v>2158</v>
       </c>
     </row>
     <row r="410" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A410" s="5" t="s">
-        <v>2212</v>
+        <v>2207</v>
       </c>
       <c r="B410" s="3" t="s">
-        <v>2164</v>
+        <v>2159</v>
       </c>
     </row>
     <row r="411" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A411" s="5" t="s">
-        <v>2213</v>
+        <v>2208</v>
       </c>
       <c r="B411" s="3" t="s">
-        <v>2165</v>
+        <v>2160</v>
       </c>
     </row>
     <row r="412" spans="1:2" x14ac:dyDescent="0.35">
@@ -10844,8 +10844,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B496"/>
   <sheetViews>
-    <sheetView topLeftCell="A384" workbookViewId="0">
-      <selection activeCell="B404" sqref="B404"/>
+    <sheetView topLeftCell="A161" workbookViewId="0">
+      <selection activeCell="B177" sqref="B177"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -11604,7 +11604,7 @@
         <v>DashboardDescription</v>
       </c>
       <c r="B94" s="7" t="s">
-        <v>2069</v>
+        <v>2068</v>
       </c>
     </row>
     <row r="95" spans="1:2" ht="130.5" x14ac:dyDescent="0.35">
@@ -12268,7 +12268,7 @@
         <v>LanguageDescription</v>
       </c>
       <c r="B177" s="7" t="s">
-        <v>2067</v>
+        <v>2214</v>
       </c>
     </row>
     <row r="178" spans="1:2" x14ac:dyDescent="0.35">
@@ -12820,7 +12820,7 @@
         <v>PasswordRequiresDigit</v>
       </c>
       <c r="B246" s="8" t="s">
-        <v>2109</v>
+        <v>2104</v>
       </c>
     </row>
     <row r="247" spans="1:2" ht="29" x14ac:dyDescent="0.35">
@@ -12828,7 +12828,7 @@
         <v>PasswordRequiresLower</v>
       </c>
       <c r="B247" s="8" t="s">
-        <v>2133</v>
+        <v>2128</v>
       </c>
     </row>
     <row r="248" spans="1:2" ht="29" x14ac:dyDescent="0.35">
@@ -12836,7 +12836,7 @@
         <v>PasswordRequiresNonAlphanumeric</v>
       </c>
       <c r="B248" s="8" t="s">
-        <v>2111</v>
+        <v>2106</v>
       </c>
     </row>
     <row r="249" spans="1:2" ht="29" x14ac:dyDescent="0.35">
@@ -12844,7 +12844,7 @@
         <v>PasswordRequiresUpper</v>
       </c>
       <c r="B249" s="8" t="s">
-        <v>2110</v>
+        <v>2105</v>
       </c>
     </row>
     <row r="250" spans="1:2" ht="58" x14ac:dyDescent="0.35">
@@ -12852,7 +12852,7 @@
         <v>PasswordRules</v>
       </c>
       <c r="B250" s="7" t="s">
-        <v>2112</v>
+        <v>2107</v>
       </c>
     </row>
     <row r="251" spans="1:2" x14ac:dyDescent="0.35">
@@ -13060,7 +13060,7 @@
         <v>RememberMe</v>
       </c>
       <c r="B276" s="8" t="s">
-        <v>2147</v>
+        <v>2142</v>
       </c>
     </row>
     <row r="277" spans="1:2" x14ac:dyDescent="0.35">
@@ -13988,7 +13988,7 @@
         <v>MyVitaeSlogan</v>
       </c>
       <c r="B392" s="8" t="s">
-        <v>2068</v>
+        <v>2067</v>
       </c>
     </row>
     <row r="393" spans="1:2" x14ac:dyDescent="0.35">
@@ -14004,7 +14004,7 @@
         <v>TermsAndConditions</v>
       </c>
       <c r="B394" s="3" t="s">
-        <v>2087</v>
+        <v>2082</v>
       </c>
     </row>
     <row r="395" spans="1:2" x14ac:dyDescent="0.35">
@@ -14012,7 +14012,7 @@
         <v>TermsAndConditionsDesc</v>
       </c>
       <c r="B395" s="3" t="s">
-        <v>2091</v>
+        <v>2086</v>
       </c>
     </row>
     <row r="396" spans="1:2" x14ac:dyDescent="0.35">
@@ -14020,7 +14020,7 @@
         <v>TermsAndConditionsError</v>
       </c>
       <c r="B396" s="3" t="s">
-        <v>2100</v>
+        <v>2095</v>
       </c>
     </row>
     <row r="397" spans="1:2" ht="29" x14ac:dyDescent="0.35">
@@ -14028,7 +14028,7 @@
         <v>PasswordCheckError</v>
       </c>
       <c r="B397" s="8" t="s">
-        <v>2105</v>
+        <v>2100</v>
       </c>
     </row>
     <row r="398" spans="1:2" x14ac:dyDescent="0.35">
@@ -14036,7 +14036,7 @@
         <v>RememberMeDesc</v>
       </c>
       <c r="B398" s="8" t="s">
-        <v>2146</v>
+        <v>2141</v>
       </c>
     </row>
     <row r="399" spans="1:2" x14ac:dyDescent="0.35">
@@ -14044,7 +14044,7 @@
         <v>QandA</v>
       </c>
       <c r="B399" s="3" t="s">
-        <v>2135</v>
+        <v>2130</v>
       </c>
     </row>
     <row r="400" spans="1:2" x14ac:dyDescent="0.35">
@@ -14052,7 +14052,7 @@
         <v>QandA_Q0</v>
       </c>
       <c r="B400" s="3" t="s">
-        <v>2136</v>
+        <v>2131</v>
       </c>
     </row>
     <row r="401" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
@@ -14060,7 +14060,7 @@
         <v>QandA_A0</v>
       </c>
       <c r="B401" s="3" t="s">
-        <v>2137</v>
+        <v>2132</v>
       </c>
     </row>
     <row r="402" spans="1:2" x14ac:dyDescent="0.35">
@@ -14068,7 +14068,7 @@
         <v>QandA_Q1</v>
       </c>
       <c r="B402" s="3" t="s">
-        <v>2138</v>
+        <v>2133</v>
       </c>
     </row>
     <row r="403" spans="1:2" ht="29" x14ac:dyDescent="0.35">
@@ -14076,7 +14076,7 @@
         <v>QandA_A1</v>
       </c>
       <c r="B403" s="3" t="s">
-        <v>2214</v>
+        <v>2209</v>
       </c>
     </row>
     <row r="404" spans="1:2" ht="29" x14ac:dyDescent="0.35">
@@ -14084,7 +14084,7 @@
         <v>QandA_Q2</v>
       </c>
       <c r="B404" s="3" t="s">
-        <v>2139</v>
+        <v>2134</v>
       </c>
     </row>
     <row r="405" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
@@ -14092,7 +14092,7 @@
         <v>QandA_A2</v>
       </c>
       <c r="B405" s="3" t="s">
-        <v>2140</v>
+        <v>2135</v>
       </c>
     </row>
     <row r="406" spans="1:2" x14ac:dyDescent="0.35">
@@ -14100,7 +14100,7 @@
         <v>QandA_Q3</v>
       </c>
       <c r="B406" s="3" t="s">
-        <v>2141</v>
+        <v>2136</v>
       </c>
     </row>
     <row r="407" spans="1:2" x14ac:dyDescent="0.35">
@@ -14108,7 +14108,7 @@
         <v>QandA_A3</v>
       </c>
       <c r="B407" s="3" t="s">
-        <v>2142</v>
+        <v>2137</v>
       </c>
     </row>
     <row r="408" spans="1:2" x14ac:dyDescent="0.35">
@@ -14116,7 +14116,7 @@
         <v>QandA_Q4</v>
       </c>
       <c r="B408" s="3" t="s">
-        <v>2143</v>
+        <v>2138</v>
       </c>
     </row>
     <row r="409" spans="1:2" ht="29" x14ac:dyDescent="0.35">
@@ -14124,7 +14124,7 @@
         <v>QandA_A4</v>
       </c>
       <c r="B409" s="3" t="s">
-        <v>2151</v>
+        <v>2146</v>
       </c>
     </row>
     <row r="410" spans="1:2" x14ac:dyDescent="0.35">
@@ -14132,7 +14132,7 @@
         <v>QandA_Q5</v>
       </c>
       <c r="B410" s="3" t="s">
-        <v>2152</v>
+        <v>2147</v>
       </c>
     </row>
     <row r="411" spans="1:2" ht="29" x14ac:dyDescent="0.35">
@@ -14140,7 +14140,7 @@
         <v>QandA_A5</v>
       </c>
       <c r="B411" s="3" t="s">
-        <v>2153</v>
+        <v>2148</v>
       </c>
     </row>
     <row r="412" spans="1:2" x14ac:dyDescent="0.35">
@@ -14578,8 +14578,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1802D85A-2FA6-4DB3-A31F-68A2D623BDD9}">
   <dimension ref="A1:B496"/>
   <sheetViews>
-    <sheetView topLeftCell="A384" workbookViewId="0">
-      <selection activeCell="B403" sqref="B403"/>
+    <sheetView topLeftCell="A157" workbookViewId="0">
+      <selection activeCell="B177" sqref="B177"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -15338,7 +15338,7 @@
         <v>DashboardDescription</v>
       </c>
       <c r="B94" s="1" t="s">
-        <v>2071</v>
+        <v>2070</v>
       </c>
     </row>
     <row r="95" spans="1:2" ht="101.5" x14ac:dyDescent="0.35">
@@ -15562,7 +15562,7 @@
         <v>EnablePasswordDescription</v>
       </c>
       <c r="B122" s="1" t="s">
-        <v>2075</v>
+        <v>2074</v>
       </c>
     </row>
     <row r="123" spans="1:2" x14ac:dyDescent="0.35">
@@ -16002,7 +16002,7 @@
         <v>LanguageDescription</v>
       </c>
       <c r="B177" s="1" t="s">
-        <v>2079</v>
+        <v>2216</v>
       </c>
     </row>
     <row r="178" spans="1:2" x14ac:dyDescent="0.35">
@@ -16554,7 +16554,7 @@
         <v>PasswordRequiresDigit</v>
       </c>
       <c r="B246" s="8" t="s">
-        <v>2128</v>
+        <v>2123</v>
       </c>
     </row>
     <row r="247" spans="1:2" x14ac:dyDescent="0.35">
@@ -16562,15 +16562,15 @@
         <v>PasswordRequiresLower</v>
       </c>
       <c r="B247" s="8" t="s">
-        <v>2129</v>
-      </c>
-    </row>
-    <row r="248" spans="1:2" x14ac:dyDescent="0.35">
+        <v>2124</v>
+      </c>
+    </row>
+    <row r="248" spans="1:2" ht="29" x14ac:dyDescent="0.35">
       <c r="A248" s="5" t="str">
         <v>PasswordRequiresNonAlphanumeric</v>
       </c>
       <c r="B248" s="8" t="s">
-        <v>2130</v>
+        <v>2125</v>
       </c>
     </row>
     <row r="249" spans="1:2" x14ac:dyDescent="0.35">
@@ -16578,15 +16578,15 @@
         <v>PasswordRequiresUpper</v>
       </c>
       <c r="B249" s="8" t="s">
-        <v>2131</v>
-      </c>
-    </row>
-    <row r="250" spans="1:2" x14ac:dyDescent="0.35">
+        <v>2126</v>
+      </c>
+    </row>
+    <row r="250" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A250" s="6" t="str">
         <v>PasswordRules</v>
       </c>
       <c r="B250" s="7" t="s">
-        <v>2132</v>
+        <v>2127</v>
       </c>
     </row>
     <row r="251" spans="1:2" x14ac:dyDescent="0.35">
@@ -17722,7 +17722,7 @@
         <v>MyVitaeSlogan</v>
       </c>
       <c r="B392" s="3" t="s">
-        <v>2083</v>
+        <v>2078</v>
       </c>
     </row>
     <row r="393" spans="1:2" x14ac:dyDescent="0.35">
@@ -17738,7 +17738,7 @@
         <v>TermsAndConditions</v>
       </c>
       <c r="B394" s="3" t="s">
-        <v>2092</v>
+        <v>2087</v>
       </c>
     </row>
     <row r="395" spans="1:2" x14ac:dyDescent="0.35">
@@ -17746,7 +17746,7 @@
         <v>TermsAndConditionsDesc</v>
       </c>
       <c r="B395" s="3" t="s">
-        <v>2093</v>
+        <v>2088</v>
       </c>
     </row>
     <row r="396" spans="1:2" x14ac:dyDescent="0.35">
@@ -17754,7 +17754,7 @@
         <v>TermsAndConditionsError</v>
       </c>
       <c r="B396" s="3" t="s">
-        <v>2101</v>
+        <v>2096</v>
       </c>
     </row>
     <row r="397" spans="1:2" ht="29" x14ac:dyDescent="0.35">
@@ -17762,7 +17762,7 @@
         <v>PasswordCheckError</v>
       </c>
       <c r="B397" s="3" t="s">
-        <v>2106</v>
+        <v>2101</v>
       </c>
     </row>
     <row r="398" spans="1:2" x14ac:dyDescent="0.35">
@@ -17770,7 +17770,7 @@
         <v>RememberMeDesc</v>
       </c>
       <c r="B398" s="3" t="s">
-        <v>2148</v>
+        <v>2143</v>
       </c>
     </row>
     <row r="399" spans="1:2" x14ac:dyDescent="0.35">
@@ -17778,7 +17778,7 @@
         <v>QandA</v>
       </c>
       <c r="B399" s="3" t="s">
-        <v>2166</v>
+        <v>2161</v>
       </c>
     </row>
     <row r="400" spans="1:2" x14ac:dyDescent="0.35">
@@ -17786,15 +17786,15 @@
         <v>QandA_Q0</v>
       </c>
       <c r="B400" s="3" t="s">
-        <v>2167</v>
-      </c>
-    </row>
-    <row r="401" spans="1:2" x14ac:dyDescent="0.35">
+        <v>2162</v>
+      </c>
+    </row>
+    <row r="401" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A401" s="5" t="str">
         <v>QandA_A0</v>
       </c>
       <c r="B401" s="3" t="s">
-        <v>2168</v>
+        <v>2163</v>
       </c>
     </row>
     <row r="402" spans="1:2" x14ac:dyDescent="0.35">
@@ -17802,7 +17802,7 @@
         <v>QandA_Q1</v>
       </c>
       <c r="B402" s="3" t="s">
-        <v>2169</v>
+        <v>2164</v>
       </c>
     </row>
     <row r="403" spans="1:2" x14ac:dyDescent="0.35">
@@ -17810,23 +17810,23 @@
         <v>QandA_A1</v>
       </c>
       <c r="B403" s="3" t="s">
-        <v>2216</v>
-      </c>
-    </row>
-    <row r="404" spans="1:2" x14ac:dyDescent="0.35">
+        <v>2211</v>
+      </c>
+    </row>
+    <row r="404" spans="1:2" ht="29" x14ac:dyDescent="0.35">
       <c r="A404" s="5" t="str">
         <v>QandA_Q2</v>
       </c>
       <c r="B404" s="3" t="s">
-        <v>2170</v>
-      </c>
-    </row>
-    <row r="405" spans="1:2" x14ac:dyDescent="0.35">
+        <v>2165</v>
+      </c>
+    </row>
+    <row r="405" spans="1:2" ht="29" x14ac:dyDescent="0.35">
       <c r="A405" s="5" t="str">
         <v>QandA_A2</v>
       </c>
       <c r="B405" s="3" t="s">
-        <v>2171</v>
+        <v>2166</v>
       </c>
     </row>
     <row r="406" spans="1:2" x14ac:dyDescent="0.35">
@@ -17834,7 +17834,7 @@
         <v>QandA_Q3</v>
       </c>
       <c r="B406" s="3" t="s">
-        <v>2172</v>
+        <v>2167</v>
       </c>
     </row>
     <row r="407" spans="1:2" x14ac:dyDescent="0.35">
@@ -17842,7 +17842,7 @@
         <v>QandA_A3</v>
       </c>
       <c r="B407" s="3" t="s">
-        <v>2173</v>
+        <v>2168</v>
       </c>
     </row>
     <row r="408" spans="1:2" x14ac:dyDescent="0.35">
@@ -17850,15 +17850,15 @@
         <v>QandA_Q4</v>
       </c>
       <c r="B408" s="3" t="s">
-        <v>2174</v>
-      </c>
-    </row>
-    <row r="409" spans="1:2" x14ac:dyDescent="0.35">
+        <v>2169</v>
+      </c>
+    </row>
+    <row r="409" spans="1:2" ht="29" x14ac:dyDescent="0.35">
       <c r="A409" s="5" t="str">
         <v>QandA_A4</v>
       </c>
       <c r="B409" s="3" t="s">
-        <v>2175</v>
+        <v>2170</v>
       </c>
     </row>
     <row r="410" spans="1:2" x14ac:dyDescent="0.35">
@@ -17866,15 +17866,15 @@
         <v>QandA_Q5</v>
       </c>
       <c r="B410" s="3" t="s">
-        <v>2176</v>
-      </c>
-    </row>
-    <row r="411" spans="1:2" x14ac:dyDescent="0.35">
+        <v>2171</v>
+      </c>
+    </row>
+    <row r="411" spans="1:2" ht="29" x14ac:dyDescent="0.35">
       <c r="A411" s="5" t="str">
         <v>QandA_A5</v>
       </c>
       <c r="B411" s="3" t="s">
-        <v>2177</v>
+        <v>2172</v>
       </c>
     </row>
     <row r="412" spans="1:2" x14ac:dyDescent="0.35">
@@ -18311,8 +18311,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{21647760-4677-48F5-BA10-2363314EC080}">
   <dimension ref="A1:B496"/>
   <sheetViews>
-    <sheetView topLeftCell="A381" workbookViewId="0">
-      <selection activeCell="B404" sqref="B404"/>
+    <sheetView topLeftCell="A172" workbookViewId="0">
+      <selection activeCell="B177" sqref="B177"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -19071,7 +19071,7 @@
         <v>DashboardDescription</v>
       </c>
       <c r="B94" s="1" t="s">
-        <v>2072</v>
+        <v>2071</v>
       </c>
     </row>
     <row r="95" spans="1:2" ht="101.5" x14ac:dyDescent="0.35">
@@ -19295,7 +19295,7 @@
         <v>EnablePasswordDescription</v>
       </c>
       <c r="B122" s="1" t="s">
-        <v>2076</v>
+        <v>2075</v>
       </c>
     </row>
     <row r="123" spans="1:2" x14ac:dyDescent="0.35">
@@ -19735,7 +19735,7 @@
         <v>LanguageDescription</v>
       </c>
       <c r="B177" s="1" t="s">
-        <v>2080</v>
+        <v>2217</v>
       </c>
     </row>
     <row r="178" spans="1:2" x14ac:dyDescent="0.35">
@@ -20287,7 +20287,7 @@
         <v>PasswordRequiresDigit</v>
       </c>
       <c r="B246" s="8" t="s">
-        <v>2123</v>
+        <v>2118</v>
       </c>
     </row>
     <row r="247" spans="1:2" x14ac:dyDescent="0.35">
@@ -20295,7 +20295,7 @@
         <v>PasswordRequiresLower</v>
       </c>
       <c r="B247" s="8" t="s">
-        <v>2124</v>
+        <v>2119</v>
       </c>
     </row>
     <row r="248" spans="1:2" x14ac:dyDescent="0.35">
@@ -20303,7 +20303,7 @@
         <v>PasswordRequiresNonAlphanumeric</v>
       </c>
       <c r="B248" s="8" t="s">
-        <v>2125</v>
+        <v>2120</v>
       </c>
     </row>
     <row r="249" spans="1:2" x14ac:dyDescent="0.35">
@@ -20311,7 +20311,7 @@
         <v>PasswordRequiresUpper</v>
       </c>
       <c r="B249" s="8" t="s">
-        <v>2126</v>
+        <v>2121</v>
       </c>
     </row>
     <row r="250" spans="1:2" x14ac:dyDescent="0.35">
@@ -20319,7 +20319,7 @@
         <v>PasswordRules</v>
       </c>
       <c r="B250" s="7" t="s">
-        <v>2127</v>
+        <v>2122</v>
       </c>
     </row>
     <row r="251" spans="1:2" x14ac:dyDescent="0.35">
@@ -21455,7 +21455,7 @@
         <v>MyVitaeSlogan</v>
       </c>
       <c r="B392" s="3" t="s">
-        <v>2084</v>
+        <v>2079</v>
       </c>
     </row>
     <row r="393" spans="1:2" x14ac:dyDescent="0.35">
@@ -21471,7 +21471,7 @@
         <v>TermsAndConditions</v>
       </c>
       <c r="B394" s="3" t="s">
-        <v>2094</v>
+        <v>2089</v>
       </c>
     </row>
     <row r="395" spans="1:2" x14ac:dyDescent="0.35">
@@ -21479,7 +21479,7 @@
         <v>TermsAndConditionsDesc</v>
       </c>
       <c r="B395" s="3" t="s">
-        <v>2096</v>
+        <v>2091</v>
       </c>
     </row>
     <row r="396" spans="1:2" x14ac:dyDescent="0.35">
@@ -21487,7 +21487,7 @@
         <v>TermsAndConditionsError</v>
       </c>
       <c r="B396" s="3" t="s">
-        <v>2102</v>
+        <v>2097</v>
       </c>
     </row>
     <row r="397" spans="1:2" x14ac:dyDescent="0.35">
@@ -21495,7 +21495,7 @@
         <v>PasswordCheckError</v>
       </c>
       <c r="B397" s="3" t="s">
-        <v>2107</v>
+        <v>2102</v>
       </c>
     </row>
     <row r="398" spans="1:2" x14ac:dyDescent="0.35">
@@ -21503,7 +21503,7 @@
         <v>RememberMeDesc</v>
       </c>
       <c r="B398" s="3" t="s">
-        <v>2149</v>
+        <v>2144</v>
       </c>
     </row>
     <row r="399" spans="1:2" x14ac:dyDescent="0.35">
@@ -21511,7 +21511,7 @@
         <v>QandA</v>
       </c>
       <c r="B399" s="3" t="s">
-        <v>2178</v>
+        <v>2173</v>
       </c>
     </row>
     <row r="400" spans="1:2" x14ac:dyDescent="0.35">
@@ -21519,15 +21519,15 @@
         <v>QandA_Q0</v>
       </c>
       <c r="B400" s="3" t="s">
-        <v>2179</v>
-      </c>
-    </row>
-    <row r="401" spans="1:2" x14ac:dyDescent="0.35">
+        <v>2174</v>
+      </c>
+    </row>
+    <row r="401" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A401" s="5" t="str">
         <v>QandA_A0</v>
       </c>
       <c r="B401" s="3" t="s">
-        <v>2180</v>
+        <v>2175</v>
       </c>
     </row>
     <row r="402" spans="1:2" x14ac:dyDescent="0.35">
@@ -21535,7 +21535,7 @@
         <v>QandA_Q1</v>
       </c>
       <c r="B402" s="3" t="s">
-        <v>2181</v>
+        <v>2176</v>
       </c>
     </row>
     <row r="403" spans="1:2" ht="29" x14ac:dyDescent="0.35">
@@ -21543,7 +21543,7 @@
         <v>QandA_A1</v>
       </c>
       <c r="B403" s="3" t="s">
-        <v>2217</v>
+        <v>2212</v>
       </c>
     </row>
     <row r="404" spans="1:2" x14ac:dyDescent="0.35">
@@ -21551,15 +21551,15 @@
         <v>QandA_Q2</v>
       </c>
       <c r="B404" s="3" t="s">
-        <v>2182</v>
-      </c>
-    </row>
-    <row r="405" spans="1:2" x14ac:dyDescent="0.35">
+        <v>2177</v>
+      </c>
+    </row>
+    <row r="405" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A405" s="5" t="str">
         <v>QandA_A2</v>
       </c>
       <c r="B405" s="3" t="s">
-        <v>2183</v>
+        <v>2178</v>
       </c>
     </row>
     <row r="406" spans="1:2" x14ac:dyDescent="0.35">
@@ -21567,7 +21567,7 @@
         <v>QandA_Q3</v>
       </c>
       <c r="B406" s="3" t="s">
-        <v>2184</v>
+        <v>2179</v>
       </c>
     </row>
     <row r="407" spans="1:2" x14ac:dyDescent="0.35">
@@ -21575,7 +21575,7 @@
         <v>QandA_A3</v>
       </c>
       <c r="B407" s="3" t="s">
-        <v>2185</v>
+        <v>2180</v>
       </c>
     </row>
     <row r="408" spans="1:2" x14ac:dyDescent="0.35">
@@ -21583,7 +21583,7 @@
         <v>QandA_Q4</v>
       </c>
       <c r="B408" s="3" t="s">
-        <v>2186</v>
+        <v>2181</v>
       </c>
     </row>
     <row r="409" spans="1:2" x14ac:dyDescent="0.35">
@@ -21591,7 +21591,7 @@
         <v>QandA_A4</v>
       </c>
       <c r="B409" s="3" t="s">
-        <v>2187</v>
+        <v>2182</v>
       </c>
     </row>
     <row r="410" spans="1:2" x14ac:dyDescent="0.35">
@@ -21599,7 +21599,7 @@
         <v>QandA_Q5</v>
       </c>
       <c r="B410" s="3" t="s">
-        <v>2188</v>
+        <v>2183</v>
       </c>
     </row>
     <row r="411" spans="1:2" x14ac:dyDescent="0.35">
@@ -21607,7 +21607,7 @@
         <v>QandA_A5</v>
       </c>
       <c r="B411" s="3" t="s">
-        <v>2189</v>
+        <v>2184</v>
       </c>
     </row>
     <row r="412" spans="1:2" x14ac:dyDescent="0.35">
@@ -22045,8 +22045,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A8220B7-2614-4C14-91F7-8D47B2A1113F}">
   <dimension ref="A1:B496"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A380" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B404" sqref="B404"/>
+    <sheetView tabSelected="1" topLeftCell="A173" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B177" sqref="B177"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -22805,7 +22805,7 @@
         <v>DashboardDescription</v>
       </c>
       <c r="B94" s="1" t="s">
-        <v>2073</v>
+        <v>2072</v>
       </c>
     </row>
     <row r="95" spans="1:2" ht="101.5" x14ac:dyDescent="0.35">
@@ -23029,7 +23029,7 @@
         <v>EnablePasswordDescription</v>
       </c>
       <c r="B122" s="1" t="s">
-        <v>2077</v>
+        <v>2076</v>
       </c>
     </row>
     <row r="123" spans="1:2" x14ac:dyDescent="0.35">
@@ -23469,7 +23469,7 @@
         <v>LanguageDescription</v>
       </c>
       <c r="B177" s="1" t="s">
-        <v>2081</v>
+        <v>2218</v>
       </c>
     </row>
     <row r="178" spans="1:2" x14ac:dyDescent="0.35">
@@ -24021,7 +24021,7 @@
         <v>PasswordRequiresDigit</v>
       </c>
       <c r="B246" s="8" t="s">
-        <v>2118</v>
+        <v>2113</v>
       </c>
     </row>
     <row r="247" spans="1:2" x14ac:dyDescent="0.35">
@@ -24029,15 +24029,15 @@
         <v>PasswordRequiresLower</v>
       </c>
       <c r="B247" s="8" t="s">
-        <v>2119</v>
-      </c>
-    </row>
-    <row r="248" spans="1:2" x14ac:dyDescent="0.35">
+        <v>2114</v>
+      </c>
+    </row>
+    <row r="248" spans="1:2" ht="29" x14ac:dyDescent="0.35">
       <c r="A248" s="5" t="str">
         <v>PasswordRequiresNonAlphanumeric</v>
       </c>
       <c r="B248" s="8" t="s">
-        <v>2120</v>
+        <v>2115</v>
       </c>
     </row>
     <row r="249" spans="1:2" x14ac:dyDescent="0.35">
@@ -24045,15 +24045,15 @@
         <v>PasswordRequiresUpper</v>
       </c>
       <c r="B249" s="8" t="s">
-        <v>2121</v>
-      </c>
-    </row>
-    <row r="250" spans="1:2" x14ac:dyDescent="0.35">
+        <v>2116</v>
+      </c>
+    </row>
+    <row r="250" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A250" s="6" t="str">
         <v>PasswordRules</v>
       </c>
       <c r="B250" s="7" t="s">
-        <v>2122</v>
+        <v>2117</v>
       </c>
     </row>
     <row r="251" spans="1:2" x14ac:dyDescent="0.35">
@@ -25189,7 +25189,7 @@
         <v>MyVitaeSlogan</v>
       </c>
       <c r="B392" s="3" t="s">
-        <v>2085</v>
+        <v>2080</v>
       </c>
     </row>
     <row r="393" spans="1:2" x14ac:dyDescent="0.35">
@@ -25205,7 +25205,7 @@
         <v>TermsAndConditions</v>
       </c>
       <c r="B394" s="3" t="s">
-        <v>2097</v>
+        <v>2092</v>
       </c>
     </row>
     <row r="395" spans="1:2" x14ac:dyDescent="0.35">
@@ -25213,7 +25213,7 @@
         <v>TermsAndConditionsDesc</v>
       </c>
       <c r="B395" s="3" t="s">
-        <v>2095</v>
+        <v>2090</v>
       </c>
     </row>
     <row r="396" spans="1:2" x14ac:dyDescent="0.35">
@@ -25221,7 +25221,7 @@
         <v>TermsAndConditionsError</v>
       </c>
       <c r="B396" s="3" t="s">
-        <v>2101</v>
+        <v>2096</v>
       </c>
     </row>
     <row r="397" spans="1:2" ht="29" x14ac:dyDescent="0.35">
@@ -25229,7 +25229,7 @@
         <v>PasswordCheckError</v>
       </c>
       <c r="B397" s="3" t="s">
-        <v>2108</v>
+        <v>2103</v>
       </c>
     </row>
     <row r="398" spans="1:2" x14ac:dyDescent="0.35">
@@ -25237,7 +25237,7 @@
         <v>RememberMeDesc</v>
       </c>
       <c r="B398" s="3" t="s">
-        <v>2150</v>
+        <v>2145</v>
       </c>
     </row>
     <row r="399" spans="1:2" x14ac:dyDescent="0.35">
@@ -25245,7 +25245,7 @@
         <v>QandA</v>
       </c>
       <c r="B399" s="3" t="s">
-        <v>2190</v>
+        <v>2185</v>
       </c>
     </row>
     <row r="400" spans="1:2" x14ac:dyDescent="0.35">
@@ -25253,15 +25253,15 @@
         <v>QandA_Q0</v>
       </c>
       <c r="B400" s="3" t="s">
-        <v>2191</v>
-      </c>
-    </row>
-    <row r="401" spans="1:2" x14ac:dyDescent="0.35">
+        <v>2186</v>
+      </c>
+    </row>
+    <row r="401" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A401" s="5" t="str">
         <v>QandA_A0</v>
       </c>
       <c r="B401" s="3" t="s">
-        <v>2192</v>
+        <v>2187</v>
       </c>
     </row>
     <row r="402" spans="1:2" x14ac:dyDescent="0.35">
@@ -25269,7 +25269,7 @@
         <v>QandA_Q1</v>
       </c>
       <c r="B402" s="3" t="s">
-        <v>2193</v>
+        <v>2188</v>
       </c>
     </row>
     <row r="403" spans="1:2" ht="29" x14ac:dyDescent="0.35">
@@ -25277,23 +25277,23 @@
         <v>QandA_A1</v>
       </c>
       <c r="B403" s="3" t="s">
-        <v>2218</v>
-      </c>
-    </row>
-    <row r="404" spans="1:2" x14ac:dyDescent="0.35">
+        <v>2213</v>
+      </c>
+    </row>
+    <row r="404" spans="1:2" ht="29" x14ac:dyDescent="0.35">
       <c r="A404" s="5" t="str">
         <v>QandA_Q2</v>
       </c>
       <c r="B404" s="3" t="s">
-        <v>2194</v>
-      </c>
-    </row>
-    <row r="405" spans="1:2" x14ac:dyDescent="0.35">
+        <v>2189</v>
+      </c>
+    </row>
+    <row r="405" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A405" s="5" t="str">
         <v>QandA_A2</v>
       </c>
       <c r="B405" s="3" t="s">
-        <v>2195</v>
+        <v>2190</v>
       </c>
     </row>
     <row r="406" spans="1:2" x14ac:dyDescent="0.35">
@@ -25301,7 +25301,7 @@
         <v>QandA_Q3</v>
       </c>
       <c r="B406" s="3" t="s">
-        <v>2196</v>
+        <v>2191</v>
       </c>
     </row>
     <row r="407" spans="1:2" x14ac:dyDescent="0.35">
@@ -25309,7 +25309,7 @@
         <v>QandA_A3</v>
       </c>
       <c r="B407" s="3" t="s">
-        <v>2197</v>
+        <v>2192</v>
       </c>
     </row>
     <row r="408" spans="1:2" x14ac:dyDescent="0.35">
@@ -25317,15 +25317,15 @@
         <v>QandA_Q4</v>
       </c>
       <c r="B408" s="3" t="s">
-        <v>2198</v>
-      </c>
-    </row>
-    <row r="409" spans="1:2" x14ac:dyDescent="0.35">
+        <v>2193</v>
+      </c>
+    </row>
+    <row r="409" spans="1:2" ht="29" x14ac:dyDescent="0.35">
       <c r="A409" s="5" t="str">
         <v>QandA_A4</v>
       </c>
       <c r="B409" s="3" t="s">
-        <v>2199</v>
+        <v>2194</v>
       </c>
     </row>
     <row r="410" spans="1:2" x14ac:dyDescent="0.35">
@@ -25333,15 +25333,15 @@
         <v>QandA_Q5</v>
       </c>
       <c r="B410" s="3" t="s">
-        <v>2200</v>
-      </c>
-    </row>
-    <row r="411" spans="1:2" x14ac:dyDescent="0.35">
+        <v>2195</v>
+      </c>
+    </row>
+    <row r="411" spans="1:2" ht="29" x14ac:dyDescent="0.35">
       <c r="A411" s="5" t="str">
         <v>QandA_A5</v>
       </c>
       <c r="B411" s="3" t="s">
-        <v>2201</v>
+        <v>2196</v>
       </c>
     </row>
     <row r="412" spans="1:2" x14ac:dyDescent="0.35">

</xml_diff>